<commit_message>
GH ACTION Autorun Mon Mar 27 15:02:38 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7AE8BC1-6E2B-48AD-A2CE-CA49C93B660D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FCF3877-FED3-4087-9AE7-F9D8309639B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -218,7 +218,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -22783,7 +22782,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
+      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23197,22 +23196,22 @@
         <v>5508</v>
       </c>
       <c r="G5" s="19">
-        <v>6253</v>
+        <v>6226</v>
       </c>
       <c r="H5" s="19">
-        <v>6047</v>
+        <v>6020</v>
       </c>
       <c r="I5" s="19">
-        <v>5693</v>
+        <v>5672</v>
       </c>
       <c r="J5" s="19">
-        <v>6136</v>
+        <v>6110</v>
       </c>
       <c r="K5" s="19">
-        <v>6488</v>
+        <v>6443</v>
       </c>
       <c r="L5" s="19">
-        <v>6206</v>
+        <v>6189</v>
       </c>
       <c r="M5" s="19">
         <v>6681</v>
@@ -23358,22 +23357,22 @@
         <v>11679</v>
       </c>
       <c r="G6" s="19">
-        <v>12639</v>
+        <v>12642</v>
       </c>
       <c r="H6" s="19">
-        <v>12733</v>
+        <v>12720</v>
       </c>
       <c r="I6" s="19">
-        <v>12053</v>
+        <v>12050</v>
       </c>
       <c r="J6" s="19">
-        <v>12553</v>
+        <v>12551</v>
       </c>
       <c r="K6" s="19">
-        <v>12246</v>
+        <v>12215</v>
       </c>
       <c r="L6" s="19">
-        <v>13260</v>
+        <v>13213</v>
       </c>
       <c r="M6" s="19">
         <v>13285</v>
@@ -23519,22 +23518,22 @@
         <v>17585</v>
       </c>
       <c r="G7" s="19">
-        <v>15583</v>
+        <v>16226</v>
       </c>
       <c r="H7" s="19">
-        <v>16537</v>
+        <v>17051</v>
       </c>
       <c r="I7" s="19">
-        <v>15018</v>
+        <v>15660</v>
       </c>
       <c r="J7" s="19">
-        <v>15881</v>
+        <v>16431</v>
       </c>
       <c r="K7" s="19">
-        <v>15615</v>
+        <v>16066</v>
       </c>
       <c r="L7" s="19">
-        <v>17259</v>
+        <v>17751</v>
       </c>
       <c r="M7" s="19">
         <v>18790</v>
@@ -23680,22 +23679,22 @@
         <v>2931</v>
       </c>
       <c r="G8" s="19">
-        <v>3860</v>
+        <v>3859</v>
       </c>
       <c r="H8" s="19">
-        <v>3469</v>
+        <v>3467</v>
       </c>
       <c r="I8" s="19">
-        <v>3670</v>
+        <v>3647</v>
       </c>
       <c r="J8" s="19">
-        <v>3912</v>
+        <v>3908</v>
       </c>
       <c r="K8" s="19">
-        <v>4428</v>
+        <v>4421</v>
       </c>
       <c r="L8" s="19">
-        <v>4346</v>
+        <v>4302</v>
       </c>
       <c r="M8" s="19">
         <v>4360</v>
@@ -23841,22 +23840,22 @@
         <v>10264</v>
       </c>
       <c r="G9" s="19">
-        <v>10029</v>
+        <v>10039</v>
       </c>
       <c r="H9" s="19">
-        <v>9490</v>
+        <v>9397</v>
       </c>
       <c r="I9" s="19">
-        <v>9113</v>
+        <v>8962</v>
       </c>
       <c r="J9" s="19">
-        <v>9801</v>
+        <v>9699</v>
       </c>
       <c r="K9" s="19">
-        <v>9899</v>
+        <v>9906</v>
       </c>
       <c r="L9" s="19">
-        <v>10253</v>
+        <v>10354</v>
       </c>
       <c r="M9" s="19">
         <v>9570</v>
@@ -24002,22 +24001,22 @@
         <v>9751</v>
       </c>
       <c r="G10" s="19">
-        <v>11667</v>
+        <v>11629</v>
       </c>
       <c r="H10" s="19">
-        <v>11366</v>
+        <v>11309</v>
       </c>
       <c r="I10" s="19">
-        <v>11935</v>
+        <v>11911</v>
       </c>
       <c r="J10" s="19">
-        <v>12070</v>
+        <v>12004</v>
       </c>
       <c r="K10" s="19">
-        <v>11514</v>
+        <v>11457</v>
       </c>
       <c r="L10" s="19">
-        <v>11442</v>
+        <v>11274</v>
       </c>
       <c r="M10" s="19">
         <v>13104</v>
@@ -24163,22 +24162,22 @@
         <v>43312</v>
       </c>
       <c r="G11" s="19">
-        <v>48157</v>
+        <v>48030</v>
       </c>
       <c r="H11" s="19">
-        <v>44092</v>
+        <v>43862</v>
       </c>
       <c r="I11" s="19">
-        <v>44123</v>
+        <v>43943</v>
       </c>
       <c r="J11" s="19">
-        <v>45882</v>
+        <v>45648</v>
       </c>
       <c r="K11" s="19">
-        <v>48859</v>
+        <v>48738</v>
       </c>
       <c r="L11" s="19">
-        <v>48325</v>
+        <v>48228</v>
       </c>
       <c r="M11" s="19">
         <v>52249</v>
@@ -24324,22 +24323,22 @@
         <v>101030</v>
       </c>
       <c r="G12" s="8">
-        <v>108188</v>
+        <v>108651</v>
       </c>
       <c r="H12" s="8">
-        <v>103734</v>
+        <v>103826</v>
       </c>
       <c r="I12" s="8">
-        <v>101605</v>
+        <v>101845</v>
       </c>
       <c r="J12" s="8">
-        <v>106235</v>
+        <v>106351</v>
       </c>
       <c r="K12" s="8">
-        <v>109049</v>
+        <v>109246</v>
       </c>
       <c r="L12" s="8">
-        <v>111091</v>
+        <v>111311</v>
       </c>
       <c r="M12" s="8">
         <v>118039</v>
@@ -24545,22 +24544,22 @@
         <v>393.62405899999999</v>
       </c>
       <c r="G15" s="19">
-        <v>450.820018</v>
+        <v>444.64685100000003</v>
       </c>
       <c r="H15" s="19">
-        <v>447.72801800000002</v>
+        <v>444.742188</v>
       </c>
       <c r="I15" s="19">
-        <v>414.59192100000001</v>
+        <v>413.33797600000003</v>
       </c>
       <c r="J15" s="19">
-        <v>459.80381399999999</v>
+        <v>454.99206600000002</v>
       </c>
       <c r="K15" s="19">
-        <v>497.84569599999998</v>
+        <v>490.41384399999998</v>
       </c>
       <c r="L15" s="19">
-        <v>488.80336699999998</v>
+        <v>487.29230899999999</v>
       </c>
       <c r="M15" s="19">
         <v>486.02968099999998</v>
@@ -24706,22 +24705,22 @@
         <v>829.83137099999999</v>
       </c>
       <c r="G16" s="19">
-        <v>904.29075799999998</v>
+        <v>906.57213899999999</v>
       </c>
       <c r="H16" s="19">
-        <v>910.93795999999998</v>
+        <v>909.75543600000003</v>
       </c>
       <c r="I16" s="19">
-        <v>878.56402100000003</v>
+        <v>879.67446500000005</v>
       </c>
       <c r="J16" s="19">
-        <v>912.45517299999995</v>
+        <v>912.27808300000004</v>
       </c>
       <c r="K16" s="19">
-        <v>924.61321299999997</v>
+        <v>920.15350999999998</v>
       </c>
       <c r="L16" s="19">
-        <v>969.13955299999998</v>
+        <v>962.79300899999998</v>
       </c>
       <c r="M16" s="19">
         <v>1028.381367</v>
@@ -24867,22 +24866,22 @@
         <v>454.22706899999997</v>
       </c>
       <c r="G17" s="19">
-        <v>476.22017899999997</v>
+        <v>474.906656</v>
       </c>
       <c r="H17" s="19">
-        <v>483.82499000000001</v>
+        <v>480.75027599999999</v>
       </c>
       <c r="I17" s="19">
-        <v>419.58892700000001</v>
+        <v>421.68528900000001</v>
       </c>
       <c r="J17" s="19">
-        <v>421.21861999999999</v>
+        <v>420.55377399999998</v>
       </c>
       <c r="K17" s="19">
-        <v>613.24761799999999</v>
+        <v>611.49292100000002</v>
       </c>
       <c r="L17" s="19">
-        <v>599.86068699999998</v>
+        <v>600.02689799999996</v>
       </c>
       <c r="M17" s="19">
         <v>580.71005000000002</v>
@@ -25028,22 +25027,22 @@
         <v>41.082461000000002</v>
       </c>
       <c r="G18" s="19">
-        <v>50.463282999999997</v>
+        <v>50.502921999999998</v>
       </c>
       <c r="H18" s="19">
-        <v>45.759475000000002</v>
+        <v>45.840166000000004</v>
       </c>
       <c r="I18" s="19">
-        <v>49.884833</v>
+        <v>46.436680000000003</v>
       </c>
       <c r="J18" s="19">
-        <v>52.567118000000001</v>
+        <v>52.560735999999999</v>
       </c>
       <c r="K18" s="19">
-        <v>58.288364999999999</v>
+        <v>58.026294</v>
       </c>
       <c r="L18" s="19">
-        <v>61.949061999999998</v>
+        <v>59.000740999999998</v>
       </c>
       <c r="M18" s="19">
         <v>61.228952999999997</v>
@@ -25189,22 +25188,22 @@
         <v>478.77222599999999</v>
       </c>
       <c r="G19" s="19">
-        <v>415.86830800000001</v>
+        <v>416.71331800000002</v>
       </c>
       <c r="H19" s="19">
-        <v>406.75820399999998</v>
+        <v>407.08307400000001</v>
       </c>
       <c r="I19" s="19">
-        <v>434.88865800000002</v>
+        <v>429.830399</v>
       </c>
       <c r="J19" s="19">
-        <v>453.39728700000001</v>
+        <v>454.415887</v>
       </c>
       <c r="K19" s="19">
-        <v>460.313197</v>
+        <v>460.30514899999997</v>
       </c>
       <c r="L19" s="19">
-        <v>463.62496099999998</v>
+        <v>467.89076899999998</v>
       </c>
       <c r="M19" s="19">
         <v>458.70701600000001</v>
@@ -25350,22 +25349,22 @@
         <v>901.81813699999998</v>
       </c>
       <c r="G20" s="19">
-        <v>1104.7375549999999</v>
+        <v>1106.46489</v>
       </c>
       <c r="H20" s="19">
-        <v>1052.6195700000001</v>
+        <v>1042.170805</v>
       </c>
       <c r="I20" s="19">
-        <v>1128.0979540000001</v>
+        <v>1122.6850159999999</v>
       </c>
       <c r="J20" s="19">
-        <v>1119.989511</v>
+        <v>1110.185884</v>
       </c>
       <c r="K20" s="19">
-        <v>1013.933806</v>
+        <v>1006.878017</v>
       </c>
       <c r="L20" s="19">
-        <v>1123.181192</v>
+        <v>1108.8886480000001</v>
       </c>
       <c r="M20" s="19">
         <v>1244.1288970000001</v>
@@ -25511,22 +25510,22 @@
         <v>984.305296</v>
       </c>
       <c r="G21" s="19">
-        <v>1051.9346680000001</v>
+        <v>1049.732385</v>
       </c>
       <c r="H21" s="19">
-        <v>1005.6013809999999</v>
+        <v>1003.817105</v>
       </c>
       <c r="I21" s="19">
-        <v>1029.321117</v>
+        <v>1028.636387</v>
       </c>
       <c r="J21" s="19">
-        <v>1102.519137</v>
+        <v>1100.134667</v>
       </c>
       <c r="K21" s="19">
-        <v>1110.381363</v>
+        <v>1108.276386</v>
       </c>
       <c r="L21" s="19">
-        <v>1128.9865460000001</v>
+        <v>1126.500579</v>
       </c>
       <c r="M21" s="19">
         <v>1229.6877569999999</v>
@@ -25672,22 +25671,22 @@
         <v>4083.6606189999998</v>
       </c>
       <c r="G22" s="8">
-        <v>4454.3347690000001</v>
+        <v>4449.5391609999997</v>
       </c>
       <c r="H22" s="8">
-        <v>4353.2295979999999</v>
+        <v>4334.1590500000002</v>
       </c>
       <c r="I22" s="8">
-        <v>4354.9374310000003</v>
+        <v>4342.286212</v>
       </c>
       <c r="J22" s="8">
-        <v>4521.9506599999995</v>
+        <v>4505.1210970000002</v>
       </c>
       <c r="K22" s="8">
-        <v>4678.6232579999996</v>
+        <v>4655.5461209999994</v>
       </c>
       <c r="L22" s="8">
-        <v>4835.5453680000001</v>
+        <v>4812.3929530000005</v>
       </c>
       <c r="M22" s="8">
         <v>5088.8737209999999</v>
@@ -25871,7 +25870,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26287,22 +26286,22 @@
         <v>6099</v>
       </c>
       <c r="G5" s="19">
-        <v>0</v>
+        <v>6061</v>
       </c>
       <c r="H5" s="19">
-        <v>0</v>
+        <v>6454</v>
       </c>
       <c r="I5" s="19">
-        <v>0</v>
+        <v>6194</v>
       </c>
       <c r="J5" s="19">
-        <v>0</v>
+        <v>6457</v>
       </c>
       <c r="K5" s="19">
-        <v>0</v>
+        <v>6539</v>
       </c>
       <c r="L5" s="19">
-        <v>0</v>
+        <v>6586</v>
       </c>
       <c r="M5" s="19">
         <v>0</v>
@@ -26449,22 +26448,22 @@
         <v>12320</v>
       </c>
       <c r="G6" s="7">
-        <v>0</v>
+        <v>13241</v>
       </c>
       <c r="H6" s="7">
-        <v>0</v>
+        <v>12782</v>
       </c>
       <c r="I6" s="7">
-        <v>0</v>
+        <v>12852</v>
       </c>
       <c r="J6" s="7">
-        <v>0</v>
+        <v>12340</v>
       </c>
       <c r="K6" s="7">
-        <v>0</v>
+        <v>12515</v>
       </c>
       <c r="L6" s="7">
-        <v>0</v>
+        <v>11992</v>
       </c>
       <c r="M6" s="7">
         <v>0</v>
@@ -26611,22 +26610,22 @@
         <v>16756</v>
       </c>
       <c r="G7" s="7">
-        <v>0</v>
+        <v>18848</v>
       </c>
       <c r="H7" s="7">
-        <v>0</v>
+        <v>18497</v>
       </c>
       <c r="I7" s="7">
-        <v>0</v>
+        <v>17694</v>
       </c>
       <c r="J7" s="7">
-        <v>0</v>
+        <v>17637</v>
       </c>
       <c r="K7" s="7">
-        <v>0</v>
+        <v>17353</v>
       </c>
       <c r="L7" s="7">
-        <v>0</v>
+        <v>16765</v>
       </c>
       <c r="M7" s="7">
         <v>0</v>
@@ -26773,22 +26772,22 @@
         <v>4088</v>
       </c>
       <c r="G8" s="7">
-        <v>0</v>
+        <v>4105</v>
       </c>
       <c r="H8" s="7">
-        <v>0</v>
+        <v>4163</v>
       </c>
       <c r="I8" s="7">
-        <v>0</v>
+        <v>4234</v>
       </c>
       <c r="J8" s="7">
-        <v>0</v>
+        <v>4775</v>
       </c>
       <c r="K8" s="7">
-        <v>0</v>
+        <v>4288</v>
       </c>
       <c r="L8" s="7">
-        <v>0</v>
+        <v>4448</v>
       </c>
       <c r="M8" s="7">
         <v>0</v>
@@ -26935,22 +26934,22 @@
         <v>10992</v>
       </c>
       <c r="G9" s="7">
-        <v>0</v>
+        <v>9572</v>
       </c>
       <c r="H9" s="7">
-        <v>0</v>
+        <v>9461</v>
       </c>
       <c r="I9" s="7">
-        <v>0</v>
+        <v>10300</v>
       </c>
       <c r="J9" s="7">
-        <v>0</v>
+        <v>10050</v>
       </c>
       <c r="K9" s="7">
-        <v>0</v>
+        <v>10278</v>
       </c>
       <c r="L9" s="7">
-        <v>0</v>
+        <v>10004</v>
       </c>
       <c r="M9" s="7">
         <v>0</v>
@@ -27097,22 +27096,22 @@
         <v>13323</v>
       </c>
       <c r="G10" s="19">
-        <v>0</v>
+        <v>14711</v>
       </c>
       <c r="H10" s="19">
-        <v>0</v>
+        <v>14796</v>
       </c>
       <c r="I10" s="19">
-        <v>0</v>
+        <v>12877</v>
       </c>
       <c r="J10" s="19">
-        <v>0</v>
+        <v>13944</v>
       </c>
       <c r="K10" s="19">
-        <v>0</v>
+        <v>13830</v>
       </c>
       <c r="L10" s="19">
-        <v>0</v>
+        <v>14619</v>
       </c>
       <c r="M10" s="19">
         <v>0</v>
@@ -27259,22 +27258,22 @@
         <v>39355</v>
       </c>
       <c r="G11" s="7">
-        <v>0</v>
+        <v>41131</v>
       </c>
       <c r="H11" s="7">
-        <v>0</v>
+        <v>40590</v>
       </c>
       <c r="I11" s="7">
-        <v>0</v>
+        <v>39566</v>
       </c>
       <c r="J11" s="7">
-        <v>0</v>
+        <v>38587</v>
       </c>
       <c r="K11" s="7">
-        <v>0</v>
+        <v>39019</v>
       </c>
       <c r="L11" s="7">
-        <v>0</v>
+        <v>38768</v>
       </c>
       <c r="M11" s="7">
         <v>0</v>
@@ -27421,22 +27420,22 @@
         <v>102933</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>107669</v>
       </c>
       <c r="H12" s="8">
-        <v>0</v>
+        <v>106743</v>
       </c>
       <c r="I12" s="8">
-        <v>0</v>
+        <v>103717</v>
       </c>
       <c r="J12" s="8">
-        <v>0</v>
+        <v>103790</v>
       </c>
       <c r="K12" s="8">
-        <v>0</v>
+        <v>103822</v>
       </c>
       <c r="L12" s="8">
-        <v>0</v>
+        <v>103182</v>
       </c>
       <c r="M12" s="8">
         <v>0</v>
@@ -27645,22 +27644,22 @@
         <v>456.74024700000001</v>
       </c>
       <c r="G15" s="19">
-        <v>0</v>
+        <v>443.31105200000002</v>
       </c>
       <c r="H15" s="19">
-        <v>0</v>
+        <v>492.69301400000001</v>
       </c>
       <c r="I15" s="19">
-        <v>0</v>
+        <v>454.65266600000001</v>
       </c>
       <c r="J15" s="19">
-        <v>0</v>
+        <v>486.92328900000001</v>
       </c>
       <c r="K15" s="19">
-        <v>0</v>
+        <v>482.55607300000003</v>
       </c>
       <c r="L15" s="19">
-        <v>0</v>
+        <v>471.20969500000001</v>
       </c>
       <c r="M15" s="19">
         <v>0</v>
@@ -27807,22 +27806,22 @@
         <v>847.61459400000001</v>
       </c>
       <c r="G16" s="7">
-        <v>0</v>
+        <v>901.21945300000004</v>
       </c>
       <c r="H16" s="7">
-        <v>0</v>
+        <v>903.55405699999994</v>
       </c>
       <c r="I16" s="7">
-        <v>0</v>
+        <v>853.31410500000004</v>
       </c>
       <c r="J16" s="7">
-        <v>0</v>
+        <v>837.315517</v>
       </c>
       <c r="K16" s="7">
-        <v>0</v>
+        <v>883.31283599999995</v>
       </c>
       <c r="L16" s="7">
-        <v>0</v>
+        <v>798.79842499999995</v>
       </c>
       <c r="M16" s="7">
         <v>0</v>
@@ -27969,22 +27968,22 @@
         <v>463.67180500000001</v>
       </c>
       <c r="G17" s="7">
-        <v>0</v>
+        <v>580.84453800000006</v>
       </c>
       <c r="H17" s="7">
-        <v>0</v>
+        <v>626.280663</v>
       </c>
       <c r="I17" s="7">
-        <v>0</v>
+        <v>545.30942400000004</v>
       </c>
       <c r="J17" s="7">
-        <v>0</v>
+        <v>577.22236599999997</v>
       </c>
       <c r="K17" s="7">
-        <v>0</v>
+        <v>491.91124200000002</v>
       </c>
       <c r="L17" s="7">
-        <v>0</v>
+        <v>552.191596</v>
       </c>
       <c r="M17" s="7">
         <v>0</v>
@@ -28131,22 +28130,22 @@
         <v>52.335751000000002</v>
       </c>
       <c r="G18" s="7">
-        <v>0</v>
+        <v>48.154744999999998</v>
       </c>
       <c r="H18" s="7">
-        <v>0</v>
+        <v>50.694625000000002</v>
       </c>
       <c r="I18" s="7">
-        <v>0</v>
+        <v>48.305501</v>
       </c>
       <c r="J18" s="7">
-        <v>0</v>
+        <v>58.714339000000002</v>
       </c>
       <c r="K18" s="7">
-        <v>0</v>
+        <v>56.807532999999999</v>
       </c>
       <c r="L18" s="7">
-        <v>0</v>
+        <v>55.489449</v>
       </c>
       <c r="M18" s="7">
         <v>0</v>
@@ -28293,22 +28292,22 @@
         <v>462.15990099999999</v>
       </c>
       <c r="G19" s="7">
-        <v>0</v>
+        <v>443.45818600000001</v>
       </c>
       <c r="H19" s="7">
-        <v>0</v>
+        <v>456.44837899999999</v>
       </c>
       <c r="I19" s="7">
-        <v>0</v>
+        <v>445.14772799999997</v>
       </c>
       <c r="J19" s="7">
-        <v>0</v>
+        <v>449.23964699999999</v>
       </c>
       <c r="K19" s="7">
-        <v>0</v>
+        <v>467.123379</v>
       </c>
       <c r="L19" s="7">
-        <v>0</v>
+        <v>445.75546700000001</v>
       </c>
       <c r="M19" s="7">
         <v>0</v>
@@ -28455,22 +28454,22 @@
         <v>1284.4992119999999</v>
       </c>
       <c r="G20" s="19">
-        <v>0</v>
+        <v>1442.369782</v>
       </c>
       <c r="H20" s="19">
-        <v>0</v>
+        <v>1398.13257</v>
       </c>
       <c r="I20" s="19">
-        <v>0</v>
+        <v>1173.676395</v>
       </c>
       <c r="J20" s="19">
-        <v>0</v>
+        <v>1357.2858630000001</v>
       </c>
       <c r="K20" s="19">
-        <v>0</v>
+        <v>1353.7928340000001</v>
       </c>
       <c r="L20" s="19">
-        <v>0</v>
+        <v>1409.8998260000001</v>
       </c>
       <c r="M20" s="19">
         <v>0</v>
@@ -28617,22 +28616,22 @@
         <v>963.02672500000006</v>
       </c>
       <c r="G21" s="7">
-        <v>0</v>
+        <v>972.01644199999998</v>
       </c>
       <c r="H21" s="7">
-        <v>0</v>
+        <v>965.34934799999996</v>
       </c>
       <c r="I21" s="7">
-        <v>0</v>
+        <v>923.63851799999998</v>
       </c>
       <c r="J21" s="7">
-        <v>0</v>
+        <v>957.78594199999998</v>
       </c>
       <c r="K21" s="7">
-        <v>0</v>
+        <v>967.64945</v>
       </c>
       <c r="L21" s="7">
-        <v>0</v>
+        <v>900.66611499999999</v>
       </c>
       <c r="M21" s="7">
         <v>0</v>
@@ -28779,22 +28778,22 @@
         <v>4530.0482349999993</v>
       </c>
       <c r="G22" s="8">
-        <v>0</v>
+        <v>4831.3741980000004</v>
       </c>
       <c r="H22" s="8">
-        <v>0</v>
+        <v>4893.1526559999993</v>
       </c>
       <c r="I22" s="8">
-        <v>0</v>
+        <v>4444.0443370000003</v>
       </c>
       <c r="J22" s="8">
-        <v>0</v>
+        <v>4724.4869630000003</v>
       </c>
       <c r="K22" s="8">
-        <v>0</v>
+        <v>4703.1533469999995</v>
       </c>
       <c r="L22" s="8">
-        <v>0</v>
+        <v>4634.0105730000005</v>
       </c>
       <c r="M22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Thu Mar 30 19:25:04 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FCF3877-FED3-4087-9AE7-F9D8309639B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDEC42C6-A13A-4CFF-85F3-E3DF85301A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -22782,7 +22782,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
+      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23214,7 +23214,7 @@
         <v>6189</v>
       </c>
       <c r="M5" s="19">
-        <v>6681</v>
+        <v>6670</v>
       </c>
       <c r="N5" s="19">
         <v>6613</v>
@@ -23375,7 +23375,7 @@
         <v>13213</v>
       </c>
       <c r="M6" s="19">
-        <v>13285</v>
+        <v>13274</v>
       </c>
       <c r="N6" s="19">
         <v>11904</v>
@@ -23536,7 +23536,7 @@
         <v>17751</v>
       </c>
       <c r="M7" s="19">
-        <v>18790</v>
+        <v>19973</v>
       </c>
       <c r="N7" s="19">
         <v>19485</v>
@@ -23697,7 +23697,7 @@
         <v>4302</v>
       </c>
       <c r="M8" s="19">
-        <v>4360</v>
+        <v>4357</v>
       </c>
       <c r="N8" s="19">
         <v>3968</v>
@@ -23858,7 +23858,7 @@
         <v>10354</v>
       </c>
       <c r="M9" s="19">
-        <v>9570</v>
+        <v>9442</v>
       </c>
       <c r="N9" s="19">
         <v>10377</v>
@@ -24019,7 +24019,7 @@
         <v>11274</v>
       </c>
       <c r="M10" s="19">
-        <v>13104</v>
+        <v>12878</v>
       </c>
       <c r="N10" s="19">
         <v>12811</v>
@@ -24180,7 +24180,7 @@
         <v>48228</v>
       </c>
       <c r="M11" s="19">
-        <v>52249</v>
+        <v>52172</v>
       </c>
       <c r="N11" s="19">
         <v>51313</v>
@@ -24341,7 +24341,7 @@
         <v>111311</v>
       </c>
       <c r="M12" s="8">
-        <v>118039</v>
+        <v>118766</v>
       </c>
       <c r="N12" s="8">
         <v>116471</v>
@@ -24562,7 +24562,7 @@
         <v>487.29230899999999</v>
       </c>
       <c r="M15" s="19">
-        <v>486.02968099999998</v>
+        <v>483.74492500000002</v>
       </c>
       <c r="N15" s="19">
         <v>469.18487399999998</v>
@@ -24723,7 +24723,7 @@
         <v>962.79300899999998</v>
       </c>
       <c r="M16" s="19">
-        <v>1028.381367</v>
+        <v>1028.625258</v>
       </c>
       <c r="N16" s="19">
         <v>858.22259899999995</v>
@@ -24884,7 +24884,7 @@
         <v>600.02689799999996</v>
       </c>
       <c r="M17" s="19">
-        <v>580.71005000000002</v>
+        <v>579.95369800000003</v>
       </c>
       <c r="N17" s="19">
         <v>560.84059400000001</v>
@@ -25045,7 +25045,7 @@
         <v>59.000740999999998</v>
       </c>
       <c r="M18" s="19">
-        <v>61.228952999999997</v>
+        <v>61.041065000000003</v>
       </c>
       <c r="N18" s="19">
         <v>54.674996999999998</v>
@@ -25206,7 +25206,7 @@
         <v>467.89076899999998</v>
       </c>
       <c r="M19" s="19">
-        <v>458.70701600000001</v>
+        <v>455.14201200000002</v>
       </c>
       <c r="N19" s="19">
         <v>501.13915300000002</v>
@@ -25367,7 +25367,7 @@
         <v>1108.8886480000001</v>
       </c>
       <c r="M20" s="19">
-        <v>1244.1288970000001</v>
+        <v>1240.558025</v>
       </c>
       <c r="N20" s="19">
         <v>1231.124028</v>
@@ -25528,7 +25528,7 @@
         <v>1126.500579</v>
       </c>
       <c r="M21" s="19">
-        <v>1229.6877569999999</v>
+        <v>1228.8055690000001</v>
       </c>
       <c r="N21" s="19">
         <v>1206.997687</v>
@@ -25689,7 +25689,7 @@
         <v>4812.3929530000005</v>
       </c>
       <c r="M22" s="8">
-        <v>5088.8737209999999</v>
+        <v>5077.8705520000003</v>
       </c>
       <c r="N22" s="8">
         <v>4882.1839319999999</v>
@@ -25870,7 +25870,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26304,7 +26304,7 @@
         <v>6586</v>
       </c>
       <c r="M5" s="19">
-        <v>0</v>
+        <v>6478</v>
       </c>
       <c r="N5" s="19">
         <v>0</v>
@@ -26466,7 +26466,7 @@
         <v>11992</v>
       </c>
       <c r="M6" s="7">
-        <v>0</v>
+        <v>12267</v>
       </c>
       <c r="N6" s="7">
         <v>0</v>
@@ -26628,7 +26628,7 @@
         <v>16765</v>
       </c>
       <c r="M7" s="7">
-        <v>0</v>
+        <v>18672</v>
       </c>
       <c r="N7" s="7">
         <v>0</v>
@@ -26790,7 +26790,7 @@
         <v>4448</v>
       </c>
       <c r="M8" s="7">
-        <v>0</v>
+        <v>4388</v>
       </c>
       <c r="N8" s="7">
         <v>0</v>
@@ -26952,7 +26952,7 @@
         <v>10004</v>
       </c>
       <c r="M9" s="7">
-        <v>0</v>
+        <v>10485</v>
       </c>
       <c r="N9" s="7">
         <v>0</v>
@@ -27114,7 +27114,7 @@
         <v>14619</v>
       </c>
       <c r="M10" s="19">
-        <v>0</v>
+        <v>13536</v>
       </c>
       <c r="N10" s="19">
         <v>0</v>
@@ -27276,7 +27276,7 @@
         <v>38768</v>
       </c>
       <c r="M11" s="7">
-        <v>0</v>
+        <v>40854</v>
       </c>
       <c r="N11" s="7">
         <v>0</v>
@@ -27438,7 +27438,7 @@
         <v>103182</v>
       </c>
       <c r="M12" s="8">
-        <v>0</v>
+        <v>106680</v>
       </c>
       <c r="N12" s="8">
         <v>0</v>
@@ -27662,7 +27662,7 @@
         <v>471.20969500000001</v>
       </c>
       <c r="M15" s="19">
-        <v>0</v>
+        <v>503.20889699999998</v>
       </c>
       <c r="N15" s="19">
         <v>0</v>
@@ -27824,7 +27824,7 @@
         <v>798.79842499999995</v>
       </c>
       <c r="M16" s="7">
-        <v>0</v>
+        <v>826.07413499999996</v>
       </c>
       <c r="N16" s="7">
         <v>0</v>
@@ -27986,7 +27986,7 @@
         <v>552.191596</v>
       </c>
       <c r="M17" s="7">
-        <v>0</v>
+        <v>597.58148800000004</v>
       </c>
       <c r="N17" s="7">
         <v>0</v>
@@ -28148,7 +28148,7 @@
         <v>55.489449</v>
       </c>
       <c r="M18" s="7">
-        <v>0</v>
+        <v>51.740797000000001</v>
       </c>
       <c r="N18" s="7">
         <v>0</v>
@@ -28310,7 +28310,7 @@
         <v>445.75546700000001</v>
       </c>
       <c r="M19" s="7">
-        <v>0</v>
+        <v>494.00620800000002</v>
       </c>
       <c r="N19" s="7">
         <v>0</v>
@@ -28472,7 +28472,7 @@
         <v>1409.8998260000001</v>
       </c>
       <c r="M20" s="19">
-        <v>0</v>
+        <v>1272.214757</v>
       </c>
       <c r="N20" s="19">
         <v>0</v>
@@ -28634,7 +28634,7 @@
         <v>900.66611499999999</v>
       </c>
       <c r="M21" s="7">
-        <v>0</v>
+        <v>960.83769700000005</v>
       </c>
       <c r="N21" s="7">
         <v>0</v>
@@ -28796,7 +28796,7 @@
         <v>4634.0105730000005</v>
       </c>
       <c r="M22" s="8">
-        <v>0</v>
+        <v>4705.6639789999999</v>
       </c>
       <c r="N22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Apr  4 17:22:30 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDEC42C6-A13A-4CFF-85F3-E3DF85301A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35093D82-5E07-4E8C-B9C7-FDE2ABDAB4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -22782,7 +22782,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23217,7 +23217,7 @@
         <v>6670</v>
       </c>
       <c r="N5" s="19">
-        <v>6613</v>
+        <v>6599</v>
       </c>
       <c r="O5" s="19">
         <v>6361</v>
@@ -23378,7 +23378,7 @@
         <v>13274</v>
       </c>
       <c r="N6" s="19">
-        <v>11904</v>
+        <v>11919</v>
       </c>
       <c r="O6" s="19">
         <v>12796</v>
@@ -23539,7 +23539,7 @@
         <v>19973</v>
       </c>
       <c r="N7" s="19">
-        <v>19485</v>
+        <v>20435</v>
       </c>
       <c r="O7" s="19">
         <v>17755</v>
@@ -23700,7 +23700,7 @@
         <v>4357</v>
       </c>
       <c r="N8" s="19">
-        <v>3968</v>
+        <v>3959</v>
       </c>
       <c r="O8" s="19">
         <v>4238</v>
@@ -23861,7 +23861,7 @@
         <v>9442</v>
       </c>
       <c r="N9" s="19">
-        <v>10377</v>
+        <v>10285</v>
       </c>
       <c r="O9" s="19">
         <v>10291</v>
@@ -24022,7 +24022,7 @@
         <v>12878</v>
       </c>
       <c r="N10" s="19">
-        <v>12811</v>
+        <v>12705</v>
       </c>
       <c r="O10" s="19">
         <v>12630</v>
@@ -24183,7 +24183,7 @@
         <v>52172</v>
       </c>
       <c r="N11" s="19">
-        <v>51313</v>
+        <v>51162</v>
       </c>
       <c r="O11" s="19">
         <v>54805</v>
@@ -24344,7 +24344,7 @@
         <v>118766</v>
       </c>
       <c r="N12" s="8">
-        <v>116471</v>
+        <v>117064</v>
       </c>
       <c r="O12" s="8">
         <v>118876</v>
@@ -24565,7 +24565,7 @@
         <v>483.74492500000002</v>
       </c>
       <c r="N15" s="19">
-        <v>469.18487399999998</v>
+        <v>466.40950700000002</v>
       </c>
       <c r="O15" s="19">
         <v>481.38831199999998</v>
@@ -24726,7 +24726,7 @@
         <v>1028.625258</v>
       </c>
       <c r="N16" s="19">
-        <v>858.22259899999995</v>
+        <v>860.89157799999998</v>
       </c>
       <c r="O16" s="19">
         <v>961.343478</v>
@@ -24887,7 +24887,7 @@
         <v>579.95369800000003</v>
       </c>
       <c r="N17" s="19">
-        <v>560.84059400000001</v>
+        <v>555.67727500000001</v>
       </c>
       <c r="O17" s="19">
         <v>544.73971900000004</v>
@@ -25048,7 +25048,7 @@
         <v>61.041065000000003</v>
       </c>
       <c r="N18" s="19">
-        <v>54.674996999999998</v>
+        <v>54.470046000000004</v>
       </c>
       <c r="O18" s="19">
         <v>58.320408</v>
@@ -25209,7 +25209,7 @@
         <v>455.14201200000002</v>
       </c>
       <c r="N19" s="19">
-        <v>501.13915300000002</v>
+        <v>494.28150199999999</v>
       </c>
       <c r="O19" s="19">
         <v>488.14388700000001</v>
@@ -25370,7 +25370,7 @@
         <v>1240.558025</v>
       </c>
       <c r="N20" s="19">
-        <v>1231.124028</v>
+        <v>1228.7149139999999</v>
       </c>
       <c r="O20" s="19">
         <v>1142.94047</v>
@@ -25531,7 +25531,7 @@
         <v>1228.8055690000001</v>
       </c>
       <c r="N21" s="19">
-        <v>1206.997687</v>
+        <v>1202.542148</v>
       </c>
       <c r="O21" s="19">
         <v>1291.5864409999999</v>
@@ -25692,7 +25692,7 @@
         <v>5077.8705520000003</v>
       </c>
       <c r="N22" s="8">
-        <v>4882.1839319999999</v>
+        <v>4862.9869699999999</v>
       </c>
       <c r="O22" s="8">
         <v>4968.4627149999997</v>
@@ -25870,7 +25870,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26307,7 +26307,7 @@
         <v>6478</v>
       </c>
       <c r="N5" s="19">
-        <v>0</v>
+        <v>6320</v>
       </c>
       <c r="O5" s="19">
         <v>0</v>
@@ -26469,7 +26469,7 @@
         <v>12267</v>
       </c>
       <c r="N6" s="7">
-        <v>0</v>
+        <v>11766</v>
       </c>
       <c r="O6" s="7">
         <v>0</v>
@@ -26631,7 +26631,7 @@
         <v>18672</v>
       </c>
       <c r="N7" s="7">
-        <v>0</v>
+        <v>19941</v>
       </c>
       <c r="O7" s="7">
         <v>0</v>
@@ -26793,7 +26793,7 @@
         <v>4388</v>
       </c>
       <c r="N8" s="7">
-        <v>0</v>
+        <v>4509</v>
       </c>
       <c r="O8" s="7">
         <v>0</v>
@@ -26955,7 +26955,7 @@
         <v>10485</v>
       </c>
       <c r="N9" s="7">
-        <v>0</v>
+        <v>12870</v>
       </c>
       <c r="O9" s="7">
         <v>0</v>
@@ -27117,7 +27117,7 @@
         <v>13536</v>
       </c>
       <c r="N10" s="19">
-        <v>0</v>
+        <v>12685</v>
       </c>
       <c r="O10" s="19">
         <v>0</v>
@@ -27279,7 +27279,7 @@
         <v>40854</v>
       </c>
       <c r="N11" s="7">
-        <v>0</v>
+        <v>39470</v>
       </c>
       <c r="O11" s="7">
         <v>0</v>
@@ -27441,7 +27441,7 @@
         <v>106680</v>
       </c>
       <c r="N12" s="8">
-        <v>0</v>
+        <v>107561</v>
       </c>
       <c r="O12" s="8">
         <v>0</v>
@@ -27665,7 +27665,7 @@
         <v>503.20889699999998</v>
       </c>
       <c r="N15" s="19">
-        <v>0</v>
+        <v>482.68787200000003</v>
       </c>
       <c r="O15" s="19">
         <v>0</v>
@@ -27827,7 +27827,7 @@
         <v>826.07413499999996</v>
       </c>
       <c r="N16" s="7">
-        <v>0</v>
+        <v>818.76770299999998</v>
       </c>
       <c r="O16" s="7">
         <v>0</v>
@@ -27989,7 +27989,7 @@
         <v>597.58148800000004</v>
       </c>
       <c r="N17" s="7">
-        <v>0</v>
+        <v>513.32603300000005</v>
       </c>
       <c r="O17" s="7">
         <v>0</v>
@@ -28151,7 +28151,7 @@
         <v>51.740797000000001</v>
       </c>
       <c r="N18" s="7">
-        <v>0</v>
+        <v>54.236482000000002</v>
       </c>
       <c r="O18" s="7">
         <v>0</v>
@@ -28313,7 +28313,7 @@
         <v>494.00620800000002</v>
       </c>
       <c r="N19" s="7">
-        <v>0</v>
+        <v>559.05307900000003</v>
       </c>
       <c r="O19" s="7">
         <v>0</v>
@@ -28475,7 +28475,7 @@
         <v>1272.214757</v>
       </c>
       <c r="N20" s="19">
-        <v>0</v>
+        <v>1196.3085900000001</v>
       </c>
       <c r="O20" s="19">
         <v>0</v>
@@ -28637,7 +28637,7 @@
         <v>960.83769700000005</v>
       </c>
       <c r="N21" s="7">
-        <v>0</v>
+        <v>910.81427099999996</v>
       </c>
       <c r="O21" s="7">
         <v>0</v>
@@ -28799,7 +28799,7 @@
         <v>4705.6639789999999</v>
       </c>
       <c r="N22" s="8">
-        <v>0</v>
+        <v>4535.1940299999997</v>
       </c>
       <c r="O22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Apr 18 20:00:04 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -23222,7 +23222,7 @@
         <v>6316</v>
       </c>
       <c r="P5" s="19">
-        <v>6534</v>
+        <v>6490</v>
       </c>
       <c r="Q5" s="19">
         <v>6741</v>
@@ -23383,7 +23383,7 @@
         <v>12787</v>
       </c>
       <c r="P6" s="19">
-        <v>12020</v>
+        <v>12034</v>
       </c>
       <c r="Q6" s="19">
         <v>11945</v>
@@ -23544,7 +23544,7 @@
         <v>18374</v>
       </c>
       <c r="P7" s="19">
-        <v>16933</v>
+        <v>17783</v>
       </c>
       <c r="Q7" s="19">
         <v>17463</v>
@@ -23705,7 +23705,7 @@
         <v>4208</v>
       </c>
       <c r="P8" s="19">
-        <v>4440</v>
+        <v>4401</v>
       </c>
       <c r="Q8" s="19">
         <v>4531</v>
@@ -23866,7 +23866,7 @@
         <v>10307</v>
       </c>
       <c r="P9" s="19">
-        <v>11163</v>
+        <v>10939</v>
       </c>
       <c r="Q9" s="19">
         <v>10743</v>
@@ -24027,7 +24027,7 @@
         <v>12614</v>
       </c>
       <c r="P10" s="19">
-        <v>11348</v>
+        <v>11349</v>
       </c>
       <c r="Q10" s="19">
         <v>11309</v>
@@ -24188,7 +24188,7 @@
         <v>54720</v>
       </c>
       <c r="P11" s="19">
-        <v>51023</v>
+        <v>50947</v>
       </c>
       <c r="Q11" s="19">
         <v>52440</v>
@@ -24349,7 +24349,7 @@
         <v>119326</v>
       </c>
       <c r="P12" s="8">
-        <v>113461</v>
+        <v>113943</v>
       </c>
       <c r="Q12" s="8">
         <v>115172</v>
@@ -24570,7 +24570,7 @@
         <v>473.37423799999999</v>
       </c>
       <c r="P15" s="19">
-        <v>491.744753</v>
+        <v>485.11397799999997</v>
       </c>
       <c r="Q15" s="19">
         <v>555.19643699999995</v>
@@ -24731,7 +24731,7 @@
         <v>961.31267200000002</v>
       </c>
       <c r="P16" s="19">
-        <v>953.54163900000003</v>
+        <v>952.53400499999998</v>
       </c>
       <c r="Q16" s="19">
         <v>876.53461000000004</v>
@@ -24892,7 +24892,7 @@
         <v>545.93595700000003</v>
       </c>
       <c r="P17" s="19">
-        <v>553.74086399999999</v>
+        <v>554.76910799999996</v>
       </c>
       <c r="Q17" s="19">
         <v>562.22682099999997</v>
@@ -25053,7 +25053,7 @@
         <v>55.939155</v>
       </c>
       <c r="P18" s="19">
-        <v>64.340154999999996</v>
+        <v>61.699232000000002</v>
       </c>
       <c r="Q18" s="19">
         <v>67.438394000000002</v>
@@ -25214,7 +25214,7 @@
         <v>488.38839300000001</v>
       </c>
       <c r="P19" s="19">
-        <v>506.97527100000002</v>
+        <v>506.36838</v>
       </c>
       <c r="Q19" s="19">
         <v>474.18720100000002</v>
@@ -25375,7 +25375,7 @@
         <v>1143.9569320000001</v>
       </c>
       <c r="P20" s="19">
-        <v>1164.3280010000001</v>
+        <v>1164.2077630000001</v>
       </c>
       <c r="Q20" s="19">
         <v>1051.721536</v>
@@ -25536,7 +25536,7 @@
         <v>1289.896857</v>
       </c>
       <c r="P21" s="19">
-        <v>1134.999039</v>
+        <v>1133.8583470000001</v>
       </c>
       <c r="Q21" s="19">
         <v>1208.2339569999999</v>
@@ -25697,7 +25697,7 @@
         <v>4958.804204</v>
       </c>
       <c r="P22" s="8">
-        <v>4869.6697219999996</v>
+        <v>4858.5508129999998</v>
       </c>
       <c r="Q22" s="8">
         <v>4795.5389560000003</v>
@@ -26312,7 +26312,7 @@
         <v>5915</v>
       </c>
       <c r="P5" s="19">
-        <v>0</v>
+        <v>6345</v>
       </c>
       <c r="Q5" s="19">
         <v>0</v>
@@ -26474,7 +26474,7 @@
         <v>11357</v>
       </c>
       <c r="P6" s="7">
-        <v>0</v>
+        <v>11348</v>
       </c>
       <c r="Q6" s="7">
         <v>0</v>
@@ -26636,7 +26636,7 @@
         <v>17688</v>
       </c>
       <c r="P7" s="7">
-        <v>0</v>
+        <v>19375</v>
       </c>
       <c r="Q7" s="7">
         <v>0</v>
@@ -26798,7 +26798,7 @@
         <v>4542</v>
       </c>
       <c r="P8" s="7">
-        <v>0</v>
+        <v>4822</v>
       </c>
       <c r="Q8" s="7">
         <v>0</v>
@@ -26960,7 +26960,7 @@
         <v>9703</v>
       </c>
       <c r="P9" s="7">
-        <v>0</v>
+        <v>11228</v>
       </c>
       <c r="Q9" s="7">
         <v>0</v>
@@ -27122,7 +27122,7 @@
         <v>13752</v>
       </c>
       <c r="P10" s="19">
-        <v>0</v>
+        <v>13857</v>
       </c>
       <c r="Q10" s="19">
         <v>0</v>
@@ -27284,7 +27284,7 @@
         <v>38318</v>
       </c>
       <c r="P11" s="7">
-        <v>0</v>
+        <v>39613</v>
       </c>
       <c r="Q11" s="7">
         <v>0</v>
@@ -27446,7 +27446,7 @@
         <v>101275</v>
       </c>
       <c r="P12" s="8">
-        <v>0</v>
+        <v>106588</v>
       </c>
       <c r="Q12" s="8">
         <v>0</v>
@@ -27670,7 +27670,7 @@
         <v>438.18934000000002</v>
       </c>
       <c r="P15" s="19">
-        <v>0</v>
+        <v>474.53636399999999</v>
       </c>
       <c r="Q15" s="19">
         <v>0</v>
@@ -27832,7 +27832,7 @@
         <v>783.68932800000005</v>
       </c>
       <c r="P16" s="7">
-        <v>0</v>
+        <v>818.33276499999999</v>
       </c>
       <c r="Q16" s="7">
         <v>0</v>
@@ -27994,7 +27994,7 @@
         <v>564.39361899999994</v>
       </c>
       <c r="P17" s="7">
-        <v>0</v>
+        <v>509.57620100000003</v>
       </c>
       <c r="Q17" s="7">
         <v>0</v>
@@ -28156,7 +28156,7 @@
         <v>57.685867999999999</v>
       </c>
       <c r="P18" s="7">
-        <v>0</v>
+        <v>66.808172999999996</v>
       </c>
       <c r="Q18" s="7">
         <v>0</v>
@@ -28318,7 +28318,7 @@
         <v>482.57338800000002</v>
       </c>
       <c r="P19" s="7">
-        <v>0</v>
+        <v>540.91893800000003</v>
       </c>
       <c r="Q19" s="7">
         <v>0</v>
@@ -28480,7 +28480,7 @@
         <v>1306.526511</v>
       </c>
       <c r="P20" s="19">
-        <v>0</v>
+        <v>1310.947643</v>
       </c>
       <c r="Q20" s="19">
         <v>0</v>
@@ -28642,7 +28642,7 @@
         <v>902.98390099999995</v>
       </c>
       <c r="P21" s="7">
-        <v>0</v>
+        <v>941.79062299999998</v>
       </c>
       <c r="Q21" s="7">
         <v>0</v>
@@ -28804,7 +28804,7 @@
         <v>4536.0419549999997</v>
       </c>
       <c r="P22" s="8">
-        <v>0</v>
+        <v>4662.910707</v>
       </c>
       <c r="Q22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Mon May 29 13:51:00 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -13318,8 +13318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16386,6 +16386,9 @@
     <mergeCell ref="A1:BA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -16394,7 +16397,7 @@
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19681,6 +19684,9 @@
     <mergeCell ref="A1:BA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -19693,7 +19699,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22769,6 +22775,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -22781,7 +22790,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23225,19 +23234,19 @@
         <v>6490</v>
       </c>
       <c r="Q5" s="19">
-        <v>6741</v>
+        <v>6718</v>
       </c>
       <c r="R5" s="19">
-        <v>6838</v>
+        <v>6812</v>
       </c>
       <c r="S5" s="19">
-        <v>6697</v>
+        <v>6647</v>
       </c>
       <c r="T5" s="19">
-        <v>6612</v>
+        <v>6583</v>
       </c>
       <c r="U5" s="19">
-        <v>6831</v>
+        <v>6803</v>
       </c>
       <c r="V5" s="19">
         <v>6785</v>
@@ -23386,19 +23395,19 @@
         <v>12034</v>
       </c>
       <c r="Q6" s="19">
-        <v>11945</v>
+        <v>11944</v>
       </c>
       <c r="R6" s="19">
-        <v>12651</v>
+        <v>12630</v>
       </c>
       <c r="S6" s="19">
-        <v>11589</v>
+        <v>11579</v>
       </c>
       <c r="T6" s="19">
-        <v>12336</v>
+        <v>12265</v>
       </c>
       <c r="U6" s="19">
-        <v>13012</v>
+        <v>12925</v>
       </c>
       <c r="V6" s="19">
         <v>12923</v>
@@ -23547,19 +23556,19 @@
         <v>17783</v>
       </c>
       <c r="Q7" s="19">
-        <v>17463</v>
+        <v>18241</v>
       </c>
       <c r="R7" s="19">
-        <v>17737</v>
+        <v>18332</v>
       </c>
       <c r="S7" s="19">
-        <v>17488</v>
+        <v>17937</v>
       </c>
       <c r="T7" s="19">
-        <v>17257</v>
+        <v>18086</v>
       </c>
       <c r="U7" s="19">
-        <v>18975</v>
+        <v>19465</v>
       </c>
       <c r="V7" s="19">
         <v>18481</v>
@@ -23708,19 +23717,19 @@
         <v>4401</v>
       </c>
       <c r="Q8" s="19">
-        <v>4531</v>
+        <v>4529</v>
       </c>
       <c r="R8" s="19">
-        <v>4561</v>
+        <v>4555</v>
       </c>
       <c r="S8" s="19">
-        <v>4383</v>
+        <v>4381</v>
       </c>
       <c r="T8" s="19">
-        <v>4094</v>
+        <v>4092</v>
       </c>
       <c r="U8" s="19">
-        <v>4051</v>
+        <v>4046</v>
       </c>
       <c r="V8" s="19">
         <v>4703</v>
@@ -23869,19 +23878,19 @@
         <v>10939</v>
       </c>
       <c r="Q9" s="19">
-        <v>10743</v>
+        <v>10721</v>
       </c>
       <c r="R9" s="19">
         <v>10684</v>
       </c>
       <c r="S9" s="19">
-        <v>10750</v>
+        <v>10625</v>
       </c>
       <c r="T9" s="19">
-        <v>10849</v>
+        <v>10851</v>
       </c>
       <c r="U9" s="19">
-        <v>9058</v>
+        <v>9071</v>
       </c>
       <c r="V9" s="19">
         <v>9576</v>
@@ -24030,19 +24039,19 @@
         <v>11349</v>
       </c>
       <c r="Q10" s="19">
-        <v>11309</v>
+        <v>11312</v>
       </c>
       <c r="R10" s="19">
-        <v>11091</v>
+        <v>10974</v>
       </c>
       <c r="S10" s="19">
-        <v>11533</v>
+        <v>11523</v>
       </c>
       <c r="T10" s="19">
-        <v>11071</v>
+        <v>11069</v>
       </c>
       <c r="U10" s="19">
-        <v>9773</v>
+        <v>9664</v>
       </c>
       <c r="V10" s="19">
         <v>10728</v>
@@ -24191,19 +24200,19 @@
         <v>50947</v>
       </c>
       <c r="Q11" s="19">
-        <v>52440</v>
+        <v>52189</v>
       </c>
       <c r="R11" s="19">
-        <v>55924</v>
+        <v>55806</v>
       </c>
       <c r="S11" s="19">
-        <v>56129</v>
+        <v>55854</v>
       </c>
       <c r="T11" s="19">
-        <v>54028</v>
+        <v>53876</v>
       </c>
       <c r="U11" s="19">
-        <v>53418</v>
+        <v>53269</v>
       </c>
       <c r="V11" s="19">
         <v>46580</v>
@@ -24352,19 +24361,19 @@
         <v>113943</v>
       </c>
       <c r="Q12" s="8">
-        <v>115172</v>
+        <v>115654</v>
       </c>
       <c r="R12" s="8">
-        <v>119486</v>
+        <v>119793</v>
       </c>
       <c r="S12" s="8">
-        <v>118569</v>
+        <v>118546</v>
       </c>
       <c r="T12" s="8">
-        <v>116247</v>
+        <v>116822</v>
       </c>
       <c r="U12" s="8">
-        <v>115118</v>
+        <v>115243</v>
       </c>
       <c r="V12" s="8">
         <v>109776</v>
@@ -24573,19 +24582,19 @@
         <v>485.11397799999997</v>
       </c>
       <c r="Q15" s="19">
-        <v>555.19643699999995</v>
+        <v>551.17688299999998</v>
       </c>
       <c r="R15" s="19">
-        <v>526.44567300000006</v>
+        <v>522.83565199999998</v>
       </c>
       <c r="S15" s="19">
-        <v>548.04846999999995</v>
+        <v>540.49227599999995</v>
       </c>
       <c r="T15" s="19">
-        <v>527.69936499999994</v>
+        <v>521.44413999999995</v>
       </c>
       <c r="U15" s="19">
-        <v>541.21490500000004</v>
+        <v>536.86192600000004</v>
       </c>
       <c r="V15" s="19">
         <v>522.878241</v>
@@ -24734,19 +24743,19 @@
         <v>952.53400499999998</v>
       </c>
       <c r="Q16" s="19">
-        <v>876.53461000000004</v>
+        <v>876.27960499999995</v>
       </c>
       <c r="R16" s="19">
-        <v>953.28585999999996</v>
+        <v>952.68658700000003</v>
       </c>
       <c r="S16" s="19">
-        <v>879.96744200000001</v>
+        <v>880.35818700000004</v>
       </c>
       <c r="T16" s="19">
-        <v>875.01599899999997</v>
+        <v>874.90772000000004</v>
       </c>
       <c r="U16" s="19">
-        <v>1027.106855</v>
+        <v>1009.54049</v>
       </c>
       <c r="V16" s="19">
         <v>1023.1000759999999</v>
@@ -24895,19 +24904,19 @@
         <v>554.76910799999996</v>
       </c>
       <c r="Q17" s="19">
-        <v>562.22682099999997</v>
+        <v>538.14593400000001</v>
       </c>
       <c r="R17" s="19">
-        <v>625.14402500000006</v>
+        <v>624.30336799999998</v>
       </c>
       <c r="S17" s="19">
-        <v>501.763777</v>
+        <v>500.40486399999998</v>
       </c>
       <c r="T17" s="19">
-        <v>535.76379199999997</v>
+        <v>528.58845199999996</v>
       </c>
       <c r="U17" s="19">
-        <v>536.25769300000002</v>
+        <v>535.50898099999995</v>
       </c>
       <c r="V17" s="19">
         <v>513.87695799999995</v>
@@ -25056,19 +25065,19 @@
         <v>61.699232000000002</v>
       </c>
       <c r="Q18" s="19">
-        <v>67.438394000000002</v>
+        <v>67.418977999999996</v>
       </c>
       <c r="R18" s="19">
-        <v>66.702438000000001</v>
+        <v>66.550061999999997</v>
       </c>
       <c r="S18" s="19">
-        <v>62.497169999999997</v>
+        <v>62.432819000000002</v>
       </c>
       <c r="T18" s="19">
-        <v>58.331285999999999</v>
+        <v>58.188654999999997</v>
       </c>
       <c r="U18" s="19">
-        <v>56.743732999999999</v>
+        <v>56.522060000000003</v>
       </c>
       <c r="V18" s="19">
         <v>60.147862000000003</v>
@@ -25217,19 +25226,19 @@
         <v>506.36838</v>
       </c>
       <c r="Q19" s="19">
-        <v>474.18720100000002</v>
+        <v>472.86283800000001</v>
       </c>
       <c r="R19" s="19">
-        <v>503.29529500000001</v>
+        <v>502.626487</v>
       </c>
       <c r="S19" s="19">
-        <v>497.685655</v>
+        <v>496.56835000000001</v>
       </c>
       <c r="T19" s="19">
-        <v>549.26969599999995</v>
+        <v>548.97047999999995</v>
       </c>
       <c r="U19" s="19">
-        <v>486.80322000000001</v>
+        <v>486.64239400000002</v>
       </c>
       <c r="V19" s="19">
         <v>463.72209099999998</v>
@@ -25378,19 +25387,19 @@
         <v>1164.2077630000001</v>
       </c>
       <c r="Q20" s="19">
-        <v>1051.721536</v>
+        <v>1053.833421</v>
       </c>
       <c r="R20" s="19">
-        <v>957.60636199999999</v>
+        <v>956.90457500000002</v>
       </c>
       <c r="S20" s="19">
-        <v>991.17258000000004</v>
+        <v>989.64519499999994</v>
       </c>
       <c r="T20" s="19">
-        <v>887.05689199999995</v>
+        <v>888.59513500000003</v>
       </c>
       <c r="U20" s="19">
-        <v>849.59546799999998</v>
+        <v>838.65342099999998</v>
       </c>
       <c r="V20" s="19">
         <v>940.15265499999998</v>
@@ -25539,19 +25548,19 @@
         <v>1133.8583470000001</v>
       </c>
       <c r="Q21" s="19">
-        <v>1208.2339569999999</v>
+        <v>1200.264598</v>
       </c>
       <c r="R21" s="19">
-        <v>1225.8682980000001</v>
+        <v>1224.41812</v>
       </c>
       <c r="S21" s="19">
-        <v>1277.676831</v>
+        <v>1272.985441</v>
       </c>
       <c r="T21" s="19">
-        <v>1217.630895</v>
+        <v>1214.0499110000001</v>
       </c>
       <c r="U21" s="19">
-        <v>1250.2926869999999</v>
+        <v>1248.7928939999999</v>
       </c>
       <c r="V21" s="19">
         <v>1082.948676</v>
@@ -25700,19 +25709,19 @@
         <v>4858.5508129999998</v>
       </c>
       <c r="Q22" s="8">
-        <v>4795.5389560000003</v>
+        <v>4759.9822569999997</v>
       </c>
       <c r="R22" s="8">
-        <v>4858.3479509999997</v>
+        <v>4850.3248509999994</v>
       </c>
       <c r="S22" s="8">
-        <v>4758.811925</v>
+        <v>4742.8871319999998</v>
       </c>
       <c r="T22" s="8">
-        <v>4650.7679250000001</v>
+        <v>4634.7444930000001</v>
       </c>
       <c r="U22" s="8">
-        <v>4748.014561</v>
+        <v>4712.5221659999997</v>
       </c>
       <c r="V22" s="8">
         <v>4606.8265589999992</v>
@@ -25868,8 +25877,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26315,19 +26324,19 @@
         <v>6345</v>
       </c>
       <c r="Q5" s="19">
-        <v>0</v>
+        <v>6384</v>
       </c>
       <c r="R5" s="19">
-        <v>0</v>
+        <v>6194</v>
       </c>
       <c r="S5" s="19">
-        <v>0</v>
+        <v>5848</v>
       </c>
       <c r="T5" s="19">
-        <v>0</v>
+        <v>5879</v>
       </c>
       <c r="U5" s="19">
-        <v>0</v>
+        <v>6094</v>
       </c>
       <c r="V5" s="19">
         <v>0</v>
@@ -26477,19 +26486,19 @@
         <v>11348</v>
       </c>
       <c r="Q6" s="7">
-        <v>0</v>
+        <v>11451</v>
       </c>
       <c r="R6" s="7">
-        <v>0</v>
+        <v>11896</v>
       </c>
       <c r="S6" s="7">
-        <v>0</v>
+        <v>11133</v>
       </c>
       <c r="T6" s="7">
-        <v>0</v>
+        <v>11716</v>
       </c>
       <c r="U6" s="7">
-        <v>0</v>
+        <v>11689</v>
       </c>
       <c r="V6" s="7">
         <v>0</v>
@@ -26639,19 +26648,19 @@
         <v>19375</v>
       </c>
       <c r="Q7" s="7">
-        <v>0</v>
+        <v>19611</v>
       </c>
       <c r="R7" s="7">
-        <v>0</v>
+        <v>20445</v>
       </c>
       <c r="S7" s="7">
-        <v>0</v>
+        <v>17797</v>
       </c>
       <c r="T7" s="7">
-        <v>0</v>
+        <v>18095</v>
       </c>
       <c r="U7" s="7">
-        <v>0</v>
+        <v>17811</v>
       </c>
       <c r="V7" s="7">
         <v>0</v>
@@ -26801,19 +26810,19 @@
         <v>4822</v>
       </c>
       <c r="Q8" s="7">
-        <v>0</v>
+        <v>4375</v>
       </c>
       <c r="R8" s="7">
-        <v>0</v>
+        <v>4599</v>
       </c>
       <c r="S8" s="7">
-        <v>0</v>
+        <v>4600</v>
       </c>
       <c r="T8" s="7">
-        <v>0</v>
+        <v>4875</v>
       </c>
       <c r="U8" s="7">
-        <v>0</v>
+        <v>4645</v>
       </c>
       <c r="V8" s="7">
         <v>0</v>
@@ -26963,19 +26972,19 @@
         <v>11228</v>
       </c>
       <c r="Q9" s="7">
-        <v>0</v>
+        <v>10593</v>
       </c>
       <c r="R9" s="7">
-        <v>0</v>
+        <v>10476</v>
       </c>
       <c r="S9" s="7">
-        <v>0</v>
+        <v>10161</v>
       </c>
       <c r="T9" s="7">
-        <v>0</v>
+        <v>10140</v>
       </c>
       <c r="U9" s="7">
-        <v>0</v>
+        <v>10276</v>
       </c>
       <c r="V9" s="7">
         <v>0</v>
@@ -27125,19 +27134,19 @@
         <v>13857</v>
       </c>
       <c r="Q10" s="19">
-        <v>0</v>
+        <v>13278</v>
       </c>
       <c r="R10" s="19">
-        <v>0</v>
+        <v>13012</v>
       </c>
       <c r="S10" s="19">
-        <v>0</v>
+        <v>11269</v>
       </c>
       <c r="T10" s="19">
-        <v>0</v>
+        <v>12171</v>
       </c>
       <c r="U10" s="19">
-        <v>0</v>
+        <v>11421</v>
       </c>
       <c r="V10" s="19">
         <v>0</v>
@@ -27287,19 +27296,19 @@
         <v>39613</v>
       </c>
       <c r="Q11" s="7">
-        <v>0</v>
+        <v>43100</v>
       </c>
       <c r="R11" s="7">
-        <v>0</v>
+        <v>42716</v>
       </c>
       <c r="S11" s="7">
-        <v>0</v>
+        <v>43917</v>
       </c>
       <c r="T11" s="7">
-        <v>0</v>
+        <v>41882</v>
       </c>
       <c r="U11" s="7">
-        <v>0</v>
+        <v>45248</v>
       </c>
       <c r="V11" s="7">
         <v>0</v>
@@ -27449,19 +27458,19 @@
         <v>106588</v>
       </c>
       <c r="Q12" s="8">
-        <v>0</v>
+        <v>108792</v>
       </c>
       <c r="R12" s="8">
-        <v>0</v>
+        <v>109338</v>
       </c>
       <c r="S12" s="8">
-        <v>0</v>
+        <v>104725</v>
       </c>
       <c r="T12" s="8">
-        <v>0</v>
+        <v>104758</v>
       </c>
       <c r="U12" s="8">
-        <v>0</v>
+        <v>107184</v>
       </c>
       <c r="V12" s="8">
         <v>0</v>
@@ -27673,19 +27682,19 @@
         <v>474.53636399999999</v>
       </c>
       <c r="Q15" s="19">
-        <v>0</v>
+        <v>497.79733900000002</v>
       </c>
       <c r="R15" s="19">
-        <v>0</v>
+        <v>470.63901099999998</v>
       </c>
       <c r="S15" s="19">
-        <v>0</v>
+        <v>442.37045699999999</v>
       </c>
       <c r="T15" s="19">
-        <v>0</v>
+        <v>440.94764700000002</v>
       </c>
       <c r="U15" s="19">
-        <v>0</v>
+        <v>458.53278699999998</v>
       </c>
       <c r="V15" s="19">
         <v>0</v>
@@ -27835,19 +27844,19 @@
         <v>818.33276499999999</v>
       </c>
       <c r="Q16" s="7">
-        <v>0</v>
+        <v>820.26349900000002</v>
       </c>
       <c r="R16" s="7">
-        <v>0</v>
+        <v>822.32434799999999</v>
       </c>
       <c r="S16" s="7">
-        <v>0</v>
+        <v>773.93702299999995</v>
       </c>
       <c r="T16" s="7">
-        <v>0</v>
+        <v>828.23167100000001</v>
       </c>
       <c r="U16" s="7">
-        <v>0</v>
+        <v>806.95998999999995</v>
       </c>
       <c r="V16" s="7">
         <v>0</v>
@@ -27997,19 +28006,19 @@
         <v>509.57620100000003</v>
       </c>
       <c r="Q17" s="7">
-        <v>0</v>
+        <v>559.76119100000005</v>
       </c>
       <c r="R17" s="7">
-        <v>0</v>
+        <v>494.38022899999999</v>
       </c>
       <c r="S17" s="7">
-        <v>0</v>
+        <v>507.82356399999998</v>
       </c>
       <c r="T17" s="7">
-        <v>0</v>
+        <v>503.87167699999998</v>
       </c>
       <c r="U17" s="7">
-        <v>0</v>
+        <v>368.55136499999998</v>
       </c>
       <c r="V17" s="7">
         <v>0</v>
@@ -28159,19 +28168,19 @@
         <v>66.808172999999996</v>
       </c>
       <c r="Q18" s="7">
-        <v>0</v>
+        <v>57.843625000000003</v>
       </c>
       <c r="R18" s="7">
-        <v>0</v>
+        <v>60.481492000000003</v>
       </c>
       <c r="S18" s="7">
-        <v>0</v>
+        <v>61.694220999999999</v>
       </c>
       <c r="T18" s="7">
-        <v>0</v>
+        <v>67.697630000000004</v>
       </c>
       <c r="U18" s="7">
-        <v>0</v>
+        <v>65.464646999999999</v>
       </c>
       <c r="V18" s="7">
         <v>0</v>
@@ -28321,19 +28330,19 @@
         <v>540.91893800000003</v>
       </c>
       <c r="Q19" s="7">
-        <v>0</v>
+        <v>509.35785900000002</v>
       </c>
       <c r="R19" s="7">
-        <v>0</v>
+        <v>478.75323500000002</v>
       </c>
       <c r="S19" s="7">
-        <v>0</v>
+        <v>421.60304600000001</v>
       </c>
       <c r="T19" s="7">
-        <v>0</v>
+        <v>454.03650199999998</v>
       </c>
       <c r="U19" s="7">
-        <v>0</v>
+        <v>466.60644600000001</v>
       </c>
       <c r="V19" s="7">
         <v>0</v>
@@ -28483,19 +28492,19 @@
         <v>1310.947643</v>
       </c>
       <c r="Q20" s="19">
-        <v>0</v>
+        <v>1233.593106</v>
       </c>
       <c r="R20" s="19">
-        <v>0</v>
+        <v>1149.510346</v>
       </c>
       <c r="S20" s="19">
-        <v>0</v>
+        <v>999.77497500000004</v>
       </c>
       <c r="T20" s="19">
-        <v>0</v>
+        <v>1082.8416589999999</v>
       </c>
       <c r="U20" s="19">
-        <v>0</v>
+        <v>982.84188900000004</v>
       </c>
       <c r="V20" s="19">
         <v>0</v>
@@ -28645,19 +28654,19 @@
         <v>941.79062299999998</v>
       </c>
       <c r="Q21" s="7">
-        <v>0</v>
+        <v>999.53377899999998</v>
       </c>
       <c r="R21" s="7">
-        <v>0</v>
+        <v>975.78376400000002</v>
       </c>
       <c r="S21" s="7">
-        <v>0</v>
+        <v>957.59569699999997</v>
       </c>
       <c r="T21" s="7">
-        <v>0</v>
+        <v>971.54684099999997</v>
       </c>
       <c r="U21" s="7">
-        <v>0</v>
+        <v>1027.445796</v>
       </c>
       <c r="V21" s="7">
         <v>0</v>
@@ -28807,19 +28816,19 @@
         <v>4662.910707</v>
       </c>
       <c r="Q22" s="8">
-        <v>0</v>
+        <v>4678.1503980000007</v>
       </c>
       <c r="R22" s="8">
-        <v>0</v>
+        <v>4451.8724249999996</v>
       </c>
       <c r="S22" s="8">
-        <v>0</v>
+        <v>4164.7989829999997</v>
       </c>
       <c r="T22" s="8">
-        <v>0</v>
+        <v>4349.1736270000001</v>
       </c>
       <c r="U22" s="8">
-        <v>0</v>
+        <v>4176.4029200000004</v>
       </c>
       <c r="V22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Fri Jul 21 15:47:24 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7867CE00-B791-41B4-82B9-6BB27B187EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -209,7 +210,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'2022'!$A:$A,'2022'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">'2023'!$A:$A,'2023'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -217,6 +218,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -457,7 +461,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -646,11 +650,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="5"/>
-    <cellStyle name="Percent 2" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1012,7 +1016,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4066,7 +4070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7152,7 +7156,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:BA54"/>
   <sheetViews>
@@ -10240,7 +10244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13315,11 +13319,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16386,18 +16390,15 @@
     <mergeCell ref="A1:BA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19684,14 +19685,11 @@
     <mergeCell ref="A1:BA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -19699,7 +19697,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22775,14 +22773,11 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -22790,7 +22785,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" sqref="A1:BA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23249,28 +23244,28 @@
         <v>6803</v>
       </c>
       <c r="V5" s="19">
-        <v>6785</v>
+        <v>6745</v>
       </c>
       <c r="W5" s="19">
-        <v>6590</v>
+        <v>6532</v>
       </c>
       <c r="X5" s="19">
-        <v>6565</v>
+        <v>6528</v>
       </c>
       <c r="Y5" s="19">
-        <v>6618</v>
+        <v>6576</v>
       </c>
       <c r="Z5" s="19">
-        <v>6387</v>
+        <v>6363</v>
       </c>
       <c r="AA5" s="19">
-        <v>6420</v>
+        <v>6402</v>
       </c>
       <c r="AB5" s="19">
-        <v>6799</v>
+        <v>6787</v>
       </c>
       <c r="AC5" s="19">
-        <v>6382</v>
+        <v>6356</v>
       </c>
       <c r="AD5" s="19">
         <v>6354</v>
@@ -23410,28 +23405,28 @@
         <v>12925</v>
       </c>
       <c r="V6" s="19">
-        <v>12923</v>
+        <v>12926</v>
       </c>
       <c r="W6" s="19">
-        <v>12036</v>
+        <v>12017</v>
       </c>
       <c r="X6" s="19">
         <v>12250</v>
       </c>
       <c r="Y6" s="19">
-        <v>12971</v>
+        <v>12953</v>
       </c>
       <c r="Z6" s="19">
-        <v>12710</v>
+        <v>12688</v>
       </c>
       <c r="AA6" s="19">
-        <v>12848</v>
+        <v>12839</v>
       </c>
       <c r="AB6" s="19">
-        <v>12210</v>
+        <v>12179</v>
       </c>
       <c r="AC6" s="19">
-        <v>13397</v>
+        <v>13335</v>
       </c>
       <c r="AD6" s="19">
         <v>12878</v>
@@ -23571,28 +23566,28 @@
         <v>19465</v>
       </c>
       <c r="V7" s="19">
-        <v>18481</v>
+        <v>19100</v>
       </c>
       <c r="W7" s="19">
-        <v>18054</v>
+        <v>18651</v>
       </c>
       <c r="X7" s="19">
-        <v>18871</v>
+        <v>19647</v>
       </c>
       <c r="Y7" s="19">
-        <v>18232</v>
+        <v>18671</v>
       </c>
       <c r="Z7" s="19">
-        <v>17655</v>
+        <v>18370</v>
       </c>
       <c r="AA7" s="19">
-        <v>19103</v>
+        <v>19898</v>
       </c>
       <c r="AB7" s="19">
-        <v>19009</v>
+        <v>19868</v>
       </c>
       <c r="AC7" s="19">
-        <v>18222</v>
+        <v>18860</v>
       </c>
       <c r="AD7" s="19">
         <v>18084</v>
@@ -23732,28 +23727,28 @@
         <v>4046</v>
       </c>
       <c r="V8" s="19">
-        <v>4703</v>
+        <v>4316</v>
       </c>
       <c r="W8" s="19">
-        <v>3901</v>
+        <v>3864</v>
       </c>
       <c r="X8" s="19">
-        <v>4268</v>
+        <v>4256</v>
       </c>
       <c r="Y8" s="19">
-        <v>4157</v>
+        <v>4148</v>
       </c>
       <c r="Z8" s="19">
-        <v>4119</v>
+        <v>4116</v>
       </c>
       <c r="AA8" s="19">
-        <v>4310</v>
+        <v>4273</v>
       </c>
       <c r="AB8" s="19">
-        <v>2905</v>
+        <v>2895</v>
       </c>
       <c r="AC8" s="19">
-        <v>3805</v>
+        <v>3799</v>
       </c>
       <c r="AD8" s="19">
         <v>3850</v>
@@ -23893,28 +23888,28 @@
         <v>9071</v>
       </c>
       <c r="V9" s="19">
-        <v>9576</v>
+        <v>9573</v>
       </c>
       <c r="W9" s="19">
-        <v>8455</v>
+        <v>8330</v>
       </c>
       <c r="X9" s="19">
-        <v>8843</v>
+        <v>8691</v>
       </c>
       <c r="Y9" s="19">
-        <v>10070</v>
+        <v>9952</v>
       </c>
       <c r="Z9" s="19">
-        <v>8574</v>
+        <v>8587</v>
       </c>
       <c r="AA9" s="19">
-        <v>10382</v>
+        <v>10387</v>
       </c>
       <c r="AB9" s="19">
-        <v>8483</v>
+        <v>8464</v>
       </c>
       <c r="AC9" s="19">
-        <v>10048</v>
+        <v>9823</v>
       </c>
       <c r="AD9" s="19">
         <v>9349</v>
@@ -24054,28 +24049,28 @@
         <v>9664</v>
       </c>
       <c r="V10" s="19">
-        <v>10728</v>
+        <v>10718</v>
       </c>
       <c r="W10" s="19">
-        <v>10275</v>
+        <v>10273</v>
       </c>
       <c r="X10" s="19">
-        <v>10899</v>
+        <v>10888</v>
       </c>
       <c r="Y10" s="19">
-        <v>10241</v>
+        <v>10099</v>
       </c>
       <c r="Z10" s="19">
-        <v>11144</v>
+        <v>11093</v>
       </c>
       <c r="AA10" s="19">
-        <v>9847</v>
+        <v>9826</v>
       </c>
       <c r="AB10" s="19">
-        <v>9993</v>
+        <v>9980</v>
       </c>
       <c r="AC10" s="19">
-        <v>10842</v>
+        <v>10822</v>
       </c>
       <c r="AD10" s="19">
         <v>9742</v>
@@ -24215,28 +24210,28 @@
         <v>53269</v>
       </c>
       <c r="V11" s="19">
-        <v>46580</v>
+        <v>46488</v>
       </c>
       <c r="W11" s="19">
-        <v>45632</v>
+        <v>45547</v>
       </c>
       <c r="X11" s="19">
-        <v>48834</v>
+        <v>48757</v>
       </c>
       <c r="Y11" s="19">
-        <v>48715</v>
+        <v>48598</v>
       </c>
       <c r="Z11" s="19">
-        <v>48231</v>
+        <v>48136</v>
       </c>
       <c r="AA11" s="19">
-        <v>46295</v>
+        <v>46213</v>
       </c>
       <c r="AB11" s="19">
-        <v>43366</v>
+        <v>43310</v>
       </c>
       <c r="AC11" s="19">
-        <v>47845</v>
+        <v>47708</v>
       </c>
       <c r="AD11" s="19">
         <v>46954</v>
@@ -24376,28 +24371,28 @@
         <v>115243</v>
       </c>
       <c r="V12" s="8">
-        <v>109776</v>
+        <v>109866</v>
       </c>
       <c r="W12" s="8">
-        <v>104943</v>
+        <v>105214</v>
       </c>
       <c r="X12" s="8">
-        <v>110530</v>
+        <v>111017</v>
       </c>
       <c r="Y12" s="8">
-        <v>111004</v>
+        <v>110997</v>
       </c>
       <c r="Z12" s="8">
-        <v>108820</v>
+        <v>109353</v>
       </c>
       <c r="AA12" s="8">
-        <v>109205</v>
+        <v>109838</v>
       </c>
       <c r="AB12" s="8">
-        <v>102765</v>
+        <v>103483</v>
       </c>
       <c r="AC12" s="8">
-        <v>110541</v>
+        <v>110703</v>
       </c>
       <c r="AD12" s="8">
         <v>107211</v>
@@ -24597,28 +24592,28 @@
         <v>536.86192600000004</v>
       </c>
       <c r="V15" s="19">
-        <v>522.878241</v>
+        <v>517.94164799999999</v>
       </c>
       <c r="W15" s="19">
-        <v>513.57559000000003</v>
+        <v>504.69518299999999</v>
       </c>
       <c r="X15" s="19">
-        <v>504.01653900000002</v>
+        <v>500.265964</v>
       </c>
       <c r="Y15" s="19">
-        <v>508.53476999999998</v>
+        <v>504.263757</v>
       </c>
       <c r="Z15" s="19">
-        <v>497.74014</v>
+        <v>494.79659400000003</v>
       </c>
       <c r="AA15" s="19">
-        <v>472.632722</v>
+        <v>471.36597399999999</v>
       </c>
       <c r="AB15" s="19">
-        <v>533.95508099999995</v>
+        <v>532.91853800000001</v>
       </c>
       <c r="AC15" s="19">
-        <v>490.36651999999998</v>
+        <v>488.45613400000002</v>
       </c>
       <c r="AD15" s="19">
         <v>486.44936799999999</v>
@@ -24758,28 +24753,28 @@
         <v>1009.54049</v>
       </c>
       <c r="V16" s="19">
-        <v>1023.1000759999999</v>
+        <v>1023.26358</v>
       </c>
       <c r="W16" s="19">
-        <v>904.17510600000003</v>
+        <v>903.48814200000004</v>
       </c>
       <c r="X16" s="19">
-        <v>912.79521599999998</v>
+        <v>912.480053</v>
       </c>
       <c r="Y16" s="19">
-        <v>1022.942935</v>
+        <v>1022.455698</v>
       </c>
       <c r="Z16" s="19">
-        <v>979.27359300000001</v>
+        <v>977.82944699999996</v>
       </c>
       <c r="AA16" s="19">
-        <v>1003.994995</v>
+        <v>1003.541155</v>
       </c>
       <c r="AB16" s="19">
-        <v>907.45244700000001</v>
+        <v>906.49024399999996</v>
       </c>
       <c r="AC16" s="19">
-        <v>1027.244416</v>
+        <v>1025.5985619999999</v>
       </c>
       <c r="AD16" s="19">
         <v>927.79104500000005</v>
@@ -24919,28 +24914,28 @@
         <v>535.50898099999995</v>
       </c>
       <c r="V17" s="19">
-        <v>513.87695799999995</v>
+        <v>514.992165</v>
       </c>
       <c r="W17" s="19">
-        <v>616.784896</v>
+        <v>617.63611500000002</v>
       </c>
       <c r="X17" s="19">
-        <v>566.06272200000001</v>
+        <v>564.75128299999994</v>
       </c>
       <c r="Y17" s="19">
-        <v>463.835354</v>
+        <v>462.85923400000001</v>
       </c>
       <c r="Z17" s="19">
-        <v>592.32104200000003</v>
+        <v>592.49319000000003</v>
       </c>
       <c r="AA17" s="19">
-        <v>598.164627</v>
+        <v>597.50664099999995</v>
       </c>
       <c r="AB17" s="19">
-        <v>549.88331100000005</v>
+        <v>549.83667100000002</v>
       </c>
       <c r="AC17" s="19">
-        <v>596.79686300000003</v>
+        <v>593.94559700000002</v>
       </c>
       <c r="AD17" s="19">
         <v>573.85811200000001</v>
@@ -25080,28 +25075,28 @@
         <v>56.522060000000003</v>
       </c>
       <c r="V18" s="19">
-        <v>60.147862000000003</v>
+        <v>57.870513000000003</v>
       </c>
       <c r="W18" s="19">
-        <v>54.392234999999999</v>
+        <v>50.581288000000001</v>
       </c>
       <c r="X18" s="19">
-        <v>52.852564999999998</v>
+        <v>52.399251</v>
       </c>
       <c r="Y18" s="19">
-        <v>54.441620999999998</v>
+        <v>54.341121000000001</v>
       </c>
       <c r="Z18" s="19">
-        <v>54.798143000000003</v>
+        <v>54.757174999999997</v>
       </c>
       <c r="AA18" s="19">
-        <v>63.190283000000001</v>
+        <v>61.191991000000002</v>
       </c>
       <c r="AB18" s="19">
-        <v>40.299790999999999</v>
+        <v>39.860756000000002</v>
       </c>
       <c r="AC18" s="19">
-        <v>54.476950000000002</v>
+        <v>54.438403000000001</v>
       </c>
       <c r="AD18" s="19">
         <v>53.185364</v>
@@ -25241,28 +25236,28 @@
         <v>486.64239400000002</v>
       </c>
       <c r="V19" s="19">
-        <v>463.72209099999998</v>
+        <v>462.50297</v>
       </c>
       <c r="W19" s="19">
-        <v>399.10927500000003</v>
+        <v>397.87539400000003</v>
       </c>
       <c r="X19" s="19">
-        <v>433.901814</v>
+        <v>429.03827899999999</v>
       </c>
       <c r="Y19" s="19">
-        <v>429.45035999999999</v>
+        <v>429.24479600000001</v>
       </c>
       <c r="Z19" s="19">
-        <v>429.099559</v>
+        <v>430.33106299999997</v>
       </c>
       <c r="AA19" s="19">
-        <v>453.37525399999998</v>
+        <v>453.62610699999999</v>
       </c>
       <c r="AB19" s="19">
-        <v>372.089201</v>
+        <v>371.65583400000003</v>
       </c>
       <c r="AC19" s="19">
-        <v>463.23593599999998</v>
+        <v>463.14434299999999</v>
       </c>
       <c r="AD19" s="19">
         <v>467.53570400000001</v>
@@ -25402,28 +25397,28 @@
         <v>838.65342099999998</v>
       </c>
       <c r="V20" s="19">
-        <v>940.15265499999998</v>
+        <v>939.21193200000005</v>
       </c>
       <c r="W20" s="19">
-        <v>831.33720600000004</v>
+        <v>831.32986000000005</v>
       </c>
       <c r="X20" s="19">
-        <v>967.18809199999998</v>
+        <v>965.96833900000001</v>
       </c>
       <c r="Y20" s="19">
-        <v>834.19719099999998</v>
+        <v>833.46183900000005</v>
       </c>
       <c r="Z20" s="19">
-        <v>967.34926199999995</v>
+        <v>965.05006200000003</v>
       </c>
       <c r="AA20" s="19">
-        <v>796.73028599999998</v>
+        <v>797.42609600000003</v>
       </c>
       <c r="AB20" s="19">
-        <v>908.43747499999995</v>
+        <v>909.34286599999996</v>
       </c>
       <c r="AC20" s="19">
-        <v>939.98175300000003</v>
+        <v>940.220913</v>
       </c>
       <c r="AD20" s="19">
         <v>884.96621100000004</v>
@@ -25563,28 +25558,28 @@
         <v>1248.7928939999999</v>
       </c>
       <c r="V21" s="19">
-        <v>1082.948676</v>
+        <v>1081.822795</v>
       </c>
       <c r="W21" s="19">
-        <v>989.93198500000005</v>
+        <v>989.74261300000001</v>
       </c>
       <c r="X21" s="19">
-        <v>1139.657279</v>
+        <v>1139.018896</v>
       </c>
       <c r="Y21" s="19">
-        <v>1063.0727039999999</v>
+        <v>1062.7640530000001</v>
       </c>
       <c r="Z21" s="19">
-        <v>1080.0218870000001</v>
+        <v>1079.319424</v>
       </c>
       <c r="AA21" s="19">
-        <v>971.67633499999999</v>
+        <v>970.87710400000003</v>
       </c>
       <c r="AB21" s="19">
-        <v>1008.254716</v>
+        <v>1007.751482</v>
       </c>
       <c r="AC21" s="19">
-        <v>1086.4416839999999</v>
+        <v>1083.1445309999999</v>
       </c>
       <c r="AD21" s="19">
         <v>1076.656798</v>
@@ -25724,28 +25719,28 @@
         <v>4712.5221659999997</v>
       </c>
       <c r="V22" s="8">
-        <v>4606.8265589999992</v>
+        <v>4597.605603</v>
       </c>
       <c r="W22" s="8">
-        <v>4309.3062930000006</v>
+        <v>4295.3485950000004</v>
       </c>
       <c r="X22" s="8">
-        <v>4576.4742269999997</v>
+        <v>4563.9220650000007</v>
       </c>
       <c r="Y22" s="8">
-        <v>4376.4749350000002</v>
+        <v>4369.3904979999998</v>
       </c>
       <c r="Z22" s="8">
-        <v>4600.6036260000001</v>
+        <v>4594.5769550000005</v>
       </c>
       <c r="AA22" s="8">
-        <v>4359.764502</v>
+        <v>4355.5350680000001</v>
       </c>
       <c r="AB22" s="8">
-        <v>4320.3720220000005</v>
+        <v>4317.8563910000003</v>
       </c>
       <c r="AC22" s="8">
-        <v>4658.5441220000002</v>
+        <v>4648.9484830000001</v>
       </c>
       <c r="AD22" s="8">
         <v>4470.4426019999992</v>
@@ -25873,12 +25868,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:BA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26339,28 +26334,28 @@
         <v>6094</v>
       </c>
       <c r="V5" s="19">
-        <v>0</v>
+        <v>5903</v>
       </c>
       <c r="W5" s="19">
-        <v>0</v>
+        <v>6111</v>
       </c>
       <c r="X5" s="19">
-        <v>0</v>
+        <v>5714</v>
       </c>
       <c r="Y5" s="19">
-        <v>0</v>
+        <v>5607</v>
       </c>
       <c r="Z5" s="19">
-        <v>0</v>
+        <v>5883</v>
       </c>
       <c r="AA5" s="19">
-        <v>0</v>
+        <v>5633</v>
       </c>
       <c r="AB5" s="19">
-        <v>0</v>
+        <v>5418</v>
       </c>
       <c r="AC5" s="19">
-        <v>0</v>
+        <v>5689</v>
       </c>
       <c r="AD5" s="19">
         <v>0</v>
@@ -26501,28 +26496,28 @@
         <v>11689</v>
       </c>
       <c r="V6" s="7">
-        <v>0</v>
+        <v>11815</v>
       </c>
       <c r="W6" s="7">
-        <v>0</v>
+        <v>11482</v>
       </c>
       <c r="X6" s="7">
-        <v>0</v>
+        <v>12124</v>
       </c>
       <c r="Y6" s="7">
-        <v>0</v>
+        <v>11455</v>
       </c>
       <c r="Z6" s="7">
-        <v>0</v>
+        <v>11939</v>
       </c>
       <c r="AA6" s="7">
-        <v>0</v>
+        <v>11646</v>
       </c>
       <c r="AB6" s="7">
-        <v>0</v>
+        <v>11164</v>
       </c>
       <c r="AC6" s="7">
-        <v>0</v>
+        <v>11259</v>
       </c>
       <c r="AD6" s="7">
         <v>0</v>
@@ -26663,28 +26658,28 @@
         <v>17811</v>
       </c>
       <c r="V7" s="7">
-        <v>0</v>
+        <v>17218</v>
       </c>
       <c r="W7" s="7">
-        <v>0</v>
+        <v>17978</v>
       </c>
       <c r="X7" s="7">
-        <v>0</v>
+        <v>17789</v>
       </c>
       <c r="Y7" s="7">
-        <v>0</v>
+        <v>18107</v>
       </c>
       <c r="Z7" s="7">
-        <v>0</v>
+        <v>19511</v>
       </c>
       <c r="AA7" s="7">
-        <v>0</v>
+        <v>17750</v>
       </c>
       <c r="AB7" s="7">
-        <v>0</v>
+        <v>19367</v>
       </c>
       <c r="AC7" s="7">
-        <v>0</v>
+        <v>20521</v>
       </c>
       <c r="AD7" s="7">
         <v>0</v>
@@ -26825,28 +26820,28 @@
         <v>4645</v>
       </c>
       <c r="V8" s="7">
-        <v>0</v>
+        <v>4326</v>
       </c>
       <c r="W8" s="7">
-        <v>0</v>
+        <v>4198</v>
       </c>
       <c r="X8" s="7">
-        <v>0</v>
+        <v>4504</v>
       </c>
       <c r="Y8" s="7">
-        <v>0</v>
+        <v>4436</v>
       </c>
       <c r="Z8" s="7">
-        <v>0</v>
+        <v>4488</v>
       </c>
       <c r="AA8" s="7">
-        <v>0</v>
+        <v>4506</v>
       </c>
       <c r="AB8" s="7">
-        <v>0</v>
+        <v>3850</v>
       </c>
       <c r="AC8" s="7">
-        <v>0</v>
+        <v>4079</v>
       </c>
       <c r="AD8" s="7">
         <v>0</v>
@@ -26987,28 +26982,28 @@
         <v>10276</v>
       </c>
       <c r="V9" s="7">
-        <v>0</v>
+        <v>9658</v>
       </c>
       <c r="W9" s="7">
-        <v>0</v>
+        <v>10986</v>
       </c>
       <c r="X9" s="7">
-        <v>0</v>
+        <v>8938</v>
       </c>
       <c r="Y9" s="7">
-        <v>0</v>
+        <v>9904</v>
       </c>
       <c r="Z9" s="7">
-        <v>0</v>
+        <v>9977</v>
       </c>
       <c r="AA9" s="7">
-        <v>0</v>
+        <v>8902</v>
       </c>
       <c r="AB9" s="7">
-        <v>0</v>
+        <v>7692</v>
       </c>
       <c r="AC9" s="7">
-        <v>0</v>
+        <v>8195</v>
       </c>
       <c r="AD9" s="7">
         <v>0</v>
@@ -27149,28 +27144,28 @@
         <v>11421</v>
       </c>
       <c r="V10" s="19">
-        <v>0</v>
+        <v>11844</v>
       </c>
       <c r="W10" s="19">
-        <v>0</v>
+        <v>10312</v>
       </c>
       <c r="X10" s="19">
-        <v>0</v>
+        <v>10900</v>
       </c>
       <c r="Y10" s="19">
-        <v>0</v>
+        <v>10552</v>
       </c>
       <c r="Z10" s="19">
-        <v>0</v>
+        <v>10129</v>
       </c>
       <c r="AA10" s="19">
-        <v>0</v>
+        <v>10161</v>
       </c>
       <c r="AB10" s="19">
-        <v>0</v>
+        <v>10591</v>
       </c>
       <c r="AC10" s="19">
-        <v>0</v>
+        <v>10494</v>
       </c>
       <c r="AD10" s="19">
         <v>0</v>
@@ -27311,28 +27306,28 @@
         <v>45248</v>
       </c>
       <c r="V11" s="7">
-        <v>0</v>
+        <v>45213</v>
       </c>
       <c r="W11" s="7">
-        <v>0</v>
+        <v>42851</v>
       </c>
       <c r="X11" s="7">
-        <v>0</v>
+        <v>42100</v>
       </c>
       <c r="Y11" s="7">
-        <v>0</v>
+        <v>44391</v>
       </c>
       <c r="Z11" s="7">
-        <v>0</v>
+        <v>41606</v>
       </c>
       <c r="AA11" s="7">
-        <v>0</v>
+        <v>38447</v>
       </c>
       <c r="AB11" s="7">
-        <v>0</v>
+        <v>21776</v>
       </c>
       <c r="AC11" s="7">
-        <v>0</v>
+        <v>27594</v>
       </c>
       <c r="AD11" s="7">
         <v>0</v>
@@ -27473,28 +27468,28 @@
         <v>107184</v>
       </c>
       <c r="V12" s="8">
-        <v>0</v>
+        <v>105977</v>
       </c>
       <c r="W12" s="8">
-        <v>0</v>
+        <v>103918</v>
       </c>
       <c r="X12" s="8">
-        <v>0</v>
+        <v>102069</v>
       </c>
       <c r="Y12" s="8">
-        <v>0</v>
+        <v>104452</v>
       </c>
       <c r="Z12" s="8">
-        <v>0</v>
+        <v>103533</v>
       </c>
       <c r="AA12" s="8">
-        <v>0</v>
+        <v>97045</v>
       </c>
       <c r="AB12" s="8">
-        <v>0</v>
+        <v>79858</v>
       </c>
       <c r="AC12" s="8">
-        <v>0</v>
+        <v>87831</v>
       </c>
       <c r="AD12" s="8">
         <v>0</v>
@@ -27697,28 +27692,28 @@
         <v>458.53278699999998</v>
       </c>
       <c r="V15" s="19">
-        <v>0</v>
+        <v>415.48274900000001</v>
       </c>
       <c r="W15" s="19">
-        <v>0</v>
+        <v>433.72582199999999</v>
       </c>
       <c r="X15" s="19">
-        <v>0</v>
+        <v>424.27063500000003</v>
       </c>
       <c r="Y15" s="19">
-        <v>0</v>
+        <v>433.658118</v>
       </c>
       <c r="Z15" s="19">
-        <v>0</v>
+        <v>431.76906100000002</v>
       </c>
       <c r="AA15" s="19">
-        <v>0</v>
+        <v>406.32294899999999</v>
       </c>
       <c r="AB15" s="19">
-        <v>0</v>
+        <v>412.20952399999999</v>
       </c>
       <c r="AC15" s="19">
-        <v>0</v>
+        <v>456.77306299999998</v>
       </c>
       <c r="AD15" s="19">
         <v>0</v>
@@ -27859,28 +27854,28 @@
         <v>806.95998999999995</v>
       </c>
       <c r="V16" s="7">
-        <v>0</v>
+        <v>802.72468000000003</v>
       </c>
       <c r="W16" s="7">
-        <v>0</v>
+        <v>778.58543499999996</v>
       </c>
       <c r="X16" s="7">
-        <v>0</v>
+        <v>821.83652400000005</v>
       </c>
       <c r="Y16" s="7">
-        <v>0</v>
+        <v>776.07931099999996</v>
       </c>
       <c r="Z16" s="7">
-        <v>0</v>
+        <v>787.45627300000001</v>
       </c>
       <c r="AA16" s="7">
-        <v>0</v>
+        <v>795.98168299999998</v>
       </c>
       <c r="AB16" s="7">
-        <v>0</v>
+        <v>750.15164900000002</v>
       </c>
       <c r="AC16" s="7">
-        <v>0</v>
+        <v>708.67453699999999</v>
       </c>
       <c r="AD16" s="7">
         <v>0</v>
@@ -28021,28 +28016,28 @@
         <v>368.55136499999998</v>
       </c>
       <c r="V17" s="7">
-        <v>0</v>
+        <v>488.59335800000002</v>
       </c>
       <c r="W17" s="7">
-        <v>0</v>
+        <v>538.76317700000004</v>
       </c>
       <c r="X17" s="7">
-        <v>0</v>
+        <v>477.33451100000002</v>
       </c>
       <c r="Y17" s="7">
-        <v>0</v>
+        <v>600.06695100000002</v>
       </c>
       <c r="Z17" s="7">
-        <v>0</v>
+        <v>550.41994</v>
       </c>
       <c r="AA17" s="7">
-        <v>0</v>
+        <v>628.21312</v>
       </c>
       <c r="AB17" s="7">
-        <v>0</v>
+        <v>582.98972200000003</v>
       </c>
       <c r="AC17" s="7">
-        <v>0</v>
+        <v>609.38806799999998</v>
       </c>
       <c r="AD17" s="7">
         <v>0</v>
@@ -28183,28 +28178,28 @@
         <v>65.464646999999999</v>
       </c>
       <c r="V18" s="7">
-        <v>0</v>
+        <v>56.386600999999999</v>
       </c>
       <c r="W18" s="7">
-        <v>0</v>
+        <v>62.160359</v>
       </c>
       <c r="X18" s="7">
-        <v>0</v>
+        <v>58.661459000000001</v>
       </c>
       <c r="Y18" s="7">
-        <v>0</v>
+        <v>59.404023000000002</v>
       </c>
       <c r="Z18" s="7">
-        <v>0</v>
+        <v>58.500211999999998</v>
       </c>
       <c r="AA18" s="7">
-        <v>0</v>
+        <v>61.894596</v>
       </c>
       <c r="AB18" s="7">
-        <v>0</v>
+        <v>60.351329999999997</v>
       </c>
       <c r="AC18" s="7">
-        <v>0</v>
+        <v>57.832172999999997</v>
       </c>
       <c r="AD18" s="7">
         <v>0</v>
@@ -28345,28 +28340,28 @@
         <v>466.60644600000001</v>
       </c>
       <c r="V19" s="7">
-        <v>0</v>
+        <v>453.20647000000002</v>
       </c>
       <c r="W19" s="7">
-        <v>0</v>
+        <v>475.640128</v>
       </c>
       <c r="X19" s="7">
-        <v>0</v>
+        <v>398.268778</v>
       </c>
       <c r="Y19" s="7">
-        <v>0</v>
+        <v>427.43161300000003</v>
       </c>
       <c r="Z19" s="7">
-        <v>0</v>
+        <v>403.74583899999999</v>
       </c>
       <c r="AA19" s="7">
-        <v>0</v>
+        <v>394.585061</v>
       </c>
       <c r="AB19" s="7">
-        <v>0</v>
+        <v>378.00727899999998</v>
       </c>
       <c r="AC19" s="7">
-        <v>0</v>
+        <v>491.01799699999998</v>
       </c>
       <c r="AD19" s="7">
         <v>0</v>
@@ -28507,28 +28502,28 @@
         <v>982.84188900000004</v>
       </c>
       <c r="V20" s="19">
-        <v>0</v>
+        <v>1079.901462</v>
       </c>
       <c r="W20" s="19">
-        <v>0</v>
+        <v>814.00307999999995</v>
       </c>
       <c r="X20" s="19">
-        <v>0</v>
+        <v>967.94014900000002</v>
       </c>
       <c r="Y20" s="19">
-        <v>0</v>
+        <v>879.01019799999995</v>
       </c>
       <c r="Z20" s="19">
-        <v>0</v>
+        <v>892.88511900000003</v>
       </c>
       <c r="AA20" s="19">
-        <v>0</v>
+        <v>935.19036300000005</v>
       </c>
       <c r="AB20" s="19">
-        <v>0</v>
+        <v>1009.999856</v>
       </c>
       <c r="AC20" s="19">
-        <v>0</v>
+        <v>951.72299699999996</v>
       </c>
       <c r="AD20" s="19">
         <v>0</v>
@@ -28669,28 +28664,28 @@
         <v>1027.445796</v>
       </c>
       <c r="V21" s="7">
-        <v>0</v>
+        <v>1035.9219900000001</v>
       </c>
       <c r="W21" s="7">
-        <v>0</v>
+        <v>1000.069224</v>
       </c>
       <c r="X21" s="7">
-        <v>0</v>
+        <v>948.19993999999997</v>
       </c>
       <c r="Y21" s="7">
-        <v>0</v>
+        <v>974.32790699999998</v>
       </c>
       <c r="Z21" s="7">
-        <v>0</v>
+        <v>957.69723099999999</v>
       </c>
       <c r="AA21" s="7">
-        <v>0</v>
+        <v>899.67968699999994</v>
       </c>
       <c r="AB21" s="7">
-        <v>0</v>
+        <v>415.64295800000002</v>
       </c>
       <c r="AC21" s="7">
-        <v>0</v>
+        <v>581.68658300000004</v>
       </c>
       <c r="AD21" s="7">
         <v>0</v>
@@ -28831,28 +28826,28 @@
         <v>4176.4029200000004</v>
       </c>
       <c r="V22" s="8">
-        <v>0</v>
+        <v>4332.21731</v>
       </c>
       <c r="W22" s="8">
-        <v>0</v>
+        <v>4102.9472249999999</v>
       </c>
       <c r="X22" s="8">
-        <v>0</v>
+        <v>4096.5119960000002</v>
       </c>
       <c r="Y22" s="8">
-        <v>0</v>
+        <v>4149.9781210000001</v>
       </c>
       <c r="Z22" s="8">
-        <v>0</v>
+        <v>4082.4736750000002</v>
       </c>
       <c r="AA22" s="8">
-        <v>0</v>
+        <v>4121.8674590000001</v>
       </c>
       <c r="AB22" s="8">
-        <v>0</v>
+        <v>3609.3523179999997</v>
       </c>
       <c r="AC22" s="8">
-        <v>0</v>
+        <v>3857.0954179999999</v>
       </c>
       <c r="AD22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jul 25 05:24:10 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7867CE00-B791-41B4-82B9-6BB27B187EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{777CB22C-FF3E-44EC-AED7-11E86F5C75B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4066,6 +4066,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -7152,6 +7155,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -10240,6 +10246,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -13315,6 +13324,9 @@
     <mergeCell ref="A1:BA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -16390,6 +16402,9 @@
     <mergeCell ref="A1:BA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -19685,6 +19700,9 @@
     <mergeCell ref="A1:BA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -22773,6 +22791,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -23268,7 +23289,7 @@
         <v>6356</v>
       </c>
       <c r="AD5" s="19">
-        <v>6354</v>
+        <v>6334</v>
       </c>
       <c r="AE5" s="19">
         <v>6627</v>
@@ -23429,7 +23450,7 @@
         <v>13335</v>
       </c>
       <c r="AD6" s="19">
-        <v>12878</v>
+        <v>12862</v>
       </c>
       <c r="AE6" s="19">
         <v>12346</v>
@@ -23590,7 +23611,7 @@
         <v>18860</v>
       </c>
       <c r="AD7" s="19">
-        <v>18084</v>
+        <v>18696</v>
       </c>
       <c r="AE7" s="19">
         <v>17373</v>
@@ -23751,7 +23772,7 @@
         <v>3799</v>
       </c>
       <c r="AD8" s="19">
-        <v>3850</v>
+        <v>3834</v>
       </c>
       <c r="AE8" s="19">
         <v>4000</v>
@@ -24073,7 +24094,7 @@
         <v>10822</v>
       </c>
       <c r="AD10" s="19">
-        <v>9742</v>
+        <v>9711</v>
       </c>
       <c r="AE10" s="19">
         <v>9656</v>
@@ -24234,7 +24255,7 @@
         <v>47708</v>
       </c>
       <c r="AD11" s="19">
-        <v>46954</v>
+        <v>46851</v>
       </c>
       <c r="AE11" s="19">
         <v>50157</v>
@@ -24395,7 +24416,7 @@
         <v>110703</v>
       </c>
       <c r="AD12" s="8">
-        <v>107211</v>
+        <v>107637</v>
       </c>
       <c r="AE12" s="8">
         <v>110952</v>
@@ -24616,7 +24637,7 @@
         <v>488.45613400000002</v>
       </c>
       <c r="AD15" s="19">
-        <v>486.44936799999999</v>
+        <v>483.95710300000002</v>
       </c>
       <c r="AE15" s="19">
         <v>521.60046</v>
@@ -24777,7 +24798,7 @@
         <v>1025.5985619999999</v>
       </c>
       <c r="AD16" s="19">
-        <v>927.79104500000005</v>
+        <v>927.86779000000001</v>
       </c>
       <c r="AE16" s="19">
         <v>910.62362599999994</v>
@@ -24938,7 +24959,7 @@
         <v>593.94559700000002</v>
       </c>
       <c r="AD17" s="19">
-        <v>573.85811200000001</v>
+        <v>573.29124000000002</v>
       </c>
       <c r="AE17" s="19">
         <v>572.16166199999998</v>
@@ -25099,7 +25120,7 @@
         <v>54.438403000000001</v>
       </c>
       <c r="AD18" s="19">
-        <v>53.185364</v>
+        <v>52.864941000000002</v>
       </c>
       <c r="AE18" s="19">
         <v>54.601064000000001</v>
@@ -25260,7 +25281,7 @@
         <v>463.14434299999999</v>
       </c>
       <c r="AD19" s="19">
-        <v>467.53570400000001</v>
+        <v>467.57713999999999</v>
       </c>
       <c r="AE19" s="19">
         <v>418.123786</v>
@@ -25421,7 +25442,7 @@
         <v>940.220913</v>
       </c>
       <c r="AD20" s="19">
-        <v>884.96621100000004</v>
+        <v>884.16366500000004</v>
       </c>
       <c r="AE20" s="19">
         <v>866.89913100000001</v>
@@ -25582,7 +25603,7 @@
         <v>1083.1445309999999</v>
       </c>
       <c r="AD21" s="19">
-        <v>1076.656798</v>
+        <v>1075.892936</v>
       </c>
       <c r="AE21" s="19">
         <v>1097.4848999999999</v>
@@ -25743,7 +25764,7 @@
         <v>4648.9484830000001</v>
       </c>
       <c r="AD22" s="8">
-        <v>4470.4426019999992</v>
+        <v>4465.6148149999999</v>
       </c>
       <c r="AE22" s="8">
         <v>4441.4946290000007</v>
@@ -26358,7 +26379,7 @@
         <v>5689</v>
       </c>
       <c r="AD5" s="19">
-        <v>0</v>
+        <v>5606</v>
       </c>
       <c r="AE5" s="19">
         <v>0</v>
@@ -26520,7 +26541,7 @@
         <v>11259</v>
       </c>
       <c r="AD6" s="7">
-        <v>0</v>
+        <v>11991</v>
       </c>
       <c r="AE6" s="7">
         <v>0</v>
@@ -26682,7 +26703,7 @@
         <v>20521</v>
       </c>
       <c r="AD7" s="7">
-        <v>0</v>
+        <v>19911</v>
       </c>
       <c r="AE7" s="7">
         <v>0</v>
@@ -26844,7 +26865,7 @@
         <v>4079</v>
       </c>
       <c r="AD8" s="7">
-        <v>0</v>
+        <v>4757</v>
       </c>
       <c r="AE8" s="7">
         <v>0</v>
@@ -27006,7 +27027,7 @@
         <v>8195</v>
       </c>
       <c r="AD9" s="7">
-        <v>0</v>
+        <v>9725</v>
       </c>
       <c r="AE9" s="7">
         <v>0</v>
@@ -27168,7 +27189,7 @@
         <v>10494</v>
       </c>
       <c r="AD10" s="19">
-        <v>0</v>
+        <v>11942</v>
       </c>
       <c r="AE10" s="19">
         <v>0</v>
@@ -27330,7 +27351,7 @@
         <v>27594</v>
       </c>
       <c r="AD11" s="7">
-        <v>0</v>
+        <v>40835</v>
       </c>
       <c r="AE11" s="7">
         <v>0</v>
@@ -27492,7 +27513,7 @@
         <v>87831</v>
       </c>
       <c r="AD12" s="8">
-        <v>0</v>
+        <v>104767</v>
       </c>
       <c r="AE12" s="8">
         <v>0</v>
@@ -27716,7 +27737,7 @@
         <v>456.77306299999998</v>
       </c>
       <c r="AD15" s="19">
-        <v>0</v>
+        <v>422.21685400000001</v>
       </c>
       <c r="AE15" s="19">
         <v>0</v>
@@ -27878,7 +27899,7 @@
         <v>708.67453699999999</v>
       </c>
       <c r="AD16" s="7">
-        <v>0</v>
+        <v>797.01322000000005</v>
       </c>
       <c r="AE16" s="7">
         <v>0</v>
@@ -28040,7 +28061,7 @@
         <v>609.38806799999998</v>
       </c>
       <c r="AD17" s="7">
-        <v>0</v>
+        <v>668.70617600000003</v>
       </c>
       <c r="AE17" s="7">
         <v>0</v>
@@ -28202,7 +28223,7 @@
         <v>57.832172999999997</v>
       </c>
       <c r="AD18" s="7">
-        <v>0</v>
+        <v>65.103791999999999</v>
       </c>
       <c r="AE18" s="7">
         <v>0</v>
@@ -28364,7 +28385,7 @@
         <v>491.01799699999998</v>
       </c>
       <c r="AD19" s="7">
-        <v>0</v>
+        <v>384.47404599999999</v>
       </c>
       <c r="AE19" s="7">
         <v>0</v>
@@ -28526,7 +28547,7 @@
         <v>951.72299699999996</v>
       </c>
       <c r="AD20" s="19">
-        <v>0</v>
+        <v>1150.8910430000001</v>
       </c>
       <c r="AE20" s="19">
         <v>0</v>
@@ -28688,7 +28709,7 @@
         <v>581.68658300000004</v>
       </c>
       <c r="AD21" s="7">
-        <v>0</v>
+        <v>943.95793700000002</v>
       </c>
       <c r="AE21" s="7">
         <v>0</v>
@@ -28850,7 +28871,7 @@
         <v>3857.0954179999999</v>
       </c>
       <c r="AD22" s="8">
-        <v>0</v>
+        <v>4432.3630679999997</v>
       </c>
       <c r="AE22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Aug  1 05:22:37 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{777CB22C-FF3E-44EC-AED7-11E86F5C75B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -210,7 +209,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'2022'!$A:$A,'2022'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">'2023'!$A:$A,'2023'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -461,7 +460,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -650,11 +649,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 3" xfId="5"/>
+    <cellStyle name="Percent 2" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1016,7 +1015,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4066,14 +4065,11 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7155,14 +7151,11 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:BA54"/>
   <sheetViews>
@@ -10246,14 +10239,11 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13324,14 +13314,11 @@
     <mergeCell ref="A1:BA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16402,14 +16389,11 @@
     <mergeCell ref="A1:BA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19700,14 +19684,11 @@
     <mergeCell ref="A1:BA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -22791,14 +22772,11 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -22806,7 +22784,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" sqref="A1:BA1"/>
+      <selection pane="bottomRight" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23292,7 +23270,7 @@
         <v>6334</v>
       </c>
       <c r="AE5" s="19">
-        <v>6627</v>
+        <v>6618</v>
       </c>
       <c r="AF5" s="19">
         <v>6316</v>
@@ -23453,7 +23431,7 @@
         <v>12862</v>
       </c>
       <c r="AE6" s="19">
-        <v>12346</v>
+        <v>12335</v>
       </c>
       <c r="AF6" s="19">
         <v>12014</v>
@@ -23614,7 +23592,7 @@
         <v>18696</v>
       </c>
       <c r="AE7" s="19">
-        <v>17373</v>
+        <v>17917</v>
       </c>
       <c r="AF7" s="19">
         <v>19442</v>
@@ -23775,7 +23753,7 @@
         <v>3834</v>
       </c>
       <c r="AE8" s="19">
-        <v>4000</v>
+        <v>3983</v>
       </c>
       <c r="AF8" s="19">
         <v>3984</v>
@@ -23936,7 +23914,7 @@
         <v>9349</v>
       </c>
       <c r="AE9" s="19">
-        <v>10793</v>
+        <v>10676</v>
       </c>
       <c r="AF9" s="19">
         <v>10171</v>
@@ -24097,7 +24075,7 @@
         <v>9711</v>
       </c>
       <c r="AE10" s="19">
-        <v>9656</v>
+        <v>9644</v>
       </c>
       <c r="AF10" s="19">
         <v>9318</v>
@@ -24258,7 +24236,7 @@
         <v>46851</v>
       </c>
       <c r="AE11" s="19">
-        <v>50157</v>
+        <v>50047</v>
       </c>
       <c r="AF11" s="19">
         <v>49527</v>
@@ -24419,7 +24397,7 @@
         <v>107637</v>
       </c>
       <c r="AE12" s="8">
-        <v>110952</v>
+        <v>111220</v>
       </c>
       <c r="AF12" s="8">
         <v>110772</v>
@@ -24640,7 +24618,7 @@
         <v>483.95710300000002</v>
       </c>
       <c r="AE15" s="19">
-        <v>521.60046</v>
+        <v>520.57220600000005</v>
       </c>
       <c r="AF15" s="19">
         <v>474.50923599999999</v>
@@ -24801,7 +24779,7 @@
         <v>927.86779000000001</v>
       </c>
       <c r="AE16" s="19">
-        <v>910.62362599999994</v>
+        <v>909.99564799999996</v>
       </c>
       <c r="AF16" s="19">
         <v>882.36902699999996</v>
@@ -24962,7 +24940,7 @@
         <v>573.29124000000002</v>
       </c>
       <c r="AE17" s="19">
-        <v>572.16166199999998</v>
+        <v>567.114777</v>
       </c>
       <c r="AF17" s="19">
         <v>568.45650499999999</v>
@@ -25123,7 +25101,7 @@
         <v>52.864941000000002</v>
       </c>
       <c r="AE18" s="19">
-        <v>54.601064000000001</v>
+        <v>54.241491000000003</v>
       </c>
       <c r="AF18" s="19">
         <v>51.567976000000002</v>
@@ -25284,7 +25262,7 @@
         <v>467.57713999999999</v>
       </c>
       <c r="AE19" s="19">
-        <v>418.123786</v>
+        <v>418.15880700000002</v>
       </c>
       <c r="AF19" s="19">
         <v>493.36618199999998</v>
@@ -25445,7 +25423,7 @@
         <v>884.16366500000004</v>
       </c>
       <c r="AE20" s="19">
-        <v>866.89913100000001</v>
+        <v>865.88985400000001</v>
       </c>
       <c r="AF20" s="19">
         <v>757.80289000000005</v>
@@ -25606,7 +25584,7 @@
         <v>1075.892936</v>
       </c>
       <c r="AE21" s="19">
-        <v>1097.4848999999999</v>
+        <v>1095.6566290000001</v>
       </c>
       <c r="AF21" s="19">
         <v>1108.6365880000001</v>
@@ -25767,7 +25745,7 @@
         <v>4465.6148149999999</v>
       </c>
       <c r="AE22" s="8">
-        <v>4441.4946290000007</v>
+        <v>4431.6294120000002</v>
       </c>
       <c r="AF22" s="8">
         <v>4336.708404</v>
@@ -25889,12 +25867,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:BA1"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26382,7 +26360,7 @@
         <v>5606</v>
       </c>
       <c r="AE5" s="19">
-        <v>0</v>
+        <v>5913</v>
       </c>
       <c r="AF5" s="19">
         <v>0</v>
@@ -26544,7 +26522,7 @@
         <v>11991</v>
       </c>
       <c r="AE6" s="7">
-        <v>0</v>
+        <v>11712</v>
       </c>
       <c r="AF6" s="7">
         <v>0</v>
@@ -26706,7 +26684,7 @@
         <v>19911</v>
       </c>
       <c r="AE7" s="7">
-        <v>0</v>
+        <v>19222</v>
       </c>
       <c r="AF7" s="7">
         <v>0</v>
@@ -26868,7 +26846,7 @@
         <v>4757</v>
       </c>
       <c r="AE8" s="7">
-        <v>0</v>
+        <v>4236</v>
       </c>
       <c r="AF8" s="7">
         <v>0</v>
@@ -27030,7 +27008,7 @@
         <v>9725</v>
       </c>
       <c r="AE9" s="7">
-        <v>0</v>
+        <v>9351</v>
       </c>
       <c r="AF9" s="7">
         <v>0</v>
@@ -27192,7 +27170,7 @@
         <v>11942</v>
       </c>
       <c r="AE10" s="19">
-        <v>0</v>
+        <v>11025</v>
       </c>
       <c r="AF10" s="19">
         <v>0</v>
@@ -27354,7 +27332,7 @@
         <v>40835</v>
       </c>
       <c r="AE11" s="7">
-        <v>0</v>
+        <v>39415</v>
       </c>
       <c r="AF11" s="7">
         <v>0</v>
@@ -27516,7 +27494,7 @@
         <v>104767</v>
       </c>
       <c r="AE12" s="8">
-        <v>0</v>
+        <v>100874</v>
       </c>
       <c r="AF12" s="8">
         <v>0</v>
@@ -27740,7 +27718,7 @@
         <v>422.21685400000001</v>
       </c>
       <c r="AE15" s="19">
-        <v>0</v>
+        <v>452.65860700000002</v>
       </c>
       <c r="AF15" s="19">
         <v>0</v>
@@ -27902,7 +27880,7 @@
         <v>797.01322000000005</v>
       </c>
       <c r="AE16" s="7">
-        <v>0</v>
+        <v>759.33742800000005</v>
       </c>
       <c r="AF16" s="7">
         <v>0</v>
@@ -28064,7 +28042,7 @@
         <v>668.70617600000003</v>
       </c>
       <c r="AE17" s="7">
-        <v>0</v>
+        <v>514.86128699999995</v>
       </c>
       <c r="AF17" s="7">
         <v>0</v>
@@ -28226,7 +28204,7 @@
         <v>65.103791999999999</v>
       </c>
       <c r="AE18" s="7">
-        <v>0</v>
+        <v>55.520687000000002</v>
       </c>
       <c r="AF18" s="7">
         <v>0</v>
@@ -28388,7 +28366,7 @@
         <v>384.47404599999999</v>
       </c>
       <c r="AE19" s="7">
-        <v>0</v>
+        <v>391.07409999999999</v>
       </c>
       <c r="AF19" s="7">
         <v>0</v>
@@ -28550,7 +28528,7 @@
         <v>1150.8910430000001</v>
       </c>
       <c r="AE20" s="19">
-        <v>0</v>
+        <v>1117.1566869999999</v>
       </c>
       <c r="AF20" s="19">
         <v>0</v>
@@ -28712,7 +28690,7 @@
         <v>943.95793700000002</v>
       </c>
       <c r="AE21" s="7">
-        <v>0</v>
+        <v>925.921828</v>
       </c>
       <c r="AF21" s="7">
         <v>0</v>
@@ -28874,7 +28852,7 @@
         <v>4432.3630679999997</v>
       </c>
       <c r="AE22" s="8">
-        <v>0</v>
+        <v>4216.5306239999991</v>
       </c>
       <c r="AF22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Wed Aug  9 05:22:17 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -22784,7 +22784,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="E38" sqref="E38"/>
+      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23273,7 +23273,7 @@
         <v>6618</v>
       </c>
       <c r="AF5" s="19">
-        <v>6316</v>
+        <v>6284</v>
       </c>
       <c r="AG5" s="19">
         <v>6336</v>
@@ -23434,7 +23434,7 @@
         <v>12335</v>
       </c>
       <c r="AF6" s="19">
-        <v>12014</v>
+        <v>11993</v>
       </c>
       <c r="AG6" s="19">
         <v>12566</v>
@@ -23595,7 +23595,7 @@
         <v>17917</v>
       </c>
       <c r="AF7" s="19">
-        <v>19442</v>
+        <v>19856</v>
       </c>
       <c r="AG7" s="19">
         <v>19833</v>
@@ -23756,7 +23756,7 @@
         <v>3983</v>
       </c>
       <c r="AF8" s="19">
-        <v>3984</v>
+        <v>3962</v>
       </c>
       <c r="AG8" s="19">
         <v>3934</v>
@@ -23917,7 +23917,7 @@
         <v>10676</v>
       </c>
       <c r="AF9" s="19">
-        <v>10171</v>
+        <v>10173</v>
       </c>
       <c r="AG9" s="19">
         <v>10094</v>
@@ -24078,7 +24078,7 @@
         <v>9644</v>
       </c>
       <c r="AF10" s="19">
-        <v>9318</v>
+        <v>9186</v>
       </c>
       <c r="AG10" s="19">
         <v>8349</v>
@@ -24239,7 +24239,7 @@
         <v>50047</v>
       </c>
       <c r="AF11" s="19">
-        <v>49527</v>
+        <v>49410</v>
       </c>
       <c r="AG11" s="19">
         <v>52160</v>
@@ -24400,7 +24400,7 @@
         <v>111220</v>
       </c>
       <c r="AF12" s="8">
-        <v>110772</v>
+        <v>110864</v>
       </c>
       <c r="AG12" s="8">
         <v>113272</v>
@@ -24621,7 +24621,7 @@
         <v>520.57220600000005</v>
       </c>
       <c r="AF15" s="19">
-        <v>474.50923599999999</v>
+        <v>470.86028299999998</v>
       </c>
       <c r="AG15" s="19">
         <v>501.47778899999997</v>
@@ -24782,7 +24782,7 @@
         <v>909.99564799999996</v>
       </c>
       <c r="AF16" s="19">
-        <v>882.36902699999996</v>
+        <v>881.86775299999999</v>
       </c>
       <c r="AG16" s="19">
         <v>932.09891800000003</v>
@@ -24943,7 +24943,7 @@
         <v>567.114777</v>
       </c>
       <c r="AF17" s="19">
-        <v>568.45650499999999</v>
+        <v>543.750001</v>
       </c>
       <c r="AG17" s="19">
         <v>543.76047000000005</v>
@@ -25104,7 +25104,7 @@
         <v>54.241491000000003</v>
       </c>
       <c r="AF18" s="19">
-        <v>51.567976000000002</v>
+        <v>51.295361999999997</v>
       </c>
       <c r="AG18" s="19">
         <v>56.709007999999997</v>
@@ -25265,7 +25265,7 @@
         <v>418.15880700000002</v>
       </c>
       <c r="AF19" s="19">
-        <v>493.36618199999998</v>
+        <v>493.34387099999998</v>
       </c>
       <c r="AG19" s="19">
         <v>452.24902700000001</v>
@@ -25426,7 +25426,7 @@
         <v>865.88985400000001</v>
       </c>
       <c r="AF20" s="19">
-        <v>757.80289000000005</v>
+        <v>740.62404600000002</v>
       </c>
       <c r="AG20" s="19">
         <v>664.07359199999996</v>
@@ -25587,7 +25587,7 @@
         <v>1095.6566290000001</v>
       </c>
       <c r="AF21" s="19">
-        <v>1108.6365880000001</v>
+        <v>1107.133484</v>
       </c>
       <c r="AG21" s="19">
         <v>1174.775582</v>
@@ -25748,7 +25748,7 @@
         <v>4431.6294120000002</v>
       </c>
       <c r="AF22" s="8">
-        <v>4336.708404</v>
+        <v>4288.8747999999996</v>
       </c>
       <c r="AG22" s="8">
         <v>4325.1443859999999</v>
@@ -25872,7 +25872,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26363,7 +26363,7 @@
         <v>5913</v>
       </c>
       <c r="AF5" s="19">
-        <v>0</v>
+        <v>5871</v>
       </c>
       <c r="AG5" s="19">
         <v>0</v>
@@ -26525,7 +26525,7 @@
         <v>11712</v>
       </c>
       <c r="AF6" s="7">
-        <v>0</v>
+        <v>12369</v>
       </c>
       <c r="AG6" s="7">
         <v>0</v>
@@ -26687,7 +26687,7 @@
         <v>19222</v>
       </c>
       <c r="AF7" s="7">
-        <v>0</v>
+        <v>19637</v>
       </c>
       <c r="AG7" s="7">
         <v>0</v>
@@ -26849,7 +26849,7 @@
         <v>4236</v>
       </c>
       <c r="AF8" s="7">
-        <v>0</v>
+        <v>4184</v>
       </c>
       <c r="AG8" s="7">
         <v>0</v>
@@ -27011,7 +27011,7 @@
         <v>9351</v>
       </c>
       <c r="AF9" s="7">
-        <v>0</v>
+        <v>9979</v>
       </c>
       <c r="AG9" s="7">
         <v>0</v>
@@ -27173,7 +27173,7 @@
         <v>11025</v>
       </c>
       <c r="AF10" s="19">
-        <v>0</v>
+        <v>10809</v>
       </c>
       <c r="AG10" s="19">
         <v>0</v>
@@ -27335,7 +27335,7 @@
         <v>39415</v>
       </c>
       <c r="AF11" s="7">
-        <v>0</v>
+        <v>42627</v>
       </c>
       <c r="AG11" s="7">
         <v>0</v>
@@ -27497,7 +27497,7 @@
         <v>100874</v>
       </c>
       <c r="AF12" s="8">
-        <v>0</v>
+        <v>105476</v>
       </c>
       <c r="AG12" s="8">
         <v>0</v>
@@ -27721,7 +27721,7 @@
         <v>452.65860700000002</v>
       </c>
       <c r="AF15" s="19">
-        <v>0</v>
+        <v>428.08640200000002</v>
       </c>
       <c r="AG15" s="19">
         <v>0</v>
@@ -27883,7 +27883,7 @@
         <v>759.33742800000005</v>
       </c>
       <c r="AF16" s="7">
-        <v>0</v>
+        <v>802.37011399999994</v>
       </c>
       <c r="AG16" s="7">
         <v>0</v>
@@ -28045,7 +28045,7 @@
         <v>514.86128699999995</v>
       </c>
       <c r="AF17" s="7">
-        <v>0</v>
+        <v>568.31929100000002</v>
       </c>
       <c r="AG17" s="7">
         <v>0</v>
@@ -28207,7 +28207,7 @@
         <v>55.520687000000002</v>
       </c>
       <c r="AF18" s="7">
-        <v>0</v>
+        <v>61.902596000000003</v>
       </c>
       <c r="AG18" s="7">
         <v>0</v>
@@ -28369,7 +28369,7 @@
         <v>391.07409999999999</v>
       </c>
       <c r="AF19" s="7">
-        <v>0</v>
+        <v>455.78434900000002</v>
       </c>
       <c r="AG19" s="7">
         <v>0</v>
@@ -28531,7 +28531,7 @@
         <v>1117.1566869999999</v>
       </c>
       <c r="AF20" s="19">
-        <v>0</v>
+        <v>1009.250854</v>
       </c>
       <c r="AG20" s="19">
         <v>0</v>
@@ -28693,7 +28693,7 @@
         <v>925.921828</v>
       </c>
       <c r="AF21" s="7">
-        <v>0</v>
+        <v>965.47461099999998</v>
       </c>
       <c r="AG21" s="7">
         <v>0</v>
@@ -28855,7 +28855,7 @@
         <v>4216.5306239999991</v>
       </c>
       <c r="AF22" s="8">
-        <v>0</v>
+        <v>4291.1882169999999</v>
       </c>
       <c r="AG22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Aug 15 05:21:41 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -22772,6 +22772,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -22784,7 +22787,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
+      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23276,7 +23279,7 @@
         <v>6284</v>
       </c>
       <c r="AG5" s="19">
-        <v>6336</v>
+        <v>6318</v>
       </c>
       <c r="AH5" s="19">
         <v>6604</v>
@@ -23437,7 +23440,7 @@
         <v>11993</v>
       </c>
       <c r="AG6" s="19">
-        <v>12566</v>
+        <v>12559</v>
       </c>
       <c r="AH6" s="19">
         <v>12580</v>
@@ -23598,7 +23601,7 @@
         <v>19856</v>
       </c>
       <c r="AG7" s="19">
-        <v>19833</v>
+        <v>20232</v>
       </c>
       <c r="AH7" s="19">
         <v>19949</v>
@@ -23759,7 +23762,7 @@
         <v>3962</v>
       </c>
       <c r="AG8" s="19">
-        <v>3934</v>
+        <v>3932</v>
       </c>
       <c r="AH8" s="19">
         <v>3909</v>
@@ -23920,7 +23923,7 @@
         <v>10173</v>
       </c>
       <c r="AG9" s="19">
-        <v>10094</v>
+        <v>9991</v>
       </c>
       <c r="AH9" s="19">
         <v>11408</v>
@@ -24081,7 +24084,7 @@
         <v>9186</v>
       </c>
       <c r="AG10" s="19">
-        <v>8349</v>
+        <v>8231</v>
       </c>
       <c r="AH10" s="19">
         <v>9136</v>
@@ -24242,7 +24245,7 @@
         <v>49410</v>
       </c>
       <c r="AG11" s="19">
-        <v>52160</v>
+        <v>52070</v>
       </c>
       <c r="AH11" s="19">
         <v>51046</v>
@@ -24403,7 +24406,7 @@
         <v>110864</v>
       </c>
       <c r="AG12" s="8">
-        <v>113272</v>
+        <v>113333</v>
       </c>
       <c r="AH12" s="8">
         <v>114632</v>
@@ -24624,7 +24627,7 @@
         <v>470.86028299999998</v>
       </c>
       <c r="AG15" s="19">
-        <v>501.47778899999997</v>
+        <v>499.84762799999999</v>
       </c>
       <c r="AH15" s="19">
         <v>528.03928699999994</v>
@@ -24785,7 +24788,7 @@
         <v>881.86775299999999</v>
       </c>
       <c r="AG16" s="19">
-        <v>932.09891800000003</v>
+        <v>931.59642099999996</v>
       </c>
       <c r="AH16" s="19">
         <v>905.64985200000001</v>
@@ -24946,7 +24949,7 @@
         <v>543.750001</v>
       </c>
       <c r="AG17" s="19">
-        <v>543.76047000000005</v>
+        <v>520.59290899999996</v>
       </c>
       <c r="AH17" s="19">
         <v>593.44917999999996</v>
@@ -25107,7 +25110,7 @@
         <v>51.295361999999997</v>
       </c>
       <c r="AG18" s="19">
-        <v>56.709007999999997</v>
+        <v>56.707538</v>
       </c>
       <c r="AH18" s="19">
         <v>56.828009000000002</v>
@@ -25268,7 +25271,7 @@
         <v>493.34387099999998</v>
       </c>
       <c r="AG19" s="19">
-        <v>452.24902700000001</v>
+        <v>452.42872799999998</v>
       </c>
       <c r="AH19" s="19">
         <v>546.42111199999999</v>
@@ -25429,7 +25432,7 @@
         <v>740.62404600000002</v>
       </c>
       <c r="AG20" s="19">
-        <v>664.07359199999996</v>
+        <v>663.24792500000001</v>
       </c>
       <c r="AH20" s="19">
         <v>782.77531499999998</v>
@@ -25590,7 +25593,7 @@
         <v>1107.133484</v>
       </c>
       <c r="AG21" s="19">
-        <v>1174.775582</v>
+        <v>1173.432282</v>
       </c>
       <c r="AH21" s="19">
         <v>1161.1797320000001</v>
@@ -25751,7 +25754,7 @@
         <v>4288.8747999999996</v>
       </c>
       <c r="AG22" s="8">
-        <v>4325.1443859999999</v>
+        <v>4297.8534309999995</v>
       </c>
       <c r="AH22" s="8">
         <v>4574.3424869999999</v>
@@ -25872,7 +25875,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26366,7 +26369,7 @@
         <v>5871</v>
       </c>
       <c r="AG5" s="19">
-        <v>0</v>
+        <v>5488</v>
       </c>
       <c r="AH5" s="19">
         <v>0</v>
@@ -26528,7 +26531,7 @@
         <v>12369</v>
       </c>
       <c r="AG6" s="7">
-        <v>0</v>
+        <v>12416</v>
       </c>
       <c r="AH6" s="7">
         <v>0</v>
@@ -26690,7 +26693,7 @@
         <v>19637</v>
       </c>
       <c r="AG7" s="7">
-        <v>0</v>
+        <v>20488</v>
       </c>
       <c r="AH7" s="7">
         <v>0</v>
@@ -26852,7 +26855,7 @@
         <v>4184</v>
       </c>
       <c r="AG8" s="7">
-        <v>0</v>
+        <v>4610</v>
       </c>
       <c r="AH8" s="7">
         <v>0</v>
@@ -27014,7 +27017,7 @@
         <v>9979</v>
       </c>
       <c r="AG9" s="7">
-        <v>0</v>
+        <v>10133</v>
       </c>
       <c r="AH9" s="7">
         <v>0</v>
@@ -27176,7 +27179,7 @@
         <v>10809</v>
       </c>
       <c r="AG10" s="19">
-        <v>0</v>
+        <v>9882</v>
       </c>
       <c r="AH10" s="19">
         <v>0</v>
@@ -27338,7 +27341,7 @@
         <v>42627</v>
       </c>
       <c r="AG11" s="7">
-        <v>0</v>
+        <v>40711</v>
       </c>
       <c r="AH11" s="7">
         <v>0</v>
@@ -27500,7 +27503,7 @@
         <v>105476</v>
       </c>
       <c r="AG12" s="8">
-        <v>0</v>
+        <v>103728</v>
       </c>
       <c r="AH12" s="8">
         <v>0</v>
@@ -27724,7 +27727,7 @@
         <v>428.08640200000002</v>
       </c>
       <c r="AG15" s="19">
-        <v>0</v>
+        <v>416.027152</v>
       </c>
       <c r="AH15" s="19">
         <v>0</v>
@@ -27886,7 +27889,7 @@
         <v>802.37011399999994</v>
       </c>
       <c r="AG16" s="7">
-        <v>0</v>
+        <v>828.43830400000002</v>
       </c>
       <c r="AH16" s="7">
         <v>0</v>
@@ -28048,7 +28051,7 @@
         <v>568.31929100000002</v>
       </c>
       <c r="AG17" s="7">
-        <v>0</v>
+        <v>625.160841</v>
       </c>
       <c r="AH17" s="7">
         <v>0</v>
@@ -28210,7 +28213,7 @@
         <v>61.902596000000003</v>
       </c>
       <c r="AG18" s="7">
-        <v>0</v>
+        <v>67.566394000000003</v>
       </c>
       <c r="AH18" s="7">
         <v>0</v>
@@ -28372,7 +28375,7 @@
         <v>455.78434900000002</v>
       </c>
       <c r="AG19" s="7">
-        <v>0</v>
+        <v>370.57557800000001</v>
       </c>
       <c r="AH19" s="7">
         <v>0</v>
@@ -28534,7 +28537,7 @@
         <v>1009.250854</v>
       </c>
       <c r="AG20" s="19">
-        <v>0</v>
+        <v>914.33445099999994</v>
       </c>
       <c r="AH20" s="19">
         <v>0</v>
@@ -28696,7 +28699,7 @@
         <v>965.47461099999998</v>
       </c>
       <c r="AG21" s="7">
-        <v>0</v>
+        <v>872.48056499999996</v>
       </c>
       <c r="AH21" s="7">
         <v>0</v>
@@ -28858,7 +28861,7 @@
         <v>4291.1882169999999</v>
       </c>
       <c r="AG22" s="8">
-        <v>0</v>
+        <v>4094.5832849999997</v>
       </c>
       <c r="AH22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Aug 22 05:21:34 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{71FB8475-193C-4AEF-BCD6-B5B91AD9B226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -209,7 +210,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'2022'!$A:$A,'2022'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">'2023'!$A:$A,'2023'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -460,7 +461,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -649,11 +650,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="5"/>
-    <cellStyle name="Percent 2" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1015,7 +1016,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4069,7 +4070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7155,7 +7156,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:BA54"/>
   <sheetViews>
@@ -10243,7 +10244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13318,7 +13319,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16393,7 +16394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19688,7 +19689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -22772,14 +22773,11 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -22787,7 +22785,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
+      <selection pane="bottomRight" sqref="A1:BA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23282,7 +23280,7 @@
         <v>6318</v>
       </c>
       <c r="AH5" s="19">
-        <v>6604</v>
+        <v>6589</v>
       </c>
       <c r="AI5" s="19">
         <v>6681</v>
@@ -23443,7 +23441,7 @@
         <v>12559</v>
       </c>
       <c r="AH6" s="19">
-        <v>12580</v>
+        <v>12576</v>
       </c>
       <c r="AI6" s="19">
         <v>11951</v>
@@ -23604,7 +23602,7 @@
         <v>20232</v>
       </c>
       <c r="AH7" s="19">
-        <v>19949</v>
+        <v>20610</v>
       </c>
       <c r="AI7" s="19">
         <v>19906</v>
@@ -23765,7 +23763,7 @@
         <v>3932</v>
       </c>
       <c r="AH8" s="19">
-        <v>3909</v>
+        <v>3903</v>
       </c>
       <c r="AI8" s="19">
         <v>4141</v>
@@ -23926,7 +23924,7 @@
         <v>9991</v>
       </c>
       <c r="AH9" s="19">
-        <v>11408</v>
+        <v>11369</v>
       </c>
       <c r="AI9" s="19">
         <v>11241</v>
@@ -24087,7 +24085,7 @@
         <v>8231</v>
       </c>
       <c r="AH10" s="19">
-        <v>9136</v>
+        <v>9145</v>
       </c>
       <c r="AI10" s="19">
         <v>9698</v>
@@ -24248,7 +24246,7 @@
         <v>52070</v>
       </c>
       <c r="AH11" s="19">
-        <v>51046</v>
+        <v>50896</v>
       </c>
       <c r="AI11" s="19">
         <v>50940</v>
@@ -24409,7 +24407,7 @@
         <v>113333</v>
       </c>
       <c r="AH12" s="8">
-        <v>114632</v>
+        <v>115088</v>
       </c>
       <c r="AI12" s="8">
         <v>114558</v>
@@ -24630,7 +24628,7 @@
         <v>499.84762799999999</v>
       </c>
       <c r="AH15" s="19">
-        <v>528.03928699999994</v>
+        <v>525.86449600000003</v>
       </c>
       <c r="AI15" s="19">
         <v>518.18334700000003</v>
@@ -24791,7 +24789,7 @@
         <v>931.59642099999996</v>
       </c>
       <c r="AH16" s="19">
-        <v>905.64985200000001</v>
+        <v>905.45995300000004</v>
       </c>
       <c r="AI16" s="19">
         <v>866.11233700000003</v>
@@ -24952,7 +24950,7 @@
         <v>520.59290899999996</v>
       </c>
       <c r="AH17" s="19">
-        <v>593.44917999999996</v>
+        <v>592.00789899999995</v>
       </c>
       <c r="AI17" s="19">
         <v>589.38980600000002</v>
@@ -25113,7 +25111,7 @@
         <v>56.707538</v>
       </c>
       <c r="AH18" s="19">
-        <v>56.828009000000002</v>
+        <v>56.727100999999998</v>
       </c>
       <c r="AI18" s="19">
         <v>58.429595999999997</v>
@@ -25274,7 +25272,7 @@
         <v>452.42872799999998</v>
       </c>
       <c r="AH19" s="19">
-        <v>546.42111199999999</v>
+        <v>545.27913000000001</v>
       </c>
       <c r="AI19" s="19">
         <v>496.513082</v>
@@ -25435,7 +25433,7 @@
         <v>663.24792500000001</v>
       </c>
       <c r="AH20" s="19">
-        <v>782.77531499999998</v>
+        <v>782.14686700000004</v>
       </c>
       <c r="AI20" s="19">
         <v>775.02782200000001</v>
@@ -25596,7 +25594,7 @@
         <v>1173.432282</v>
       </c>
       <c r="AH21" s="19">
-        <v>1161.1797320000001</v>
+        <v>1159.559972</v>
       </c>
       <c r="AI21" s="19">
         <v>1130.766016</v>
@@ -25757,7 +25755,7 @@
         <v>4297.8534309999995</v>
       </c>
       <c r="AH22" s="8">
-        <v>4574.3424869999999</v>
+        <v>4567.0454179999997</v>
       </c>
       <c r="AI22" s="8">
         <v>4434.4220060000007</v>
@@ -25870,12 +25868,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection sqref="A1:BA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26372,7 +26370,7 @@
         <v>5488</v>
       </c>
       <c r="AH5" s="19">
-        <v>0</v>
+        <v>5720</v>
       </c>
       <c r="AI5" s="19">
         <v>0</v>
@@ -26534,7 +26532,7 @@
         <v>12416</v>
       </c>
       <c r="AH6" s="7">
-        <v>0</v>
+        <v>12355</v>
       </c>
       <c r="AI6" s="7">
         <v>0</v>
@@ -26696,7 +26694,7 @@
         <v>20488</v>
       </c>
       <c r="AH7" s="7">
-        <v>0</v>
+        <v>20527</v>
       </c>
       <c r="AI7" s="7">
         <v>0</v>
@@ -26858,7 +26856,7 @@
         <v>4610</v>
       </c>
       <c r="AH8" s="7">
-        <v>0</v>
+        <v>4701</v>
       </c>
       <c r="AI8" s="7">
         <v>0</v>
@@ -27020,7 +27018,7 @@
         <v>10133</v>
       </c>
       <c r="AH9" s="7">
-        <v>0</v>
+        <v>9736</v>
       </c>
       <c r="AI9" s="7">
         <v>0</v>
@@ -27182,7 +27180,7 @@
         <v>9882</v>
       </c>
       <c r="AH10" s="19">
-        <v>0</v>
+        <v>10198</v>
       </c>
       <c r="AI10" s="19">
         <v>0</v>
@@ -27344,7 +27342,7 @@
         <v>40711</v>
       </c>
       <c r="AH11" s="7">
-        <v>0</v>
+        <v>41067</v>
       </c>
       <c r="AI11" s="7">
         <v>0</v>
@@ -27506,7 +27504,7 @@
         <v>103728</v>
       </c>
       <c r="AH12" s="8">
-        <v>0</v>
+        <v>104304</v>
       </c>
       <c r="AI12" s="8">
         <v>0</v>
@@ -27730,7 +27728,7 @@
         <v>416.027152</v>
       </c>
       <c r="AH15" s="19">
-        <v>0</v>
+        <v>434.27642800000001</v>
       </c>
       <c r="AI15" s="19">
         <v>0</v>
@@ -27892,7 +27890,7 @@
         <v>828.43830400000002</v>
       </c>
       <c r="AH16" s="7">
-        <v>0</v>
+        <v>797.96354599999995</v>
       </c>
       <c r="AI16" s="7">
         <v>0</v>
@@ -28054,7 +28052,7 @@
         <v>625.160841</v>
       </c>
       <c r="AH17" s="7">
-        <v>0</v>
+        <v>595.55138199999999</v>
       </c>
       <c r="AI17" s="7">
         <v>0</v>
@@ -28216,7 +28214,7 @@
         <v>67.566394000000003</v>
       </c>
       <c r="AH18" s="7">
-        <v>0</v>
+        <v>62.391016999999998</v>
       </c>
       <c r="AI18" s="7">
         <v>0</v>
@@ -28378,7 +28376,7 @@
         <v>370.57557800000001</v>
       </c>
       <c r="AH19" s="7">
-        <v>0</v>
+        <v>411.70692000000003</v>
       </c>
       <c r="AI19" s="7">
         <v>0</v>
@@ -28540,7 +28538,7 @@
         <v>914.33445099999994</v>
       </c>
       <c r="AH20" s="19">
-        <v>0</v>
+        <v>989.09914700000002</v>
       </c>
       <c r="AI20" s="19">
         <v>0</v>
@@ -28702,7 +28700,7 @@
         <v>872.48056499999996</v>
       </c>
       <c r="AH21" s="7">
-        <v>0</v>
+        <v>960.33806200000004</v>
       </c>
       <c r="AI21" s="7">
         <v>0</v>
@@ -28864,7 +28862,7 @@
         <v>4094.5832849999997</v>
       </c>
       <c r="AH22" s="8">
-        <v>0</v>
+        <v>4251.3265019999999</v>
       </c>
       <c r="AI22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Aug 29 05:21:45 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71FB8475-193C-4AEF-BCD6-B5B91AD9B226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -210,7 +209,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'2022'!$A:$A,'2022'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">'2023'!$A:$A,'2023'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -461,7 +460,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -650,11 +649,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 3" xfId="5"/>
+    <cellStyle name="Percent 2" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1016,7 +1015,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4070,7 +4069,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7156,7 +7155,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:BA54"/>
   <sheetViews>
@@ -10244,7 +10243,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13319,7 +13318,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16394,7 +16393,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19689,7 +19688,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -22777,7 +22776,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -22785,7 +22784,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" sqref="A1:BA1"/>
+      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23283,7 +23282,7 @@
         <v>6589</v>
       </c>
       <c r="AI5" s="19">
-        <v>6681</v>
+        <v>6655</v>
       </c>
       <c r="AJ5" s="19">
         <v>6760</v>
@@ -23444,7 +23443,7 @@
         <v>12576</v>
       </c>
       <c r="AI6" s="19">
-        <v>11951</v>
+        <v>11939</v>
       </c>
       <c r="AJ6" s="19">
         <v>12411</v>
@@ -23605,7 +23604,7 @@
         <v>20610</v>
       </c>
       <c r="AI7" s="19">
-        <v>19906</v>
+        <v>20712</v>
       </c>
       <c r="AJ7" s="19">
         <v>19343</v>
@@ -23766,7 +23765,7 @@
         <v>3903</v>
       </c>
       <c r="AI8" s="19">
-        <v>4141</v>
+        <v>4085</v>
       </c>
       <c r="AJ8" s="19">
         <v>4246</v>
@@ -23927,7 +23926,7 @@
         <v>11369</v>
       </c>
       <c r="AI9" s="19">
-        <v>11241</v>
+        <v>11252</v>
       </c>
       <c r="AJ9" s="19">
         <v>9932</v>
@@ -24088,7 +24087,7 @@
         <v>9145</v>
       </c>
       <c r="AI10" s="19">
-        <v>9698</v>
+        <v>9684</v>
       </c>
       <c r="AJ10" s="19">
         <v>8911</v>
@@ -24249,7 +24248,7 @@
         <v>50896</v>
       </c>
       <c r="AI11" s="19">
-        <v>50940</v>
+        <v>50790</v>
       </c>
       <c r="AJ11" s="19">
         <v>52996</v>
@@ -24410,7 +24409,7 @@
         <v>115088</v>
       </c>
       <c r="AI12" s="8">
-        <v>114558</v>
+        <v>115117</v>
       </c>
       <c r="AJ12" s="8">
         <v>114599</v>
@@ -24631,7 +24630,7 @@
         <v>525.86449600000003</v>
       </c>
       <c r="AI15" s="19">
-        <v>518.18334700000003</v>
+        <v>517.13303900000005</v>
       </c>
       <c r="AJ15" s="19">
         <v>527.83306900000002</v>
@@ -24792,7 +24791,7 @@
         <v>905.45995300000004</v>
       </c>
       <c r="AI16" s="19">
-        <v>866.11233700000003</v>
+        <v>868.201413</v>
       </c>
       <c r="AJ16" s="19">
         <v>899.74568199999999</v>
@@ -24953,7 +24952,7 @@
         <v>592.00789899999995</v>
       </c>
       <c r="AI17" s="19">
-        <v>589.38980600000002</v>
+        <v>588.277017</v>
       </c>
       <c r="AJ17" s="19">
         <v>586.73105699999996</v>
@@ -25114,7 +25113,7 @@
         <v>56.727100999999998</v>
       </c>
       <c r="AI18" s="19">
-        <v>58.429595999999997</v>
+        <v>56.688443999999997</v>
       </c>
       <c r="AJ18" s="19">
         <v>62.525658999999997</v>
@@ -25275,7 +25274,7 @@
         <v>545.27913000000001</v>
       </c>
       <c r="AI19" s="19">
-        <v>496.513082</v>
+        <v>497.97739200000001</v>
       </c>
       <c r="AJ19" s="19">
         <v>443.56388199999998</v>
@@ -25436,7 +25435,7 @@
         <v>782.14686700000004</v>
       </c>
       <c r="AI20" s="19">
-        <v>775.02782200000001</v>
+        <v>773.69365600000003</v>
       </c>
       <c r="AJ20" s="19">
         <v>757.74621400000001</v>
@@ -25597,7 +25596,7 @@
         <v>1159.559972</v>
       </c>
       <c r="AI21" s="19">
-        <v>1130.766016</v>
+        <v>1129.4320760000001</v>
       </c>
       <c r="AJ21" s="19">
         <v>1153.183002</v>
@@ -25758,7 +25757,7 @@
         <v>4567.0454179999997</v>
       </c>
       <c r="AI22" s="8">
-        <v>4434.4220060000007</v>
+        <v>4431.403037</v>
       </c>
       <c r="AJ22" s="8">
         <v>4431.3285649999998</v>
@@ -25868,12 +25867,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:BA1"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26373,7 +26372,7 @@
         <v>5720</v>
       </c>
       <c r="AI5" s="19">
-        <v>0</v>
+        <v>6127</v>
       </c>
       <c r="AJ5" s="19">
         <v>0</v>
@@ -26535,7 +26534,7 @@
         <v>12355</v>
       </c>
       <c r="AI6" s="7">
-        <v>0</v>
+        <v>12298</v>
       </c>
       <c r="AJ6" s="7">
         <v>0</v>
@@ -26697,7 +26696,7 @@
         <v>20527</v>
       </c>
       <c r="AI7" s="7">
-        <v>0</v>
+        <v>15659</v>
       </c>
       <c r="AJ7" s="7">
         <v>0</v>
@@ -26859,7 +26858,7 @@
         <v>4701</v>
       </c>
       <c r="AI8" s="7">
-        <v>0</v>
+        <v>4437</v>
       </c>
       <c r="AJ8" s="7">
         <v>0</v>
@@ -27021,7 +27020,7 @@
         <v>9736</v>
       </c>
       <c r="AI9" s="7">
-        <v>0</v>
+        <v>9108</v>
       </c>
       <c r="AJ9" s="7">
         <v>0</v>
@@ -27183,7 +27182,7 @@
         <v>10198</v>
       </c>
       <c r="AI10" s="19">
-        <v>0</v>
+        <v>11169</v>
       </c>
       <c r="AJ10" s="19">
         <v>0</v>
@@ -27345,7 +27344,7 @@
         <v>41067</v>
       </c>
       <c r="AI11" s="7">
-        <v>0</v>
+        <v>38316</v>
       </c>
       <c r="AJ11" s="7">
         <v>0</v>
@@ -27507,7 +27506,7 @@
         <v>104304</v>
       </c>
       <c r="AI12" s="8">
-        <v>0</v>
+        <v>97114</v>
       </c>
       <c r="AJ12" s="8">
         <v>0</v>
@@ -27731,7 +27730,7 @@
         <v>434.27642800000001</v>
       </c>
       <c r="AI15" s="19">
-        <v>0</v>
+        <v>459.14135499999998</v>
       </c>
       <c r="AJ15" s="19">
         <v>0</v>
@@ -27893,7 +27892,7 @@
         <v>797.96354599999995</v>
       </c>
       <c r="AI16" s="7">
-        <v>0</v>
+        <v>829.32071399999995</v>
       </c>
       <c r="AJ16" s="7">
         <v>0</v>
@@ -28055,7 +28054,7 @@
         <v>595.55138199999999</v>
       </c>
       <c r="AI17" s="7">
-        <v>0</v>
+        <v>514.93327999999997</v>
       </c>
       <c r="AJ17" s="7">
         <v>0</v>
@@ -28217,7 +28216,7 @@
         <v>62.391016999999998</v>
       </c>
       <c r="AI18" s="7">
-        <v>0</v>
+        <v>60.478881999999999</v>
       </c>
       <c r="AJ18" s="7">
         <v>0</v>
@@ -28379,7 +28378,7 @@
         <v>411.70692000000003</v>
       </c>
       <c r="AI19" s="7">
-        <v>0</v>
+        <v>401.20988499999999</v>
       </c>
       <c r="AJ19" s="7">
         <v>0</v>
@@ -28541,7 +28540,7 @@
         <v>989.09914700000002</v>
       </c>
       <c r="AI20" s="19">
-        <v>0</v>
+        <v>1061.8927659999999</v>
       </c>
       <c r="AJ20" s="19">
         <v>0</v>
@@ -28703,7 +28702,7 @@
         <v>960.33806200000004</v>
       </c>
       <c r="AI21" s="7">
-        <v>0</v>
+        <v>860.75445100000002</v>
       </c>
       <c r="AJ21" s="7">
         <v>0</v>
@@ -28865,7 +28864,7 @@
         <v>4251.3265019999999</v>
       </c>
       <c r="AI22" s="8">
-        <v>0</v>
+        <v>4187.7313329999997</v>
       </c>
       <c r="AJ22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Wed Sep  6 05:21:32 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -22784,7 +22784,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23285,7 +23285,7 @@
         <v>6655</v>
       </c>
       <c r="AJ5" s="19">
-        <v>6760</v>
+        <v>6733</v>
       </c>
       <c r="AK5" s="19">
         <v>6416</v>
@@ -23446,7 +23446,7 @@
         <v>11939</v>
       </c>
       <c r="AJ6" s="19">
-        <v>12411</v>
+        <v>12287</v>
       </c>
       <c r="AK6" s="19">
         <v>11691</v>
@@ -23607,7 +23607,7 @@
         <v>20712</v>
       </c>
       <c r="AJ7" s="19">
-        <v>19343</v>
+        <v>20105</v>
       </c>
       <c r="AK7" s="19">
         <v>18855</v>
@@ -23768,7 +23768,7 @@
         <v>4085</v>
       </c>
       <c r="AJ8" s="19">
-        <v>4246</v>
+        <v>4243</v>
       </c>
       <c r="AK8" s="19">
         <v>3876</v>
@@ -23929,7 +23929,7 @@
         <v>11252</v>
       </c>
       <c r="AJ9" s="19">
-        <v>9932</v>
+        <v>9697</v>
       </c>
       <c r="AK9" s="19">
         <v>10283</v>
@@ -24090,7 +24090,7 @@
         <v>9684</v>
       </c>
       <c r="AJ10" s="19">
-        <v>8911</v>
+        <v>8930</v>
       </c>
       <c r="AK10" s="19">
         <v>10373</v>
@@ -24251,7 +24251,7 @@
         <v>50790</v>
       </c>
       <c r="AJ11" s="19">
-        <v>52996</v>
+        <v>52839</v>
       </c>
       <c r="AK11" s="19">
         <v>46331</v>
@@ -24412,7 +24412,7 @@
         <v>115117</v>
       </c>
       <c r="AJ12" s="8">
-        <v>114599</v>
+        <v>114834</v>
       </c>
       <c r="AK12" s="8">
         <v>107825</v>
@@ -24633,7 +24633,7 @@
         <v>517.13303900000005</v>
       </c>
       <c r="AJ15" s="19">
-        <v>527.83306900000002</v>
+        <v>524.56151599999998</v>
       </c>
       <c r="AK15" s="19">
         <v>489.73348099999998</v>
@@ -24794,7 +24794,7 @@
         <v>868.201413</v>
       </c>
       <c r="AJ16" s="19">
-        <v>899.74568199999999</v>
+        <v>890.116263</v>
       </c>
       <c r="AK16" s="19">
         <v>821.83972900000003</v>
@@ -24955,7 +24955,7 @@
         <v>588.277017</v>
       </c>
       <c r="AJ17" s="19">
-        <v>586.73105699999996</v>
+        <v>586.09682899999996</v>
       </c>
       <c r="AK17" s="19">
         <v>531.56183399999998</v>
@@ -25116,7 +25116,7 @@
         <v>56.688443999999997</v>
       </c>
       <c r="AJ18" s="19">
-        <v>62.525658999999997</v>
+        <v>62.481541999999997</v>
       </c>
       <c r="AK18" s="19">
         <v>56.740982000000002</v>
@@ -25277,7 +25277,7 @@
         <v>497.97739200000001</v>
       </c>
       <c r="AJ19" s="19">
-        <v>443.56388199999998</v>
+        <v>443.10229299999997</v>
       </c>
       <c r="AK19" s="19">
         <v>453.409515</v>
@@ -25438,7 +25438,7 @@
         <v>773.69365600000003</v>
       </c>
       <c r="AJ20" s="19">
-        <v>757.74621400000001</v>
+        <v>759.63975600000003</v>
       </c>
       <c r="AK20" s="19">
         <v>946.67852800000003</v>
@@ -25599,7 +25599,7 @@
         <v>1129.4320760000001</v>
       </c>
       <c r="AJ21" s="19">
-        <v>1153.183002</v>
+        <v>1153.0830060000001</v>
       </c>
       <c r="AK21" s="19">
         <v>1003.803734</v>
@@ -25760,7 +25760,7 @@
         <v>4431.403037</v>
       </c>
       <c r="AJ22" s="8">
-        <v>4431.3285649999998</v>
+        <v>4419.0812050000004</v>
       </c>
       <c r="AK22" s="8">
         <v>4303.7678029999997</v>
@@ -25872,7 +25872,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26375,7 +26375,7 @@
         <v>6127</v>
       </c>
       <c r="AJ5" s="19">
-        <v>0</v>
+        <v>6135</v>
       </c>
       <c r="AK5" s="19">
         <v>0</v>
@@ -26537,7 +26537,7 @@
         <v>12298</v>
       </c>
       <c r="AJ6" s="7">
-        <v>0</v>
+        <v>12480</v>
       </c>
       <c r="AK6" s="7">
         <v>0</v>
@@ -26699,7 +26699,7 @@
         <v>15659</v>
       </c>
       <c r="AJ7" s="7">
-        <v>0</v>
+        <v>19256</v>
       </c>
       <c r="AK7" s="7">
         <v>0</v>
@@ -26861,7 +26861,7 @@
         <v>4437</v>
       </c>
       <c r="AJ8" s="7">
-        <v>0</v>
+        <v>4309</v>
       </c>
       <c r="AK8" s="7">
         <v>0</v>
@@ -27023,7 +27023,7 @@
         <v>9108</v>
       </c>
       <c r="AJ9" s="7">
-        <v>0</v>
+        <v>9268</v>
       </c>
       <c r="AK9" s="7">
         <v>0</v>
@@ -27185,7 +27185,7 @@
         <v>11169</v>
       </c>
       <c r="AJ10" s="19">
-        <v>0</v>
+        <v>11103</v>
       </c>
       <c r="AK10" s="19">
         <v>0</v>
@@ -27347,7 +27347,7 @@
         <v>38316</v>
       </c>
       <c r="AJ11" s="7">
-        <v>0</v>
+        <v>39287</v>
       </c>
       <c r="AK11" s="7">
         <v>0</v>
@@ -27509,7 +27509,7 @@
         <v>97114</v>
       </c>
       <c r="AJ12" s="8">
-        <v>0</v>
+        <v>101838</v>
       </c>
       <c r="AK12" s="8">
         <v>0</v>
@@ -27733,7 +27733,7 @@
         <v>459.14135499999998</v>
       </c>
       <c r="AJ15" s="19">
-        <v>0</v>
+        <v>477.95193799999998</v>
       </c>
       <c r="AK15" s="19">
         <v>0</v>
@@ -27895,7 +27895,7 @@
         <v>829.32071399999995</v>
       </c>
       <c r="AJ16" s="7">
-        <v>0</v>
+        <v>827.81147699999997</v>
       </c>
       <c r="AK16" s="7">
         <v>0</v>
@@ -28057,7 +28057,7 @@
         <v>514.93327999999997</v>
       </c>
       <c r="AJ17" s="7">
-        <v>0</v>
+        <v>576.19058900000005</v>
       </c>
       <c r="AK17" s="7">
         <v>0</v>
@@ -28219,7 +28219,7 @@
         <v>60.478881999999999</v>
       </c>
       <c r="AJ18" s="7">
-        <v>0</v>
+        <v>60.502398999999997</v>
       </c>
       <c r="AK18" s="7">
         <v>0</v>
@@ -28381,7 +28381,7 @@
         <v>401.20988499999999</v>
       </c>
       <c r="AJ19" s="7">
-        <v>0</v>
+        <v>361.42696799999999</v>
       </c>
       <c r="AK19" s="7">
         <v>0</v>
@@ -28543,7 +28543,7 @@
         <v>1061.8927659999999</v>
       </c>
       <c r="AJ20" s="19">
-        <v>0</v>
+        <v>1087.203634</v>
       </c>
       <c r="AK20" s="19">
         <v>0</v>
@@ -28705,7 +28705,7 @@
         <v>860.75445100000002</v>
       </c>
       <c r="AJ21" s="7">
-        <v>0</v>
+        <v>846.67003699999998</v>
       </c>
       <c r="AK21" s="7">
         <v>0</v>
@@ -28867,7 +28867,7 @@
         <v>4187.7313329999997</v>
       </c>
       <c r="AJ22" s="8">
-        <v>0</v>
+        <v>4237.7570420000002</v>
       </c>
       <c r="AK22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Sep 12 05:22:30 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -22772,6 +22772,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -22779,12 +22782,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23288,7 +23291,7 @@
         <v>6733</v>
       </c>
       <c r="AK5" s="19">
-        <v>6416</v>
+        <v>6394</v>
       </c>
       <c r="AL5" s="19">
         <v>6433</v>
@@ -23449,7 +23452,7 @@
         <v>12287</v>
       </c>
       <c r="AK6" s="19">
-        <v>11691</v>
+        <v>11665</v>
       </c>
       <c r="AL6" s="19">
         <v>11950</v>
@@ -23610,7 +23613,7 @@
         <v>20105</v>
       </c>
       <c r="AK7" s="19">
-        <v>18855</v>
+        <v>19587</v>
       </c>
       <c r="AL7" s="19">
         <v>18968</v>
@@ -23771,7 +23774,7 @@
         <v>4243</v>
       </c>
       <c r="AK8" s="19">
-        <v>3876</v>
+        <v>3889</v>
       </c>
       <c r="AL8" s="19">
         <v>3828</v>
@@ -24093,7 +24096,7 @@
         <v>8930</v>
       </c>
       <c r="AK10" s="19">
-        <v>10373</v>
+        <v>10357</v>
       </c>
       <c r="AL10" s="19">
         <v>12531</v>
@@ -24254,7 +24257,7 @@
         <v>52839</v>
       </c>
       <c r="AK11" s="19">
-        <v>46331</v>
+        <v>46310</v>
       </c>
       <c r="AL11" s="19">
         <v>50611</v>
@@ -24415,7 +24418,7 @@
         <v>114834</v>
       </c>
       <c r="AK12" s="8">
-        <v>107825</v>
+        <v>108485</v>
       </c>
       <c r="AL12" s="8">
         <v>115366</v>
@@ -24636,7 +24639,7 @@
         <v>524.56151599999998</v>
       </c>
       <c r="AK15" s="19">
-        <v>489.73348099999998</v>
+        <v>487.86275699999999</v>
       </c>
       <c r="AL15" s="19">
         <v>515.20376099999999</v>
@@ -24797,7 +24800,7 @@
         <v>890.116263</v>
       </c>
       <c r="AK16" s="19">
-        <v>821.83972900000003</v>
+        <v>821.99920699999996</v>
       </c>
       <c r="AL16" s="19">
         <v>844.37060199999996</v>
@@ -24958,7 +24961,7 @@
         <v>586.09682899999996</v>
       </c>
       <c r="AK17" s="19">
-        <v>531.56183399999998</v>
+        <v>531.54656399999999</v>
       </c>
       <c r="AL17" s="19">
         <v>586.21940400000005</v>
@@ -25119,7 +25122,7 @@
         <v>62.481541999999997</v>
       </c>
       <c r="AK18" s="19">
-        <v>56.740982000000002</v>
+        <v>56.811768000000001</v>
       </c>
       <c r="AL18" s="19">
         <v>57.144962999999997</v>
@@ -25280,7 +25283,7 @@
         <v>443.10229299999997</v>
       </c>
       <c r="AK19" s="19">
-        <v>453.409515</v>
+        <v>453.36718500000001</v>
       </c>
       <c r="AL19" s="19">
         <v>419.26886999999999</v>
@@ -25441,7 +25444,7 @@
         <v>759.63975600000003</v>
       </c>
       <c r="AK20" s="19">
-        <v>946.67852800000003</v>
+        <v>946.28463399999998</v>
       </c>
       <c r="AL20" s="19">
         <v>1179.116434</v>
@@ -25602,7 +25605,7 @@
         <v>1153.0830060000001</v>
       </c>
       <c r="AK21" s="19">
-        <v>1003.803734</v>
+        <v>1003.581827</v>
       </c>
       <c r="AL21" s="19">
         <v>1173.1981479999999</v>
@@ -25763,7 +25766,7 @@
         <v>4419.0812050000004</v>
       </c>
       <c r="AK22" s="8">
-        <v>4303.7678029999997</v>
+        <v>4301.4539420000001</v>
       </c>
       <c r="AL22" s="8">
         <v>4774.5221820000006</v>
@@ -25871,8 +25874,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26378,7 +26381,7 @@
         <v>6135</v>
       </c>
       <c r="AK5" s="19">
-        <v>0</v>
+        <v>5743</v>
       </c>
       <c r="AL5" s="19">
         <v>0</v>
@@ -26540,7 +26543,7 @@
         <v>12480</v>
       </c>
       <c r="AK6" s="7">
-        <v>0</v>
+        <v>11892</v>
       </c>
       <c r="AL6" s="7">
         <v>0</v>
@@ -26702,7 +26705,7 @@
         <v>19256</v>
       </c>
       <c r="AK7" s="7">
-        <v>0</v>
+        <v>20237</v>
       </c>
       <c r="AL7" s="7">
         <v>0</v>
@@ -26864,7 +26867,7 @@
         <v>4309</v>
       </c>
       <c r="AK8" s="7">
-        <v>0</v>
+        <v>4491</v>
       </c>
       <c r="AL8" s="7">
         <v>0</v>
@@ -27026,7 +27029,7 @@
         <v>9268</v>
       </c>
       <c r="AK9" s="7">
-        <v>0</v>
+        <v>10210</v>
       </c>
       <c r="AL9" s="7">
         <v>0</v>
@@ -27188,7 +27191,7 @@
         <v>11103</v>
       </c>
       <c r="AK10" s="19">
-        <v>0</v>
+        <v>12428</v>
       </c>
       <c r="AL10" s="19">
         <v>0</v>
@@ -27350,7 +27353,7 @@
         <v>39287</v>
       </c>
       <c r="AK11" s="7">
-        <v>0</v>
+        <v>37249</v>
       </c>
       <c r="AL11" s="7">
         <v>0</v>
@@ -27512,7 +27515,7 @@
         <v>101838</v>
       </c>
       <c r="AK12" s="8">
-        <v>0</v>
+        <v>102250</v>
       </c>
       <c r="AL12" s="8">
         <v>0</v>
@@ -27736,7 +27739,7 @@
         <v>477.95193799999998</v>
       </c>
       <c r="AK15" s="19">
-        <v>0</v>
+        <v>421.91737799999999</v>
       </c>
       <c r="AL15" s="19">
         <v>0</v>
@@ -27898,7 +27901,7 @@
         <v>827.81147699999997</v>
       </c>
       <c r="AK16" s="7">
-        <v>0</v>
+        <v>825.90069200000005</v>
       </c>
       <c r="AL16" s="7">
         <v>0</v>
@@ -28060,7 +28063,7 @@
         <v>576.19058900000005</v>
       </c>
       <c r="AK17" s="7">
-        <v>0</v>
+        <v>571.79369199999996</v>
       </c>
       <c r="AL17" s="7">
         <v>0</v>
@@ -28222,7 +28225,7 @@
         <v>60.502398999999997</v>
       </c>
       <c r="AK18" s="7">
-        <v>0</v>
+        <v>61.965994999999999</v>
       </c>
       <c r="AL18" s="7">
         <v>0</v>
@@ -28384,7 +28387,7 @@
         <v>361.42696799999999</v>
       </c>
       <c r="AK19" s="7">
-        <v>0</v>
+        <v>476.060294</v>
       </c>
       <c r="AL19" s="7">
         <v>0</v>
@@ -28546,7 +28549,7 @@
         <v>1087.203634</v>
       </c>
       <c r="AK20" s="19">
-        <v>0</v>
+        <v>1116.3297500000001</v>
       </c>
       <c r="AL20" s="19">
         <v>0</v>
@@ -28708,7 +28711,7 @@
         <v>846.67003699999998</v>
       </c>
       <c r="AK21" s="7">
-        <v>0</v>
+        <v>829.43938600000001</v>
       </c>
       <c r="AL21" s="7">
         <v>0</v>
@@ -28870,7 +28873,7 @@
         <v>4237.7570420000002</v>
       </c>
       <c r="AK22" s="8">
-        <v>0</v>
+        <v>4303.4071869999998</v>
       </c>
       <c r="AL22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Sep 19 05:23:28 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -22772,9 +22772,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -22787,7 +22784,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="K42" sqref="K42"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23294,7 +23291,7 @@
         <v>6394</v>
       </c>
       <c r="AL5" s="19">
-        <v>6433</v>
+        <v>6415</v>
       </c>
       <c r="AM5" s="19">
         <v>6699</v>
@@ -23455,7 +23452,7 @@
         <v>11665</v>
       </c>
       <c r="AL6" s="19">
-        <v>11950</v>
+        <v>11924</v>
       </c>
       <c r="AM6" s="19">
         <v>11909</v>
@@ -23616,7 +23613,7 @@
         <v>19587</v>
       </c>
       <c r="AL7" s="19">
-        <v>18968</v>
+        <v>19514</v>
       </c>
       <c r="AM7" s="19">
         <v>19923</v>
@@ -23777,7 +23774,7 @@
         <v>3889</v>
       </c>
       <c r="AL8" s="19">
-        <v>3828</v>
+        <v>3810</v>
       </c>
       <c r="AM8" s="19">
         <v>4083</v>
@@ -23938,7 +23935,7 @@
         <v>10283</v>
       </c>
       <c r="AL9" s="19">
-        <v>11045</v>
+        <v>10939</v>
       </c>
       <c r="AM9" s="19">
         <v>7562</v>
@@ -24099,7 +24096,7 @@
         <v>10357</v>
       </c>
       <c r="AL10" s="19">
-        <v>12531</v>
+        <v>12530</v>
       </c>
       <c r="AM10" s="19">
         <v>12228</v>
@@ -24260,7 +24257,7 @@
         <v>46310</v>
       </c>
       <c r="AL11" s="19">
-        <v>50611</v>
+        <v>50524</v>
       </c>
       <c r="AM11" s="19">
         <v>45422</v>
@@ -24421,7 +24418,7 @@
         <v>108485</v>
       </c>
       <c r="AL12" s="8">
-        <v>115366</v>
+        <v>115656</v>
       </c>
       <c r="AM12" s="8">
         <v>107826</v>
@@ -24642,7 +24639,7 @@
         <v>487.86275699999999</v>
       </c>
       <c r="AL15" s="19">
-        <v>515.20376099999999</v>
+        <v>513.29454999999996</v>
       </c>
       <c r="AM15" s="19">
         <v>521.34197200000006</v>
@@ -24803,7 +24800,7 @@
         <v>821.99920699999996</v>
       </c>
       <c r="AL16" s="19">
-        <v>844.37060199999996</v>
+        <v>843.77446799999996</v>
       </c>
       <c r="AM16" s="19">
         <v>809.44283099999996</v>
@@ -24964,7 +24961,7 @@
         <v>531.54656399999999</v>
       </c>
       <c r="AL17" s="19">
-        <v>586.21940400000005</v>
+        <v>579.219605</v>
       </c>
       <c r="AM17" s="19">
         <v>546.17005800000004</v>
@@ -25125,7 +25122,7 @@
         <v>56.811768000000001</v>
       </c>
       <c r="AL18" s="19">
-        <v>57.144962999999997</v>
+        <v>56.917349999999999</v>
       </c>
       <c r="AM18" s="19">
         <v>55.393833000000001</v>
@@ -25286,7 +25283,7 @@
         <v>453.36718500000001</v>
       </c>
       <c r="AL19" s="19">
-        <v>419.26886999999999</v>
+        <v>411.55637200000001</v>
       </c>
       <c r="AM19" s="19">
         <v>341.77711900000003</v>
@@ -25447,7 +25444,7 @@
         <v>946.28463399999998</v>
       </c>
       <c r="AL20" s="19">
-        <v>1179.116434</v>
+        <v>1184.545652</v>
       </c>
       <c r="AM20" s="19">
         <v>1111.2315249999999</v>
@@ -25608,7 +25605,7 @@
         <v>1003.581827</v>
       </c>
       <c r="AL21" s="19">
-        <v>1173.1981479999999</v>
+        <v>1172.4710210000001</v>
       </c>
       <c r="AM21" s="19">
         <v>1010.748098</v>
@@ -25769,7 +25766,7 @@
         <v>4301.4539420000001</v>
       </c>
       <c r="AL22" s="8">
-        <v>4774.5221820000006</v>
+        <v>4761.7790180000002</v>
       </c>
       <c r="AM22" s="8">
         <v>4396.1054359999998</v>
@@ -25875,7 +25872,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38:H39"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26384,7 +26381,7 @@
         <v>5743</v>
       </c>
       <c r="AL5" s="19">
-        <v>0</v>
+        <v>5942</v>
       </c>
       <c r="AM5" s="19">
         <v>0</v>
@@ -26546,7 +26543,7 @@
         <v>11892</v>
       </c>
       <c r="AL6" s="7">
-        <v>0</v>
+        <v>12203</v>
       </c>
       <c r="AM6" s="7">
         <v>0</v>
@@ -26708,7 +26705,7 @@
         <v>20237</v>
       </c>
       <c r="AL7" s="7">
-        <v>0</v>
+        <v>17729</v>
       </c>
       <c r="AM7" s="7">
         <v>0</v>
@@ -26870,7 +26867,7 @@
         <v>4491</v>
       </c>
       <c r="AL8" s="7">
-        <v>0</v>
+        <v>4773</v>
       </c>
       <c r="AM8" s="7">
         <v>0</v>
@@ -27032,7 +27029,7 @@
         <v>10210</v>
       </c>
       <c r="AL9" s="7">
-        <v>0</v>
+        <v>10435</v>
       </c>
       <c r="AM9" s="7">
         <v>0</v>
@@ -27194,7 +27191,7 @@
         <v>12428</v>
       </c>
       <c r="AL10" s="19">
-        <v>0</v>
+        <v>13014</v>
       </c>
       <c r="AM10" s="19">
         <v>0</v>
@@ -27356,7 +27353,7 @@
         <v>37249</v>
       </c>
       <c r="AL11" s="7">
-        <v>0</v>
+        <v>40798</v>
       </c>
       <c r="AM11" s="7">
         <v>0</v>
@@ -27518,7 +27515,7 @@
         <v>102250</v>
       </c>
       <c r="AL12" s="8">
-        <v>0</v>
+        <v>104894</v>
       </c>
       <c r="AM12" s="8">
         <v>0</v>
@@ -27742,7 +27739,7 @@
         <v>421.91737799999999</v>
       </c>
       <c r="AL15" s="19">
-        <v>0</v>
+        <v>453.115228</v>
       </c>
       <c r="AM15" s="19">
         <v>0</v>
@@ -27904,7 +27901,7 @@
         <v>825.90069200000005</v>
       </c>
       <c r="AL16" s="7">
-        <v>0</v>
+        <v>857.56252099999995</v>
       </c>
       <c r="AM16" s="7">
         <v>0</v>
@@ -28066,7 +28063,7 @@
         <v>571.79369199999996</v>
       </c>
       <c r="AL17" s="7">
-        <v>0</v>
+        <v>520.32689500000004</v>
       </c>
       <c r="AM17" s="7">
         <v>0</v>
@@ -28228,7 +28225,7 @@
         <v>61.965994999999999</v>
       </c>
       <c r="AL18" s="7">
-        <v>0</v>
+        <v>64.228583999999998</v>
       </c>
       <c r="AM18" s="7">
         <v>0</v>
@@ -28390,7 +28387,7 @@
         <v>476.060294</v>
       </c>
       <c r="AL19" s="7">
-        <v>0</v>
+        <v>458.12219199999998</v>
       </c>
       <c r="AM19" s="7">
         <v>0</v>
@@ -28552,7 +28549,7 @@
         <v>1116.3297500000001</v>
       </c>
       <c r="AL20" s="19">
-        <v>0</v>
+        <v>1157.946289</v>
       </c>
       <c r="AM20" s="19">
         <v>0</v>
@@ -28714,7 +28711,7 @@
         <v>829.43938600000001</v>
       </c>
       <c r="AL21" s="7">
-        <v>0</v>
+        <v>919.41972299999998</v>
       </c>
       <c r="AM21" s="7">
         <v>0</v>
@@ -28876,7 +28873,7 @@
         <v>4303.4071869999998</v>
       </c>
       <c r="AL22" s="8">
-        <v>0</v>
+        <v>4430.7214320000003</v>
       </c>
       <c r="AM22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Sep 26 05:22:11 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -22772,6 +22772,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -22779,12 +22782,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23294,7 +23297,7 @@
         <v>6415</v>
       </c>
       <c r="AM5" s="19">
-        <v>6699</v>
+        <v>6689</v>
       </c>
       <c r="AN5" s="19">
         <v>6559</v>
@@ -23455,7 +23458,7 @@
         <v>11924</v>
       </c>
       <c r="AM6" s="19">
-        <v>11909</v>
+        <v>11795</v>
       </c>
       <c r="AN6" s="19">
         <v>11831</v>
@@ -23616,7 +23619,7 @@
         <v>19514</v>
       </c>
       <c r="AM7" s="19">
-        <v>19923</v>
+        <v>20443</v>
       </c>
       <c r="AN7" s="19">
         <v>19805</v>
@@ -23777,7 +23780,7 @@
         <v>3810</v>
       </c>
       <c r="AM8" s="19">
-        <v>4083</v>
+        <v>4074</v>
       </c>
       <c r="AN8" s="19">
         <v>4463</v>
@@ -23938,7 +23941,7 @@
         <v>10939</v>
       </c>
       <c r="AM9" s="19">
-        <v>7562</v>
+        <v>7381</v>
       </c>
       <c r="AN9" s="19">
         <v>9393</v>
@@ -24099,7 +24102,7 @@
         <v>12530</v>
       </c>
       <c r="AM10" s="19">
-        <v>12228</v>
+        <v>12195</v>
       </c>
       <c r="AN10" s="19">
         <v>14200</v>
@@ -24260,7 +24263,7 @@
         <v>50524</v>
       </c>
       <c r="AM11" s="19">
-        <v>45422</v>
+        <v>45525</v>
       </c>
       <c r="AN11" s="19">
         <v>50591</v>
@@ -24421,7 +24424,7 @@
         <v>115656</v>
       </c>
       <c r="AM12" s="8">
-        <v>107826</v>
+        <v>108102</v>
       </c>
       <c r="AN12" s="8">
         <v>116842</v>
@@ -24642,7 +24645,7 @@
         <v>513.29454999999996</v>
       </c>
       <c r="AM15" s="19">
-        <v>521.34197200000006</v>
+        <v>521.01743699999997</v>
       </c>
       <c r="AN15" s="19">
         <v>483.47938599999998</v>
@@ -24803,7 +24806,7 @@
         <v>843.77446799999996</v>
       </c>
       <c r="AM16" s="19">
-        <v>809.44283099999996</v>
+        <v>807.58786299999997</v>
       </c>
       <c r="AN16" s="19">
         <v>826.41212700000005</v>
@@ -24964,7 +24967,7 @@
         <v>579.219605</v>
       </c>
       <c r="AM17" s="19">
-        <v>546.17005800000004</v>
+        <v>545.59080600000004</v>
       </c>
       <c r="AN17" s="19">
         <v>571.17974600000002</v>
@@ -25125,7 +25128,7 @@
         <v>56.917349999999999</v>
       </c>
       <c r="AM18" s="19">
-        <v>55.393833000000001</v>
+        <v>55.202246000000002</v>
       </c>
       <c r="AN18" s="19">
         <v>54.356985000000002</v>
@@ -25286,7 +25289,7 @@
         <v>411.55637200000001</v>
       </c>
       <c r="AM19" s="19">
-        <v>341.77711900000003</v>
+        <v>336.92512099999999</v>
       </c>
       <c r="AN19" s="19">
         <v>361.19014099999998</v>
@@ -25447,7 +25450,7 @@
         <v>1184.545652</v>
       </c>
       <c r="AM20" s="19">
-        <v>1111.2315249999999</v>
+        <v>1110.694753</v>
       </c>
       <c r="AN20" s="19">
         <v>1272.4153659999999</v>
@@ -25608,7 +25611,7 @@
         <v>1172.4710210000001</v>
       </c>
       <c r="AM21" s="19">
-        <v>1010.748098</v>
+        <v>1012.613606</v>
       </c>
       <c r="AN21" s="19">
         <v>1108.021808</v>
@@ -25769,7 +25772,7 @@
         <v>4761.7790180000002</v>
       </c>
       <c r="AM22" s="8">
-        <v>4396.1054359999998</v>
+        <v>4389.631832</v>
       </c>
       <c r="AN22" s="8">
         <v>4677.0555590000004</v>
@@ -25871,8 +25874,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26384,7 +26387,7 @@
         <v>5942</v>
       </c>
       <c r="AM5" s="19">
-        <v>0</v>
+        <v>5985</v>
       </c>
       <c r="AN5" s="19">
         <v>0</v>
@@ -26546,7 +26549,7 @@
         <v>12203</v>
       </c>
       <c r="AM6" s="7">
-        <v>0</v>
+        <v>12102</v>
       </c>
       <c r="AN6" s="7">
         <v>0</v>
@@ -26708,7 +26711,7 @@
         <v>17729</v>
       </c>
       <c r="AM7" s="7">
-        <v>0</v>
+        <v>20289</v>
       </c>
       <c r="AN7" s="7">
         <v>0</v>
@@ -26870,7 +26873,7 @@
         <v>4773</v>
       </c>
       <c r="AM8" s="7">
-        <v>0</v>
+        <v>4988</v>
       </c>
       <c r="AN8" s="7">
         <v>0</v>
@@ -27032,7 +27035,7 @@
         <v>10435</v>
       </c>
       <c r="AM9" s="7">
-        <v>0</v>
+        <v>9543</v>
       </c>
       <c r="AN9" s="7">
         <v>0</v>
@@ -27194,7 +27197,7 @@
         <v>13014</v>
       </c>
       <c r="AM10" s="19">
-        <v>0</v>
+        <v>14549</v>
       </c>
       <c r="AN10" s="19">
         <v>0</v>
@@ -27356,7 +27359,7 @@
         <v>40798</v>
       </c>
       <c r="AM11" s="7">
-        <v>0</v>
+        <v>41926</v>
       </c>
       <c r="AN11" s="7">
         <v>0</v>
@@ -27518,7 +27521,7 @@
         <v>104894</v>
       </c>
       <c r="AM12" s="8">
-        <v>0</v>
+        <v>109382</v>
       </c>
       <c r="AN12" s="8">
         <v>0</v>
@@ -27742,7 +27745,7 @@
         <v>453.115228</v>
       </c>
       <c r="AM15" s="19">
-        <v>0</v>
+        <v>447.72177799999997</v>
       </c>
       <c r="AN15" s="19">
         <v>0</v>
@@ -27904,7 +27907,7 @@
         <v>857.56252099999995</v>
       </c>
       <c r="AM16" s="7">
-        <v>0</v>
+        <v>816.82095900000002</v>
       </c>
       <c r="AN16" s="7">
         <v>0</v>
@@ -28066,7 +28069,7 @@
         <v>520.32689500000004</v>
       </c>
       <c r="AM17" s="7">
-        <v>0</v>
+        <v>531.17191200000002</v>
       </c>
       <c r="AN17" s="7">
         <v>0</v>
@@ -28228,7 +28231,7 @@
         <v>64.228583999999998</v>
       </c>
       <c r="AM18" s="7">
-        <v>0</v>
+        <v>68.635548999999997</v>
       </c>
       <c r="AN18" s="7">
         <v>0</v>
@@ -28390,7 +28393,7 @@
         <v>458.12219199999998</v>
       </c>
       <c r="AM19" s="7">
-        <v>0</v>
+        <v>420.62093399999998</v>
       </c>
       <c r="AN19" s="7">
         <v>0</v>
@@ -28552,7 +28555,7 @@
         <v>1157.946289</v>
       </c>
       <c r="AM20" s="19">
-        <v>0</v>
+        <v>1360.5035929999999</v>
       </c>
       <c r="AN20" s="19">
         <v>0</v>
@@ -28714,7 +28717,7 @@
         <v>919.41972299999998</v>
       </c>
       <c r="AM21" s="7">
-        <v>0</v>
+        <v>977.00921100000005</v>
       </c>
       <c r="AN21" s="7">
         <v>0</v>
@@ -28876,7 +28879,7 @@
         <v>4430.7214320000003</v>
       </c>
       <c r="AM22" s="8">
-        <v>0</v>
+        <v>4622.4839360000005</v>
       </c>
       <c r="AN22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Wed Oct  4 05:24:26 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -22787,7 +22787,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomRight" activeCell="F39" sqref="F38:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23300,7 +23300,7 @@
         <v>6689</v>
       </c>
       <c r="AN5" s="19">
-        <v>6559</v>
+        <v>6544</v>
       </c>
       <c r="AO5" s="19">
         <v>6601</v>
@@ -23461,7 +23461,7 @@
         <v>11795</v>
       </c>
       <c r="AN6" s="19">
-        <v>11831</v>
+        <v>11827</v>
       </c>
       <c r="AO6" s="19">
         <v>12149</v>
@@ -23622,7 +23622,7 @@
         <v>20443</v>
       </c>
       <c r="AN7" s="19">
-        <v>19805</v>
+        <v>20598</v>
       </c>
       <c r="AO7" s="19">
         <v>18944</v>
@@ -23783,7 +23783,7 @@
         <v>4074</v>
       </c>
       <c r="AN8" s="19">
-        <v>4463</v>
+        <v>4449</v>
       </c>
       <c r="AO8" s="19">
         <v>4013</v>
@@ -23944,7 +23944,7 @@
         <v>7381</v>
       </c>
       <c r="AN9" s="19">
-        <v>9393</v>
+        <v>9423</v>
       </c>
       <c r="AO9" s="19">
         <v>9373</v>
@@ -24105,7 +24105,7 @@
         <v>12195</v>
       </c>
       <c r="AN10" s="19">
-        <v>14200</v>
+        <v>14126</v>
       </c>
       <c r="AO10" s="19">
         <v>15394</v>
@@ -24266,7 +24266,7 @@
         <v>45525</v>
       </c>
       <c r="AN11" s="19">
-        <v>50591</v>
+        <v>50466</v>
       </c>
       <c r="AO11" s="19">
         <v>49446</v>
@@ -24427,7 +24427,7 @@
         <v>108102</v>
       </c>
       <c r="AN12" s="8">
-        <v>116842</v>
+        <v>117433</v>
       </c>
       <c r="AO12" s="8">
         <v>115920</v>
@@ -24648,7 +24648,7 @@
         <v>521.01743699999997</v>
       </c>
       <c r="AN15" s="19">
-        <v>483.47938599999998</v>
+        <v>479.431104</v>
       </c>
       <c r="AO15" s="19">
         <v>494.66531600000002</v>
@@ -24809,7 +24809,7 @@
         <v>807.58786299999997</v>
       </c>
       <c r="AN16" s="19">
-        <v>826.41212700000005</v>
+        <v>826.28208600000005</v>
       </c>
       <c r="AO16" s="19">
         <v>826.45504100000005</v>
@@ -24970,7 +24970,7 @@
         <v>545.59080600000004</v>
       </c>
       <c r="AN17" s="19">
-        <v>571.17974600000002</v>
+        <v>570.92526399999997</v>
       </c>
       <c r="AO17" s="19">
         <v>456.641077</v>
@@ -25131,7 +25131,7 @@
         <v>55.202246000000002</v>
       </c>
       <c r="AN18" s="19">
-        <v>54.356985000000002</v>
+        <v>54.152121000000001</v>
       </c>
       <c r="AO18" s="19">
         <v>51.659765999999998</v>
@@ -25292,7 +25292,7 @@
         <v>336.92512099999999</v>
       </c>
       <c r="AN19" s="19">
-        <v>361.19014099999998</v>
+        <v>364.19976500000001</v>
       </c>
       <c r="AO19" s="19">
         <v>381.95059199999997</v>
@@ -25453,7 +25453,7 @@
         <v>1110.694753</v>
       </c>
       <c r="AN20" s="19">
-        <v>1272.4153659999999</v>
+        <v>1268.875397</v>
       </c>
       <c r="AO20" s="19">
         <v>1397.462383</v>
@@ -25614,7 +25614,7 @@
         <v>1012.613606</v>
       </c>
       <c r="AN21" s="19">
-        <v>1108.021808</v>
+        <v>1105.9637540000001</v>
       </c>
       <c r="AO21" s="19">
         <v>1120.38499</v>
@@ -25775,7 +25775,7 @@
         <v>4389.631832</v>
       </c>
       <c r="AN22" s="8">
-        <v>4677.0555590000004</v>
+        <v>4669.8294910000004</v>
       </c>
       <c r="AO22" s="8">
         <v>4729.2191650000004</v>
@@ -25875,7 +25875,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26390,7 +26390,7 @@
         <v>5985</v>
       </c>
       <c r="AN5" s="19">
-        <v>0</v>
+        <v>5780</v>
       </c>
       <c r="AO5" s="19">
         <v>0</v>
@@ -26552,7 +26552,7 @@
         <v>12102</v>
       </c>
       <c r="AN6" s="7">
-        <v>0</v>
+        <v>11559</v>
       </c>
       <c r="AO6" s="7">
         <v>0</v>
@@ -26714,7 +26714,7 @@
         <v>20289</v>
       </c>
       <c r="AN7" s="7">
-        <v>0</v>
+        <v>20471</v>
       </c>
       <c r="AO7" s="7">
         <v>0</v>
@@ -26876,7 +26876,7 @@
         <v>4988</v>
       </c>
       <c r="AN8" s="7">
-        <v>0</v>
+        <v>5217</v>
       </c>
       <c r="AO8" s="7">
         <v>0</v>
@@ -27038,7 +27038,7 @@
         <v>9543</v>
       </c>
       <c r="AN9" s="7">
-        <v>0</v>
+        <v>10011</v>
       </c>
       <c r="AO9" s="7">
         <v>0</v>
@@ -27200,7 +27200,7 @@
         <v>14549</v>
       </c>
       <c r="AN10" s="19">
-        <v>0</v>
+        <v>15208</v>
       </c>
       <c r="AO10" s="19">
         <v>0</v>
@@ -27362,7 +27362,7 @@
         <v>41926</v>
       </c>
       <c r="AN11" s="7">
-        <v>0</v>
+        <v>41438</v>
       </c>
       <c r="AO11" s="7">
         <v>0</v>
@@ -27524,7 +27524,7 @@
         <v>109382</v>
       </c>
       <c r="AN12" s="8">
-        <v>0</v>
+        <v>109684</v>
       </c>
       <c r="AO12" s="8">
         <v>0</v>
@@ -27748,7 +27748,7 @@
         <v>447.72177799999997</v>
       </c>
       <c r="AN15" s="19">
-        <v>0</v>
+        <v>426.14194199999997</v>
       </c>
       <c r="AO15" s="19">
         <v>0</v>
@@ -27910,7 +27910,7 @@
         <v>816.82095900000002</v>
       </c>
       <c r="AN16" s="7">
-        <v>0</v>
+        <v>788.05608099999995</v>
       </c>
       <c r="AO16" s="7">
         <v>0</v>
@@ -28072,7 +28072,7 @@
         <v>531.17191200000002</v>
       </c>
       <c r="AN17" s="7">
-        <v>0</v>
+        <v>634.70223999999996</v>
       </c>
       <c r="AO17" s="7">
         <v>0</v>
@@ -28234,7 +28234,7 @@
         <v>68.635548999999997</v>
       </c>
       <c r="AN18" s="7">
-        <v>0</v>
+        <v>72.163685000000001</v>
       </c>
       <c r="AO18" s="7">
         <v>0</v>
@@ -28396,7 +28396,7 @@
         <v>420.62093399999998</v>
       </c>
       <c r="AN19" s="7">
-        <v>0</v>
+        <v>424.03746799999999</v>
       </c>
       <c r="AO19" s="7">
         <v>0</v>
@@ -28558,7 +28558,7 @@
         <v>1360.5035929999999</v>
       </c>
       <c r="AN20" s="19">
-        <v>0</v>
+        <v>1502.291872</v>
       </c>
       <c r="AO20" s="19">
         <v>0</v>
@@ -28720,7 +28720,7 @@
         <v>977.00921100000005</v>
       </c>
       <c r="AN21" s="7">
-        <v>0</v>
+        <v>904.89198199999998</v>
       </c>
       <c r="AO21" s="7">
         <v>0</v>
@@ -28882,7 +28882,7 @@
         <v>4622.4839360000005</v>
       </c>
       <c r="AN22" s="8">
-        <v>0</v>
+        <v>4752.2852700000003</v>
       </c>
       <c r="AO22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Wed Oct 11 05:22:14 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -22787,7 +22787,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="F39" sqref="F38:F39"/>
+      <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23303,7 +23303,7 @@
         <v>6544</v>
       </c>
       <c r="AO5" s="19">
-        <v>6601</v>
+        <v>6581</v>
       </c>
       <c r="AP5" s="19">
         <v>6357</v>
@@ -23464,7 +23464,7 @@
         <v>11827</v>
       </c>
       <c r="AO6" s="19">
-        <v>12149</v>
+        <v>12133</v>
       </c>
       <c r="AP6" s="19">
         <v>11420</v>
@@ -23625,7 +23625,7 @@
         <v>20598</v>
       </c>
       <c r="AO7" s="19">
-        <v>18944</v>
+        <v>19992</v>
       </c>
       <c r="AP7" s="19">
         <v>19676</v>
@@ -23786,7 +23786,7 @@
         <v>4449</v>
       </c>
       <c r="AO8" s="19">
-        <v>4013</v>
+        <v>4011</v>
       </c>
       <c r="AP8" s="19">
         <v>4124</v>
@@ -23947,7 +23947,7 @@
         <v>9423</v>
       </c>
       <c r="AO9" s="19">
-        <v>9373</v>
+        <v>9256</v>
       </c>
       <c r="AP9" s="19">
         <v>10327</v>
@@ -24108,7 +24108,7 @@
         <v>14126</v>
       </c>
       <c r="AO10" s="19">
-        <v>15394</v>
+        <v>15376</v>
       </c>
       <c r="AP10" s="19">
         <v>15791</v>
@@ -24269,7 +24269,7 @@
         <v>50466</v>
       </c>
       <c r="AO11" s="19">
-        <v>49446</v>
+        <v>49385</v>
       </c>
       <c r="AP11" s="19">
         <v>46403</v>
@@ -24430,7 +24430,7 @@
         <v>117433</v>
       </c>
       <c r="AO12" s="8">
-        <v>115920</v>
+        <v>116734</v>
       </c>
       <c r="AP12" s="8">
         <v>114098</v>
@@ -24651,7 +24651,7 @@
         <v>479.431104</v>
       </c>
       <c r="AO15" s="19">
-        <v>494.66531600000002</v>
+        <v>491.77408400000002</v>
       </c>
       <c r="AP15" s="19">
         <v>457.22720900000002</v>
@@ -24812,7 +24812,7 @@
         <v>826.28208600000005</v>
       </c>
       <c r="AO16" s="19">
-        <v>826.45504100000005</v>
+        <v>826.09751800000004</v>
       </c>
       <c r="AP16" s="19">
         <v>793.65536999999995</v>
@@ -24973,7 +24973,7 @@
         <v>570.92526399999997</v>
       </c>
       <c r="AO17" s="19">
-        <v>456.641077</v>
+        <v>474.20423599999998</v>
       </c>
       <c r="AP17" s="19">
         <v>489.297574</v>
@@ -25134,7 +25134,7 @@
         <v>54.152121000000001</v>
       </c>
       <c r="AO18" s="19">
-        <v>51.659765999999998</v>
+        <v>51.589692999999997</v>
       </c>
       <c r="AP18" s="19">
         <v>53.710757000000001</v>
@@ -25295,7 +25295,7 @@
         <v>364.19976500000001</v>
       </c>
       <c r="AO19" s="19">
-        <v>381.95059199999997</v>
+        <v>381.91619700000001</v>
       </c>
       <c r="AP19" s="19">
         <v>409.33619800000002</v>
@@ -25456,7 +25456,7 @@
         <v>1268.875397</v>
       </c>
       <c r="AO20" s="19">
-        <v>1397.462383</v>
+        <v>1395.6897269999999</v>
       </c>
       <c r="AP20" s="19">
         <v>1478.0898400000001</v>
@@ -25617,7 +25617,7 @@
         <v>1105.9637540000001</v>
       </c>
       <c r="AO21" s="19">
-        <v>1120.38499</v>
+        <v>1120.342969</v>
       </c>
       <c r="AP21" s="19">
         <v>1043.7050839999999</v>
@@ -25778,7 +25778,7 @@
         <v>4669.8294910000004</v>
       </c>
       <c r="AO22" s="8">
-        <v>4729.2191650000004</v>
+        <v>4741.6144240000003</v>
       </c>
       <c r="AP22" s="8">
         <v>4725.0220319999999</v>
@@ -25875,7 +25875,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E39" sqref="E38:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26393,7 +26393,7 @@
         <v>5780</v>
       </c>
       <c r="AO5" s="19">
-        <v>0</v>
+        <v>5957</v>
       </c>
       <c r="AP5" s="19">
         <v>0</v>
@@ -26555,7 +26555,7 @@
         <v>11559</v>
       </c>
       <c r="AO6" s="7">
-        <v>0</v>
+        <v>11951</v>
       </c>
       <c r="AP6" s="7">
         <v>0</v>
@@ -26717,7 +26717,7 @@
         <v>20471</v>
       </c>
       <c r="AO7" s="7">
-        <v>0</v>
+        <v>19934</v>
       </c>
       <c r="AP7" s="7">
         <v>0</v>
@@ -26879,7 +26879,7 @@
         <v>5217</v>
       </c>
       <c r="AO8" s="7">
-        <v>0</v>
+        <v>5071</v>
       </c>
       <c r="AP8" s="7">
         <v>0</v>
@@ -27041,7 +27041,7 @@
         <v>10011</v>
       </c>
       <c r="AO9" s="7">
-        <v>0</v>
+        <v>10757</v>
       </c>
       <c r="AP9" s="7">
         <v>0</v>
@@ -27203,7 +27203,7 @@
         <v>15208</v>
       </c>
       <c r="AO10" s="19">
-        <v>0</v>
+        <v>16251</v>
       </c>
       <c r="AP10" s="19">
         <v>0</v>
@@ -27365,7 +27365,7 @@
         <v>41438</v>
       </c>
       <c r="AO11" s="7">
-        <v>0</v>
+        <v>40294</v>
       </c>
       <c r="AP11" s="7">
         <v>0</v>
@@ -27527,7 +27527,7 @@
         <v>109684</v>
       </c>
       <c r="AO12" s="8">
-        <v>0</v>
+        <v>110215</v>
       </c>
       <c r="AP12" s="8">
         <v>0</v>
@@ -27751,7 +27751,7 @@
         <v>426.14194199999997</v>
       </c>
       <c r="AO15" s="19">
-        <v>0</v>
+        <v>453.26573000000002</v>
       </c>
       <c r="AP15" s="19">
         <v>0</v>
@@ -27913,7 +27913,7 @@
         <v>788.05608099999995</v>
       </c>
       <c r="AO16" s="7">
-        <v>0</v>
+        <v>810.61133900000004</v>
       </c>
       <c r="AP16" s="7">
         <v>0</v>
@@ -28075,7 +28075,7 @@
         <v>634.70223999999996</v>
       </c>
       <c r="AO17" s="7">
-        <v>0</v>
+        <v>599.29353600000002</v>
       </c>
       <c r="AP17" s="7">
         <v>0</v>
@@ -28237,7 +28237,7 @@
         <v>72.163685000000001</v>
       </c>
       <c r="AO18" s="7">
-        <v>0</v>
+        <v>71.428331</v>
       </c>
       <c r="AP18" s="7">
         <v>0</v>
@@ -28399,7 +28399,7 @@
         <v>424.03746799999999</v>
       </c>
       <c r="AO19" s="7">
-        <v>0</v>
+        <v>418.30478599999998</v>
       </c>
       <c r="AP19" s="7">
         <v>0</v>
@@ -28561,7 +28561,7 @@
         <v>1502.291872</v>
       </c>
       <c r="AO20" s="19">
-        <v>0</v>
+        <v>1466.612709</v>
       </c>
       <c r="AP20" s="19">
         <v>0</v>
@@ -28723,7 +28723,7 @@
         <v>904.89198199999998</v>
       </c>
       <c r="AO21" s="7">
-        <v>0</v>
+        <v>940.44672600000001</v>
       </c>
       <c r="AP21" s="7">
         <v>0</v>
@@ -28885,7 +28885,7 @@
         <v>4752.2852700000003</v>
       </c>
       <c r="AO22" s="8">
-        <v>0</v>
+        <v>4759.9631570000001</v>
       </c>
       <c r="AP22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Oct 17 05:22:22 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -22772,9 +22772,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -22787,7 +22784,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23306,7 +23303,7 @@
         <v>6581</v>
       </c>
       <c r="AP5" s="19">
-        <v>6357</v>
+        <v>6348</v>
       </c>
       <c r="AQ5" s="19">
         <v>6498</v>
@@ -23467,7 +23464,7 @@
         <v>12133</v>
       </c>
       <c r="AP6" s="19">
-        <v>11420</v>
+        <v>11408</v>
       </c>
       <c r="AQ6" s="19">
         <v>11857</v>
@@ -23628,7 +23625,7 @@
         <v>19992</v>
       </c>
       <c r="AP7" s="19">
-        <v>19676</v>
+        <v>20649</v>
       </c>
       <c r="AQ7" s="19">
         <v>18337</v>
@@ -23789,7 +23786,7 @@
         <v>4011</v>
       </c>
       <c r="AP8" s="19">
-        <v>4124</v>
+        <v>4119</v>
       </c>
       <c r="AQ8" s="19">
         <v>3999</v>
@@ -23950,7 +23947,7 @@
         <v>9256</v>
       </c>
       <c r="AP9" s="19">
-        <v>10327</v>
+        <v>10329</v>
       </c>
       <c r="AQ9" s="19">
         <v>11475</v>
@@ -24111,7 +24108,7 @@
         <v>15376</v>
       </c>
       <c r="AP10" s="19">
-        <v>15791</v>
+        <v>15730</v>
       </c>
       <c r="AQ10" s="19">
         <v>16472</v>
@@ -24272,7 +24269,7 @@
         <v>49385</v>
       </c>
       <c r="AP11" s="19">
-        <v>46403</v>
+        <v>46424</v>
       </c>
       <c r="AQ11" s="19">
         <v>45087</v>
@@ -24433,7 +24430,7 @@
         <v>116734</v>
       </c>
       <c r="AP12" s="8">
-        <v>114098</v>
+        <v>115007</v>
       </c>
       <c r="AQ12" s="8">
         <v>113725</v>
@@ -24654,7 +24651,7 @@
         <v>491.77408400000002</v>
       </c>
       <c r="AP15" s="19">
-        <v>457.22720900000002</v>
+        <v>454.892404</v>
       </c>
       <c r="AQ15" s="19">
         <v>500.54783400000002</v>
@@ -24815,7 +24812,7 @@
         <v>826.09751800000004</v>
       </c>
       <c r="AP16" s="19">
-        <v>793.65536999999995</v>
+        <v>793.84245099999998</v>
       </c>
       <c r="AQ16" s="19">
         <v>793.66749300000004</v>
@@ -24976,7 +24973,7 @@
         <v>474.20423599999998</v>
       </c>
       <c r="AP17" s="19">
-        <v>489.297574</v>
+        <v>489.14712200000002</v>
       </c>
       <c r="AQ17" s="19">
         <v>623.07083</v>
@@ -25137,7 +25134,7 @@
         <v>51.589692999999997</v>
       </c>
       <c r="AP18" s="19">
-        <v>53.710757000000001</v>
+        <v>53.644734999999997</v>
       </c>
       <c r="AQ18" s="19">
         <v>56.821790999999997</v>
@@ -25298,7 +25295,7 @@
         <v>381.91619700000001</v>
       </c>
       <c r="AP19" s="19">
-        <v>409.33619800000002</v>
+        <v>409.41935699999999</v>
       </c>
       <c r="AQ19" s="19">
         <v>440.67939899999999</v>
@@ -25459,7 +25456,7 @@
         <v>1395.6897269999999</v>
       </c>
       <c r="AP20" s="19">
-        <v>1478.0898400000001</v>
+        <v>1468.2030299999999</v>
       </c>
       <c r="AQ20" s="19">
         <v>1536.938142</v>
@@ -25620,7 +25617,7 @@
         <v>1120.342969</v>
       </c>
       <c r="AP21" s="19">
-        <v>1043.7050839999999</v>
+        <v>1044.880056</v>
       </c>
       <c r="AQ21" s="19">
         <v>1077.573449</v>
@@ -25781,7 +25778,7 @@
         <v>4741.6144240000003</v>
       </c>
       <c r="AP22" s="8">
-        <v>4725.0220319999999</v>
+        <v>4714.0291550000002</v>
       </c>
       <c r="AQ22" s="8">
         <v>5029.2989379999999</v>
@@ -25875,7 +25872,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E38:E39"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26396,7 +26393,7 @@
         <v>5957</v>
       </c>
       <c r="AP5" s="19">
-        <v>0</v>
+        <v>5566</v>
       </c>
       <c r="AQ5" s="19">
         <v>0</v>
@@ -26558,7 +26555,7 @@
         <v>11951</v>
       </c>
       <c r="AP6" s="7">
-        <v>0</v>
+        <v>12157</v>
       </c>
       <c r="AQ6" s="7">
         <v>0</v>
@@ -26720,7 +26717,7 @@
         <v>19934</v>
       </c>
       <c r="AP7" s="7">
-        <v>0</v>
+        <v>18757</v>
       </c>
       <c r="AQ7" s="7">
         <v>0</v>
@@ -26882,7 +26879,7 @@
         <v>5071</v>
       </c>
       <c r="AP8" s="7">
-        <v>0</v>
+        <v>4641</v>
       </c>
       <c r="AQ8" s="7">
         <v>0</v>
@@ -27044,7 +27041,7 @@
         <v>10757</v>
       </c>
       <c r="AP9" s="7">
-        <v>0</v>
+        <v>9702</v>
       </c>
       <c r="AQ9" s="7">
         <v>0</v>
@@ -27206,7 +27203,7 @@
         <v>16251</v>
       </c>
       <c r="AP10" s="19">
-        <v>0</v>
+        <v>15314</v>
       </c>
       <c r="AQ10" s="19">
         <v>0</v>
@@ -27368,7 +27365,7 @@
         <v>40294</v>
       </c>
       <c r="AP11" s="7">
-        <v>0</v>
+        <v>39331</v>
       </c>
       <c r="AQ11" s="7">
         <v>0</v>
@@ -27530,7 +27527,7 @@
         <v>110215</v>
       </c>
       <c r="AP12" s="8">
-        <v>0</v>
+        <v>105468</v>
       </c>
       <c r="AQ12" s="8">
         <v>0</v>
@@ -27754,7 +27751,7 @@
         <v>453.26573000000002</v>
       </c>
       <c r="AP15" s="19">
-        <v>0</v>
+        <v>415.21233799999999</v>
       </c>
       <c r="AQ15" s="19">
         <v>0</v>
@@ -27916,7 +27913,7 @@
         <v>810.61133900000004</v>
       </c>
       <c r="AP16" s="7">
-        <v>0</v>
+        <v>838.05247699999995</v>
       </c>
       <c r="AQ16" s="7">
         <v>0</v>
@@ -28078,7 +28075,7 @@
         <v>599.29353600000002</v>
       </c>
       <c r="AP17" s="7">
-        <v>0</v>
+        <v>629.89371700000004</v>
       </c>
       <c r="AQ17" s="7">
         <v>0</v>
@@ -28240,7 +28237,7 @@
         <v>71.428331</v>
       </c>
       <c r="AP18" s="7">
-        <v>0</v>
+        <v>61.485888000000003</v>
       </c>
       <c r="AQ18" s="7">
         <v>0</v>
@@ -28402,7 +28399,7 @@
         <v>418.30478599999998</v>
       </c>
       <c r="AP19" s="7">
-        <v>0</v>
+        <v>411.84829500000001</v>
       </c>
       <c r="AQ19" s="7">
         <v>0</v>
@@ -28564,7 +28561,7 @@
         <v>1466.612709</v>
       </c>
       <c r="AP20" s="19">
-        <v>0</v>
+        <v>1505.6943879999999</v>
       </c>
       <c r="AQ20" s="19">
         <v>0</v>
@@ -28726,7 +28723,7 @@
         <v>940.44672600000001</v>
       </c>
       <c r="AP21" s="7">
-        <v>0</v>
+        <v>866.54798700000003</v>
       </c>
       <c r="AQ21" s="7">
         <v>0</v>
@@ -28888,7 +28885,7 @@
         <v>4759.9631570000001</v>
       </c>
       <c r="AP22" s="8">
-        <v>0</v>
+        <v>4728.7350900000001</v>
       </c>
       <c r="AQ22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Oct 24 05:22:11 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -22784,7 +22784,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23306,7 +23306,7 @@
         <v>6348</v>
       </c>
       <c r="AQ5" s="19">
-        <v>6498</v>
+        <v>6480</v>
       </c>
       <c r="AR5" s="19">
         <v>6530</v>
@@ -23467,7 +23467,7 @@
         <v>11408</v>
       </c>
       <c r="AQ6" s="19">
-        <v>11857</v>
+        <v>11732</v>
       </c>
       <c r="AR6" s="19">
         <v>12052</v>
@@ -23628,7 +23628,7 @@
         <v>20649</v>
       </c>
       <c r="AQ7" s="19">
-        <v>18337</v>
+        <v>19280</v>
       </c>
       <c r="AR7" s="19">
         <v>16367</v>
@@ -23789,7 +23789,7 @@
         <v>4119</v>
       </c>
       <c r="AQ8" s="19">
-        <v>3999</v>
+        <v>3996</v>
       </c>
       <c r="AR8" s="19">
         <v>4665</v>
@@ -23950,7 +23950,7 @@
         <v>10329</v>
       </c>
       <c r="AQ9" s="19">
-        <v>11475</v>
+        <v>11430</v>
       </c>
       <c r="AR9" s="19">
         <v>10827</v>
@@ -24111,7 +24111,7 @@
         <v>15730</v>
       </c>
       <c r="AQ10" s="19">
-        <v>16472</v>
+        <v>16679</v>
       </c>
       <c r="AR10" s="19">
         <v>14672</v>
@@ -24272,7 +24272,7 @@
         <v>46424</v>
       </c>
       <c r="AQ11" s="19">
-        <v>45087</v>
+        <v>44938</v>
       </c>
       <c r="AR11" s="19">
         <v>45151</v>
@@ -24433,7 +24433,7 @@
         <v>115007</v>
       </c>
       <c r="AQ12" s="8">
-        <v>113725</v>
+        <v>114535</v>
       </c>
       <c r="AR12" s="8">
         <v>110264</v>
@@ -24654,7 +24654,7 @@
         <v>454.892404</v>
       </c>
       <c r="AQ15" s="19">
-        <v>500.54783400000002</v>
+        <v>497.84841299999999</v>
       </c>
       <c r="AR15" s="19">
         <v>491.28521599999999</v>
@@ -24815,7 +24815,7 @@
         <v>793.84245099999998</v>
       </c>
       <c r="AQ16" s="19">
-        <v>793.66749300000004</v>
+        <v>787.65963099999999</v>
       </c>
       <c r="AR16" s="19">
         <v>839.51689299999998</v>
@@ -24976,7 +24976,7 @@
         <v>489.14712200000002</v>
       </c>
       <c r="AQ17" s="19">
-        <v>623.07083</v>
+        <v>622.595823</v>
       </c>
       <c r="AR17" s="19">
         <v>644.76174900000001</v>
@@ -25137,7 +25137,7 @@
         <v>53.644734999999997</v>
       </c>
       <c r="AQ18" s="19">
-        <v>56.821790999999997</v>
+        <v>56.755087000000003</v>
       </c>
       <c r="AR18" s="19">
         <v>62.720484999999996</v>
@@ -25298,7 +25298,7 @@
         <v>409.41935699999999</v>
       </c>
       <c r="AQ19" s="19">
-        <v>440.67939899999999</v>
+        <v>446.20862899999997</v>
       </c>
       <c r="AR19" s="19">
         <v>459.39371999999997</v>
@@ -25459,7 +25459,7 @@
         <v>1468.2030299999999</v>
       </c>
       <c r="AQ20" s="19">
-        <v>1536.938142</v>
+        <v>1541.5027170000001</v>
       </c>
       <c r="AR20" s="19">
         <v>1346.452513</v>
@@ -25620,7 +25620,7 @@
         <v>1044.880056</v>
       </c>
       <c r="AQ21" s="19">
-        <v>1077.573449</v>
+        <v>1076.4139869999999</v>
       </c>
       <c r="AR21" s="19">
         <v>1069.457803</v>
@@ -25781,7 +25781,7 @@
         <v>4714.0291550000002</v>
       </c>
       <c r="AQ22" s="8">
-        <v>5029.2989379999999</v>
+        <v>5028.9842870000002</v>
       </c>
       <c r="AR22" s="8">
         <v>4913.5883789999998</v>
@@ -25872,7 +25872,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26396,7 +26396,7 @@
         <v>5566</v>
       </c>
       <c r="AQ5" s="19">
-        <v>0</v>
+        <v>5523</v>
       </c>
       <c r="AR5" s="19">
         <v>0</v>
@@ -26558,7 +26558,7 @@
         <v>12157</v>
       </c>
       <c r="AQ6" s="7">
-        <v>0</v>
+        <v>12298</v>
       </c>
       <c r="AR6" s="7">
         <v>0</v>
@@ -26720,7 +26720,7 @@
         <v>18757</v>
       </c>
       <c r="AQ7" s="7">
-        <v>0</v>
+        <v>19523</v>
       </c>
       <c r="AR7" s="7">
         <v>0</v>
@@ -26882,7 +26882,7 @@
         <v>4641</v>
       </c>
       <c r="AQ8" s="7">
-        <v>0</v>
+        <v>4911</v>
       </c>
       <c r="AR8" s="7">
         <v>0</v>
@@ -27044,7 +27044,7 @@
         <v>9702</v>
       </c>
       <c r="AQ9" s="7">
-        <v>0</v>
+        <v>9486</v>
       </c>
       <c r="AR9" s="7">
         <v>0</v>
@@ -27206,7 +27206,7 @@
         <v>15314</v>
       </c>
       <c r="AQ10" s="19">
-        <v>0</v>
+        <v>16412</v>
       </c>
       <c r="AR10" s="19">
         <v>0</v>
@@ -27368,7 +27368,7 @@
         <v>39331</v>
       </c>
       <c r="AQ11" s="7">
-        <v>0</v>
+        <v>41162</v>
       </c>
       <c r="AR11" s="7">
         <v>0</v>
@@ -27530,7 +27530,7 @@
         <v>105468</v>
       </c>
       <c r="AQ12" s="8">
-        <v>0</v>
+        <v>109315</v>
       </c>
       <c r="AR12" s="8">
         <v>0</v>
@@ -27754,7 +27754,7 @@
         <v>415.21233799999999</v>
       </c>
       <c r="AQ15" s="19">
-        <v>0</v>
+        <v>436.81901599999998</v>
       </c>
       <c r="AR15" s="19">
         <v>0</v>
@@ -27916,7 +27916,7 @@
         <v>838.05247699999995</v>
       </c>
       <c r="AQ16" s="7">
-        <v>0</v>
+        <v>839.25483699999995</v>
       </c>
       <c r="AR16" s="7">
         <v>0</v>
@@ -28078,7 +28078,7 @@
         <v>629.89371700000004</v>
       </c>
       <c r="AQ17" s="7">
-        <v>0</v>
+        <v>573.95665799999995</v>
       </c>
       <c r="AR17" s="7">
         <v>0</v>
@@ -28240,7 +28240,7 @@
         <v>61.485888000000003</v>
       </c>
       <c r="AQ18" s="7">
-        <v>0</v>
+        <v>77.333590999999998</v>
       </c>
       <c r="AR18" s="7">
         <v>0</v>
@@ -28402,7 +28402,7 @@
         <v>411.84829500000001</v>
       </c>
       <c r="AQ19" s="7">
-        <v>0</v>
+        <v>420.31390699999997</v>
       </c>
       <c r="AR19" s="7">
         <v>0</v>
@@ -28564,7 +28564,7 @@
         <v>1505.6943879999999</v>
       </c>
       <c r="AQ20" s="19">
-        <v>0</v>
+        <v>1569.0897210000001</v>
       </c>
       <c r="AR20" s="19">
         <v>0</v>
@@ -28726,7 +28726,7 @@
         <v>866.54798700000003</v>
       </c>
       <c r="AQ21" s="7">
-        <v>0</v>
+        <v>911.84274600000003</v>
       </c>
       <c r="AR21" s="7">
         <v>0</v>
@@ -28888,7 +28888,7 @@
         <v>4728.7350900000001</v>
       </c>
       <c r="AQ22" s="8">
-        <v>0</v>
+        <v>4828.6104760000007</v>
       </c>
       <c r="AR22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Oct 31 05:22:22 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -22772,6 +22772,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -22784,7 +22787,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23309,7 +23312,7 @@
         <v>6480</v>
       </c>
       <c r="AR5" s="19">
-        <v>6530</v>
+        <v>6499</v>
       </c>
       <c r="AS5" s="19">
         <v>6509</v>
@@ -23470,7 +23473,7 @@
         <v>11732</v>
       </c>
       <c r="AR6" s="19">
-        <v>12052</v>
+        <v>12040</v>
       </c>
       <c r="AS6" s="19">
         <v>11934</v>
@@ -23631,7 +23634,7 @@
         <v>19280</v>
       </c>
       <c r="AR7" s="19">
-        <v>16367</v>
+        <v>17023</v>
       </c>
       <c r="AS7" s="19">
         <v>17204</v>
@@ -23792,7 +23795,7 @@
         <v>3996</v>
       </c>
       <c r="AR8" s="19">
-        <v>4665</v>
+        <v>4620</v>
       </c>
       <c r="AS8" s="19">
         <v>4424</v>
@@ -23953,7 +23956,7 @@
         <v>11430</v>
       </c>
       <c r="AR9" s="19">
-        <v>10827</v>
+        <v>10837</v>
       </c>
       <c r="AS9" s="19">
         <v>11238</v>
@@ -24114,7 +24117,7 @@
         <v>16679</v>
       </c>
       <c r="AR10" s="19">
-        <v>14672</v>
+        <v>14560</v>
       </c>
       <c r="AS10" s="19">
         <v>15259</v>
@@ -24275,7 +24278,7 @@
         <v>44938</v>
       </c>
       <c r="AR11" s="19">
-        <v>45151</v>
+        <v>44976</v>
       </c>
       <c r="AS11" s="19">
         <v>45261</v>
@@ -24436,7 +24439,7 @@
         <v>114535</v>
       </c>
       <c r="AR12" s="8">
-        <v>110264</v>
+        <v>110555</v>
       </c>
       <c r="AS12" s="8">
         <v>111829</v>
@@ -24657,7 +24660,7 @@
         <v>497.84841299999999</v>
       </c>
       <c r="AR15" s="19">
-        <v>491.28521599999999</v>
+        <v>487.778212</v>
       </c>
       <c r="AS15" s="19">
         <v>494.27261199999998</v>
@@ -24818,7 +24821,7 @@
         <v>787.65963099999999</v>
       </c>
       <c r="AR16" s="19">
-        <v>839.51689299999998</v>
+        <v>838.70392400000003</v>
       </c>
       <c r="AS16" s="19">
         <v>814.82662100000005</v>
@@ -24979,7 +24982,7 @@
         <v>622.595823</v>
       </c>
       <c r="AR17" s="19">
-        <v>644.76174900000001</v>
+        <v>645.22791800000005</v>
       </c>
       <c r="AS17" s="19">
         <v>576.01996599999995</v>
@@ -25140,7 +25143,7 @@
         <v>56.755087000000003</v>
       </c>
       <c r="AR18" s="19">
-        <v>62.720484999999996</v>
+        <v>62.309002</v>
       </c>
       <c r="AS18" s="19">
         <v>58.535254999999999</v>
@@ -25301,7 +25304,7 @@
         <v>446.20862899999997</v>
       </c>
       <c r="AR19" s="19">
-        <v>459.39371999999997</v>
+        <v>459.52981599999998</v>
       </c>
       <c r="AS19" s="19">
         <v>499.16213800000003</v>
@@ -25462,7 +25465,7 @@
         <v>1541.5027170000001</v>
       </c>
       <c r="AR20" s="19">
-        <v>1346.452513</v>
+        <v>1332.774334</v>
       </c>
       <c r="AS20" s="19">
         <v>1376.206046</v>
@@ -25623,7 +25626,7 @@
         <v>1076.4139869999999</v>
       </c>
       <c r="AR21" s="19">
-        <v>1069.457803</v>
+        <v>1065.465508</v>
       </c>
       <c r="AS21" s="19">
         <v>1042.6754249999999</v>
@@ -25784,7 +25787,7 @@
         <v>5028.9842870000002</v>
       </c>
       <c r="AR22" s="8">
-        <v>4913.5883789999998</v>
+        <v>4891.7887140000003</v>
       </c>
       <c r="AS22" s="8">
         <v>4861.6980629999998</v>
@@ -25872,7 +25875,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26399,7 +26402,7 @@
         <v>5523</v>
       </c>
       <c r="AR5" s="19">
-        <v>0</v>
+        <v>5652</v>
       </c>
       <c r="AS5" s="19">
         <v>0</v>
@@ -26561,7 +26564,7 @@
         <v>12298</v>
       </c>
       <c r="AR6" s="7">
-        <v>0</v>
+        <v>12390</v>
       </c>
       <c r="AS6" s="7">
         <v>0</v>
@@ -26723,7 +26726,7 @@
         <v>19523</v>
       </c>
       <c r="AR7" s="7">
-        <v>0</v>
+        <v>18243</v>
       </c>
       <c r="AS7" s="7">
         <v>0</v>
@@ -26885,7 +26888,7 @@
         <v>4911</v>
       </c>
       <c r="AR8" s="7">
-        <v>0</v>
+        <v>4989</v>
       </c>
       <c r="AS8" s="7">
         <v>0</v>
@@ -27047,7 +27050,7 @@
         <v>9486</v>
       </c>
       <c r="AR9" s="7">
-        <v>0</v>
+        <v>9440</v>
       </c>
       <c r="AS9" s="7">
         <v>0</v>
@@ -27209,7 +27212,7 @@
         <v>16412</v>
       </c>
       <c r="AR10" s="19">
-        <v>0</v>
+        <v>14915</v>
       </c>
       <c r="AS10" s="19">
         <v>0</v>
@@ -27371,7 +27374,7 @@
         <v>41162</v>
       </c>
       <c r="AR11" s="7">
-        <v>0</v>
+        <v>39252</v>
       </c>
       <c r="AS11" s="7">
         <v>0</v>
@@ -27533,7 +27536,7 @@
         <v>109315</v>
       </c>
       <c r="AR12" s="8">
-        <v>0</v>
+        <v>104881</v>
       </c>
       <c r="AS12" s="8">
         <v>0</v>
@@ -27757,7 +27760,7 @@
         <v>436.81901599999998</v>
       </c>
       <c r="AR15" s="19">
-        <v>0</v>
+        <v>413.95728000000003</v>
       </c>
       <c r="AS15" s="19">
         <v>0</v>
@@ -27919,7 +27922,7 @@
         <v>839.25483699999995</v>
       </c>
       <c r="AR16" s="7">
-        <v>0</v>
+        <v>883.51841200000001</v>
       </c>
       <c r="AS16" s="7">
         <v>0</v>
@@ -28081,7 +28084,7 @@
         <v>573.95665799999995</v>
       </c>
       <c r="AR17" s="7">
-        <v>0</v>
+        <v>574.248606</v>
       </c>
       <c r="AS17" s="7">
         <v>0</v>
@@ -28243,7 +28246,7 @@
         <v>77.333590999999998</v>
       </c>
       <c r="AR18" s="7">
-        <v>0</v>
+        <v>71.167961000000005</v>
       </c>
       <c r="AS18" s="7">
         <v>0</v>
@@ -28405,7 +28408,7 @@
         <v>420.31390699999997</v>
       </c>
       <c r="AR19" s="7">
-        <v>0</v>
+        <v>422.05681900000002</v>
       </c>
       <c r="AS19" s="7">
         <v>0</v>
@@ -28567,7 +28570,7 @@
         <v>1569.0897210000001</v>
       </c>
       <c r="AR20" s="19">
-        <v>0</v>
+        <v>1541.593351</v>
       </c>
       <c r="AS20" s="19">
         <v>0</v>
@@ -28729,7 +28732,7 @@
         <v>911.84274600000003</v>
       </c>
       <c r="AR21" s="7">
-        <v>0</v>
+        <v>924.635896</v>
       </c>
       <c r="AS21" s="7">
         <v>0</v>
@@ -28891,7 +28894,7 @@
         <v>4828.6104760000007</v>
       </c>
       <c r="AR22" s="8">
-        <v>0</v>
+        <v>4831.1783249999999</v>
       </c>
       <c r="AS22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Nov  7 05:23:54 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -22772,9 +22772,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -22782,12 +22779,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23315,7 +23312,7 @@
         <v>6499</v>
       </c>
       <c r="AS5" s="19">
-        <v>6509</v>
+        <v>6485</v>
       </c>
       <c r="AT5" s="19">
         <v>6206</v>
@@ -23476,7 +23473,7 @@
         <v>12040</v>
       </c>
       <c r="AS6" s="19">
-        <v>11934</v>
+        <v>11921</v>
       </c>
       <c r="AT6" s="19">
         <v>12157</v>
@@ -23637,7 +23634,7 @@
         <v>17023</v>
       </c>
       <c r="AS7" s="19">
-        <v>17204</v>
+        <v>17673</v>
       </c>
       <c r="AT7" s="19">
         <v>17687</v>
@@ -23798,7 +23795,7 @@
         <v>4620</v>
       </c>
       <c r="AS8" s="19">
-        <v>4424</v>
+        <v>4411</v>
       </c>
       <c r="AT8" s="19">
         <v>4062</v>
@@ -23959,7 +23956,7 @@
         <v>10837</v>
       </c>
       <c r="AS9" s="19">
-        <v>11238</v>
+        <v>11120</v>
       </c>
       <c r="AT9" s="19">
         <v>9380</v>
@@ -24120,7 +24117,7 @@
         <v>14560</v>
       </c>
       <c r="AS10" s="19">
-        <v>15259</v>
+        <v>15250</v>
       </c>
       <c r="AT10" s="19">
         <v>14612</v>
@@ -24281,7 +24278,7 @@
         <v>44976</v>
       </c>
       <c r="AS11" s="19">
-        <v>45261</v>
+        <v>45160</v>
       </c>
       <c r="AT11" s="19">
         <v>43856</v>
@@ -24442,7 +24439,7 @@
         <v>110555</v>
       </c>
       <c r="AS12" s="8">
-        <v>111829</v>
+        <v>112020</v>
       </c>
       <c r="AT12" s="8">
         <v>107960</v>
@@ -24663,7 +24660,7 @@
         <v>487.778212</v>
       </c>
       <c r="AS15" s="19">
-        <v>494.27261199999998</v>
+        <v>492.33599400000003</v>
       </c>
       <c r="AT15" s="19">
         <v>456.40343899999999</v>
@@ -24824,7 +24821,7 @@
         <v>838.70392400000003</v>
       </c>
       <c r="AS16" s="19">
-        <v>814.82662100000005</v>
+        <v>812.03479000000004</v>
       </c>
       <c r="AT16" s="19">
         <v>814.17363499999999</v>
@@ -24985,7 +24982,7 @@
         <v>645.22791800000005</v>
       </c>
       <c r="AS17" s="19">
-        <v>576.01996599999995</v>
+        <v>575.186691</v>
       </c>
       <c r="AT17" s="19">
         <v>481.01507700000002</v>
@@ -25146,7 +25143,7 @@
         <v>62.309002</v>
       </c>
       <c r="AS18" s="19">
-        <v>58.535254999999999</v>
+        <v>58.491612000000003</v>
       </c>
       <c r="AT18" s="19">
         <v>55.581164000000001</v>
@@ -25307,7 +25304,7 @@
         <v>459.52981599999998</v>
       </c>
       <c r="AS19" s="19">
-        <v>499.16213800000003</v>
+        <v>499.13068299999998</v>
       </c>
       <c r="AT19" s="19">
         <v>390.82899500000002</v>
@@ -25468,7 +25465,7 @@
         <v>1332.774334</v>
       </c>
       <c r="AS20" s="19">
-        <v>1376.206046</v>
+        <v>1373.250939</v>
       </c>
       <c r="AT20" s="19">
         <v>1336.597137</v>
@@ -25629,7 +25626,7 @@
         <v>1065.465508</v>
       </c>
       <c r="AS21" s="19">
-        <v>1042.6754249999999</v>
+        <v>1040.396493</v>
       </c>
       <c r="AT21" s="19">
         <v>1013.083017</v>
@@ -25790,7 +25787,7 @@
         <v>4891.7887140000003</v>
       </c>
       <c r="AS22" s="8">
-        <v>4861.6980629999998</v>
+        <v>4850.8272020000004</v>
       </c>
       <c r="AT22" s="8">
         <v>4547.6824639999995</v>
@@ -25874,8 +25871,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26405,7 +26402,7 @@
         <v>5652</v>
       </c>
       <c r="AS5" s="19">
-        <v>0</v>
+        <v>6028</v>
       </c>
       <c r="AT5" s="19">
         <v>0</v>
@@ -26567,7 +26564,7 @@
         <v>12390</v>
       </c>
       <c r="AS6" s="7">
-        <v>0</v>
+        <v>12529</v>
       </c>
       <c r="AT6" s="7">
         <v>0</v>
@@ -26729,7 +26726,7 @@
         <v>18243</v>
       </c>
       <c r="AS7" s="7">
-        <v>0</v>
+        <v>19503</v>
       </c>
       <c r="AT7" s="7">
         <v>0</v>
@@ -26891,7 +26888,7 @@
         <v>4989</v>
       </c>
       <c r="AS8" s="7">
-        <v>0</v>
+        <v>4590</v>
       </c>
       <c r="AT8" s="7">
         <v>0</v>
@@ -27053,7 +27050,7 @@
         <v>9440</v>
       </c>
       <c r="AS9" s="7">
-        <v>0</v>
+        <v>10443</v>
       </c>
       <c r="AT9" s="7">
         <v>0</v>
@@ -27215,7 +27212,7 @@
         <v>14915</v>
       </c>
       <c r="AS10" s="19">
-        <v>0</v>
+        <v>15310</v>
       </c>
       <c r="AT10" s="19">
         <v>0</v>
@@ -27377,7 +27374,7 @@
         <v>39252</v>
       </c>
       <c r="AS11" s="7">
-        <v>0</v>
+        <v>36679</v>
       </c>
       <c r="AT11" s="7">
         <v>0</v>
@@ -27539,7 +27536,7 @@
         <v>104881</v>
       </c>
       <c r="AS12" s="8">
-        <v>0</v>
+        <v>105082</v>
       </c>
       <c r="AT12" s="8">
         <v>0</v>
@@ -27763,7 +27760,7 @@
         <v>413.95728000000003</v>
       </c>
       <c r="AS15" s="19">
-        <v>0</v>
+        <v>447.052076</v>
       </c>
       <c r="AT15" s="19">
         <v>0</v>
@@ -27925,7 +27922,7 @@
         <v>883.51841200000001</v>
       </c>
       <c r="AS16" s="7">
-        <v>0</v>
+        <v>894.59904400000005</v>
       </c>
       <c r="AT16" s="7">
         <v>0</v>
@@ -28087,7 +28084,7 @@
         <v>574.248606</v>
       </c>
       <c r="AS17" s="7">
-        <v>0</v>
+        <v>535.51196000000004</v>
       </c>
       <c r="AT17" s="7">
         <v>0</v>
@@ -28249,7 +28246,7 @@
         <v>71.167961000000005</v>
       </c>
       <c r="AS18" s="7">
-        <v>0</v>
+        <v>65.691602000000003</v>
       </c>
       <c r="AT18" s="7">
         <v>0</v>
@@ -28411,7 +28408,7 @@
         <v>422.05681900000002</v>
       </c>
       <c r="AS19" s="7">
-        <v>0</v>
+        <v>466.18692499999997</v>
       </c>
       <c r="AT19" s="7">
         <v>0</v>
@@ -28573,7 +28570,7 @@
         <v>1541.593351</v>
       </c>
       <c r="AS20" s="19">
-        <v>0</v>
+        <v>1507.2264929999999</v>
       </c>
       <c r="AT20" s="19">
         <v>0</v>
@@ -28735,7 +28732,7 @@
         <v>924.635896</v>
       </c>
       <c r="AS21" s="7">
-        <v>0</v>
+        <v>760.97466899999995</v>
       </c>
       <c r="AT21" s="7">
         <v>0</v>
@@ -28897,7 +28894,7 @@
         <v>4831.1783249999999</v>
       </c>
       <c r="AS22" s="8">
-        <v>0</v>
+        <v>4677.2427690000004</v>
       </c>
       <c r="AT22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Wed Nov 15 05:25:32 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -22784,7 +22784,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D35:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23315,7 +23315,7 @@
         <v>6485</v>
       </c>
       <c r="AT5" s="19">
-        <v>6206</v>
+        <v>6179</v>
       </c>
       <c r="AU5" s="19">
         <v>6506</v>
@@ -23476,7 +23476,7 @@
         <v>11921</v>
       </c>
       <c r="AT6" s="19">
-        <v>12157</v>
+        <v>12139</v>
       </c>
       <c r="AU6" s="19">
         <v>12175</v>
@@ -23637,7 +23637,7 @@
         <v>17673</v>
       </c>
       <c r="AT7" s="19">
-        <v>17687</v>
+        <v>18552</v>
       </c>
       <c r="AU7" s="19">
         <v>17974</v>
@@ -23798,7 +23798,7 @@
         <v>4411</v>
       </c>
       <c r="AT8" s="19">
-        <v>4062</v>
+        <v>4057</v>
       </c>
       <c r="AU8" s="19">
         <v>4270</v>
@@ -23959,7 +23959,7 @@
         <v>11120</v>
       </c>
       <c r="AT9" s="19">
-        <v>9380</v>
+        <v>9385</v>
       </c>
       <c r="AU9" s="19">
         <v>10117</v>
@@ -24120,7 +24120,7 @@
         <v>15250</v>
       </c>
       <c r="AT10" s="19">
-        <v>14612</v>
+        <v>14635</v>
       </c>
       <c r="AU10" s="19">
         <v>15783</v>
@@ -24281,7 +24281,7 @@
         <v>45160</v>
       </c>
       <c r="AT11" s="19">
-        <v>43856</v>
+        <v>43749</v>
       </c>
       <c r="AU11" s="19">
         <v>43658</v>
@@ -24442,7 +24442,7 @@
         <v>112020</v>
       </c>
       <c r="AT12" s="8">
-        <v>107960</v>
+        <v>108696</v>
       </c>
       <c r="AU12" s="8">
         <v>110483</v>
@@ -24663,7 +24663,7 @@
         <v>492.33599400000003</v>
       </c>
       <c r="AT15" s="19">
-        <v>456.40343899999999</v>
+        <v>454.376959</v>
       </c>
       <c r="AU15" s="19">
         <v>490.69789300000002</v>
@@ -24824,7 +24824,7 @@
         <v>812.03479000000004</v>
       </c>
       <c r="AT16" s="19">
-        <v>814.17363499999999</v>
+        <v>814.01198899999997</v>
       </c>
       <c r="AU16" s="19">
         <v>820.01279</v>
@@ -24985,7 +24985,7 @@
         <v>575.186691</v>
       </c>
       <c r="AT17" s="19">
-        <v>481.01507700000002</v>
+        <v>479.98988800000001</v>
       </c>
       <c r="AU17" s="19">
         <v>573.06620599999997</v>
@@ -25146,7 +25146,7 @@
         <v>58.491612000000003</v>
       </c>
       <c r="AT18" s="19">
-        <v>55.581164000000001</v>
+        <v>55.54045</v>
       </c>
       <c r="AU18" s="19">
         <v>55.430866999999999</v>
@@ -25307,7 +25307,7 @@
         <v>499.13068299999998</v>
       </c>
       <c r="AT19" s="19">
-        <v>390.82899500000002</v>
+        <v>390.83495499999998</v>
       </c>
       <c r="AU19" s="19">
         <v>439.13479999999998</v>
@@ -25468,7 +25468,7 @@
         <v>1373.250939</v>
       </c>
       <c r="AT20" s="19">
-        <v>1336.597137</v>
+        <v>1336.3384599999999</v>
       </c>
       <c r="AU20" s="19">
         <v>1444.362903</v>
@@ -25629,7 +25629,7 @@
         <v>1040.396493</v>
       </c>
       <c r="AT21" s="19">
-        <v>1013.083017</v>
+        <v>1010.253921</v>
       </c>
       <c r="AU21" s="19">
         <v>1053.7069859999999</v>
@@ -25790,7 +25790,7 @@
         <v>4850.8272020000004</v>
       </c>
       <c r="AT22" s="8">
-        <v>4547.6824639999995</v>
+        <v>4541.346622</v>
       </c>
       <c r="AU22" s="8">
         <v>4876.4124449999999</v>
@@ -25872,7 +25872,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26405,7 +26405,7 @@
         <v>6028</v>
       </c>
       <c r="AT5" s="19">
-        <v>0</v>
+        <v>5798</v>
       </c>
       <c r="AU5" s="19">
         <v>0</v>
@@ -26567,7 +26567,7 @@
         <v>12529</v>
       </c>
       <c r="AT6" s="7">
-        <v>0</v>
+        <v>13020</v>
       </c>
       <c r="AU6" s="7">
         <v>0</v>
@@ -26729,7 +26729,7 @@
         <v>19503</v>
       </c>
       <c r="AT7" s="7">
-        <v>0</v>
+        <v>19483</v>
       </c>
       <c r="AU7" s="7">
         <v>0</v>
@@ -26891,7 +26891,7 @@
         <v>4590</v>
       </c>
       <c r="AT8" s="7">
-        <v>0</v>
+        <v>4727</v>
       </c>
       <c r="AU8" s="7">
         <v>0</v>
@@ -27053,7 +27053,7 @@
         <v>10443</v>
       </c>
       <c r="AT9" s="7">
-        <v>0</v>
+        <v>11367</v>
       </c>
       <c r="AU9" s="7">
         <v>0</v>
@@ -27215,7 +27215,7 @@
         <v>15310</v>
       </c>
       <c r="AT10" s="19">
-        <v>0</v>
+        <v>14332</v>
       </c>
       <c r="AU10" s="19">
         <v>0</v>
@@ -27377,7 +27377,7 @@
         <v>36679</v>
       </c>
       <c r="AT11" s="7">
-        <v>0</v>
+        <v>40038</v>
       </c>
       <c r="AU11" s="7">
         <v>0</v>
@@ -27539,7 +27539,7 @@
         <v>105082</v>
       </c>
       <c r="AT12" s="8">
-        <v>0</v>
+        <v>108765</v>
       </c>
       <c r="AU12" s="8">
         <v>0</v>
@@ -27763,7 +27763,7 @@
         <v>447.052076</v>
       </c>
       <c r="AT15" s="19">
-        <v>0</v>
+        <v>431.289469</v>
       </c>
       <c r="AU15" s="19">
         <v>0</v>
@@ -27925,7 +27925,7 @@
         <v>894.59904400000005</v>
       </c>
       <c r="AT16" s="7">
-        <v>0</v>
+        <v>946.93562999999995</v>
       </c>
       <c r="AU16" s="7">
         <v>0</v>
@@ -28087,7 +28087,7 @@
         <v>535.51196000000004</v>
       </c>
       <c r="AT17" s="7">
-        <v>0</v>
+        <v>474.83860800000002</v>
       </c>
       <c r="AU17" s="7">
         <v>0</v>
@@ -28249,7 +28249,7 @@
         <v>65.691602000000003</v>
       </c>
       <c r="AT18" s="7">
-        <v>0</v>
+        <v>63.640169999999998</v>
       </c>
       <c r="AU18" s="7">
         <v>0</v>
@@ -28411,7 +28411,7 @@
         <v>466.18692499999997</v>
       </c>
       <c r="AT19" s="7">
-        <v>0</v>
+        <v>467.72137600000002</v>
       </c>
       <c r="AU19" s="7">
         <v>0</v>
@@ -28573,7 +28573,7 @@
         <v>1507.2264929999999</v>
       </c>
       <c r="AT20" s="19">
-        <v>0</v>
+        <v>1423.9756070000001</v>
       </c>
       <c r="AU20" s="19">
         <v>0</v>
@@ -28735,7 +28735,7 @@
         <v>760.97466899999995</v>
       </c>
       <c r="AT21" s="7">
-        <v>0</v>
+        <v>965.85286299999996</v>
       </c>
       <c r="AU21" s="7">
         <v>0</v>
@@ -28897,7 +28897,7 @@
         <v>4677.2427690000004</v>
       </c>
       <c r="AT22" s="8">
-        <v>0</v>
+        <v>4774.2537229999998</v>
       </c>
       <c r="AU22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Nov 21 05:23:03 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -22772,6 +22772,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -22779,12 +22782,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="D36" sqref="D35:D36"/>
+      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23318,7 +23321,7 @@
         <v>6179</v>
       </c>
       <c r="AU5" s="19">
-        <v>6506</v>
+        <v>6439</v>
       </c>
       <c r="AV5" s="19">
         <v>6434</v>
@@ -23479,7 +23482,7 @@
         <v>12139</v>
       </c>
       <c r="AU6" s="19">
-        <v>12175</v>
+        <v>12167</v>
       </c>
       <c r="AV6" s="19">
         <v>11899</v>
@@ -23640,7 +23643,7 @@
         <v>18552</v>
       </c>
       <c r="AU7" s="19">
-        <v>17974</v>
+        <v>18910</v>
       </c>
       <c r="AV7" s="19">
         <v>18772</v>
@@ -23801,7 +23804,7 @@
         <v>4057</v>
       </c>
       <c r="AU8" s="19">
-        <v>4270</v>
+        <v>4266</v>
       </c>
       <c r="AV8" s="19">
         <v>3731</v>
@@ -23962,7 +23965,7 @@
         <v>9385</v>
       </c>
       <c r="AU9" s="19">
-        <v>10117</v>
+        <v>9996</v>
       </c>
       <c r="AV9" s="19">
         <v>11160</v>
@@ -24123,7 +24126,7 @@
         <v>14635</v>
       </c>
       <c r="AU10" s="19">
-        <v>15783</v>
+        <v>15665</v>
       </c>
       <c r="AV10" s="19">
         <v>15483</v>
@@ -24284,7 +24287,7 @@
         <v>43749</v>
       </c>
       <c r="AU11" s="19">
-        <v>43658</v>
+        <v>43557</v>
       </c>
       <c r="AV11" s="19">
         <v>41186</v>
@@ -24445,7 +24448,7 @@
         <v>108696</v>
       </c>
       <c r="AU12" s="8">
-        <v>110483</v>
+        <v>111000</v>
       </c>
       <c r="AV12" s="8">
         <v>108665</v>
@@ -24666,7 +24669,7 @@
         <v>454.376959</v>
       </c>
       <c r="AU15" s="19">
-        <v>490.69789300000002</v>
+        <v>486.31085999999999</v>
       </c>
       <c r="AV15" s="19">
         <v>477.18595199999999</v>
@@ -24827,7 +24830,7 @@
         <v>814.01198899999997</v>
       </c>
       <c r="AU16" s="19">
-        <v>820.01279</v>
+        <v>819.47908399999994</v>
       </c>
       <c r="AV16" s="19">
         <v>845.50511800000004</v>
@@ -24988,7 +24991,7 @@
         <v>479.98988800000001</v>
       </c>
       <c r="AU17" s="19">
-        <v>573.06620599999997</v>
+        <v>572.199701</v>
       </c>
       <c r="AV17" s="19">
         <v>480.42448899999999</v>
@@ -25149,7 +25152,7 @@
         <v>55.54045</v>
       </c>
       <c r="AU18" s="19">
-        <v>55.430866999999999</v>
+        <v>55.433745999999999</v>
       </c>
       <c r="AV18" s="19">
         <v>51.513334999999998</v>
@@ -25310,7 +25313,7 @@
         <v>390.83495499999998</v>
       </c>
       <c r="AU19" s="19">
-        <v>439.13479999999998</v>
+        <v>439.03695499999998</v>
       </c>
       <c r="AV19" s="19">
         <v>523.47889399999997</v>
@@ -25471,7 +25474,7 @@
         <v>1336.3384599999999</v>
       </c>
       <c r="AU20" s="19">
-        <v>1444.362903</v>
+        <v>1442.281412</v>
       </c>
       <c r="AV20" s="19">
         <v>1402.549937</v>
@@ -25632,7 +25635,7 @@
         <v>1010.253921</v>
       </c>
       <c r="AU21" s="19">
-        <v>1053.7069859999999</v>
+        <v>1051.357706</v>
       </c>
       <c r="AV21" s="19">
         <v>979.87685199999999</v>
@@ -25793,7 +25796,7 @@
         <v>4541.346622</v>
       </c>
       <c r="AU22" s="8">
-        <v>4876.4124449999999</v>
+        <v>4866.0994639999999</v>
       </c>
       <c r="AV22" s="8">
         <v>4760.5345770000004</v>
@@ -25871,8 +25874,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F37" sqref="F36:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26408,7 +26411,7 @@
         <v>5798</v>
       </c>
       <c r="AU5" s="19">
-        <v>0</v>
+        <v>6285</v>
       </c>
       <c r="AV5" s="19">
         <v>0</v>
@@ -26570,7 +26573,7 @@
         <v>13020</v>
       </c>
       <c r="AU6" s="7">
-        <v>0</v>
+        <v>13283</v>
       </c>
       <c r="AV6" s="7">
         <v>0</v>
@@ -26732,7 +26735,7 @@
         <v>19483</v>
       </c>
       <c r="AU7" s="7">
-        <v>0</v>
+        <v>19617</v>
       </c>
       <c r="AV7" s="7">
         <v>0</v>
@@ -26894,7 +26897,7 @@
         <v>4727</v>
       </c>
       <c r="AU8" s="7">
-        <v>0</v>
+        <v>4921</v>
       </c>
       <c r="AV8" s="7">
         <v>0</v>
@@ -27056,7 +27059,7 @@
         <v>11367</v>
       </c>
       <c r="AU9" s="7">
-        <v>0</v>
+        <v>10430</v>
       </c>
       <c r="AV9" s="7">
         <v>0</v>
@@ -27218,7 +27221,7 @@
         <v>14332</v>
       </c>
       <c r="AU10" s="19">
-        <v>0</v>
+        <v>14951</v>
       </c>
       <c r="AV10" s="19">
         <v>0</v>
@@ -27380,7 +27383,7 @@
         <v>40038</v>
       </c>
       <c r="AU11" s="7">
-        <v>0</v>
+        <v>38254</v>
       </c>
       <c r="AV11" s="7">
         <v>0</v>
@@ -27542,7 +27545,7 @@
         <v>108765</v>
       </c>
       <c r="AU12" s="8">
-        <v>0</v>
+        <v>107741</v>
       </c>
       <c r="AV12" s="8">
         <v>0</v>
@@ -27766,7 +27769,7 @@
         <v>431.289469</v>
       </c>
       <c r="AU15" s="19">
-        <v>0</v>
+        <v>469.00431500000002</v>
       </c>
       <c r="AV15" s="19">
         <v>0</v>
@@ -27928,7 +27931,7 @@
         <v>946.93562999999995</v>
       </c>
       <c r="AU16" s="7">
-        <v>0</v>
+        <v>925.71202000000005</v>
       </c>
       <c r="AV16" s="7">
         <v>0</v>
@@ -28090,7 +28093,7 @@
         <v>474.83860800000002</v>
       </c>
       <c r="AU17" s="7">
-        <v>0</v>
+        <v>555.82336499999997</v>
       </c>
       <c r="AV17" s="7">
         <v>0</v>
@@ -28252,7 +28255,7 @@
         <v>63.640169999999998</v>
       </c>
       <c r="AU18" s="7">
-        <v>0</v>
+        <v>71.092873999999995</v>
       </c>
       <c r="AV18" s="7">
         <v>0</v>
@@ -28414,7 +28417,7 @@
         <v>467.72137600000002</v>
       </c>
       <c r="AU19" s="7">
-        <v>0</v>
+        <v>449.01658300000003</v>
       </c>
       <c r="AV19" s="7">
         <v>0</v>
@@ -28576,7 +28579,7 @@
         <v>1423.9756070000001</v>
       </c>
       <c r="AU20" s="19">
-        <v>0</v>
+        <v>1526.804995</v>
       </c>
       <c r="AV20" s="19">
         <v>0</v>
@@ -28738,7 +28741,7 @@
         <v>965.85286299999996</v>
       </c>
       <c r="AU21" s="7">
-        <v>0</v>
+        <v>890.68457100000001</v>
       </c>
       <c r="AV21" s="7">
         <v>0</v>
@@ -28900,7 +28903,7 @@
         <v>4774.2537229999998</v>
       </c>
       <c r="AU22" s="8">
-        <v>0</v>
+        <v>4888.138723</v>
       </c>
       <c r="AV22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Nov 28 05:22:29 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4048CA2E-2DD9-4086-95D0-6BA6B3649FE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -209,7 +210,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'2022'!$A:$A,'2022'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">'2023'!$A:$A,'2023'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -217,9 +218,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -460,7 +458,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -649,11 +647,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="5"/>
-    <cellStyle name="Percent 2" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1015,7 +1013,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4069,7 +4067,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7155,7 +7153,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:BA54"/>
   <sheetViews>
@@ -10243,7 +10241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13318,7 +13316,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16393,7 +16391,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19688,7 +19686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -22772,14 +22770,11 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -22787,7 +22782,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23324,7 +23319,7 @@
         <v>6439</v>
       </c>
       <c r="AV5" s="19">
-        <v>6434</v>
+        <v>6408</v>
       </c>
       <c r="AW5" s="19">
         <v>6466</v>
@@ -23485,7 +23480,7 @@
         <v>12167</v>
       </c>
       <c r="AV6" s="19">
-        <v>11899</v>
+        <v>11805</v>
       </c>
       <c r="AW6" s="19">
         <v>12424</v>
@@ -23646,7 +23641,7 @@
         <v>18910</v>
       </c>
       <c r="AV7" s="19">
-        <v>18772</v>
+        <v>19769</v>
       </c>
       <c r="AW7" s="19">
         <v>18593</v>
@@ -23807,7 +23802,7 @@
         <v>4266</v>
       </c>
       <c r="AV8" s="19">
-        <v>3731</v>
+        <v>3727</v>
       </c>
       <c r="AW8" s="19">
         <v>4671</v>
@@ -23968,7 +23963,7 @@
         <v>9996</v>
       </c>
       <c r="AV9" s="19">
-        <v>11160</v>
+        <v>11055</v>
       </c>
       <c r="AW9" s="19">
         <v>9114</v>
@@ -24129,7 +24124,7 @@
         <v>15665</v>
       </c>
       <c r="AV10" s="19">
-        <v>15483</v>
+        <v>15480</v>
       </c>
       <c r="AW10" s="19">
         <v>15509</v>
@@ -24290,7 +24285,7 @@
         <v>43557</v>
       </c>
       <c r="AV11" s="19">
-        <v>41186</v>
+        <v>41079</v>
       </c>
       <c r="AW11" s="19">
         <v>42884</v>
@@ -24451,7 +24446,7 @@
         <v>111000</v>
       </c>
       <c r="AV12" s="8">
-        <v>108665</v>
+        <v>109323</v>
       </c>
       <c r="AW12" s="8">
         <v>109661</v>
@@ -24672,7 +24667,7 @@
         <v>486.31085999999999</v>
       </c>
       <c r="AV15" s="19">
-        <v>477.18595199999999</v>
+        <v>474.17004400000002</v>
       </c>
       <c r="AW15" s="19">
         <v>467.69939299999999</v>
@@ -24833,7 +24828,7 @@
         <v>819.47908399999994</v>
       </c>
       <c r="AV16" s="19">
-        <v>845.50511800000004</v>
+        <v>839.85170400000004</v>
       </c>
       <c r="AW16" s="19">
         <v>874.28392699999995</v>
@@ -24994,7 +24989,7 @@
         <v>572.199701</v>
       </c>
       <c r="AV17" s="19">
-        <v>480.42448899999999</v>
+        <v>478.86316399999998</v>
       </c>
       <c r="AW17" s="19">
         <v>481.86904700000002</v>
@@ -25155,7 +25150,7 @@
         <v>55.433745999999999</v>
       </c>
       <c r="AV18" s="19">
-        <v>51.513334999999998</v>
+        <v>51.464913000000003</v>
       </c>
       <c r="AW18" s="19">
         <v>56.399445999999998</v>
@@ -25316,7 +25311,7 @@
         <v>439.03695499999998</v>
       </c>
       <c r="AV19" s="19">
-        <v>523.47889399999997</v>
+        <v>524.22870599999999</v>
       </c>
       <c r="AW19" s="19">
         <v>403.21295700000002</v>
@@ -25477,7 +25472,7 @@
         <v>1442.281412</v>
       </c>
       <c r="AV20" s="19">
-        <v>1402.549937</v>
+        <v>1402.4785910000001</v>
       </c>
       <c r="AW20" s="19">
         <v>1450.6636590000001</v>
@@ -25638,7 +25633,7 @@
         <v>1051.357706</v>
       </c>
       <c r="AV21" s="19">
-        <v>979.87685199999999</v>
+        <v>978.20554700000002</v>
       </c>
       <c r="AW21" s="19">
         <v>1044.8588999999999</v>
@@ -25799,7 +25794,7 @@
         <v>4866.0994639999999</v>
       </c>
       <c r="AV22" s="8">
-        <v>4760.5345770000004</v>
+        <v>4749.2626689999997</v>
       </c>
       <c r="AW22" s="8">
         <v>4778.9873290000005</v>
@@ -25863,19 +25858,16 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F37" sqref="F36:F37"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26414,7 +26406,7 @@
         <v>6285</v>
       </c>
       <c r="AV5" s="19">
-        <v>0</v>
+        <v>6041</v>
       </c>
       <c r="AW5" s="19">
         <v>0</v>
@@ -26576,7 +26568,7 @@
         <v>13283</v>
       </c>
       <c r="AV6" s="7">
-        <v>0</v>
+        <v>12323</v>
       </c>
       <c r="AW6" s="7">
         <v>0</v>
@@ -26738,7 +26730,7 @@
         <v>19617</v>
       </c>
       <c r="AV7" s="7">
-        <v>0</v>
+        <v>18576</v>
       </c>
       <c r="AW7" s="7">
         <v>0</v>
@@ -26900,7 +26892,7 @@
         <v>4921</v>
       </c>
       <c r="AV8" s="7">
-        <v>0</v>
+        <v>4378</v>
       </c>
       <c r="AW8" s="7">
         <v>0</v>
@@ -27062,7 +27054,7 @@
         <v>10430</v>
       </c>
       <c r="AV9" s="7">
-        <v>0</v>
+        <v>8463</v>
       </c>
       <c r="AW9" s="7">
         <v>0</v>
@@ -27224,7 +27216,7 @@
         <v>14951</v>
       </c>
       <c r="AV10" s="19">
-        <v>0</v>
+        <v>14127</v>
       </c>
       <c r="AW10" s="19">
         <v>0</v>
@@ -27386,7 +27378,7 @@
         <v>38254</v>
       </c>
       <c r="AV11" s="7">
-        <v>0</v>
+        <v>40158</v>
       </c>
       <c r="AW11" s="7">
         <v>0</v>
@@ -27548,7 +27540,7 @@
         <v>107741</v>
       </c>
       <c r="AV12" s="8">
-        <v>0</v>
+        <v>104066</v>
       </c>
       <c r="AW12" s="8">
         <v>0</v>
@@ -27772,7 +27764,7 @@
         <v>469.00431500000002</v>
       </c>
       <c r="AV15" s="19">
-        <v>0</v>
+        <v>464.85895299999999</v>
       </c>
       <c r="AW15" s="19">
         <v>0</v>
@@ -27934,7 +27926,7 @@
         <v>925.71202000000005</v>
       </c>
       <c r="AV16" s="7">
-        <v>0</v>
+        <v>887.33977800000002</v>
       </c>
       <c r="AW16" s="7">
         <v>0</v>
@@ -28096,7 +28088,7 @@
         <v>555.82336499999997</v>
       </c>
       <c r="AV17" s="7">
-        <v>0</v>
+        <v>487.59617100000003</v>
       </c>
       <c r="AW17" s="7">
         <v>0</v>
@@ -28258,7 +28250,7 @@
         <v>71.092873999999995</v>
       </c>
       <c r="AV18" s="7">
-        <v>0</v>
+        <v>65.225431999999998</v>
       </c>
       <c r="AW18" s="7">
         <v>0</v>
@@ -28420,7 +28412,7 @@
         <v>449.01658300000003</v>
       </c>
       <c r="AV19" s="7">
-        <v>0</v>
+        <v>386.00406099999998</v>
       </c>
       <c r="AW19" s="7">
         <v>0</v>
@@ -28582,7 +28574,7 @@
         <v>1526.804995</v>
       </c>
       <c r="AV20" s="19">
-        <v>0</v>
+        <v>1414.814081</v>
       </c>
       <c r="AW20" s="19">
         <v>0</v>
@@ -28744,7 +28736,7 @@
         <v>890.68457100000001</v>
       </c>
       <c r="AV21" s="7">
-        <v>0</v>
+        <v>908.04903400000001</v>
       </c>
       <c r="AW21" s="7">
         <v>0</v>
@@ -28906,7 +28898,7 @@
         <v>4888.138723</v>
       </c>
       <c r="AV22" s="8">
-        <v>0</v>
+        <v>4613.8875099999996</v>
       </c>
       <c r="AW22" s="8">
         <v>0</v>
@@ -29033,8 +29025,5 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GH ACTION Autorun Tue Dec  5 05:22:45 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4048CA2E-2DD9-4086-95D0-6BA6B3649FE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A118F2-CE01-422B-B4B0-C08EF9347CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,7 +580,7 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -595,7 +595,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -608,7 +608,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment textRotation="75"/>
     </xf>
     <xf numFmtId="16" fontId="7" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -617,7 +617,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -638,10 +638,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1033,61 +1030,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
     </row>
     <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
@@ -4088,61 +4085,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
     </row>
     <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -7175,61 +7172,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
     </row>
     <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -10258,61 +10255,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
     </row>
     <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -13333,61 +13330,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
     </row>
     <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -16409,61 +16406,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
@@ -19707,61 +19704,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
     </row>
     <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
@@ -19926,160 +19923,160 @@
       <c r="A3" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="6">
         <v>44199</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="6">
         <v>44206</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="6">
         <v>44213</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="6">
         <v>44220</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="6">
         <v>44227</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="6">
         <v>44234</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="6">
         <v>44241</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="6">
         <v>44248</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="6">
         <v>44255</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="6">
         <v>44262</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="6">
         <v>44269</v>
       </c>
-      <c r="M3" s="26">
+      <c r="M3" s="6">
         <v>44276</v>
       </c>
-      <c r="N3" s="26">
+      <c r="N3" s="6">
         <v>44283</v>
       </c>
-      <c r="O3" s="26">
+      <c r="O3" s="6">
         <v>44290</v>
       </c>
-      <c r="P3" s="26">
+      <c r="P3" s="6">
         <v>44297</v>
       </c>
-      <c r="Q3" s="26">
+      <c r="Q3" s="6">
         <v>44304</v>
       </c>
-      <c r="R3" s="26">
+      <c r="R3" s="6">
         <v>44311</v>
       </c>
-      <c r="S3" s="26">
+      <c r="S3" s="6">
         <v>44318</v>
       </c>
-      <c r="T3" s="26">
+      <c r="T3" s="6">
         <v>44325</v>
       </c>
-      <c r="U3" s="26">
+      <c r="U3" s="6">
         <v>44332</v>
       </c>
-      <c r="V3" s="26">
+      <c r="V3" s="6">
         <v>44339</v>
       </c>
-      <c r="W3" s="26">
+      <c r="W3" s="6">
         <v>44346</v>
       </c>
-      <c r="X3" s="26">
+      <c r="X3" s="6">
         <v>44353</v>
       </c>
-      <c r="Y3" s="26">
+      <c r="Y3" s="6">
         <v>44360</v>
       </c>
-      <c r="Z3" s="26">
+      <c r="Z3" s="6">
         <v>44367</v>
       </c>
-      <c r="AA3" s="26">
+      <c r="AA3" s="6">
         <v>44374</v>
       </c>
-      <c r="AB3" s="26">
+      <c r="AB3" s="6">
         <v>44381</v>
       </c>
-      <c r="AC3" s="26">
+      <c r="AC3" s="6">
         <v>44388</v>
       </c>
-      <c r="AD3" s="26">
+      <c r="AD3" s="6">
         <v>44395</v>
       </c>
-      <c r="AE3" s="26">
+      <c r="AE3" s="6">
         <v>44402</v>
       </c>
-      <c r="AF3" s="26">
+      <c r="AF3" s="6">
         <v>44409</v>
       </c>
-      <c r="AG3" s="26">
+      <c r="AG3" s="6">
         <v>44416</v>
       </c>
-      <c r="AH3" s="26">
+      <c r="AH3" s="6">
         <v>44423</v>
       </c>
-      <c r="AI3" s="26">
+      <c r="AI3" s="6">
         <v>44430</v>
       </c>
-      <c r="AJ3" s="26">
+      <c r="AJ3" s="6">
         <v>44437</v>
       </c>
-      <c r="AK3" s="26">
+      <c r="AK3" s="6">
         <v>44444</v>
       </c>
-      <c r="AL3" s="26">
+      <c r="AL3" s="6">
         <v>44451</v>
       </c>
-      <c r="AM3" s="26">
+      <c r="AM3" s="6">
         <v>44458</v>
       </c>
-      <c r="AN3" s="26">
+      <c r="AN3" s="6">
         <v>44465</v>
       </c>
-      <c r="AO3" s="26">
+      <c r="AO3" s="6">
         <v>44472</v>
       </c>
-      <c r="AP3" s="26">
+      <c r="AP3" s="6">
         <v>44479</v>
       </c>
-      <c r="AQ3" s="26">
+      <c r="AQ3" s="6">
         <v>44486</v>
       </c>
-      <c r="AR3" s="26">
+      <c r="AR3" s="6">
         <v>44493</v>
       </c>
-      <c r="AS3" s="26">
+      <c r="AS3" s="6">
         <v>44500</v>
       </c>
-      <c r="AT3" s="26">
+      <c r="AT3" s="6">
         <v>44507</v>
       </c>
-      <c r="AU3" s="26">
+      <c r="AU3" s="6">
         <v>44514</v>
       </c>
-      <c r="AV3" s="26">
+      <c r="AV3" s="6">
         <v>44521</v>
       </c>
-      <c r="AW3" s="26">
+      <c r="AW3" s="6">
         <v>44528</v>
       </c>
-      <c r="AX3" s="26">
+      <c r="AX3" s="6">
         <v>44535</v>
       </c>
-      <c r="AY3" s="26">
+      <c r="AY3" s="6">
         <v>44542</v>
       </c>
-      <c r="AZ3" s="26">
+      <c r="AZ3" s="6">
         <v>44549</v>
       </c>
-      <c r="BA3" s="26">
+      <c r="BA3" s="6">
         <v>44556</v>
       </c>
     </row>
@@ -22782,7 +22779,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22795,61 +22792,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
     </row>
     <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
@@ -23322,7 +23319,7 @@
         <v>6408</v>
       </c>
       <c r="AW5" s="19">
-        <v>6466</v>
+        <v>6422</v>
       </c>
       <c r="AX5" s="19">
         <v>6293</v>
@@ -23483,7 +23480,7 @@
         <v>11805</v>
       </c>
       <c r="AW6" s="19">
-        <v>12424</v>
+        <v>12486</v>
       </c>
       <c r="AX6" s="19">
         <v>11657</v>
@@ -23644,7 +23641,7 @@
         <v>19769</v>
       </c>
       <c r="AW7" s="19">
-        <v>18593</v>
+        <v>19601</v>
       </c>
       <c r="AX7" s="19">
         <v>18090</v>
@@ -23805,7 +23802,7 @@
         <v>3727</v>
       </c>
       <c r="AW8" s="19">
-        <v>4671</v>
+        <v>4569</v>
       </c>
       <c r="AX8" s="19">
         <v>4435</v>
@@ -23966,7 +23963,7 @@
         <v>11055</v>
       </c>
       <c r="AW9" s="19">
-        <v>9114</v>
+        <v>9130</v>
       </c>
       <c r="AX9" s="19">
         <v>11081</v>
@@ -24127,7 +24124,7 @@
         <v>15480</v>
       </c>
       <c r="AW10" s="19">
-        <v>15509</v>
+        <v>15383</v>
       </c>
       <c r="AX10" s="19">
         <v>14192</v>
@@ -24288,7 +24285,7 @@
         <v>41079</v>
       </c>
       <c r="AW11" s="19">
-        <v>42884</v>
+        <v>42822</v>
       </c>
       <c r="AX11" s="19">
         <v>41250</v>
@@ -24449,7 +24446,7 @@
         <v>109323</v>
       </c>
       <c r="AW12" s="8">
-        <v>109661</v>
+        <v>110413</v>
       </c>
       <c r="AX12" s="8">
         <v>106998</v>
@@ -24670,7 +24667,7 @@
         <v>474.17004400000002</v>
       </c>
       <c r="AW15" s="19">
-        <v>467.69939299999999</v>
+        <v>465.23953999999998</v>
       </c>
       <c r="AX15" s="19">
         <v>471.36564299999998</v>
@@ -24831,7 +24828,7 @@
         <v>839.85170400000004</v>
       </c>
       <c r="AW16" s="19">
-        <v>874.28392699999995</v>
+        <v>878.432997</v>
       </c>
       <c r="AX16" s="19">
         <v>805.15687400000002</v>
@@ -24992,7 +24989,7 @@
         <v>478.86316399999998</v>
       </c>
       <c r="AW17" s="19">
-        <v>481.86904700000002</v>
+        <v>482.124819</v>
       </c>
       <c r="AX17" s="19">
         <v>577.32030799999995</v>
@@ -25153,7 +25150,7 @@
         <v>51.464913000000003</v>
       </c>
       <c r="AW18" s="19">
-        <v>56.399445999999998</v>
+        <v>54.723756999999999</v>
       </c>
       <c r="AX18" s="19">
         <v>55.494872000000001</v>
@@ -25314,7 +25311,7 @@
         <v>524.22870599999999</v>
       </c>
       <c r="AW19" s="19">
-        <v>403.21295700000002</v>
+        <v>403.93306699999999</v>
       </c>
       <c r="AX19" s="19">
         <v>500.15290399999998</v>
@@ -25475,7 +25472,7 @@
         <v>1402.4785910000001</v>
       </c>
       <c r="AW20" s="19">
-        <v>1450.6636590000001</v>
+        <v>1437.694753</v>
       </c>
       <c r="AX20" s="19">
         <v>1279.091394</v>
@@ -25636,7 +25633,7 @@
         <v>978.20554700000002</v>
       </c>
       <c r="AW21" s="19">
-        <v>1044.8588999999999</v>
+        <v>1044.070923</v>
       </c>
       <c r="AX21" s="19">
         <v>1004.732848</v>
@@ -25797,7 +25794,7 @@
         <v>4749.2626689999997</v>
       </c>
       <c r="AW22" s="8">
-        <v>4778.9873290000005</v>
+        <v>4766.2198560000006</v>
       </c>
       <c r="AX22" s="8">
         <v>4693.3148429999992</v>
@@ -25867,7 +25864,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25880,61 +25877,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
     </row>
     <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -26099,160 +26096,160 @@
       <c r="A3" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="6">
         <v>44927</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="6">
         <v>44934</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="6">
         <v>44941</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="6">
         <v>44948</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="6">
         <v>44955</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="6">
         <v>44962</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="6">
         <v>44969</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="6">
         <v>44976</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="6">
         <v>44983</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="6">
         <v>44990</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="6">
         <v>44997</v>
       </c>
-      <c r="M3" s="26">
+      <c r="M3" s="6">
         <v>45004</v>
       </c>
-      <c r="N3" s="26">
+      <c r="N3" s="6">
         <v>45011</v>
       </c>
-      <c r="O3" s="26">
+      <c r="O3" s="6">
         <v>45018</v>
       </c>
-      <c r="P3" s="26">
+      <c r="P3" s="6">
         <v>45025</v>
       </c>
-      <c r="Q3" s="26">
+      <c r="Q3" s="6">
         <v>45032</v>
       </c>
-      <c r="R3" s="26">
+      <c r="R3" s="6">
         <v>45039</v>
       </c>
-      <c r="S3" s="26">
+      <c r="S3" s="6">
         <v>45046</v>
       </c>
-      <c r="T3" s="26">
+      <c r="T3" s="6">
         <v>45053</v>
       </c>
-      <c r="U3" s="26">
+      <c r="U3" s="6">
         <v>45060</v>
       </c>
-      <c r="V3" s="26">
+      <c r="V3" s="6">
         <v>45067</v>
       </c>
-      <c r="W3" s="26">
+      <c r="W3" s="6">
         <v>45074</v>
       </c>
-      <c r="X3" s="26">
+      <c r="X3" s="6">
         <v>45081</v>
       </c>
-      <c r="Y3" s="26">
+      <c r="Y3" s="6">
         <v>45088</v>
       </c>
-      <c r="Z3" s="26">
+      <c r="Z3" s="6">
         <v>45095</v>
       </c>
-      <c r="AA3" s="26">
+      <c r="AA3" s="6">
         <v>45102</v>
       </c>
-      <c r="AB3" s="26">
+      <c r="AB3" s="6">
         <v>45109</v>
       </c>
-      <c r="AC3" s="26">
+      <c r="AC3" s="6">
         <v>45116</v>
       </c>
-      <c r="AD3" s="26">
+      <c r="AD3" s="6">
         <v>45123</v>
       </c>
-      <c r="AE3" s="26">
+      <c r="AE3" s="6">
         <v>45130</v>
       </c>
-      <c r="AF3" s="26">
+      <c r="AF3" s="6">
         <v>45137</v>
       </c>
-      <c r="AG3" s="26">
+      <c r="AG3" s="6">
         <v>45144</v>
       </c>
-      <c r="AH3" s="26">
+      <c r="AH3" s="6">
         <v>45151</v>
       </c>
-      <c r="AI3" s="26">
+      <c r="AI3" s="6">
         <v>45158</v>
       </c>
-      <c r="AJ3" s="26">
+      <c r="AJ3" s="6">
         <v>45165</v>
       </c>
-      <c r="AK3" s="26">
+      <c r="AK3" s="6">
         <v>45172</v>
       </c>
-      <c r="AL3" s="26">
+      <c r="AL3" s="6">
         <v>45179</v>
       </c>
-      <c r="AM3" s="26">
+      <c r="AM3" s="6">
         <v>45186</v>
       </c>
-      <c r="AN3" s="26">
+      <c r="AN3" s="6">
         <v>45193</v>
       </c>
-      <c r="AO3" s="26">
+      <c r="AO3" s="6">
         <v>45200</v>
       </c>
-      <c r="AP3" s="26">
+      <c r="AP3" s="6">
         <v>45207</v>
       </c>
-      <c r="AQ3" s="26">
+      <c r="AQ3" s="6">
         <v>45214</v>
       </c>
-      <c r="AR3" s="26">
+      <c r="AR3" s="6">
         <v>45221</v>
       </c>
-      <c r="AS3" s="26">
+      <c r="AS3" s="6">
         <v>45228</v>
       </c>
-      <c r="AT3" s="26">
+      <c r="AT3" s="6">
         <v>45235</v>
       </c>
-      <c r="AU3" s="26">
+      <c r="AU3" s="6">
         <v>45242</v>
       </c>
-      <c r="AV3" s="26">
+      <c r="AV3" s="6">
         <v>45249</v>
       </c>
-      <c r="AW3" s="26">
+      <c r="AW3" s="6">
         <v>45256</v>
       </c>
-      <c r="AX3" s="26">
+      <c r="AX3" s="6">
         <v>45263</v>
       </c>
-      <c r="AY3" s="26">
+      <c r="AY3" s="6">
         <v>45270</v>
       </c>
-      <c r="AZ3" s="26">
+      <c r="AZ3" s="6">
         <v>45277</v>
       </c>
-      <c r="BA3" s="26">
+      <c r="BA3" s="6">
         <v>45284</v>
       </c>
       <c r="BB3"/>
@@ -26409,7 +26406,7 @@
         <v>6041</v>
       </c>
       <c r="AW5" s="19">
-        <v>0</v>
+        <v>6067</v>
       </c>
       <c r="AX5" s="19">
         <v>0</v>
@@ -26571,7 +26568,7 @@
         <v>12323</v>
       </c>
       <c r="AW6" s="7">
-        <v>0</v>
+        <v>13140</v>
       </c>
       <c r="AX6" s="7">
         <v>0</v>
@@ -26733,7 +26730,7 @@
         <v>18576</v>
       </c>
       <c r="AW7" s="7">
-        <v>0</v>
+        <v>18123</v>
       </c>
       <c r="AX7" s="7">
         <v>0</v>
@@ -26895,7 +26892,7 @@
         <v>4378</v>
       </c>
       <c r="AW8" s="7">
-        <v>0</v>
+        <v>4738</v>
       </c>
       <c r="AX8" s="7">
         <v>0</v>
@@ -27057,7 +27054,7 @@
         <v>8463</v>
       </c>
       <c r="AW9" s="7">
-        <v>0</v>
+        <v>10685</v>
       </c>
       <c r="AX9" s="7">
         <v>0</v>
@@ -27219,7 +27216,7 @@
         <v>14127</v>
       </c>
       <c r="AW10" s="19">
-        <v>0</v>
+        <v>13416</v>
       </c>
       <c r="AX10" s="19">
         <v>0</v>
@@ -27381,7 +27378,7 @@
         <v>40158</v>
       </c>
       <c r="AW11" s="7">
-        <v>0</v>
+        <v>42446</v>
       </c>
       <c r="AX11" s="7">
         <v>0</v>
@@ -27543,7 +27540,7 @@
         <v>104066</v>
       </c>
       <c r="AW12" s="8">
-        <v>0</v>
+        <v>108615</v>
       </c>
       <c r="AX12" s="8">
         <v>0</v>
@@ -27767,7 +27764,7 @@
         <v>464.85895299999999</v>
       </c>
       <c r="AW15" s="19">
-        <v>0</v>
+        <v>452.84101800000002</v>
       </c>
       <c r="AX15" s="19">
         <v>0</v>
@@ -27929,7 +27926,7 @@
         <v>887.33977800000002</v>
       </c>
       <c r="AW16" s="7">
-        <v>0</v>
+        <v>950.074296</v>
       </c>
       <c r="AX16" s="7">
         <v>0</v>
@@ -28091,7 +28088,7 @@
         <v>487.59617100000003</v>
       </c>
       <c r="AW17" s="7">
-        <v>0</v>
+        <v>512.009274</v>
       </c>
       <c r="AX17" s="7">
         <v>0</v>
@@ -28253,7 +28250,7 @@
         <v>65.225431999999998</v>
       </c>
       <c r="AW18" s="7">
-        <v>0</v>
+        <v>64.451792999999995</v>
       </c>
       <c r="AX18" s="7">
         <v>0</v>
@@ -28415,7 +28412,7 @@
         <v>386.00406099999998</v>
       </c>
       <c r="AW19" s="7">
-        <v>0</v>
+        <v>459.34115800000001</v>
       </c>
       <c r="AX19" s="7">
         <v>0</v>
@@ -28577,7 +28574,7 @@
         <v>1414.814081</v>
       </c>
       <c r="AW20" s="19">
-        <v>0</v>
+        <v>1286.8551580000001</v>
       </c>
       <c r="AX20" s="19">
         <v>0</v>
@@ -28739,7 +28736,7 @@
         <v>908.04903400000001</v>
       </c>
       <c r="AW21" s="7">
-        <v>0</v>
+        <v>1021.3936210000001</v>
       </c>
       <c r="AX21" s="7">
         <v>0</v>
@@ -28901,7 +28898,7 @@
         <v>4613.8875099999996</v>
       </c>
       <c r="AW22" s="8">
-        <v>0</v>
+        <v>4746.9663180000007</v>
       </c>
       <c r="AX22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Dec 12 05:22:48 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A118F2-CE01-422B-B4B0-C08EF9347CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CBF19D-A659-4D11-9B1B-FCCE208A5E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -19686,12 +19686,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22779,7 +22779,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomRight" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23322,7 +23322,7 @@
         <v>6422</v>
       </c>
       <c r="AX5" s="19">
-        <v>6293</v>
+        <v>6261</v>
       </c>
       <c r="AY5" s="19">
         <v>6056</v>
@@ -23483,7 +23483,7 @@
         <v>12486</v>
       </c>
       <c r="AX6" s="19">
-        <v>11657</v>
+        <v>11629</v>
       </c>
       <c r="AY6" s="19">
         <v>11973</v>
@@ -23644,7 +23644,7 @@
         <v>19601</v>
       </c>
       <c r="AX7" s="19">
-        <v>18090</v>
+        <v>18829</v>
       </c>
       <c r="AY7" s="19">
         <v>16697</v>
@@ -23805,7 +23805,7 @@
         <v>4569</v>
       </c>
       <c r="AX8" s="19">
-        <v>4435</v>
+        <v>4287</v>
       </c>
       <c r="AY8" s="19">
         <v>4305</v>
@@ -23966,7 +23966,7 @@
         <v>9130</v>
       </c>
       <c r="AX9" s="19">
-        <v>11081</v>
+        <v>11072</v>
       </c>
       <c r="AY9" s="19">
         <v>9208</v>
@@ -24127,7 +24127,7 @@
         <v>15383</v>
       </c>
       <c r="AX10" s="19">
-        <v>14192</v>
+        <v>14207</v>
       </c>
       <c r="AY10" s="19">
         <v>14512</v>
@@ -24288,7 +24288,7 @@
         <v>42822</v>
       </c>
       <c r="AX11" s="19">
-        <v>41250</v>
+        <v>41170</v>
       </c>
       <c r="AY11" s="19">
         <v>43076</v>
@@ -24449,7 +24449,7 @@
         <v>110413</v>
       </c>
       <c r="AX12" s="8">
-        <v>106998</v>
+        <v>107455</v>
       </c>
       <c r="AY12" s="8">
         <v>105827</v>
@@ -24670,7 +24670,7 @@
         <v>465.23953999999998</v>
       </c>
       <c r="AX15" s="19">
-        <v>471.36564299999998</v>
+        <v>469.36145800000003</v>
       </c>
       <c r="AY15" s="19">
         <v>455.92156399999999</v>
@@ -24831,7 +24831,7 @@
         <v>878.432997</v>
       </c>
       <c r="AX16" s="19">
-        <v>805.15687400000002</v>
+        <v>804.54120599999999</v>
       </c>
       <c r="AY16" s="19">
         <v>843.74641499999996</v>
@@ -24992,7 +24992,7 @@
         <v>482.124819</v>
       </c>
       <c r="AX17" s="19">
-        <v>577.32030799999995</v>
+        <v>577.72562800000003</v>
       </c>
       <c r="AY17" s="19">
         <v>508.591386</v>
@@ -25153,7 +25153,7 @@
         <v>54.723756999999999</v>
       </c>
       <c r="AX18" s="19">
-        <v>55.494872000000001</v>
+        <v>53.027901999999997</v>
       </c>
       <c r="AY18" s="19">
         <v>53.694839000000002</v>
@@ -25314,7 +25314,7 @@
         <v>403.93306699999999</v>
       </c>
       <c r="AX19" s="19">
-        <v>500.15290399999998</v>
+        <v>499.80282699999998</v>
       </c>
       <c r="AY19" s="19">
         <v>418.44617799999997</v>
@@ -25475,7 +25475,7 @@
         <v>1437.694753</v>
       </c>
       <c r="AX20" s="19">
-        <v>1279.091394</v>
+        <v>1282.6093450000001</v>
       </c>
       <c r="AY20" s="19">
         <v>1420.8044950000001</v>
@@ -25636,7 +25636,7 @@
         <v>1044.070923</v>
       </c>
       <c r="AX21" s="19">
-        <v>1004.732848</v>
+        <v>1003.687999</v>
       </c>
       <c r="AY21" s="19">
         <v>1005.521257</v>
@@ -25797,7 +25797,7 @@
         <v>4766.2198560000006</v>
       </c>
       <c r="AX22" s="8">
-        <v>4693.3148429999992</v>
+        <v>4690.7563649999993</v>
       </c>
       <c r="AY22" s="8">
         <v>4706.7261340000005</v>
@@ -25863,8 +25863,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26409,7 +26409,7 @@
         <v>6067</v>
       </c>
       <c r="AX5" s="19">
-        <v>0</v>
+        <v>5859</v>
       </c>
       <c r="AY5" s="19">
         <v>0</v>
@@ -26571,7 +26571,7 @@
         <v>13140</v>
       </c>
       <c r="AX6" s="7">
-        <v>0</v>
+        <v>12760</v>
       </c>
       <c r="AY6" s="7">
         <v>0</v>
@@ -26733,7 +26733,7 @@
         <v>18123</v>
       </c>
       <c r="AX7" s="7">
-        <v>0</v>
+        <v>17145</v>
       </c>
       <c r="AY7" s="7">
         <v>0</v>
@@ -26895,7 +26895,7 @@
         <v>4738</v>
       </c>
       <c r="AX8" s="7">
-        <v>0</v>
+        <v>5072</v>
       </c>
       <c r="AY8" s="7">
         <v>0</v>
@@ -27057,7 +27057,7 @@
         <v>10685</v>
       </c>
       <c r="AX9" s="7">
-        <v>0</v>
+        <v>8723</v>
       </c>
       <c r="AY9" s="7">
         <v>0</v>
@@ -27219,7 +27219,7 @@
         <v>13416</v>
       </c>
       <c r="AX10" s="19">
-        <v>0</v>
+        <v>13980</v>
       </c>
       <c r="AY10" s="19">
         <v>0</v>
@@ -27381,7 +27381,7 @@
         <v>42446</v>
       </c>
       <c r="AX11" s="7">
-        <v>0</v>
+        <v>41515</v>
       </c>
       <c r="AY11" s="7">
         <v>0</v>
@@ -27543,7 +27543,7 @@
         <v>108615</v>
       </c>
       <c r="AX12" s="8">
-        <v>0</v>
+        <v>105054</v>
       </c>
       <c r="AY12" s="8">
         <v>0</v>
@@ -27767,7 +27767,7 @@
         <v>452.84101800000002</v>
       </c>
       <c r="AX15" s="19">
-        <v>0</v>
+        <v>426.452989</v>
       </c>
       <c r="AY15" s="19">
         <v>0</v>
@@ -27929,7 +27929,7 @@
         <v>950.074296</v>
       </c>
       <c r="AX16" s="7">
-        <v>0</v>
+        <v>945.47032300000001</v>
       </c>
       <c r="AY16" s="7">
         <v>0</v>
@@ -28091,7 +28091,7 @@
         <v>512.009274</v>
       </c>
       <c r="AX17" s="7">
-        <v>0</v>
+        <v>480.54639800000001</v>
       </c>
       <c r="AY17" s="7">
         <v>0</v>
@@ -28253,7 +28253,7 @@
         <v>64.451792999999995</v>
       </c>
       <c r="AX18" s="7">
-        <v>0</v>
+        <v>64.893192999999997</v>
       </c>
       <c r="AY18" s="7">
         <v>0</v>
@@ -28415,7 +28415,7 @@
         <v>459.34115800000001</v>
       </c>
       <c r="AX19" s="7">
-        <v>0</v>
+        <v>413.78705100000002</v>
       </c>
       <c r="AY19" s="7">
         <v>0</v>
@@ -28577,7 +28577,7 @@
         <v>1286.8551580000001</v>
       </c>
       <c r="AX20" s="19">
-        <v>0</v>
+        <v>1328.845151</v>
       </c>
       <c r="AY20" s="19">
         <v>0</v>
@@ -28739,7 +28739,7 @@
         <v>1021.3936210000001</v>
       </c>
       <c r="AX21" s="7">
-        <v>0</v>
+        <v>984.25070500000004</v>
       </c>
       <c r="AY21" s="7">
         <v>0</v>
@@ -28901,7 +28901,7 @@
         <v>4746.9663180000007</v>
       </c>
       <c r="AX22" s="8">
-        <v>0</v>
+        <v>4644.2458099999994</v>
       </c>
       <c r="AY22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Thu Dec 14 05:22:13 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CBF19D-A659-4D11-9B1B-FCCE208A5E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A118F2-CE01-422B-B4B0-C08EF9347CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -19686,12 +19686,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22779,7 +22779,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="E38" sqref="E38"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23322,7 +23322,7 @@
         <v>6422</v>
       </c>
       <c r="AX5" s="19">
-        <v>6261</v>
+        <v>6293</v>
       </c>
       <c r="AY5" s="19">
         <v>6056</v>
@@ -23483,7 +23483,7 @@
         <v>12486</v>
       </c>
       <c r="AX6" s="19">
-        <v>11629</v>
+        <v>11657</v>
       </c>
       <c r="AY6" s="19">
         <v>11973</v>
@@ -23644,7 +23644,7 @@
         <v>19601</v>
       </c>
       <c r="AX7" s="19">
-        <v>18829</v>
+        <v>18090</v>
       </c>
       <c r="AY7" s="19">
         <v>16697</v>
@@ -23805,7 +23805,7 @@
         <v>4569</v>
       </c>
       <c r="AX8" s="19">
-        <v>4287</v>
+        <v>4435</v>
       </c>
       <c r="AY8" s="19">
         <v>4305</v>
@@ -23966,7 +23966,7 @@
         <v>9130</v>
       </c>
       <c r="AX9" s="19">
-        <v>11072</v>
+        <v>11081</v>
       </c>
       <c r="AY9" s="19">
         <v>9208</v>
@@ -24127,7 +24127,7 @@
         <v>15383</v>
       </c>
       <c r="AX10" s="19">
-        <v>14207</v>
+        <v>14192</v>
       </c>
       <c r="AY10" s="19">
         <v>14512</v>
@@ -24288,7 +24288,7 @@
         <v>42822</v>
       </c>
       <c r="AX11" s="19">
-        <v>41170</v>
+        <v>41250</v>
       </c>
       <c r="AY11" s="19">
         <v>43076</v>
@@ -24449,7 +24449,7 @@
         <v>110413</v>
       </c>
       <c r="AX12" s="8">
-        <v>107455</v>
+        <v>106998</v>
       </c>
       <c r="AY12" s="8">
         <v>105827</v>
@@ -24670,7 +24670,7 @@
         <v>465.23953999999998</v>
       </c>
       <c r="AX15" s="19">
-        <v>469.36145800000003</v>
+        <v>471.36564299999998</v>
       </c>
       <c r="AY15" s="19">
         <v>455.92156399999999</v>
@@ -24831,7 +24831,7 @@
         <v>878.432997</v>
       </c>
       <c r="AX16" s="19">
-        <v>804.54120599999999</v>
+        <v>805.15687400000002</v>
       </c>
       <c r="AY16" s="19">
         <v>843.74641499999996</v>
@@ -24992,7 +24992,7 @@
         <v>482.124819</v>
       </c>
       <c r="AX17" s="19">
-        <v>577.72562800000003</v>
+        <v>577.32030799999995</v>
       </c>
       <c r="AY17" s="19">
         <v>508.591386</v>
@@ -25153,7 +25153,7 @@
         <v>54.723756999999999</v>
       </c>
       <c r="AX18" s="19">
-        <v>53.027901999999997</v>
+        <v>55.494872000000001</v>
       </c>
       <c r="AY18" s="19">
         <v>53.694839000000002</v>
@@ -25314,7 +25314,7 @@
         <v>403.93306699999999</v>
       </c>
       <c r="AX19" s="19">
-        <v>499.80282699999998</v>
+        <v>500.15290399999998</v>
       </c>
       <c r="AY19" s="19">
         <v>418.44617799999997</v>
@@ -25475,7 +25475,7 @@
         <v>1437.694753</v>
       </c>
       <c r="AX20" s="19">
-        <v>1282.6093450000001</v>
+        <v>1279.091394</v>
       </c>
       <c r="AY20" s="19">
         <v>1420.8044950000001</v>
@@ -25636,7 +25636,7 @@
         <v>1044.070923</v>
       </c>
       <c r="AX21" s="19">
-        <v>1003.687999</v>
+        <v>1004.732848</v>
       </c>
       <c r="AY21" s="19">
         <v>1005.521257</v>
@@ -25797,7 +25797,7 @@
         <v>4766.2198560000006</v>
       </c>
       <c r="AX22" s="8">
-        <v>4690.7563649999993</v>
+        <v>4693.3148429999992</v>
       </c>
       <c r="AY22" s="8">
         <v>4706.7261340000005</v>
@@ -25863,8 +25863,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26409,7 +26409,7 @@
         <v>6067</v>
       </c>
       <c r="AX5" s="19">
-        <v>5859</v>
+        <v>0</v>
       </c>
       <c r="AY5" s="19">
         <v>0</v>
@@ -26571,7 +26571,7 @@
         <v>13140</v>
       </c>
       <c r="AX6" s="7">
-        <v>12760</v>
+        <v>0</v>
       </c>
       <c r="AY6" s="7">
         <v>0</v>
@@ -26733,7 +26733,7 @@
         <v>18123</v>
       </c>
       <c r="AX7" s="7">
-        <v>17145</v>
+        <v>0</v>
       </c>
       <c r="AY7" s="7">
         <v>0</v>
@@ -26895,7 +26895,7 @@
         <v>4738</v>
       </c>
       <c r="AX8" s="7">
-        <v>5072</v>
+        <v>0</v>
       </c>
       <c r="AY8" s="7">
         <v>0</v>
@@ -27057,7 +27057,7 @@
         <v>10685</v>
       </c>
       <c r="AX9" s="7">
-        <v>8723</v>
+        <v>0</v>
       </c>
       <c r="AY9" s="7">
         <v>0</v>
@@ -27219,7 +27219,7 @@
         <v>13416</v>
       </c>
       <c r="AX10" s="19">
-        <v>13980</v>
+        <v>0</v>
       </c>
       <c r="AY10" s="19">
         <v>0</v>
@@ -27381,7 +27381,7 @@
         <v>42446</v>
       </c>
       <c r="AX11" s="7">
-        <v>41515</v>
+        <v>0</v>
       </c>
       <c r="AY11" s="7">
         <v>0</v>
@@ -27543,7 +27543,7 @@
         <v>108615</v>
       </c>
       <c r="AX12" s="8">
-        <v>105054</v>
+        <v>0</v>
       </c>
       <c r="AY12" s="8">
         <v>0</v>
@@ -27767,7 +27767,7 @@
         <v>452.84101800000002</v>
       </c>
       <c r="AX15" s="19">
-        <v>426.452989</v>
+        <v>0</v>
       </c>
       <c r="AY15" s="19">
         <v>0</v>
@@ -27929,7 +27929,7 @@
         <v>950.074296</v>
       </c>
       <c r="AX16" s="7">
-        <v>945.47032300000001</v>
+        <v>0</v>
       </c>
       <c r="AY16" s="7">
         <v>0</v>
@@ -28091,7 +28091,7 @@
         <v>512.009274</v>
       </c>
       <c r="AX17" s="7">
-        <v>480.54639800000001</v>
+        <v>0</v>
       </c>
       <c r="AY17" s="7">
         <v>0</v>
@@ -28253,7 +28253,7 @@
         <v>64.451792999999995</v>
       </c>
       <c r="AX18" s="7">
-        <v>64.893192999999997</v>
+        <v>0</v>
       </c>
       <c r="AY18" s="7">
         <v>0</v>
@@ -28415,7 +28415,7 @@
         <v>459.34115800000001</v>
       </c>
       <c r="AX19" s="7">
-        <v>413.78705100000002</v>
+        <v>0</v>
       </c>
       <c r="AY19" s="7">
         <v>0</v>
@@ -28577,7 +28577,7 @@
         <v>1286.8551580000001</v>
       </c>
       <c r="AX20" s="19">
-        <v>1328.845151</v>
+        <v>0</v>
       </c>
       <c r="AY20" s="19">
         <v>0</v>
@@ -28739,7 +28739,7 @@
         <v>1021.3936210000001</v>
       </c>
       <c r="AX21" s="7">
-        <v>984.25070500000004</v>
+        <v>0</v>
       </c>
       <c r="AY21" s="7">
         <v>0</v>
@@ -28901,7 +28901,7 @@
         <v>4746.9663180000007</v>
       </c>
       <c r="AX22" s="8">
-        <v>4644.2458099999994</v>
+        <v>0</v>
       </c>
       <c r="AY22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Dec 19 05:22:30 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A118F2-CE01-422B-B4B0-C08EF9347CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C33940-0F5A-4759-AC83-3A52DA329F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -19686,12 +19686,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BA54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22779,7 +22779,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomRight" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23322,10 +23322,10 @@
         <v>6422</v>
       </c>
       <c r="AX5" s="19">
-        <v>6293</v>
+        <v>6261</v>
       </c>
       <c r="AY5" s="19">
-        <v>6056</v>
+        <v>6026</v>
       </c>
       <c r="AZ5" s="19">
         <v>5040</v>
@@ -23483,10 +23483,10 @@
         <v>12486</v>
       </c>
       <c r="AX6" s="19">
-        <v>11657</v>
+        <v>11629</v>
       </c>
       <c r="AY6" s="19">
-        <v>11973</v>
+        <v>11940</v>
       </c>
       <c r="AZ6" s="19">
         <v>10183</v>
@@ -23644,10 +23644,10 @@
         <v>19601</v>
       </c>
       <c r="AX7" s="19">
-        <v>18090</v>
+        <v>18829</v>
       </c>
       <c r="AY7" s="19">
-        <v>16697</v>
+        <v>17397</v>
       </c>
       <c r="AZ7" s="19">
         <v>14879</v>
@@ -23805,10 +23805,10 @@
         <v>4569</v>
       </c>
       <c r="AX8" s="19">
-        <v>4435</v>
+        <v>4287</v>
       </c>
       <c r="AY8" s="19">
-        <v>4305</v>
+        <v>4290</v>
       </c>
       <c r="AZ8" s="19">
         <v>3614</v>
@@ -23966,10 +23966,10 @@
         <v>9130</v>
       </c>
       <c r="AX9" s="19">
-        <v>11081</v>
+        <v>11072</v>
       </c>
       <c r="AY9" s="19">
-        <v>9208</v>
+        <v>9088</v>
       </c>
       <c r="AZ9" s="19">
         <v>5668</v>
@@ -24127,10 +24127,10 @@
         <v>15383</v>
       </c>
       <c r="AX10" s="19">
-        <v>14192</v>
+        <v>14207</v>
       </c>
       <c r="AY10" s="19">
-        <v>14512</v>
+        <v>14330</v>
       </c>
       <c r="AZ10" s="19">
         <v>11917</v>
@@ -24288,10 +24288,10 @@
         <v>42822</v>
       </c>
       <c r="AX11" s="19">
-        <v>41250</v>
+        <v>41170</v>
       </c>
       <c r="AY11" s="19">
-        <v>43076</v>
+        <v>42982</v>
       </c>
       <c r="AZ11" s="19">
         <v>31158</v>
@@ -24449,10 +24449,10 @@
         <v>110413</v>
       </c>
       <c r="AX12" s="8">
-        <v>106998</v>
+        <v>107455</v>
       </c>
       <c r="AY12" s="8">
-        <v>105827</v>
+        <v>106053</v>
       </c>
       <c r="AZ12" s="8">
         <v>82459</v>
@@ -24670,10 +24670,10 @@
         <v>465.23953999999998</v>
       </c>
       <c r="AX15" s="19">
-        <v>471.36564299999998</v>
+        <v>469.36145800000003</v>
       </c>
       <c r="AY15" s="19">
-        <v>455.92156399999999</v>
+        <v>453.522627</v>
       </c>
       <c r="AZ15" s="19">
         <v>357.46771999999999</v>
@@ -24831,10 +24831,10 @@
         <v>878.432997</v>
       </c>
       <c r="AX16" s="19">
-        <v>805.15687400000002</v>
+        <v>804.54120599999999</v>
       </c>
       <c r="AY16" s="19">
-        <v>843.74641499999996</v>
+        <v>843.15540399999998</v>
       </c>
       <c r="AZ16" s="19">
         <v>713.24548600000003</v>
@@ -24992,10 +24992,10 @@
         <v>482.124819</v>
       </c>
       <c r="AX17" s="19">
-        <v>577.32030799999995</v>
+        <v>577.72562800000003</v>
       </c>
       <c r="AY17" s="19">
-        <v>508.591386</v>
+        <v>506.82070700000003</v>
       </c>
       <c r="AZ17" s="19">
         <v>421.07592499999998</v>
@@ -25153,10 +25153,10 @@
         <v>54.723756999999999</v>
       </c>
       <c r="AX18" s="19">
-        <v>55.494872000000001</v>
+        <v>53.027901999999997</v>
       </c>
       <c r="AY18" s="19">
-        <v>53.694839000000002</v>
+        <v>53.683435000000003</v>
       </c>
       <c r="AZ18" s="19">
         <v>48.471234000000003</v>
@@ -25314,10 +25314,10 @@
         <v>403.93306699999999</v>
       </c>
       <c r="AX19" s="19">
-        <v>500.15290399999998</v>
+        <v>499.80282699999998</v>
       </c>
       <c r="AY19" s="19">
-        <v>418.44617799999997</v>
+        <v>417.91065300000002</v>
       </c>
       <c r="AZ19" s="19">
         <v>218.110658</v>
@@ -25475,10 +25475,10 @@
         <v>1437.694753</v>
       </c>
       <c r="AX20" s="19">
-        <v>1279.091394</v>
+        <v>1282.6093450000001</v>
       </c>
       <c r="AY20" s="19">
-        <v>1420.8044950000001</v>
+        <v>1407.218061</v>
       </c>
       <c r="AZ20" s="19">
         <v>1062.9517490000001</v>
@@ -25636,10 +25636,10 @@
         <v>1044.070923</v>
       </c>
       <c r="AX21" s="19">
-        <v>1004.732848</v>
+        <v>1003.687999</v>
       </c>
       <c r="AY21" s="19">
-        <v>1005.521257</v>
+        <v>1004.360185</v>
       </c>
       <c r="AZ21" s="19">
         <v>711.72899600000005</v>
@@ -25797,10 +25797,10 @@
         <v>4766.2198560000006</v>
       </c>
       <c r="AX22" s="8">
-        <v>4693.3148429999992</v>
+        <v>4690.7563649999993</v>
       </c>
       <c r="AY22" s="8">
-        <v>4706.7261340000005</v>
+        <v>4686.6710720000001</v>
       </c>
       <c r="AZ22" s="8">
         <v>3533.0517680000003</v>
@@ -25863,8 +25863,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ32" sqref="AJ32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26409,10 +26409,10 @@
         <v>6067</v>
       </c>
       <c r="AX5" s="19">
-        <v>0</v>
+        <v>5859</v>
       </c>
       <c r="AY5" s="19">
-        <v>0</v>
+        <v>5952</v>
       </c>
       <c r="AZ5" s="19">
         <v>0</v>
@@ -26571,10 +26571,10 @@
         <v>13140</v>
       </c>
       <c r="AX6" s="7">
-        <v>0</v>
+        <v>12760</v>
       </c>
       <c r="AY6" s="7">
-        <v>0</v>
+        <v>13045</v>
       </c>
       <c r="AZ6" s="7">
         <v>0</v>
@@ -26733,10 +26733,10 @@
         <v>18123</v>
       </c>
       <c r="AX7" s="7">
-        <v>0</v>
+        <v>17145</v>
       </c>
       <c r="AY7" s="7">
-        <v>0</v>
+        <v>19061</v>
       </c>
       <c r="AZ7" s="7">
         <v>0</v>
@@ -26895,10 +26895,10 @@
         <v>4738</v>
       </c>
       <c r="AX8" s="7">
-        <v>0</v>
+        <v>5072</v>
       </c>
       <c r="AY8" s="7">
-        <v>0</v>
+        <v>5220</v>
       </c>
       <c r="AZ8" s="7">
         <v>0</v>
@@ -27057,10 +27057,10 @@
         <v>10685</v>
       </c>
       <c r="AX9" s="7">
-        <v>0</v>
+        <v>8723</v>
       </c>
       <c r="AY9" s="7">
-        <v>0</v>
+        <v>8890</v>
       </c>
       <c r="AZ9" s="7">
         <v>0</v>
@@ -27219,10 +27219,10 @@
         <v>13416</v>
       </c>
       <c r="AX10" s="19">
-        <v>0</v>
+        <v>13980</v>
       </c>
       <c r="AY10" s="19">
-        <v>0</v>
+        <v>13485</v>
       </c>
       <c r="AZ10" s="19">
         <v>0</v>
@@ -27381,10 +27381,10 @@
         <v>42446</v>
       </c>
       <c r="AX11" s="7">
-        <v>0</v>
+        <v>41515</v>
       </c>
       <c r="AY11" s="7">
-        <v>0</v>
+        <v>43919</v>
       </c>
       <c r="AZ11" s="7">
         <v>0</v>
@@ -27543,10 +27543,10 @@
         <v>108615</v>
       </c>
       <c r="AX12" s="8">
-        <v>0</v>
+        <v>105054</v>
       </c>
       <c r="AY12" s="8">
-        <v>0</v>
+        <v>109572</v>
       </c>
       <c r="AZ12" s="8">
         <v>0</v>
@@ -27767,10 +27767,10 @@
         <v>452.84101800000002</v>
       </c>
       <c r="AX15" s="19">
-        <v>0</v>
+        <v>426.452989</v>
       </c>
       <c r="AY15" s="19">
-        <v>0</v>
+        <v>437.59148099999999</v>
       </c>
       <c r="AZ15" s="19">
         <v>0</v>
@@ -27929,10 +27929,10 @@
         <v>950.074296</v>
       </c>
       <c r="AX16" s="7">
-        <v>0</v>
+        <v>945.47032300000001</v>
       </c>
       <c r="AY16" s="7">
-        <v>0</v>
+        <v>953.87813300000005</v>
       </c>
       <c r="AZ16" s="7">
         <v>0</v>
@@ -28091,10 +28091,10 @@
         <v>512.009274</v>
       </c>
       <c r="AX17" s="7">
-        <v>0</v>
+        <v>480.54639800000001</v>
       </c>
       <c r="AY17" s="7">
-        <v>0</v>
+        <v>489.13018499999998</v>
       </c>
       <c r="AZ17" s="7">
         <v>0</v>
@@ -28253,10 +28253,10 @@
         <v>64.451792999999995</v>
       </c>
       <c r="AX18" s="7">
-        <v>0</v>
+        <v>64.893192999999997</v>
       </c>
       <c r="AY18" s="7">
-        <v>0</v>
+        <v>77.609941000000006</v>
       </c>
       <c r="AZ18" s="7">
         <v>0</v>
@@ -28415,10 +28415,10 @@
         <v>459.34115800000001</v>
       </c>
       <c r="AX19" s="7">
-        <v>0</v>
+        <v>413.78705100000002</v>
       </c>
       <c r="AY19" s="7">
-        <v>0</v>
+        <v>370.854581</v>
       </c>
       <c r="AZ19" s="7">
         <v>0</v>
@@ -28577,10 +28577,10 @@
         <v>1286.8551580000001</v>
       </c>
       <c r="AX20" s="19">
-        <v>0</v>
+        <v>1328.845151</v>
       </c>
       <c r="AY20" s="19">
-        <v>0</v>
+        <v>1309.9274230000001</v>
       </c>
       <c r="AZ20" s="19">
         <v>0</v>
@@ -28739,10 +28739,10 @@
         <v>1021.3936210000001</v>
       </c>
       <c r="AX21" s="7">
-        <v>0</v>
+        <v>984.25070500000004</v>
       </c>
       <c r="AY21" s="7">
-        <v>0</v>
+        <v>999.25665500000002</v>
       </c>
       <c r="AZ21" s="7">
         <v>0</v>
@@ -28901,10 +28901,10 @@
         <v>4746.9663180000007</v>
       </c>
       <c r="AX22" s="8">
-        <v>0</v>
+        <v>4644.2458099999994</v>
       </c>
       <c r="AY22" s="8">
-        <v>0</v>
+        <v>4638.2483990000001</v>
       </c>
       <c r="AZ22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Aug 27 05:24:59 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{102D5B61-12B4-4471-A502-69F510694E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7001F03-BDF6-4466-B844-66E81361E031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -922,16 +922,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="9"/>
+    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1310,12 +1310,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2658,12 +2658,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -3974,22 +3974,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.44140625" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.42578125" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4046,7 +4046,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4369,13 +4369,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>5922</v>
       </c>
       <c r="AI5" s="15">
-        <v>0</v>
+        <v>4724</v>
       </c>
       <c r="AJ5" s="15">
         <v>0</v>
@@ -4537,7 +4537,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>13011</v>
       </c>
       <c r="AI6" s="6">
-        <v>0</v>
+        <v>10292</v>
       </c>
       <c r="AJ6" s="6">
         <v>0</v>
@@ -4699,7 +4699,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>14949</v>
       </c>
       <c r="AI7" s="6">
-        <v>0</v>
+        <v>15168</v>
       </c>
       <c r="AJ7" s="6">
         <v>0</v>
@@ -4861,7 +4861,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>4081</v>
       </c>
       <c r="AI8" s="6">
-        <v>0</v>
+        <v>3396</v>
       </c>
       <c r="AJ8" s="6">
         <v>0</v>
@@ -5023,7 +5023,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>8842</v>
       </c>
       <c r="AI9" s="6">
-        <v>0</v>
+        <v>7250</v>
       </c>
       <c r="AJ9" s="6">
         <v>0</v>
@@ -5185,7 +5185,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>12130</v>
       </c>
       <c r="AI10" s="15">
-        <v>0</v>
+        <v>8727</v>
       </c>
       <c r="AJ10" s="15">
         <v>0</v>
@@ -5347,7 +5347,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>39058</v>
       </c>
       <c r="AI11" s="6">
-        <v>0</v>
+        <v>28728</v>
       </c>
       <c r="AJ11" s="6">
         <v>0</v>
@@ -5509,7 +5509,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>97993</v>
       </c>
       <c r="AI12" s="7">
-        <v>0</v>
+        <v>78285</v>
       </c>
       <c r="AJ12" s="7">
         <v>0</v>
@@ -5671,7 +5671,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5727,13 +5727,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>450.18517000000003</v>
       </c>
       <c r="AI15" s="15">
-        <v>0</v>
+        <v>336.97846700000002</v>
       </c>
       <c r="AJ15" s="15">
         <v>0</v>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>953.28650700000003</v>
       </c>
       <c r="AI16" s="6">
-        <v>0</v>
+        <v>706.90092900000002</v>
       </c>
       <c r="AJ16" s="6">
         <v>0</v>
@@ -6057,7 +6057,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>648.69403</v>
       </c>
       <c r="AI17" s="6">
-        <v>0</v>
+        <v>344.75138600000002</v>
       </c>
       <c r="AJ17" s="6">
         <v>0</v>
@@ -6219,7 +6219,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>72.158365000000003</v>
       </c>
       <c r="AI18" s="6">
-        <v>0</v>
+        <v>44.145868999999998</v>
       </c>
       <c r="AJ18" s="6">
         <v>0</v>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>361.26725900000002</v>
       </c>
       <c r="AI19" s="6">
-        <v>0</v>
+        <v>307.15985599999999</v>
       </c>
       <c r="AJ19" s="6">
         <v>0</v>
@@ -6543,7 +6543,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>1147.503254</v>
       </c>
       <c r="AI20" s="15">
-        <v>0</v>
+        <v>740.64947099999995</v>
       </c>
       <c r="AJ20" s="15">
         <v>0</v>
@@ -6705,7 +6705,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>931.29774999999995</v>
       </c>
       <c r="AI21" s="6">
-        <v>0</v>
+        <v>602.18869299999994</v>
       </c>
       <c r="AJ21" s="6">
         <v>0</v>
@@ -6867,7 +6867,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6971,7 +6971,7 @@
         <v>4564.3923350000005</v>
       </c>
       <c r="AI22" s="7">
-        <v>0</v>
+        <v>3082.7746710000001</v>
       </c>
       <c r="AJ22" s="7">
         <v>0</v>
@@ -7029,100 +7029,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -7137,9 +7137,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -7155,16 +7152,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="17"/>
+    <col min="54" max="16384" width="6.7109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -7221,7 +7218,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7382,7 +7379,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7544,12 +7541,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7710,7 +7707,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7871,7 +7868,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -8032,7 +8029,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8193,7 +8190,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8354,7 +8351,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8515,7 +8512,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8676,7 +8673,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8837,7 +8834,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8892,12 +8889,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -9058,7 +9055,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9219,7 +9216,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9380,7 +9377,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9541,7 +9538,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9702,7 +9699,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9863,7 +9860,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -10024,7 +10021,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10185,38 +10182,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -10245,16 +10242,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -10311,7 +10308,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10472,7 +10469,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10633,12 +10630,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10799,7 +10796,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -10960,7 +10957,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11121,7 +11118,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11282,7 +11279,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11443,7 +11440,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11604,7 +11601,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11765,7 +11762,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11926,7 +11923,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -11981,12 +11978,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12147,7 +12144,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12308,7 +12305,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12469,7 +12466,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12630,7 +12627,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12791,7 +12788,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -12952,7 +12949,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13113,7 +13110,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13274,38 +13271,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13330,16 +13327,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -13396,7 +13393,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13557,7 +13554,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13719,12 +13716,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13885,7 +13882,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14046,7 +14043,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14207,7 +14204,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14368,7 +14365,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14529,7 +14526,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14690,7 +14687,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14851,7 +14848,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15012,7 +15009,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15067,12 +15064,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15233,7 +15230,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15394,7 +15391,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15555,7 +15552,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15716,7 +15713,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15877,7 +15874,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16038,7 +16035,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16199,7 +16196,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16360,38 +16357,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16408,16 +16405,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -16474,7 +16471,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16635,7 +16632,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16797,12 +16794,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -16963,7 +16960,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17124,7 +17121,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17285,7 +17282,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17446,7 +17443,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17607,7 +17604,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17768,7 +17765,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17929,7 +17926,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18090,7 +18087,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18145,12 +18142,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18311,7 +18308,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18472,7 +18469,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18633,7 +18630,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18794,7 +18791,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -18955,7 +18952,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19116,7 +19113,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19277,7 +19274,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19438,38 +19435,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19486,17 +19483,17 @@
       <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -19553,7 +19550,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -19717,7 +19714,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -19879,7 +19876,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -20043,12 +20040,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -20212,7 +20209,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -20376,7 +20373,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -20540,7 +20537,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -20704,7 +20701,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -20868,7 +20865,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -21032,7 +21029,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -21196,7 +21193,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -21360,7 +21357,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -21416,12 +21413,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -21585,7 +21582,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -21749,7 +21746,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -21913,7 +21910,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -22077,7 +22074,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -22241,7 +22238,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -22405,7 +22402,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -22569,7 +22566,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -22733,38 +22730,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22785,16 +22782,16 @@
       <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -22851,7 +22848,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -23012,7 +23009,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -23174,12 +23171,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -23340,7 +23337,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -23501,7 +23498,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -23662,7 +23659,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -23823,7 +23820,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -23984,7 +23981,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -24145,7 +24142,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -24306,7 +24303,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -24467,7 +24464,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -24522,12 +24519,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -24688,7 +24685,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -24849,7 +24846,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -25010,7 +25007,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -25171,7 +25168,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -25332,7 +25329,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -25493,7 +25490,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -25654,7 +25651,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -25815,40 +25812,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25876,16 +25873,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -25942,7 +25939,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26103,7 +26100,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26265,12 +26262,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26431,7 +26428,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26592,7 +26589,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26753,7 +26750,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26914,7 +26911,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27075,7 +27072,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27236,7 +27233,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27397,7 +27394,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27558,7 +27555,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27613,12 +27610,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27779,7 +27776,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27940,7 +27937,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28101,7 +28098,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28262,7 +28259,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28423,7 +28420,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28584,7 +28581,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28745,7 +28742,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28906,40 +28903,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -28960,23 +28957,23 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -29033,7 +29030,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29194,7 +29191,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29356,12 +29353,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29465,7 +29462,7 @@
         <v>5696</v>
       </c>
       <c r="AI5" s="15">
-        <v>6127</v>
+        <v>6111</v>
       </c>
       <c r="AJ5" s="15">
         <v>6135</v>
@@ -29522,7 +29519,7 @@
         <v>4445</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29626,7 +29623,7 @@
         <v>12339</v>
       </c>
       <c r="AI6" s="15">
-        <v>12298</v>
+        <v>12269</v>
       </c>
       <c r="AJ6" s="15">
         <v>12480</v>
@@ -29683,7 +29680,7 @@
         <v>11733</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29787,7 +29784,7 @@
         <v>21449</v>
       </c>
       <c r="AI7" s="15">
-        <v>15659</v>
+        <v>16187</v>
       </c>
       <c r="AJ7" s="15">
         <v>19256</v>
@@ -29844,7 +29841,7 @@
         <v>15028</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -29948,7 +29945,7 @@
         <v>4685</v>
       </c>
       <c r="AI8" s="15">
-        <v>4437</v>
+        <v>4428</v>
       </c>
       <c r="AJ8" s="15">
         <v>4309</v>
@@ -30005,7 +30002,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30109,7 +30106,7 @@
         <v>9734</v>
       </c>
       <c r="AI9" s="15">
-        <v>9108</v>
+        <v>9262</v>
       </c>
       <c r="AJ9" s="15">
         <v>9268</v>
@@ -30166,7 +30163,7 @@
         <v>8123</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30270,7 +30267,7 @@
         <v>10200</v>
       </c>
       <c r="AI10" s="15">
-        <v>11169</v>
+        <v>11171</v>
       </c>
       <c r="AJ10" s="15">
         <v>11103</v>
@@ -30327,7 +30324,7 @@
         <v>9903</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30431,7 +30428,7 @@
         <v>40937</v>
       </c>
       <c r="AI11" s="15">
-        <v>38316</v>
+        <v>38235</v>
       </c>
       <c r="AJ11" s="15">
         <v>39287</v>
@@ -30488,7 +30485,7 @@
         <v>34137</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30592,7 +30589,7 @@
         <v>105040</v>
       </c>
       <c r="AI12" s="7">
-        <v>97114</v>
+        <v>97663</v>
       </c>
       <c r="AJ12" s="7">
         <v>101838</v>
@@ -30649,7 +30646,7 @@
         <v>85879</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30704,12 +30701,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30813,7 +30810,7 @@
         <v>433.43205999999998</v>
       </c>
       <c r="AI15" s="15">
-        <v>459.14135499999998</v>
+        <v>458.180678</v>
       </c>
       <c r="AJ15" s="15">
         <v>477.95193799999998</v>
@@ -30870,7 +30867,7 @@
         <v>299.51857200000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -30974,7 +30971,7 @@
         <v>797.39188300000001</v>
       </c>
       <c r="AI16" s="15">
-        <v>829.32071399999995</v>
+        <v>829.12899600000003</v>
       </c>
       <c r="AJ16" s="15">
         <v>827.81147699999997</v>
@@ -31031,7 +31028,7 @@
         <v>889.37489700000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31135,7 +31132,7 @@
         <v>592.99947799999995</v>
       </c>
       <c r="AI17" s="15">
-        <v>514.93327999999997</v>
+        <v>514.06320200000005</v>
       </c>
       <c r="AJ17" s="15">
         <v>576.19058900000005</v>
@@ -31192,7 +31189,7 @@
         <v>534.04841199999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31296,7 +31293,7 @@
         <v>61.886968000000003</v>
       </c>
       <c r="AI18" s="15">
-        <v>60.478881999999999</v>
+        <v>60.222265</v>
       </c>
       <c r="AJ18" s="15">
         <v>60.502398999999997</v>
@@ -31353,7 +31350,7 @@
         <v>38.940157999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31457,7 +31454,7 @@
         <v>411.55973</v>
       </c>
       <c r="AI19" s="15">
-        <v>401.20988499999999</v>
+        <v>403.48586599999999</v>
       </c>
       <c r="AJ19" s="15">
         <v>361.42696799999999</v>
@@ -31514,7 +31511,7 @@
         <v>363.77720699999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31618,7 +31615,7 @@
         <v>986.26180499999998</v>
       </c>
       <c r="AI20" s="15">
-        <v>1061.8927659999999</v>
+        <v>1061.514457</v>
       </c>
       <c r="AJ20" s="15">
         <v>1087.203634</v>
@@ -31675,7 +31672,7 @@
         <v>993.71548499999994</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31779,7 +31776,7 @@
         <v>959.27766999999994</v>
       </c>
       <c r="AI21" s="15">
-        <v>860.75445100000002</v>
+        <v>859.92707499999995</v>
       </c>
       <c r="AJ21" s="15">
         <v>846.67003699999998</v>
@@ -31836,7 +31833,7 @@
         <v>756.39903700000002</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -31940,7 +31937,7 @@
         <v>4242.8095940000003</v>
       </c>
       <c r="AI22" s="7">
-        <v>4187.7313329999997</v>
+        <v>4186.5225389999996</v>
       </c>
       <c r="AJ22" s="7">
         <v>4237.7570420000002</v>
@@ -31997,40 +31994,40 @@
         <v>3875.773768</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32043,8 +32040,5 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GH ACTION Autorun Wed Sep  4 05:26:46 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7001F03-BDF6-4466-B844-66E81361E031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1615C84F-EE82-42A2-98FD-5BDCC0D3ACDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3977,7 +3977,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4482,7 +4482,7 @@
         <v>4724</v>
       </c>
       <c r="AJ5" s="15">
-        <v>0</v>
+        <v>5247</v>
       </c>
       <c r="AK5" s="15">
         <v>0</v>
@@ -4644,7 +4644,7 @@
         <v>10292</v>
       </c>
       <c r="AJ6" s="6">
-        <v>0</v>
+        <v>11935</v>
       </c>
       <c r="AK6" s="6">
         <v>0</v>
@@ -4806,7 +4806,7 @@
         <v>15168</v>
       </c>
       <c r="AJ7" s="6">
-        <v>0</v>
+        <v>19412</v>
       </c>
       <c r="AK7" s="6">
         <v>0</v>
@@ -4968,7 +4968,7 @@
         <v>3396</v>
       </c>
       <c r="AJ8" s="6">
-        <v>0</v>
+        <v>4144</v>
       </c>
       <c r="AK8" s="6">
         <v>0</v>
@@ -5130,7 +5130,7 @@
         <v>7250</v>
       </c>
       <c r="AJ9" s="6">
-        <v>0</v>
+        <v>8621</v>
       </c>
       <c r="AK9" s="6">
         <v>0</v>
@@ -5292,7 +5292,7 @@
         <v>8727</v>
       </c>
       <c r="AJ10" s="15">
-        <v>0</v>
+        <v>11555</v>
       </c>
       <c r="AK10" s="15">
         <v>0</v>
@@ -5454,7 +5454,7 @@
         <v>28728</v>
       </c>
       <c r="AJ11" s="6">
-        <v>0</v>
+        <v>35373</v>
       </c>
       <c r="AK11" s="6">
         <v>0</v>
@@ -5616,7 +5616,7 @@
         <v>78285</v>
       </c>
       <c r="AJ12" s="7">
-        <v>0</v>
+        <v>96287</v>
       </c>
       <c r="AK12" s="7">
         <v>0</v>
@@ -5840,7 +5840,7 @@
         <v>336.97846700000002</v>
       </c>
       <c r="AJ15" s="15">
-        <v>0</v>
+        <v>391.73318799999998</v>
       </c>
       <c r="AK15" s="15">
         <v>0</v>
@@ -6002,7 +6002,7 @@
         <v>706.90092900000002</v>
       </c>
       <c r="AJ16" s="6">
-        <v>0</v>
+        <v>880.103342</v>
       </c>
       <c r="AK16" s="6">
         <v>0</v>
@@ -6164,7 +6164,7 @@
         <v>344.75138600000002</v>
       </c>
       <c r="AJ17" s="6">
-        <v>0</v>
+        <v>552.36141399999997</v>
       </c>
       <c r="AK17" s="6">
         <v>0</v>
@@ -6326,7 +6326,7 @@
         <v>44.145868999999998</v>
       </c>
       <c r="AJ18" s="6">
-        <v>0</v>
+        <v>60.779040999999999</v>
       </c>
       <c r="AK18" s="6">
         <v>0</v>
@@ -6488,7 +6488,7 @@
         <v>307.15985599999999</v>
       </c>
       <c r="AJ19" s="6">
-        <v>0</v>
+        <v>358.97626300000002</v>
       </c>
       <c r="AK19" s="6">
         <v>0</v>
@@ -6650,7 +6650,7 @@
         <v>740.64947099999995</v>
       </c>
       <c r="AJ20" s="15">
-        <v>0</v>
+        <v>1076.9260509999999</v>
       </c>
       <c r="AK20" s="15">
         <v>0</v>
@@ -6812,7 +6812,7 @@
         <v>602.18869299999994</v>
       </c>
       <c r="AJ21" s="6">
-        <v>0</v>
+        <v>883.33743300000003</v>
       </c>
       <c r="AK21" s="6">
         <v>0</v>
@@ -6974,7 +6974,7 @@
         <v>3082.7746710000001</v>
       </c>
       <c r="AJ22" s="7">
-        <v>0</v>
+        <v>4204.2167319999999</v>
       </c>
       <c r="AK22" s="7">
         <v>0</v>
@@ -25870,7 +25870,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28957,11 +28957,11 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29465,7 +29465,7 @@
         <v>6111</v>
       </c>
       <c r="AJ5" s="15">
-        <v>6135</v>
+        <v>6125</v>
       </c>
       <c r="AK5" s="15">
         <v>5743</v>
@@ -29626,7 +29626,7 @@
         <v>12269</v>
       </c>
       <c r="AJ6" s="15">
-        <v>12480</v>
+        <v>12459</v>
       </c>
       <c r="AK6" s="15">
         <v>11892</v>
@@ -29787,7 +29787,7 @@
         <v>16187</v>
       </c>
       <c r="AJ7" s="15">
-        <v>19256</v>
+        <v>19562</v>
       </c>
       <c r="AK7" s="15">
         <v>20237</v>
@@ -29948,7 +29948,7 @@
         <v>4428</v>
       </c>
       <c r="AJ8" s="15">
-        <v>4309</v>
+        <v>4305</v>
       </c>
       <c r="AK8" s="15">
         <v>4491</v>
@@ -30109,7 +30109,7 @@
         <v>9262</v>
       </c>
       <c r="AJ9" s="15">
-        <v>9268</v>
+        <v>9273</v>
       </c>
       <c r="AK9" s="15">
         <v>10210</v>
@@ -30270,7 +30270,7 @@
         <v>11171</v>
       </c>
       <c r="AJ10" s="15">
-        <v>11103</v>
+        <v>11047</v>
       </c>
       <c r="AK10" s="15">
         <v>12428</v>
@@ -30431,7 +30431,7 @@
         <v>38235</v>
       </c>
       <c r="AJ11" s="15">
-        <v>39287</v>
+        <v>39203</v>
       </c>
       <c r="AK11" s="15">
         <v>37249</v>
@@ -30592,7 +30592,7 @@
         <v>97663</v>
       </c>
       <c r="AJ12" s="7">
-        <v>101838</v>
+        <v>101974</v>
       </c>
       <c r="AK12" s="7">
         <v>102250</v>
@@ -30813,7 +30813,7 @@
         <v>458.180678</v>
       </c>
       <c r="AJ15" s="15">
-        <v>477.95193799999998</v>
+        <v>476.72680100000002</v>
       </c>
       <c r="AK15" s="15">
         <v>421.91737799999999</v>
@@ -30974,7 +30974,7 @@
         <v>829.12899600000003</v>
       </c>
       <c r="AJ16" s="15">
-        <v>827.81147699999997</v>
+        <v>826.34678499999995</v>
       </c>
       <c r="AK16" s="15">
         <v>825.90069200000005</v>
@@ -31135,7 +31135,7 @@
         <v>514.06320200000005</v>
       </c>
       <c r="AJ17" s="15">
-        <v>576.19058900000005</v>
+        <v>574.34882600000003</v>
       </c>
       <c r="AK17" s="15">
         <v>571.79369199999996</v>
@@ -31296,7 +31296,7 @@
         <v>60.222265</v>
       </c>
       <c r="AJ18" s="15">
-        <v>60.502398999999997</v>
+        <v>60.390579000000002</v>
       </c>
       <c r="AK18" s="15">
         <v>61.965994999999999</v>
@@ -31457,7 +31457,7 @@
         <v>403.48586599999999</v>
       </c>
       <c r="AJ19" s="15">
-        <v>361.42696799999999</v>
+        <v>361.41434600000002</v>
       </c>
       <c r="AK19" s="15">
         <v>476.060294</v>
@@ -31618,7 +31618,7 @@
         <v>1061.514457</v>
       </c>
       <c r="AJ20" s="15">
-        <v>1087.203634</v>
+        <v>1086.4407590000001</v>
       </c>
       <c r="AK20" s="15">
         <v>1116.3297500000001</v>
@@ -31779,7 +31779,7 @@
         <v>859.92707499999995</v>
       </c>
       <c r="AJ21" s="15">
-        <v>846.67003699999998</v>
+        <v>845.41139099999998</v>
       </c>
       <c r="AK21" s="15">
         <v>829.43938600000001</v>
@@ -31940,7 +31940,7 @@
         <v>4186.5225389999996</v>
       </c>
       <c r="AJ22" s="7">
-        <v>4237.7570420000002</v>
+        <v>4231.079487</v>
       </c>
       <c r="AK22" s="7">
         <v>4303.4071869999998</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Sep 10 05:25:57 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1615C84F-EE82-42A2-98FD-5BDCC0D3ACDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C4CE6EF-C3F8-4219-963D-0B1DF9A76089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -919,19 +919,19 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="9"/>
+    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1310,12 +1310,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2658,12 +2658,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -3964,6 +3964,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -3977,19 +3980,19 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.42578125" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.44140625" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4046,7 +4049,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4207,7 +4210,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4369,13 +4372,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4485,7 +4488,7 @@
         <v>5247</v>
       </c>
       <c r="AK5" s="15">
-        <v>0</v>
+        <v>5559</v>
       </c>
       <c r="AL5" s="15">
         <v>0</v>
@@ -4537,7 +4540,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4647,7 +4650,7 @@
         <v>11935</v>
       </c>
       <c r="AK6" s="6">
-        <v>0</v>
+        <v>11624</v>
       </c>
       <c r="AL6" s="6">
         <v>0</v>
@@ -4699,7 +4702,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4809,7 +4812,7 @@
         <v>19412</v>
       </c>
       <c r="AK7" s="6">
-        <v>0</v>
+        <v>19195</v>
       </c>
       <c r="AL7" s="6">
         <v>0</v>
@@ -4861,7 +4864,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4971,7 +4974,7 @@
         <v>4144</v>
       </c>
       <c r="AK8" s="6">
-        <v>0</v>
+        <v>4107</v>
       </c>
       <c r="AL8" s="6">
         <v>0</v>
@@ -5023,7 +5026,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5133,7 +5136,7 @@
         <v>8621</v>
       </c>
       <c r="AK9" s="6">
-        <v>0</v>
+        <v>8599</v>
       </c>
       <c r="AL9" s="6">
         <v>0</v>
@@ -5185,7 +5188,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5295,7 +5298,7 @@
         <v>11555</v>
       </c>
       <c r="AK10" s="15">
-        <v>0</v>
+        <v>12166</v>
       </c>
       <c r="AL10" s="15">
         <v>0</v>
@@ -5347,7 +5350,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5457,7 +5460,7 @@
         <v>35373</v>
       </c>
       <c r="AK11" s="6">
-        <v>0</v>
+        <v>38385</v>
       </c>
       <c r="AL11" s="6">
         <v>0</v>
@@ -5509,7 +5512,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5619,7 +5622,7 @@
         <v>96287</v>
       </c>
       <c r="AK12" s="7">
-        <v>0</v>
+        <v>99635</v>
       </c>
       <c r="AL12" s="7">
         <v>0</v>
@@ -5671,7 +5674,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5727,13 +5730,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5843,7 +5846,7 @@
         <v>391.73318799999998</v>
       </c>
       <c r="AK15" s="15">
-        <v>0</v>
+        <v>394.86603700000001</v>
       </c>
       <c r="AL15" s="15">
         <v>0</v>
@@ -5895,7 +5898,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -6005,7 +6008,7 @@
         <v>880.103342</v>
       </c>
       <c r="AK16" s="6">
-        <v>0</v>
+        <v>815.923317</v>
       </c>
       <c r="AL16" s="6">
         <v>0</v>
@@ -6057,7 +6060,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6167,7 +6170,7 @@
         <v>552.36141399999997</v>
       </c>
       <c r="AK17" s="6">
-        <v>0</v>
+        <v>588.57835399999999</v>
       </c>
       <c r="AL17" s="6">
         <v>0</v>
@@ -6219,7 +6222,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6329,7 +6332,7 @@
         <v>60.779040999999999</v>
       </c>
       <c r="AK18" s="6">
-        <v>0</v>
+        <v>68.022459999999995</v>
       </c>
       <c r="AL18" s="6">
         <v>0</v>
@@ -6381,7 +6384,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6491,7 +6494,7 @@
         <v>358.97626300000002</v>
       </c>
       <c r="AK19" s="6">
-        <v>0</v>
+        <v>372.73333100000002</v>
       </c>
       <c r="AL19" s="6">
         <v>0</v>
@@ -6543,7 +6546,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6653,7 +6656,7 @@
         <v>1076.9260509999999</v>
       </c>
       <c r="AK20" s="15">
-        <v>0</v>
+        <v>1165.080271</v>
       </c>
       <c r="AL20" s="15">
         <v>0</v>
@@ -6705,7 +6708,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6815,7 +6818,7 @@
         <v>883.33743300000003</v>
       </c>
       <c r="AK21" s="6">
-        <v>0</v>
+        <v>939.34409700000003</v>
       </c>
       <c r="AL21" s="6">
         <v>0</v>
@@ -6867,7 +6870,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6977,7 +6980,7 @@
         <v>4204.2167319999999</v>
       </c>
       <c r="AK22" s="7">
-        <v>0</v>
+        <v>4344.5478670000002</v>
       </c>
       <c r="AL22" s="7">
         <v>0</v>
@@ -7029,100 +7032,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -7137,6 +7140,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -7149,19 +7155,19 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="17"/>
+    <col min="54" max="16384" width="6.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -7218,7 +7224,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7379,7 +7385,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7541,12 +7547,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7707,7 +7713,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7868,7 +7874,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -8029,7 +8035,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8190,7 +8196,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8351,7 +8357,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8512,7 +8518,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8673,7 +8679,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8834,7 +8840,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8889,12 +8895,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -9055,7 +9061,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9216,7 +9222,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9377,7 +9383,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9538,7 +9544,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9699,7 +9705,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9860,7 +9866,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -10021,7 +10027,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10182,38 +10188,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -10236,22 +10242,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -10308,7 +10314,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10469,7 +10475,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10630,12 +10636,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10796,7 +10802,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -10957,7 +10963,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11118,7 +11124,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11279,7 +11285,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11440,7 +11446,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11601,7 +11607,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11762,7 +11768,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11923,7 +11929,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -11978,12 +11984,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12144,7 +12150,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12305,7 +12311,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12466,7 +12472,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12627,7 +12633,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12788,7 +12794,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -12949,7 +12955,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13110,7 +13116,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13271,38 +13277,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13324,19 +13330,19 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -13393,7 +13399,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13554,7 +13560,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13716,12 +13722,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13882,7 +13888,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14043,7 +14049,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14204,7 +14210,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14365,7 +14371,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14526,7 +14532,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14687,7 +14693,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14848,7 +14854,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15009,7 +15015,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15064,12 +15070,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15230,7 +15236,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15391,7 +15397,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15552,7 +15558,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15713,7 +15719,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15874,7 +15880,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16035,7 +16041,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16196,7 +16202,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16357,38 +16363,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16402,19 +16408,19 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -16471,7 +16477,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16632,7 +16638,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16794,12 +16800,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -16960,7 +16966,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17121,7 +17127,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17282,7 +17288,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17443,7 +17449,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17604,7 +17610,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17765,7 +17771,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17926,7 +17932,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18087,7 +18093,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18142,12 +18148,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18308,7 +18314,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18469,7 +18475,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18630,7 +18636,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18791,7 +18797,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -18952,7 +18958,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19113,7 +19119,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19274,7 +19280,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19435,38 +19441,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19480,20 +19486,20 @@
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -19550,7 +19556,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -19714,7 +19720,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -19876,7 +19882,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -20040,12 +20046,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -20209,7 +20215,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -20373,7 +20379,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -20537,7 +20543,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -20701,7 +20707,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -20865,7 +20871,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -21029,7 +21035,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -21193,7 +21199,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -21357,7 +21363,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -21413,12 +21419,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -21582,7 +21588,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -21746,7 +21752,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -21910,7 +21916,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -22074,7 +22080,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -22238,7 +22244,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -22402,7 +22408,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -22566,7 +22572,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -22730,38 +22736,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22776,22 +22782,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -22848,7 +22854,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -23009,7 +23015,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -23171,12 +23177,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -23337,7 +23343,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -23498,7 +23504,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -23659,7 +23665,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -23820,7 +23826,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -23981,7 +23987,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -24142,7 +24148,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -24303,7 +24309,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -24464,7 +24470,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -24519,12 +24525,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -24685,7 +24691,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -24846,7 +24852,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -25007,7 +25013,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -25168,7 +25174,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -25329,7 +25335,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -25490,7 +25496,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -25651,7 +25657,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -25812,40 +25818,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25858,6 +25864,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -25867,22 +25876,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -25939,7 +25948,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26100,7 +26109,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26262,12 +26271,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26428,7 +26437,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26589,7 +26598,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26750,7 +26759,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26911,7 +26920,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27072,7 +27081,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27233,7 +27242,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27394,7 +27403,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27555,7 +27564,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27610,12 +27619,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27776,7 +27785,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27937,7 +27946,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28098,7 +28107,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28259,7 +28268,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28420,7 +28429,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28581,7 +28590,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28742,7 +28751,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28903,40 +28912,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -28958,22 +28967,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -29030,7 +29039,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29191,7 +29200,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29353,12 +29362,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29468,7 +29477,7 @@
         <v>6125</v>
       </c>
       <c r="AK5" s="15">
-        <v>5743</v>
+        <v>5731</v>
       </c>
       <c r="AL5" s="15">
         <v>5942</v>
@@ -29519,7 +29528,7 @@
         <v>4445</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29629,7 +29638,7 @@
         <v>12459</v>
       </c>
       <c r="AK6" s="15">
-        <v>11892</v>
+        <v>11882</v>
       </c>
       <c r="AL6" s="15">
         <v>12203</v>
@@ -29680,7 +29689,7 @@
         <v>11733</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29790,7 +29799,7 @@
         <v>19562</v>
       </c>
       <c r="AK7" s="15">
-        <v>20237</v>
+        <v>20820</v>
       </c>
       <c r="AL7" s="15">
         <v>17729</v>
@@ -29841,7 +29850,7 @@
         <v>15028</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -29951,7 +29960,7 @@
         <v>4305</v>
       </c>
       <c r="AK8" s="15">
-        <v>4491</v>
+        <v>4485</v>
       </c>
       <c r="AL8" s="15">
         <v>4773</v>
@@ -30002,7 +30011,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30112,7 +30121,7 @@
         <v>9273</v>
       </c>
       <c r="AK9" s="15">
-        <v>10210</v>
+        <v>10208</v>
       </c>
       <c r="AL9" s="15">
         <v>10435</v>
@@ -30163,7 +30172,7 @@
         <v>8123</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30273,7 +30282,7 @@
         <v>11047</v>
       </c>
       <c r="AK10" s="15">
-        <v>12428</v>
+        <v>12410</v>
       </c>
       <c r="AL10" s="15">
         <v>13014</v>
@@ -30324,7 +30333,7 @@
         <v>9903</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30434,7 +30443,7 @@
         <v>39203</v>
       </c>
       <c r="AK11" s="15">
-        <v>37249</v>
+        <v>37172</v>
       </c>
       <c r="AL11" s="15">
         <v>40798</v>
@@ -30485,7 +30494,7 @@
         <v>34137</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30595,7 +30604,7 @@
         <v>101974</v>
       </c>
       <c r="AK12" s="7">
-        <v>102250</v>
+        <v>102708</v>
       </c>
       <c r="AL12" s="7">
         <v>104894</v>
@@ -30646,7 +30655,7 @@
         <v>85879</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30701,12 +30710,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30816,7 +30825,7 @@
         <v>476.72680100000002</v>
       </c>
       <c r="AK15" s="15">
-        <v>421.91737799999999</v>
+        <v>420.03667100000001</v>
       </c>
       <c r="AL15" s="15">
         <v>453.115228</v>
@@ -30867,7 +30876,7 @@
         <v>299.51857200000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -30977,7 +30986,7 @@
         <v>826.34678499999995</v>
       </c>
       <c r="AK16" s="15">
-        <v>825.90069200000005</v>
+        <v>825.47227999999996</v>
       </c>
       <c r="AL16" s="15">
         <v>857.56252099999995</v>
@@ -31028,7 +31037,7 @@
         <v>889.37489700000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31138,7 +31147,7 @@
         <v>574.34882600000003</v>
       </c>
       <c r="AK17" s="15">
-        <v>571.79369199999996</v>
+        <v>570.16733999999997</v>
       </c>
       <c r="AL17" s="15">
         <v>520.32689500000004</v>
@@ -31189,7 +31198,7 @@
         <v>534.04841199999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31299,7 +31308,7 @@
         <v>60.390579000000002</v>
       </c>
       <c r="AK18" s="15">
-        <v>61.965994999999999</v>
+        <v>61.886457</v>
       </c>
       <c r="AL18" s="15">
         <v>64.228583999999998</v>
@@ -31350,7 +31359,7 @@
         <v>38.940157999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31460,7 +31469,7 @@
         <v>361.41434600000002</v>
       </c>
       <c r="AK19" s="15">
-        <v>476.060294</v>
+        <v>476.12888900000002</v>
       </c>
       <c r="AL19" s="15">
         <v>458.12219199999998</v>
@@ -31511,7 +31520,7 @@
         <v>363.77720699999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31621,7 +31630,7 @@
         <v>1086.4407590000001</v>
       </c>
       <c r="AK20" s="15">
-        <v>1116.3297500000001</v>
+        <v>1117.4824000000001</v>
       </c>
       <c r="AL20" s="15">
         <v>1157.946289</v>
@@ -31672,7 +31681,7 @@
         <v>993.71548499999994</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31782,7 +31791,7 @@
         <v>845.41139099999998</v>
       </c>
       <c r="AK21" s="15">
-        <v>829.43938600000001</v>
+        <v>828.24070400000005</v>
       </c>
       <c r="AL21" s="15">
         <v>919.41972299999998</v>
@@ -31833,7 +31842,7 @@
         <v>756.39903700000002</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -31943,7 +31952,7 @@
         <v>4231.079487</v>
       </c>
       <c r="AK22" s="7">
-        <v>4303.4071869999998</v>
+        <v>4299.4147409999996</v>
       </c>
       <c r="AL22" s="7">
         <v>4430.7214320000003</v>
@@ -31994,40 +32003,40 @@
         <v>3875.773768</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32040,5 +32049,8 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GH ACTION Autorun Tue Sep 17 05:26:01 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C4CE6EF-C3F8-4219-963D-0B1DF9A76089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD478FF-10A7-444C-A4CC-AD5A54841DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -919,19 +919,19 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="9"/>
+    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1310,12 +1310,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2658,12 +2658,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -3964,9 +3964,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -3975,24 +3972,24 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.44140625" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.42578125" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4049,7 +4046,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4210,7 +4207,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4372,13 +4369,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4491,7 +4488,7 @@
         <v>5559</v>
       </c>
       <c r="AL5" s="15">
-        <v>0</v>
+        <v>5388</v>
       </c>
       <c r="AM5" s="15">
         <v>0</v>
@@ -4540,7 +4537,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4653,7 +4650,7 @@
         <v>11624</v>
       </c>
       <c r="AL6" s="6">
-        <v>0</v>
+        <v>11318</v>
       </c>
       <c r="AM6" s="6">
         <v>0</v>
@@ -4702,7 +4699,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4815,7 +4812,7 @@
         <v>19195</v>
       </c>
       <c r="AL7" s="6">
-        <v>0</v>
+        <v>16776</v>
       </c>
       <c r="AM7" s="6">
         <v>0</v>
@@ -4864,7 +4861,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4977,7 +4974,7 @@
         <v>4107</v>
       </c>
       <c r="AL8" s="6">
-        <v>0</v>
+        <v>4017</v>
       </c>
       <c r="AM8" s="6">
         <v>0</v>
@@ -5026,7 +5023,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5139,7 +5136,7 @@
         <v>8599</v>
       </c>
       <c r="AL9" s="6">
-        <v>0</v>
+        <v>9754</v>
       </c>
       <c r="AM9" s="6">
         <v>0</v>
@@ -5188,7 +5185,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5301,7 +5298,7 @@
         <v>12166</v>
       </c>
       <c r="AL10" s="15">
-        <v>0</v>
+        <v>14814</v>
       </c>
       <c r="AM10" s="15">
         <v>0</v>
@@ -5350,7 +5347,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5463,7 +5460,7 @@
         <v>38385</v>
       </c>
       <c r="AL11" s="6">
-        <v>0</v>
+        <v>40565</v>
       </c>
       <c r="AM11" s="6">
         <v>0</v>
@@ -5512,7 +5509,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5625,7 +5622,7 @@
         <v>99635</v>
       </c>
       <c r="AL12" s="7">
-        <v>0</v>
+        <v>102632</v>
       </c>
       <c r="AM12" s="7">
         <v>0</v>
@@ -5674,7 +5671,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5730,13 +5727,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5849,7 +5846,7 @@
         <v>394.86603700000001</v>
       </c>
       <c r="AL15" s="15">
-        <v>0</v>
+        <v>402.85448400000001</v>
       </c>
       <c r="AM15" s="15">
         <v>0</v>
@@ -5898,7 +5895,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -6011,7 +6008,7 @@
         <v>815.923317</v>
       </c>
       <c r="AL16" s="6">
-        <v>0</v>
+        <v>822.49362599999995</v>
       </c>
       <c r="AM16" s="6">
         <v>0</v>
@@ -6060,7 +6057,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6173,7 +6170,7 @@
         <v>588.57835399999999</v>
       </c>
       <c r="AL17" s="6">
-        <v>0</v>
+        <v>458.094829</v>
       </c>
       <c r="AM17" s="6">
         <v>0</v>
@@ -6222,7 +6219,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6335,7 +6332,7 @@
         <v>68.022459999999995</v>
       </c>
       <c r="AL18" s="6">
-        <v>0</v>
+        <v>63.541631000000002</v>
       </c>
       <c r="AM18" s="6">
         <v>0</v>
@@ -6384,7 +6381,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6497,7 +6494,7 @@
         <v>372.73333100000002</v>
       </c>
       <c r="AL19" s="6">
-        <v>0</v>
+        <v>412.930792</v>
       </c>
       <c r="AM19" s="6">
         <v>0</v>
@@ -6546,7 +6543,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6659,7 +6656,7 @@
         <v>1165.080271</v>
       </c>
       <c r="AL20" s="15">
-        <v>0</v>
+        <v>1398.5743379999999</v>
       </c>
       <c r="AM20" s="15">
         <v>0</v>
@@ -6708,7 +6705,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6821,7 +6818,7 @@
         <v>939.34409700000003</v>
       </c>
       <c r="AL21" s="6">
-        <v>0</v>
+        <v>981.90933500000006</v>
       </c>
       <c r="AM21" s="6">
         <v>0</v>
@@ -6870,7 +6867,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6983,7 +6980,7 @@
         <v>4344.5478670000002</v>
       </c>
       <c r="AL22" s="7">
-        <v>0</v>
+        <v>4540.3990350000004</v>
       </c>
       <c r="AM22" s="7">
         <v>0</v>
@@ -7032,100 +7029,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -7140,9 +7137,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -7155,19 +7149,19 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="17"/>
+    <col min="54" max="16384" width="6.7109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -7224,7 +7218,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7385,7 +7379,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7547,12 +7541,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7713,7 +7707,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7874,7 +7868,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -8035,7 +8029,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8196,7 +8190,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8357,7 +8351,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8518,7 +8512,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8679,7 +8673,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8840,7 +8834,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8895,12 +8889,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -9061,7 +9055,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9222,7 +9216,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9383,7 +9377,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9544,7 +9538,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9705,7 +9699,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9866,7 +9860,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -10027,7 +10021,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10188,38 +10182,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -10242,22 +10236,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -10314,7 +10308,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10475,7 +10469,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10636,12 +10630,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10802,7 +10796,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -10963,7 +10957,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11124,7 +11118,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11285,7 +11279,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11446,7 +11440,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11607,7 +11601,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11768,7 +11762,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11929,7 +11923,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -11984,12 +11978,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12150,7 +12144,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12311,7 +12305,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12472,7 +12466,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12633,7 +12627,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12794,7 +12788,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -12955,7 +12949,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13116,7 +13110,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13277,38 +13271,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13330,19 +13324,19 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -13399,7 +13393,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13560,7 +13554,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13722,12 +13716,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13888,7 +13882,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14049,7 +14043,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14210,7 +14204,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14371,7 +14365,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14532,7 +14526,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14693,7 +14687,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14854,7 +14848,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15015,7 +15009,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15070,12 +15064,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15236,7 +15230,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15397,7 +15391,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15558,7 +15552,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15719,7 +15713,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15880,7 +15874,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16041,7 +16035,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16202,7 +16196,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16363,38 +16357,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16408,19 +16402,19 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -16477,7 +16471,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16638,7 +16632,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16800,12 +16794,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -16966,7 +16960,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17127,7 +17121,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17288,7 +17282,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17449,7 +17443,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17610,7 +17604,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17771,7 +17765,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17932,7 +17926,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18093,7 +18087,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18148,12 +18142,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18314,7 +18308,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18475,7 +18469,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18636,7 +18630,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18797,7 +18791,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -18958,7 +18952,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19119,7 +19113,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19280,7 +19274,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19441,38 +19435,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19486,20 +19480,20 @@
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -19556,7 +19550,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -19720,7 +19714,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -19882,7 +19876,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -20046,12 +20040,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -20215,7 +20209,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -20379,7 +20373,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -20543,7 +20537,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -20707,7 +20701,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -20871,7 +20865,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -21035,7 +21029,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -21199,7 +21193,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -21363,7 +21357,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -21419,12 +21413,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -21588,7 +21582,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -21752,7 +21746,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -21916,7 +21910,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -22080,7 +22074,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -22244,7 +22238,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -22408,7 +22402,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -22572,7 +22566,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -22736,38 +22730,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22782,22 +22776,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -22854,7 +22848,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -23015,7 +23009,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -23177,12 +23171,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -23343,7 +23337,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -23504,7 +23498,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -23665,7 +23659,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -23826,7 +23820,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -23987,7 +23981,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -24148,7 +24142,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -24309,7 +24303,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -24470,7 +24464,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -24525,12 +24519,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -24691,7 +24685,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -24852,7 +24846,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -25013,7 +25007,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -25174,7 +25168,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -25335,7 +25329,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -25496,7 +25490,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -25657,7 +25651,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -25818,40 +25812,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25864,9 +25858,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -25876,22 +25867,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -25948,7 +25939,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26109,7 +26100,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26271,12 +26262,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26437,7 +26428,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26598,7 +26589,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26759,7 +26750,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26920,7 +26911,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27081,7 +27072,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27242,7 +27233,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27403,7 +27394,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27564,7 +27555,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27619,12 +27610,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27785,7 +27776,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27946,7 +27937,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28107,7 +28098,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28268,7 +28259,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28429,7 +28420,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28590,7 +28581,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28751,7 +28742,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28912,40 +28903,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -28965,24 +28956,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -29039,7 +29030,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29200,7 +29191,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29362,12 +29353,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29480,7 +29471,7 @@
         <v>5731</v>
       </c>
       <c r="AL5" s="15">
-        <v>5942</v>
+        <v>5923</v>
       </c>
       <c r="AM5" s="15">
         <v>5985</v>
@@ -29528,7 +29519,7 @@
         <v>4445</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29641,7 +29632,7 @@
         <v>11882</v>
       </c>
       <c r="AL6" s="15">
-        <v>12203</v>
+        <v>12198</v>
       </c>
       <c r="AM6" s="15">
         <v>12102</v>
@@ -29689,7 +29680,7 @@
         <v>11733</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29802,7 +29793,7 @@
         <v>20820</v>
       </c>
       <c r="AL7" s="15">
-        <v>17729</v>
+        <v>18214</v>
       </c>
       <c r="AM7" s="15">
         <v>20289</v>
@@ -29850,7 +29841,7 @@
         <v>15028</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -29963,7 +29954,7 @@
         <v>4485</v>
       </c>
       <c r="AL8" s="15">
-        <v>4773</v>
+        <v>4767</v>
       </c>
       <c r="AM8" s="15">
         <v>4988</v>
@@ -30011,7 +30002,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30124,7 +30115,7 @@
         <v>10208</v>
       </c>
       <c r="AL9" s="15">
-        <v>10435</v>
+        <v>10240</v>
       </c>
       <c r="AM9" s="15">
         <v>9543</v>
@@ -30172,7 +30163,7 @@
         <v>8123</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30285,7 +30276,7 @@
         <v>12410</v>
       </c>
       <c r="AL10" s="15">
-        <v>13014</v>
+        <v>12996</v>
       </c>
       <c r="AM10" s="15">
         <v>14549</v>
@@ -30333,7 +30324,7 @@
         <v>9903</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30446,7 +30437,7 @@
         <v>37172</v>
       </c>
       <c r="AL11" s="15">
-        <v>40798</v>
+        <v>40740</v>
       </c>
       <c r="AM11" s="15">
         <v>41926</v>
@@ -30494,7 +30485,7 @@
         <v>34137</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30607,7 +30598,7 @@
         <v>102708</v>
       </c>
       <c r="AL12" s="7">
-        <v>104894</v>
+        <v>105078</v>
       </c>
       <c r="AM12" s="7">
         <v>109382</v>
@@ -30655,7 +30646,7 @@
         <v>85879</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30710,12 +30701,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30828,7 +30819,7 @@
         <v>420.03667100000001</v>
       </c>
       <c r="AL15" s="15">
-        <v>453.115228</v>
+        <v>452.45527600000003</v>
       </c>
       <c r="AM15" s="15">
         <v>447.72177799999997</v>
@@ -30876,7 +30867,7 @@
         <v>299.51857200000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -30989,7 +30980,7 @@
         <v>825.47227999999996</v>
       </c>
       <c r="AL16" s="15">
-        <v>857.56252099999995</v>
+        <v>856.94078300000001</v>
       </c>
       <c r="AM16" s="15">
         <v>816.82095900000002</v>
@@ -31037,7 +31028,7 @@
         <v>889.37489700000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31150,7 +31141,7 @@
         <v>570.16733999999997</v>
       </c>
       <c r="AL17" s="15">
-        <v>520.32689500000004</v>
+        <v>519.23125300000004</v>
       </c>
       <c r="AM17" s="15">
         <v>531.17191200000002</v>
@@ -31198,7 +31189,7 @@
         <v>534.04841199999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31311,7 +31302,7 @@
         <v>61.886457</v>
       </c>
       <c r="AL18" s="15">
-        <v>64.228583999999998</v>
+        <v>64.136240999999998</v>
       </c>
       <c r="AM18" s="15">
         <v>68.635548999999997</v>
@@ -31359,7 +31350,7 @@
         <v>38.940157999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31472,7 +31463,7 @@
         <v>476.12888900000002</v>
       </c>
       <c r="AL19" s="15">
-        <v>458.12219199999998</v>
+        <v>453.58616799999999</v>
       </c>
       <c r="AM19" s="15">
         <v>420.62093399999998</v>
@@ -31520,7 +31511,7 @@
         <v>363.77720699999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31633,7 +31624,7 @@
         <v>1117.4824000000001</v>
       </c>
       <c r="AL20" s="15">
-        <v>1157.946289</v>
+        <v>1156.1470380000001</v>
       </c>
       <c r="AM20" s="15">
         <v>1360.5035929999999</v>
@@ -31681,7 +31672,7 @@
         <v>993.71548499999994</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31794,7 +31785,7 @@
         <v>828.24070400000005</v>
       </c>
       <c r="AL21" s="15">
-        <v>919.41972299999998</v>
+        <v>918.25736199999994</v>
       </c>
       <c r="AM21" s="15">
         <v>977.00921100000005</v>
@@ -31842,7 +31833,7 @@
         <v>756.39903700000002</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -31955,7 +31946,7 @@
         <v>4299.4147409999996</v>
       </c>
       <c r="AL22" s="7">
-        <v>4430.7214320000003</v>
+        <v>4420.7541209999999</v>
       </c>
       <c r="AM22" s="7">
         <v>4622.4839360000005</v>
@@ -32003,40 +31994,40 @@
         <v>3875.773768</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32049,8 +32040,5 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GH ACTION Autorun Tue Sep 24 05:26:37 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD478FF-10A7-444C-A4CC-AD5A54841DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE374CA-D360-4EA3-AEAD-A6926F774BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -3972,12 +3972,12 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4491,7 +4491,7 @@
         <v>5388</v>
       </c>
       <c r="AM5" s="15">
-        <v>0</v>
+        <v>5765</v>
       </c>
       <c r="AN5" s="15">
         <v>0</v>
@@ -4653,7 +4653,7 @@
         <v>11318</v>
       </c>
       <c r="AM6" s="6">
-        <v>0</v>
+        <v>11760</v>
       </c>
       <c r="AN6" s="6">
         <v>0</v>
@@ -4815,7 +4815,7 @@
         <v>16776</v>
       </c>
       <c r="AM7" s="6">
-        <v>0</v>
+        <v>17767</v>
       </c>
       <c r="AN7" s="6">
         <v>0</v>
@@ -4977,7 +4977,7 @@
         <v>4017</v>
       </c>
       <c r="AM8" s="6">
-        <v>0</v>
+        <v>4477</v>
       </c>
       <c r="AN8" s="6">
         <v>0</v>
@@ -5139,7 +5139,7 @@
         <v>9754</v>
       </c>
       <c r="AM9" s="6">
-        <v>0</v>
+        <v>7761</v>
       </c>
       <c r="AN9" s="6">
         <v>0</v>
@@ -5301,7 +5301,7 @@
         <v>14814</v>
       </c>
       <c r="AM10" s="15">
-        <v>0</v>
+        <v>14680</v>
       </c>
       <c r="AN10" s="15">
         <v>0</v>
@@ -5463,7 +5463,7 @@
         <v>40565</v>
       </c>
       <c r="AM11" s="6">
-        <v>0</v>
+        <v>39665</v>
       </c>
       <c r="AN11" s="6">
         <v>0</v>
@@ -5625,7 +5625,7 @@
         <v>102632</v>
       </c>
       <c r="AM12" s="7">
-        <v>0</v>
+        <v>101875</v>
       </c>
       <c r="AN12" s="7">
         <v>0</v>
@@ -5849,7 +5849,7 @@
         <v>402.85448400000001</v>
       </c>
       <c r="AM15" s="15">
-        <v>0</v>
+        <v>431.709701</v>
       </c>
       <c r="AN15" s="15">
         <v>0</v>
@@ -6011,7 +6011,7 @@
         <v>822.49362599999995</v>
       </c>
       <c r="AM16" s="6">
-        <v>0</v>
+        <v>875.01216199999999</v>
       </c>
       <c r="AN16" s="6">
         <v>0</v>
@@ -6173,7 +6173,7 @@
         <v>458.094829</v>
       </c>
       <c r="AM17" s="6">
-        <v>0</v>
+        <v>498.29941300000002</v>
       </c>
       <c r="AN17" s="6">
         <v>0</v>
@@ -6335,7 +6335,7 @@
         <v>63.541631000000002</v>
       </c>
       <c r="AM18" s="6">
-        <v>0</v>
+        <v>62.42559</v>
       </c>
       <c r="AN18" s="6">
         <v>0</v>
@@ -6497,7 +6497,7 @@
         <v>412.930792</v>
       </c>
       <c r="AM19" s="6">
-        <v>0</v>
+        <v>328.34344499999997</v>
       </c>
       <c r="AN19" s="6">
         <v>0</v>
@@ -6659,7 +6659,7 @@
         <v>1398.5743379999999</v>
       </c>
       <c r="AM20" s="15">
-        <v>0</v>
+        <v>1345.620682</v>
       </c>
       <c r="AN20" s="15">
         <v>0</v>
@@ -6821,7 +6821,7 @@
         <v>981.90933500000006</v>
       </c>
       <c r="AM21" s="6">
-        <v>0</v>
+        <v>938.05947700000002</v>
       </c>
       <c r="AN21" s="6">
         <v>0</v>
@@ -6983,7 +6983,7 @@
         <v>4540.3990350000004</v>
       </c>
       <c r="AM22" s="7">
-        <v>0</v>
+        <v>4479.4704699999993</v>
       </c>
       <c r="AN22" s="7">
         <v>0</v>
@@ -28956,12 +28956,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="T32" sqref="T32"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29474,7 +29474,7 @@
         <v>5923</v>
       </c>
       <c r="AM5" s="15">
-        <v>5985</v>
+        <v>5960</v>
       </c>
       <c r="AN5" s="15">
         <v>5780</v>
@@ -29635,7 +29635,7 @@
         <v>12198</v>
       </c>
       <c r="AM6" s="15">
-        <v>12102</v>
+        <v>12094</v>
       </c>
       <c r="AN6" s="15">
         <v>11559</v>
@@ -29796,7 +29796,7 @@
         <v>18214</v>
       </c>
       <c r="AM7" s="15">
-        <v>20289</v>
+        <v>20971</v>
       </c>
       <c r="AN7" s="15">
         <v>20471</v>
@@ -29957,7 +29957,7 @@
         <v>4767</v>
       </c>
       <c r="AM8" s="15">
-        <v>4988</v>
+        <v>4951</v>
       </c>
       <c r="AN8" s="15">
         <v>5217</v>
@@ -30118,7 +30118,7 @@
         <v>10240</v>
       </c>
       <c r="AM9" s="15">
-        <v>9543</v>
+        <v>9538</v>
       </c>
       <c r="AN9" s="15">
         <v>10011</v>
@@ -30279,7 +30279,7 @@
         <v>12996</v>
       </c>
       <c r="AM10" s="15">
-        <v>14549</v>
+        <v>14462</v>
       </c>
       <c r="AN10" s="15">
         <v>15208</v>
@@ -30440,7 +30440,7 @@
         <v>40740</v>
       </c>
       <c r="AM11" s="15">
-        <v>41926</v>
+        <v>41817</v>
       </c>
       <c r="AN11" s="15">
         <v>41438</v>
@@ -30601,7 +30601,7 @@
         <v>105078</v>
       </c>
       <c r="AM12" s="7">
-        <v>109382</v>
+        <v>109793</v>
       </c>
       <c r="AN12" s="7">
         <v>109684</v>
@@ -30822,7 +30822,7 @@
         <v>452.45527600000003</v>
       </c>
       <c r="AM15" s="15">
-        <v>447.72177799999997</v>
+        <v>446.39435400000002</v>
       </c>
       <c r="AN15" s="15">
         <v>426.14194199999997</v>
@@ -30983,7 +30983,7 @@
         <v>856.94078300000001</v>
       </c>
       <c r="AM16" s="15">
-        <v>816.82095900000002</v>
+        <v>816.49973199999999</v>
       </c>
       <c r="AN16" s="15">
         <v>788.05608099999995</v>
@@ -31144,7 +31144,7 @@
         <v>519.23125300000004</v>
       </c>
       <c r="AM17" s="15">
-        <v>531.17191200000002</v>
+        <v>530.45867399999997</v>
       </c>
       <c r="AN17" s="15">
         <v>634.70223999999996</v>
@@ -31305,7 +31305,7 @@
         <v>64.136240999999998</v>
       </c>
       <c r="AM18" s="15">
-        <v>68.635548999999997</v>
+        <v>67.648559000000006</v>
       </c>
       <c r="AN18" s="15">
         <v>72.163685000000001</v>
@@ -31466,7 +31466,7 @@
         <v>453.58616799999999</v>
       </c>
       <c r="AM19" s="15">
-        <v>420.62093399999998</v>
+        <v>420.53968200000003</v>
       </c>
       <c r="AN19" s="15">
         <v>424.03746799999999</v>
@@ -31627,7 +31627,7 @@
         <v>1156.1470380000001</v>
       </c>
       <c r="AM20" s="15">
-        <v>1360.5035929999999</v>
+        <v>1355.807564</v>
       </c>
       <c r="AN20" s="15">
         <v>1502.291872</v>
@@ -31788,7 +31788,7 @@
         <v>918.25736199999994</v>
       </c>
       <c r="AM21" s="15">
-        <v>977.00921100000005</v>
+        <v>975.61884799999996</v>
       </c>
       <c r="AN21" s="15">
         <v>904.89198199999998</v>
@@ -31949,7 +31949,7 @@
         <v>4420.7541209999999</v>
       </c>
       <c r="AM22" s="7">
-        <v>4622.4839360000005</v>
+        <v>4612.9674130000003</v>
       </c>
       <c r="AN22" s="7">
         <v>4752.2852700000003</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Wed Oct  2 05:26:16 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE374CA-D360-4EA3-AEAD-A6926F774BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E38FFF2-3B16-4641-BD5F-8CF4680EFFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3977,7 +3977,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4494,7 +4494,7 @@
         <v>5765</v>
       </c>
       <c r="AN5" s="15">
-        <v>0</v>
+        <v>5623</v>
       </c>
       <c r="AO5" s="15">
         <v>0</v>
@@ -4656,7 +4656,7 @@
         <v>11760</v>
       </c>
       <c r="AN6" s="6">
-        <v>0</v>
+        <v>12013</v>
       </c>
       <c r="AO6" s="6">
         <v>0</v>
@@ -4818,7 +4818,7 @@
         <v>17767</v>
       </c>
       <c r="AN7" s="6">
-        <v>0</v>
+        <v>18814</v>
       </c>
       <c r="AO7" s="6">
         <v>0</v>
@@ -4980,7 +4980,7 @@
         <v>4477</v>
       </c>
       <c r="AN8" s="6">
-        <v>0</v>
+        <v>4409</v>
       </c>
       <c r="AO8" s="6">
         <v>0</v>
@@ -5142,7 +5142,7 @@
         <v>7761</v>
       </c>
       <c r="AN9" s="6">
-        <v>0</v>
+        <v>9396</v>
       </c>
       <c r="AO9" s="6">
         <v>0</v>
@@ -5304,7 +5304,7 @@
         <v>14680</v>
       </c>
       <c r="AN10" s="15">
-        <v>0</v>
+        <v>15780</v>
       </c>
       <c r="AO10" s="15">
         <v>0</v>
@@ -5466,7 +5466,7 @@
         <v>39665</v>
       </c>
       <c r="AN11" s="6">
-        <v>0</v>
+        <v>41442</v>
       </c>
       <c r="AO11" s="6">
         <v>0</v>
@@ -5628,7 +5628,7 @@
         <v>101875</v>
       </c>
       <c r="AN12" s="7">
-        <v>0</v>
+        <v>107477</v>
       </c>
       <c r="AO12" s="7">
         <v>0</v>
@@ -5852,7 +5852,7 @@
         <v>431.709701</v>
       </c>
       <c r="AN15" s="15">
-        <v>0</v>
+        <v>428.208324</v>
       </c>
       <c r="AO15" s="15">
         <v>0</v>
@@ -6014,7 +6014,7 @@
         <v>875.01216199999999</v>
       </c>
       <c r="AN16" s="6">
-        <v>0</v>
+        <v>882.51763200000005</v>
       </c>
       <c r="AO16" s="6">
         <v>0</v>
@@ -6176,7 +6176,7 @@
         <v>498.29941300000002</v>
       </c>
       <c r="AN17" s="6">
-        <v>0</v>
+        <v>477.66669899999999</v>
       </c>
       <c r="AO17" s="6">
         <v>0</v>
@@ -6338,7 +6338,7 @@
         <v>62.42559</v>
       </c>
       <c r="AN18" s="6">
-        <v>0</v>
+        <v>62.525210999999999</v>
       </c>
       <c r="AO18" s="6">
         <v>0</v>
@@ -6500,7 +6500,7 @@
         <v>328.34344499999997</v>
       </c>
       <c r="AN19" s="6">
-        <v>0</v>
+        <v>417.123761</v>
       </c>
       <c r="AO19" s="6">
         <v>0</v>
@@ -6662,7 +6662,7 @@
         <v>1345.620682</v>
       </c>
       <c r="AN20" s="15">
-        <v>0</v>
+        <v>1449.538268</v>
       </c>
       <c r="AO20" s="15">
         <v>0</v>
@@ -6824,7 +6824,7 @@
         <v>938.05947700000002</v>
       </c>
       <c r="AN21" s="6">
-        <v>0</v>
+        <v>1014.4135649999999</v>
       </c>
       <c r="AO21" s="6">
         <v>0</v>
@@ -6986,7 +6986,7 @@
         <v>4479.4704699999993</v>
       </c>
       <c r="AN22" s="7">
-        <v>0</v>
+        <v>4731.9934599999997</v>
       </c>
       <c r="AO22" s="7">
         <v>0</v>
@@ -25870,7 +25870,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28961,7 +28961,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29477,7 +29477,7 @@
         <v>5960</v>
       </c>
       <c r="AN5" s="15">
-        <v>5780</v>
+        <v>5774</v>
       </c>
       <c r="AO5" s="15">
         <v>5957</v>
@@ -29638,7 +29638,7 @@
         <v>12094</v>
       </c>
       <c r="AN6" s="15">
-        <v>11559</v>
+        <v>11555</v>
       </c>
       <c r="AO6" s="15">
         <v>11951</v>
@@ -29799,7 +29799,7 @@
         <v>20971</v>
       </c>
       <c r="AN7" s="15">
-        <v>20471</v>
+        <v>21137</v>
       </c>
       <c r="AO7" s="15">
         <v>19934</v>
@@ -29960,7 +29960,7 @@
         <v>4951</v>
       </c>
       <c r="AN8" s="15">
-        <v>5217</v>
+        <v>5191</v>
       </c>
       <c r="AO8" s="15">
         <v>5071</v>
@@ -30121,7 +30121,7 @@
         <v>9538</v>
       </c>
       <c r="AN9" s="15">
-        <v>10011</v>
+        <v>9852</v>
       </c>
       <c r="AO9" s="15">
         <v>10757</v>
@@ -30282,7 +30282,7 @@
         <v>14462</v>
       </c>
       <c r="AN10" s="15">
-        <v>15208</v>
+        <v>15094</v>
       </c>
       <c r="AO10" s="15">
         <v>16251</v>
@@ -30443,7 +30443,7 @@
         <v>41817</v>
       </c>
       <c r="AN11" s="15">
-        <v>41438</v>
+        <v>41335</v>
       </c>
       <c r="AO11" s="15">
         <v>40294</v>
@@ -30604,7 +30604,7 @@
         <v>109793</v>
       </c>
       <c r="AN12" s="7">
-        <v>109684</v>
+        <v>109938</v>
       </c>
       <c r="AO12" s="7">
         <v>110215</v>
@@ -30825,7 +30825,7 @@
         <v>446.39435400000002</v>
       </c>
       <c r="AN15" s="15">
-        <v>426.14194199999997</v>
+        <v>425.69115299999999</v>
       </c>
       <c r="AO15" s="15">
         <v>453.26573000000002</v>
@@ -30986,7 +30986,7 @@
         <v>816.49973199999999</v>
       </c>
       <c r="AN16" s="15">
-        <v>788.05608099999995</v>
+        <v>788.10276799999997</v>
       </c>
       <c r="AO16" s="15">
         <v>810.61133900000004</v>
@@ -31147,7 +31147,7 @@
         <v>530.45867399999997</v>
       </c>
       <c r="AN17" s="15">
-        <v>634.70223999999996</v>
+        <v>628.191147</v>
       </c>
       <c r="AO17" s="15">
         <v>599.29353600000002</v>
@@ -31308,7 +31308,7 @@
         <v>67.648559000000006</v>
       </c>
       <c r="AN18" s="15">
-        <v>72.163685000000001</v>
+        <v>71.646172000000007</v>
       </c>
       <c r="AO18" s="15">
         <v>71.428331</v>
@@ -31469,7 +31469,7 @@
         <v>420.53968200000003</v>
       </c>
       <c r="AN19" s="15">
-        <v>424.03746799999999</v>
+        <v>424.03642300000001</v>
       </c>
       <c r="AO19" s="15">
         <v>418.30478599999998</v>
@@ -31630,7 +31630,7 @@
         <v>1355.807564</v>
       </c>
       <c r="AN20" s="15">
-        <v>1502.291872</v>
+        <v>1494.2954850000001</v>
       </c>
       <c r="AO20" s="15">
         <v>1466.612709</v>
@@ -31791,7 +31791,7 @@
         <v>975.61884799999996</v>
       </c>
       <c r="AN21" s="15">
-        <v>904.89198199999998</v>
+        <v>903.24244299999998</v>
       </c>
       <c r="AO21" s="15">
         <v>940.44672600000001</v>
@@ -31952,7 +31952,7 @@
         <v>4612.9674130000003</v>
       </c>
       <c r="AN22" s="7">
-        <v>4752.2852700000003</v>
+        <v>4735.2055909999999</v>
       </c>
       <c r="AO22" s="7">
         <v>4759.9631570000001</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Oct  8 05:25:59 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E38FFF2-3B16-4641-BD5F-8CF4680EFFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD1871B-4609-49F5-834E-F43BE7F7A5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3977,7 +3977,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4497,7 +4497,7 @@
         <v>5623</v>
       </c>
       <c r="AO5" s="15">
-        <v>0</v>
+        <v>5436</v>
       </c>
       <c r="AP5" s="15">
         <v>0</v>
@@ -4659,7 +4659,7 @@
         <v>12013</v>
       </c>
       <c r="AO6" s="6">
-        <v>0</v>
+        <v>12217</v>
       </c>
       <c r="AP6" s="6">
         <v>0</v>
@@ -4821,7 +4821,7 @@
         <v>18814</v>
       </c>
       <c r="AO7" s="6">
-        <v>0</v>
+        <v>18962</v>
       </c>
       <c r="AP7" s="6">
         <v>0</v>
@@ -4983,7 +4983,7 @@
         <v>4409</v>
       </c>
       <c r="AO8" s="6">
-        <v>0</v>
+        <v>4362</v>
       </c>
       <c r="AP8" s="6">
         <v>0</v>
@@ -5145,7 +5145,7 @@
         <v>9396</v>
       </c>
       <c r="AO9" s="6">
-        <v>0</v>
+        <v>9248</v>
       </c>
       <c r="AP9" s="6">
         <v>0</v>
@@ -5307,7 +5307,7 @@
         <v>15780</v>
       </c>
       <c r="AO10" s="15">
-        <v>0</v>
+        <v>15045</v>
       </c>
       <c r="AP10" s="15">
         <v>0</v>
@@ -5469,7 +5469,7 @@
         <v>41442</v>
       </c>
       <c r="AO11" s="6">
-        <v>0</v>
+        <v>39909</v>
       </c>
       <c r="AP11" s="6">
         <v>0</v>
@@ -5631,7 +5631,7 @@
         <v>107477</v>
       </c>
       <c r="AO12" s="7">
-        <v>0</v>
+        <v>105179</v>
       </c>
       <c r="AP12" s="7">
         <v>0</v>
@@ -5855,7 +5855,7 @@
         <v>428.208324</v>
       </c>
       <c r="AO15" s="15">
-        <v>0</v>
+        <v>393.90864299999998</v>
       </c>
       <c r="AP15" s="15">
         <v>0</v>
@@ -6017,7 +6017,7 @@
         <v>882.51763200000005</v>
       </c>
       <c r="AO16" s="6">
-        <v>0</v>
+        <v>888.39569100000006</v>
       </c>
       <c r="AP16" s="6">
         <v>0</v>
@@ -6179,7 +6179,7 @@
         <v>477.66669899999999</v>
       </c>
       <c r="AO17" s="6">
-        <v>0</v>
+        <v>548.23373700000002</v>
       </c>
       <c r="AP17" s="6">
         <v>0</v>
@@ -6341,7 +6341,7 @@
         <v>62.525210999999999</v>
       </c>
       <c r="AO18" s="6">
-        <v>0</v>
+        <v>67.510356000000002</v>
       </c>
       <c r="AP18" s="6">
         <v>0</v>
@@ -6503,7 +6503,7 @@
         <v>417.123761</v>
       </c>
       <c r="AO19" s="6">
-        <v>0</v>
+        <v>412.70193799999998</v>
       </c>
       <c r="AP19" s="6">
         <v>0</v>
@@ -6665,7 +6665,7 @@
         <v>1449.538268</v>
       </c>
       <c r="AO20" s="15">
-        <v>0</v>
+        <v>1334.407504</v>
       </c>
       <c r="AP20" s="15">
         <v>0</v>
@@ -6827,7 +6827,7 @@
         <v>1014.4135649999999</v>
       </c>
       <c r="AO21" s="6">
-        <v>0</v>
+        <v>914.81456800000001</v>
       </c>
       <c r="AP21" s="6">
         <v>0</v>
@@ -6989,7 +6989,7 @@
         <v>4731.9934599999997</v>
       </c>
       <c r="AO22" s="7">
-        <v>0</v>
+        <v>4559.9724369999994</v>
       </c>
       <c r="AP22" s="7">
         <v>0</v>
@@ -25870,7 +25870,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28961,7 +28961,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29480,7 +29480,7 @@
         <v>5774</v>
       </c>
       <c r="AO5" s="15">
-        <v>5957</v>
+        <v>5962</v>
       </c>
       <c r="AP5" s="15">
         <v>5566</v>
@@ -29641,7 +29641,7 @@
         <v>11555</v>
       </c>
       <c r="AO6" s="15">
-        <v>11951</v>
+        <v>11942</v>
       </c>
       <c r="AP6" s="15">
         <v>12157</v>
@@ -29802,7 +29802,7 @@
         <v>21137</v>
       </c>
       <c r="AO7" s="15">
-        <v>19934</v>
+        <v>20546</v>
       </c>
       <c r="AP7" s="15">
         <v>18757</v>
@@ -29963,7 +29963,7 @@
         <v>5191</v>
       </c>
       <c r="AO8" s="15">
-        <v>5071</v>
+        <v>5037</v>
       </c>
       <c r="AP8" s="15">
         <v>4641</v>
@@ -30124,7 +30124,7 @@
         <v>9852</v>
       </c>
       <c r="AO9" s="15">
-        <v>10757</v>
+        <v>10587</v>
       </c>
       <c r="AP9" s="15">
         <v>9702</v>
@@ -30285,7 +30285,7 @@
         <v>15094</v>
       </c>
       <c r="AO10" s="15">
-        <v>16251</v>
+        <v>16142</v>
       </c>
       <c r="AP10" s="15">
         <v>15314</v>
@@ -30446,7 +30446,7 @@
         <v>41335</v>
       </c>
       <c r="AO11" s="15">
-        <v>40294</v>
+        <v>40192</v>
       </c>
       <c r="AP11" s="15">
         <v>39331</v>
@@ -30607,7 +30607,7 @@
         <v>109938</v>
       </c>
       <c r="AO12" s="7">
-        <v>110215</v>
+        <v>110408</v>
       </c>
       <c r="AP12" s="7">
         <v>105468</v>
@@ -30828,7 +30828,7 @@
         <v>425.69115299999999</v>
       </c>
       <c r="AO15" s="15">
-        <v>453.26573000000002</v>
+        <v>454.44031799999999</v>
       </c>
       <c r="AP15" s="15">
         <v>415.21233799999999</v>
@@ -30989,7 +30989,7 @@
         <v>788.10276799999997</v>
       </c>
       <c r="AO16" s="15">
-        <v>810.61133900000004</v>
+        <v>810.64133100000004</v>
       </c>
       <c r="AP16" s="15">
         <v>838.05247699999995</v>
@@ -31150,7 +31150,7 @@
         <v>628.191147</v>
       </c>
       <c r="AO17" s="15">
-        <v>599.29353600000002</v>
+        <v>597.15577499999995</v>
       </c>
       <c r="AP17" s="15">
         <v>629.89371700000004</v>
@@ -31311,7 +31311,7 @@
         <v>71.646172000000007</v>
       </c>
       <c r="AO18" s="15">
-        <v>71.428331</v>
+        <v>70.922612000000001</v>
       </c>
       <c r="AP18" s="15">
         <v>61.485888000000003</v>
@@ -31472,7 +31472,7 @@
         <v>424.03642300000001</v>
       </c>
       <c r="AO19" s="15">
-        <v>418.30478599999998</v>
+        <v>407.12536699999998</v>
       </c>
       <c r="AP19" s="15">
         <v>411.84829500000001</v>
@@ -31633,7 +31633,7 @@
         <v>1494.2954850000001</v>
       </c>
       <c r="AO20" s="15">
-        <v>1466.612709</v>
+        <v>1465.01449</v>
       </c>
       <c r="AP20" s="15">
         <v>1505.6943879999999</v>
@@ -31794,7 +31794,7 @@
         <v>903.24244299999998</v>
       </c>
       <c r="AO21" s="15">
-        <v>940.44672600000001</v>
+        <v>938.22674700000005</v>
       </c>
       <c r="AP21" s="15">
         <v>866.54798700000003</v>
@@ -31955,7 +31955,7 @@
         <v>4735.2055909999999</v>
       </c>
       <c r="AO22" s="7">
-        <v>4759.9631570000001</v>
+        <v>4743.52664</v>
       </c>
       <c r="AP22" s="7">
         <v>4728.7350900000001</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Wed Oct 16 05:27:10 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD1871B-4609-49F5-834E-F43BE7F7A5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F102A7-3820-42BC-804F-F8FD36882321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3977,7 +3977,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4500,7 +4500,7 @@
         <v>5436</v>
       </c>
       <c r="AP5" s="15">
-        <v>0</v>
+        <v>5544</v>
       </c>
       <c r="AQ5" s="15">
         <v>0</v>
@@ -4662,7 +4662,7 @@
         <v>12217</v>
       </c>
       <c r="AP6" s="6">
-        <v>0</v>
+        <v>12658</v>
       </c>
       <c r="AQ6" s="6">
         <v>0</v>
@@ -4824,7 +4824,7 @@
         <v>18962</v>
       </c>
       <c r="AP7" s="6">
-        <v>0</v>
+        <v>19635</v>
       </c>
       <c r="AQ7" s="6">
         <v>0</v>
@@ -4986,7 +4986,7 @@
         <v>4362</v>
       </c>
       <c r="AP8" s="6">
-        <v>0</v>
+        <v>4242</v>
       </c>
       <c r="AQ8" s="6">
         <v>0</v>
@@ -5148,7 +5148,7 @@
         <v>9248</v>
       </c>
       <c r="AP9" s="6">
-        <v>0</v>
+        <v>10333</v>
       </c>
       <c r="AQ9" s="6">
         <v>0</v>
@@ -5310,7 +5310,7 @@
         <v>15045</v>
       </c>
       <c r="AP10" s="15">
-        <v>0</v>
+        <v>16014</v>
       </c>
       <c r="AQ10" s="15">
         <v>0</v>
@@ -5472,7 +5472,7 @@
         <v>39909</v>
       </c>
       <c r="AP11" s="6">
-        <v>0</v>
+        <v>40869</v>
       </c>
       <c r="AQ11" s="6">
         <v>0</v>
@@ -5634,7 +5634,7 @@
         <v>105179</v>
       </c>
       <c r="AP12" s="7">
-        <v>0</v>
+        <v>109295</v>
       </c>
       <c r="AQ12" s="7">
         <v>0</v>
@@ -5858,7 +5858,7 @@
         <v>393.90864299999998</v>
       </c>
       <c r="AP15" s="15">
-        <v>0</v>
+        <v>425.80954500000001</v>
       </c>
       <c r="AQ15" s="15">
         <v>0</v>
@@ -6020,7 +6020,7 @@
         <v>888.39569100000006</v>
       </c>
       <c r="AP16" s="6">
-        <v>0</v>
+        <v>959.89508499999999</v>
       </c>
       <c r="AQ16" s="6">
         <v>0</v>
@@ -6182,7 +6182,7 @@
         <v>548.23373700000002</v>
       </c>
       <c r="AP17" s="6">
-        <v>0</v>
+        <v>427.00622299999998</v>
       </c>
       <c r="AQ17" s="6">
         <v>0</v>
@@ -6344,7 +6344,7 @@
         <v>67.510356000000002</v>
       </c>
       <c r="AP18" s="6">
-        <v>0</v>
+        <v>69.146095000000003</v>
       </c>
       <c r="AQ18" s="6">
         <v>0</v>
@@ -6506,7 +6506,7 @@
         <v>412.70193799999998</v>
       </c>
       <c r="AP19" s="6">
-        <v>0</v>
+        <v>433.769948</v>
       </c>
       <c r="AQ19" s="6">
         <v>0</v>
@@ -6668,7 +6668,7 @@
         <v>1334.407504</v>
       </c>
       <c r="AP20" s="15">
-        <v>0</v>
+        <v>1497.982735</v>
       </c>
       <c r="AQ20" s="15">
         <v>0</v>
@@ -6830,7 +6830,7 @@
         <v>914.81456800000001</v>
       </c>
       <c r="AP21" s="6">
-        <v>0</v>
+        <v>965.27094</v>
       </c>
       <c r="AQ21" s="6">
         <v>0</v>
@@ -6992,7 +6992,7 @@
         <v>4559.9724369999994</v>
       </c>
       <c r="AP22" s="7">
-        <v>0</v>
+        <v>4778.8805710000006</v>
       </c>
       <c r="AQ22" s="7">
         <v>0</v>
@@ -28961,7 +28961,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29483,7 +29483,7 @@
         <v>5962</v>
       </c>
       <c r="AP5" s="15">
-        <v>5566</v>
+        <v>5589</v>
       </c>
       <c r="AQ5" s="15">
         <v>5523</v>
@@ -29644,7 +29644,7 @@
         <v>11942</v>
       </c>
       <c r="AP6" s="15">
-        <v>12157</v>
+        <v>12118</v>
       </c>
       <c r="AQ6" s="15">
         <v>12298</v>
@@ -29805,7 +29805,7 @@
         <v>20546</v>
       </c>
       <c r="AP7" s="15">
-        <v>18757</v>
+        <v>19481</v>
       </c>
       <c r="AQ7" s="15">
         <v>19523</v>
@@ -29966,7 +29966,7 @@
         <v>5037</v>
       </c>
       <c r="AP8" s="15">
-        <v>4641</v>
+        <v>4635</v>
       </c>
       <c r="AQ8" s="15">
         <v>4911</v>
@@ -30127,7 +30127,7 @@
         <v>10587</v>
       </c>
       <c r="AP9" s="15">
-        <v>9702</v>
+        <v>9648</v>
       </c>
       <c r="AQ9" s="15">
         <v>9486</v>
@@ -30288,7 +30288,7 @@
         <v>16142</v>
       </c>
       <c r="AP10" s="15">
-        <v>15314</v>
+        <v>15318</v>
       </c>
       <c r="AQ10" s="15">
         <v>16412</v>
@@ -30449,7 +30449,7 @@
         <v>40192</v>
       </c>
       <c r="AP11" s="15">
-        <v>39331</v>
+        <v>39274</v>
       </c>
       <c r="AQ11" s="15">
         <v>41162</v>
@@ -30610,7 +30610,7 @@
         <v>110408</v>
       </c>
       <c r="AP12" s="7">
-        <v>105468</v>
+        <v>106063</v>
       </c>
       <c r="AQ12" s="7">
         <v>109315</v>
@@ -30831,7 +30831,7 @@
         <v>454.44031799999999</v>
       </c>
       <c r="AP15" s="15">
-        <v>415.21233799999999</v>
+        <v>415.06086499999998</v>
       </c>
       <c r="AQ15" s="15">
         <v>436.81901599999998</v>
@@ -30992,7 +30992,7 @@
         <v>810.64133100000004</v>
       </c>
       <c r="AP16" s="15">
-        <v>838.05247699999995</v>
+        <v>837.08477300000004</v>
       </c>
       <c r="AQ16" s="15">
         <v>839.25483699999995</v>
@@ -31153,7 +31153,7 @@
         <v>597.15577499999995</v>
       </c>
       <c r="AP17" s="15">
-        <v>629.89371700000004</v>
+        <v>628.27750200000003</v>
       </c>
       <c r="AQ17" s="15">
         <v>573.95665799999995</v>
@@ -31314,7 +31314,7 @@
         <v>70.922612000000001</v>
       </c>
       <c r="AP18" s="15">
-        <v>61.485888000000003</v>
+        <v>61.308174000000001</v>
       </c>
       <c r="AQ18" s="15">
         <v>77.333590999999998</v>
@@ -31475,7 +31475,7 @@
         <v>407.12536699999998</v>
       </c>
       <c r="AP19" s="15">
-        <v>411.84829500000001</v>
+        <v>411.70982900000001</v>
       </c>
       <c r="AQ19" s="15">
         <v>420.31390699999997</v>
@@ -31636,7 +31636,7 @@
         <v>1465.01449</v>
       </c>
       <c r="AP20" s="15">
-        <v>1505.6943879999999</v>
+        <v>1506.9180739999999</v>
       </c>
       <c r="AQ20" s="15">
         <v>1569.0897210000001</v>
@@ -31797,7 +31797,7 @@
         <v>938.22674700000005</v>
       </c>
       <c r="AP21" s="15">
-        <v>866.54798700000003</v>
+        <v>864.74065099999996</v>
       </c>
       <c r="AQ21" s="15">
         <v>911.84274600000003</v>
@@ -31958,7 +31958,7 @@
         <v>4743.52664</v>
       </c>
       <c r="AP22" s="7">
-        <v>4728.7350900000001</v>
+        <v>4725.0998680000002</v>
       </c>
       <c r="AQ22" s="7">
         <v>4828.6104760000007</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Oct 22 05:26:32 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F102A7-3820-42BC-804F-F8FD36882321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECC8B5A-93CC-4B4F-8C87-AFFCBD9EA148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3977,7 +3977,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
+      <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4503,7 +4503,7 @@
         <v>5544</v>
       </c>
       <c r="AQ5" s="15">
-        <v>0</v>
+        <v>5571</v>
       </c>
       <c r="AR5" s="15">
         <v>0</v>
@@ -4665,7 +4665,7 @@
         <v>12658</v>
       </c>
       <c r="AQ6" s="6">
-        <v>0</v>
+        <v>12243</v>
       </c>
       <c r="AR6" s="6">
         <v>0</v>
@@ -4827,7 +4827,7 @@
         <v>19635</v>
       </c>
       <c r="AQ7" s="6">
-        <v>0</v>
+        <v>17628</v>
       </c>
       <c r="AR7" s="6">
         <v>0</v>
@@ -4989,7 +4989,7 @@
         <v>4242</v>
       </c>
       <c r="AQ8" s="6">
-        <v>0</v>
+        <v>3820</v>
       </c>
       <c r="AR8" s="6">
         <v>0</v>
@@ -5151,7 +5151,7 @@
         <v>10333</v>
       </c>
       <c r="AQ9" s="6">
-        <v>0</v>
+        <v>9998</v>
       </c>
       <c r="AR9" s="6">
         <v>0</v>
@@ -5313,7 +5313,7 @@
         <v>16014</v>
       </c>
       <c r="AQ10" s="15">
-        <v>0</v>
+        <v>15106</v>
       </c>
       <c r="AR10" s="15">
         <v>0</v>
@@ -5475,7 +5475,7 @@
         <v>40869</v>
       </c>
       <c r="AQ11" s="6">
-        <v>0</v>
+        <v>39108</v>
       </c>
       <c r="AR11" s="6">
         <v>0</v>
@@ -5637,7 +5637,7 @@
         <v>109295</v>
       </c>
       <c r="AQ12" s="7">
-        <v>0</v>
+        <v>103474</v>
       </c>
       <c r="AR12" s="7">
         <v>0</v>
@@ -5861,7 +5861,7 @@
         <v>425.80954500000001</v>
       </c>
       <c r="AQ15" s="15">
-        <v>0</v>
+        <v>417.67195299999997</v>
       </c>
       <c r="AR15" s="15">
         <v>0</v>
@@ -6023,7 +6023,7 @@
         <v>959.89508499999999</v>
       </c>
       <c r="AQ16" s="6">
-        <v>0</v>
+        <v>874.09404300000006</v>
       </c>
       <c r="AR16" s="6">
         <v>0</v>
@@ -6185,7 +6185,7 @@
         <v>427.00622299999998</v>
       </c>
       <c r="AQ17" s="6">
-        <v>0</v>
+        <v>519.33369800000003</v>
       </c>
       <c r="AR17" s="6">
         <v>0</v>
@@ -6347,7 +6347,7 @@
         <v>69.146095000000003</v>
       </c>
       <c r="AQ18" s="6">
-        <v>0</v>
+        <v>54.156249000000003</v>
       </c>
       <c r="AR18" s="6">
         <v>0</v>
@@ -6509,7 +6509,7 @@
         <v>433.769948</v>
       </c>
       <c r="AQ19" s="6">
-        <v>0</v>
+        <v>432.83984700000002</v>
       </c>
       <c r="AR19" s="6">
         <v>0</v>
@@ -6671,7 +6671,7 @@
         <v>1497.982735</v>
       </c>
       <c r="AQ20" s="15">
-        <v>0</v>
+        <v>1352.5772730000001</v>
       </c>
       <c r="AR20" s="15">
         <v>0</v>
@@ -6833,7 +6833,7 @@
         <v>965.27094</v>
       </c>
       <c r="AQ21" s="6">
-        <v>0</v>
+        <v>917.04974700000002</v>
       </c>
       <c r="AR21" s="6">
         <v>0</v>
@@ -6995,7 +6995,7 @@
         <v>4778.8805710000006</v>
       </c>
       <c r="AQ22" s="7">
-        <v>0</v>
+        <v>4567.7228100000002</v>
       </c>
       <c r="AR22" s="7">
         <v>0</v>
@@ -25870,7 +25870,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28961,7 +28961,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29486,7 +29486,7 @@
         <v>5589</v>
       </c>
       <c r="AQ5" s="15">
-        <v>5523</v>
+        <v>5510</v>
       </c>
       <c r="AR5" s="15">
         <v>5652</v>
@@ -29647,7 +29647,7 @@
         <v>12118</v>
       </c>
       <c r="AQ6" s="15">
-        <v>12298</v>
+        <v>12285</v>
       </c>
       <c r="AR6" s="15">
         <v>12390</v>
@@ -29808,7 +29808,7 @@
         <v>19481</v>
       </c>
       <c r="AQ7" s="15">
-        <v>19523</v>
+        <v>20581</v>
       </c>
       <c r="AR7" s="15">
         <v>18243</v>
@@ -29969,7 +29969,7 @@
         <v>4635</v>
       </c>
       <c r="AQ8" s="15">
-        <v>4911</v>
+        <v>4862</v>
       </c>
       <c r="AR8" s="15">
         <v>4989</v>
@@ -30130,7 +30130,7 @@
         <v>9648</v>
       </c>
       <c r="AQ9" s="15">
-        <v>9486</v>
+        <v>9484</v>
       </c>
       <c r="AR9" s="15">
         <v>9440</v>
@@ -30291,7 +30291,7 @@
         <v>15318</v>
       </c>
       <c r="AQ10" s="15">
-        <v>16412</v>
+        <v>16368</v>
       </c>
       <c r="AR10" s="15">
         <v>14915</v>
@@ -30452,7 +30452,7 @@
         <v>39274</v>
       </c>
       <c r="AQ11" s="15">
-        <v>41162</v>
+        <v>41043</v>
       </c>
       <c r="AR11" s="15">
         <v>39252</v>
@@ -30613,7 +30613,7 @@
         <v>106063</v>
       </c>
       <c r="AQ12" s="7">
-        <v>109315</v>
+        <v>110133</v>
       </c>
       <c r="AR12" s="7">
         <v>104881</v>
@@ -30834,7 +30834,7 @@
         <v>415.06086499999998</v>
       </c>
       <c r="AQ15" s="15">
-        <v>436.81901599999998</v>
+        <v>435.95195100000001</v>
       </c>
       <c r="AR15" s="15">
         <v>413.95728000000003</v>
@@ -30995,7 +30995,7 @@
         <v>837.08477300000004</v>
       </c>
       <c r="AQ16" s="15">
-        <v>839.25483699999995</v>
+        <v>838.33325200000002</v>
       </c>
       <c r="AR16" s="15">
         <v>883.51841200000001</v>
@@ -31156,7 +31156,7 @@
         <v>628.27750200000003</v>
       </c>
       <c r="AQ17" s="15">
-        <v>573.95665799999995</v>
+        <v>572.18091500000003</v>
       </c>
       <c r="AR17" s="15">
         <v>574.248606</v>
@@ -31317,7 +31317,7 @@
         <v>61.308174000000001</v>
       </c>
       <c r="AQ18" s="15">
-        <v>77.333590999999998</v>
+        <v>75.853785000000002</v>
       </c>
       <c r="AR18" s="15">
         <v>71.167961000000005</v>
@@ -31478,7 +31478,7 @@
         <v>411.70982900000001</v>
       </c>
       <c r="AQ19" s="15">
-        <v>420.31390699999997</v>
+        <v>420.22598299999999</v>
       </c>
       <c r="AR19" s="15">
         <v>422.05681900000002</v>
@@ -31639,7 +31639,7 @@
         <v>1506.9180739999999</v>
       </c>
       <c r="AQ20" s="15">
-        <v>1569.0897210000001</v>
+        <v>1567.263457</v>
       </c>
       <c r="AR20" s="15">
         <v>1541.593351</v>
@@ -31800,7 +31800,7 @@
         <v>864.74065099999996</v>
       </c>
       <c r="AQ21" s="15">
-        <v>911.84274600000003</v>
+        <v>910.33158900000001</v>
       </c>
       <c r="AR21" s="15">
         <v>924.635896</v>
@@ -31961,7 +31961,7 @@
         <v>4725.0998680000002</v>
       </c>
       <c r="AQ22" s="7">
-        <v>4828.6104760000007</v>
+        <v>4820.1409320000002</v>
       </c>
       <c r="AR22" s="7">
         <v>4831.1783249999999</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Oct 29 05:27:24 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECC8B5A-93CC-4B4F-8C87-AFFCBD9EA148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FD62A45-6C8D-48B1-AC87-191938E8790F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -919,19 +919,19 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="9"/>
+    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1310,12 +1310,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2658,12 +2658,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -3977,19 +3977,19 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.42578125" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.44140625" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4046,7 +4046,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4369,13 +4369,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>5571</v>
       </c>
       <c r="AR5" s="15">
-        <v>0</v>
+        <v>5637</v>
       </c>
       <c r="AS5" s="15">
         <v>0</v>
@@ -4537,7 +4537,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>12243</v>
       </c>
       <c r="AR6" s="6">
-        <v>0</v>
+        <v>12046</v>
       </c>
       <c r="AS6" s="6">
         <v>0</v>
@@ -4699,7 +4699,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4830,7 +4830,7 @@
         <v>17628</v>
       </c>
       <c r="AR7" s="6">
-        <v>0</v>
+        <v>20312</v>
       </c>
       <c r="AS7" s="6">
         <v>0</v>
@@ -4861,7 +4861,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>3820</v>
       </c>
       <c r="AR8" s="6">
-        <v>0</v>
+        <v>4335</v>
       </c>
       <c r="AS8" s="6">
         <v>0</v>
@@ -5023,7 +5023,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>9998</v>
       </c>
       <c r="AR9" s="6">
-        <v>0</v>
+        <v>7366</v>
       </c>
       <c r="AS9" s="6">
         <v>0</v>
@@ -5185,7 +5185,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>15106</v>
       </c>
       <c r="AR10" s="15">
-        <v>0</v>
+        <v>16441</v>
       </c>
       <c r="AS10" s="15">
         <v>0</v>
@@ -5347,7 +5347,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>39108</v>
       </c>
       <c r="AR11" s="6">
-        <v>0</v>
+        <v>43549</v>
       </c>
       <c r="AS11" s="6">
         <v>0</v>
@@ -5509,7 +5509,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>103474</v>
       </c>
       <c r="AR12" s="7">
-        <v>0</v>
+        <v>109686</v>
       </c>
       <c r="AS12" s="7">
         <v>0</v>
@@ -5671,7 +5671,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5727,13 +5727,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>417.67195299999997</v>
       </c>
       <c r="AR15" s="15">
-        <v>0</v>
+        <v>426.85339299999998</v>
       </c>
       <c r="AS15" s="15">
         <v>0</v>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>874.09404300000006</v>
       </c>
       <c r="AR16" s="6">
-        <v>0</v>
+        <v>878.838978</v>
       </c>
       <c r="AS16" s="6">
         <v>0</v>
@@ -6057,7 +6057,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>519.33369800000003</v>
       </c>
       <c r="AR17" s="6">
-        <v>0</v>
+        <v>526.36218899999994</v>
       </c>
       <c r="AS17" s="6">
         <v>0</v>
@@ -6219,7 +6219,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6350,7 +6350,7 @@
         <v>54.156249000000003</v>
       </c>
       <c r="AR18" s="6">
-        <v>0</v>
+        <v>66.348393000000002</v>
       </c>
       <c r="AS18" s="6">
         <v>0</v>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v>432.83984700000002</v>
       </c>
       <c r="AR19" s="6">
-        <v>0</v>
+        <v>307.04768899999999</v>
       </c>
       <c r="AS19" s="6">
         <v>0</v>
@@ -6543,7 +6543,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>1352.5772730000001</v>
       </c>
       <c r="AR20" s="15">
-        <v>0</v>
+        <v>1531.614065</v>
       </c>
       <c r="AS20" s="15">
         <v>0</v>
@@ -6705,7 +6705,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6836,7 +6836,7 @@
         <v>917.04974700000002</v>
       </c>
       <c r="AR21" s="6">
-        <v>0</v>
+        <v>1013.434178</v>
       </c>
       <c r="AS21" s="6">
         <v>0</v>
@@ -6867,7 +6867,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6998,7 +6998,7 @@
         <v>4567.7228100000002</v>
       </c>
       <c r="AR22" s="7">
-        <v>0</v>
+        <v>4750.4988849999991</v>
       </c>
       <c r="AS22" s="7">
         <v>0</v>
@@ -7029,100 +7029,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -7137,6 +7137,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -7149,19 +7152,19 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="17"/>
+    <col min="54" max="16384" width="6.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -7218,7 +7221,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7379,7 +7382,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7541,12 +7544,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7707,7 +7710,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7868,7 +7871,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -8029,7 +8032,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8190,7 +8193,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8351,7 +8354,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8512,7 +8515,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8673,7 +8676,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8834,7 +8837,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8889,12 +8892,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -9055,7 +9058,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9216,7 +9219,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9377,7 +9380,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9538,7 +9541,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9699,7 +9702,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9860,7 +9863,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -10021,7 +10024,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10182,38 +10185,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -10236,22 +10239,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -10308,7 +10311,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10469,7 +10472,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10630,12 +10633,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10796,7 +10799,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -10957,7 +10960,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11118,7 +11121,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11279,7 +11282,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11440,7 +11443,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11601,7 +11604,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11762,7 +11765,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11923,7 +11926,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -11978,12 +11981,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12144,7 +12147,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12305,7 +12308,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12466,7 +12469,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12627,7 +12630,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12788,7 +12791,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -12949,7 +12952,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13110,7 +13113,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13271,38 +13274,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13324,19 +13327,19 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -13393,7 +13396,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13554,7 +13557,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13716,12 +13719,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13882,7 +13885,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14043,7 +14046,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14204,7 +14207,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14365,7 +14368,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14526,7 +14529,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14687,7 +14690,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14848,7 +14851,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15009,7 +15012,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15064,12 +15067,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15230,7 +15233,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15391,7 +15394,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15552,7 +15555,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15713,7 +15716,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15874,7 +15877,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16035,7 +16038,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16196,7 +16199,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16357,38 +16360,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16402,19 +16405,19 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -16471,7 +16474,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16632,7 +16635,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16794,12 +16797,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -16960,7 +16963,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17121,7 +17124,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17282,7 +17285,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17443,7 +17446,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17604,7 +17607,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17765,7 +17768,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17926,7 +17929,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18087,7 +18090,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18142,12 +18145,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18308,7 +18311,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18469,7 +18472,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18630,7 +18633,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18791,7 +18794,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -18952,7 +18955,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19113,7 +19116,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19274,7 +19277,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19435,38 +19438,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19480,20 +19483,20 @@
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -19550,7 +19553,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -19714,7 +19717,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -19876,7 +19879,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -20040,12 +20043,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -20209,7 +20212,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -20373,7 +20376,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -20537,7 +20540,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -20701,7 +20704,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -20865,7 +20868,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -21029,7 +21032,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -21193,7 +21196,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -21357,7 +21360,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -21413,12 +21416,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -21582,7 +21585,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -21746,7 +21749,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -21910,7 +21913,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -22074,7 +22077,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -22238,7 +22241,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -22402,7 +22405,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -22566,7 +22569,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -22730,38 +22733,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22776,22 +22779,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -22848,7 +22851,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -23009,7 +23012,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -23171,12 +23174,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -23337,7 +23340,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -23498,7 +23501,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -23659,7 +23662,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -23820,7 +23823,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -23981,7 +23984,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -24142,7 +24145,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -24303,7 +24306,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -24464,7 +24467,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -24519,12 +24522,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -24685,7 +24688,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -24846,7 +24849,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -25007,7 +25010,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -25168,7 +25171,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -25329,7 +25332,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -25490,7 +25493,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -25651,7 +25654,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -25812,40 +25815,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25867,22 +25870,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -25939,7 +25942,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26100,7 +26103,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26262,12 +26265,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26428,7 +26431,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26589,7 +26592,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26750,7 +26753,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26911,7 +26914,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27072,7 +27075,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27233,7 +27236,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27394,7 +27397,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27555,7 +27558,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27610,12 +27613,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27776,7 +27779,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27937,7 +27940,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28098,7 +28101,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28259,7 +28262,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28420,7 +28423,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28581,7 +28584,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28742,7 +28745,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28903,40 +28906,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -28958,22 +28961,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -29030,7 +29033,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29191,7 +29194,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29353,12 +29356,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29489,7 +29492,7 @@
         <v>5510</v>
       </c>
       <c r="AR5" s="15">
-        <v>5652</v>
+        <v>5643</v>
       </c>
       <c r="AS5" s="15">
         <v>6028</v>
@@ -29519,7 +29522,7 @@
         <v>4445</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29650,7 +29653,7 @@
         <v>12285</v>
       </c>
       <c r="AR6" s="15">
-        <v>12390</v>
+        <v>12345</v>
       </c>
       <c r="AS6" s="15">
         <v>12529</v>
@@ -29680,7 +29683,7 @@
         <v>11733</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29811,7 +29814,7 @@
         <v>20581</v>
       </c>
       <c r="AR7" s="15">
-        <v>18243</v>
+        <v>19120</v>
       </c>
       <c r="AS7" s="15">
         <v>19503</v>
@@ -29841,7 +29844,7 @@
         <v>15028</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -29972,7 +29975,7 @@
         <v>4862</v>
       </c>
       <c r="AR8" s="15">
-        <v>4989</v>
+        <v>4983</v>
       </c>
       <c r="AS8" s="15">
         <v>4590</v>
@@ -30002,7 +30005,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30133,7 +30136,7 @@
         <v>9484</v>
       </c>
       <c r="AR9" s="15">
-        <v>9440</v>
+        <v>9444</v>
       </c>
       <c r="AS9" s="15">
         <v>10443</v>
@@ -30163,7 +30166,7 @@
         <v>8123</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30294,7 +30297,7 @@
         <v>16368</v>
       </c>
       <c r="AR10" s="15">
-        <v>14915</v>
+        <v>14930</v>
       </c>
       <c r="AS10" s="15">
         <v>15310</v>
@@ -30324,7 +30327,7 @@
         <v>9903</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30455,7 +30458,7 @@
         <v>41043</v>
       </c>
       <c r="AR11" s="15">
-        <v>39252</v>
+        <v>39158</v>
       </c>
       <c r="AS11" s="15">
         <v>36679</v>
@@ -30485,7 +30488,7 @@
         <v>34137</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30616,7 +30619,7 @@
         <v>110133</v>
       </c>
       <c r="AR12" s="7">
-        <v>104881</v>
+        <v>105623</v>
       </c>
       <c r="AS12" s="7">
         <v>105082</v>
@@ -30646,7 +30649,7 @@
         <v>85879</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30701,12 +30704,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30837,7 +30840,7 @@
         <v>435.95195100000001</v>
       </c>
       <c r="AR15" s="15">
-        <v>413.95728000000003</v>
+        <v>413.19035400000001</v>
       </c>
       <c r="AS15" s="15">
         <v>447.052076</v>
@@ -30867,7 +30870,7 @@
         <v>299.51857200000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -30998,7 +31001,7 @@
         <v>838.33325200000002</v>
       </c>
       <c r="AR16" s="15">
-        <v>883.51841200000001</v>
+        <v>879.88279499999999</v>
       </c>
       <c r="AS16" s="15">
         <v>894.59904400000005</v>
@@ -31028,7 +31031,7 @@
         <v>889.37489700000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31159,7 +31162,7 @@
         <v>572.18091500000003</v>
       </c>
       <c r="AR17" s="15">
-        <v>574.248606</v>
+        <v>572.46850099999995</v>
       </c>
       <c r="AS17" s="15">
         <v>535.51196000000004</v>
@@ -31189,7 +31192,7 @@
         <v>534.04841199999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31320,7 +31323,7 @@
         <v>75.853785000000002</v>
       </c>
       <c r="AR18" s="15">
-        <v>71.167961000000005</v>
+        <v>71.025507000000005</v>
       </c>
       <c r="AS18" s="15">
         <v>65.691602000000003</v>
@@ -31350,7 +31353,7 @@
         <v>38.940157999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31481,7 +31484,7 @@
         <v>420.22598299999999</v>
       </c>
       <c r="AR19" s="15">
-        <v>422.05681900000002</v>
+        <v>422.15675099999999</v>
       </c>
       <c r="AS19" s="15">
         <v>466.18692499999997</v>
@@ -31511,7 +31514,7 @@
         <v>363.77720699999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31642,7 +31645,7 @@
         <v>1567.263457</v>
       </c>
       <c r="AR20" s="15">
-        <v>1541.593351</v>
+        <v>1545.036443</v>
       </c>
       <c r="AS20" s="15">
         <v>1507.2264929999999</v>
@@ -31672,7 +31675,7 @@
         <v>993.71548499999994</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31803,7 +31806,7 @@
         <v>910.33158900000001</v>
       </c>
       <c r="AR21" s="15">
-        <v>924.635896</v>
+        <v>923.15671699999996</v>
       </c>
       <c r="AS21" s="15">
         <v>760.97466899999995</v>
@@ -31833,7 +31836,7 @@
         <v>756.39903700000002</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -31964,7 +31967,7 @@
         <v>4820.1409320000002</v>
       </c>
       <c r="AR22" s="7">
-        <v>4831.1783249999999</v>
+        <v>4826.9170679999997</v>
       </c>
       <c r="AS22" s="7">
         <v>4677.2427690000004</v>
@@ -31994,40 +31997,40 @@
         <v>3875.773768</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32040,5 +32043,8 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GH ACTION Autorun Tue Nov  5 05:26:28 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FD62A45-6C8D-48B1-AC87-191938E8790F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFDDC1D-2FDD-49E7-A18A-BDDACEC7EEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -919,19 +919,19 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="9"/>
+    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1310,12 +1310,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2658,12 +2658,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -3977,19 +3977,19 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.44140625" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.42578125" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4046,7 +4046,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4369,13 +4369,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>5637</v>
       </c>
       <c r="AS5" s="15">
-        <v>0</v>
+        <v>5675</v>
       </c>
       <c r="AT5" s="15">
         <v>0</v>
@@ -4537,7 +4537,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>12046</v>
       </c>
       <c r="AS6" s="6">
-        <v>0</v>
+        <v>12635</v>
       </c>
       <c r="AT6" s="6">
         <v>0</v>
@@ -4699,7 +4699,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>20312</v>
       </c>
       <c r="AS7" s="6">
-        <v>0</v>
+        <v>19109</v>
       </c>
       <c r="AT7" s="6">
         <v>0</v>
@@ -4861,7 +4861,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>4335</v>
       </c>
       <c r="AS8" s="6">
-        <v>0</v>
+        <v>3788</v>
       </c>
       <c r="AT8" s="6">
         <v>0</v>
@@ -5023,7 +5023,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>7366</v>
       </c>
       <c r="AS9" s="6">
-        <v>0</v>
+        <v>9428</v>
       </c>
       <c r="AT9" s="6">
         <v>0</v>
@@ -5185,7 +5185,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>16441</v>
       </c>
       <c r="AS10" s="15">
-        <v>0</v>
+        <v>16277</v>
       </c>
       <c r="AT10" s="15">
         <v>0</v>
@@ -5347,7 +5347,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>43549</v>
       </c>
       <c r="AS11" s="6">
-        <v>0</v>
+        <v>41497</v>
       </c>
       <c r="AT11" s="6">
         <v>0</v>
@@ -5509,7 +5509,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>109686</v>
       </c>
       <c r="AS12" s="7">
-        <v>0</v>
+        <v>108409</v>
       </c>
       <c r="AT12" s="7">
         <v>0</v>
@@ -5671,7 +5671,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5727,13 +5727,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>426.85339299999998</v>
       </c>
       <c r="AS15" s="15">
-        <v>0</v>
+        <v>423.848096</v>
       </c>
       <c r="AT15" s="15">
         <v>0</v>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>878.838978</v>
       </c>
       <c r="AS16" s="6">
-        <v>0</v>
+        <v>906.96721200000002</v>
       </c>
       <c r="AT16" s="6">
         <v>0</v>
@@ -6057,7 +6057,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>526.36218899999994</v>
       </c>
       <c r="AS17" s="6">
-        <v>0</v>
+        <v>568.45972600000005</v>
       </c>
       <c r="AT17" s="6">
         <v>0</v>
@@ -6219,7 +6219,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>66.348393000000002</v>
       </c>
       <c r="AS18" s="6">
-        <v>0</v>
+        <v>54.787115</v>
       </c>
       <c r="AT18" s="6">
         <v>0</v>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6515,7 +6515,7 @@
         <v>307.04768899999999</v>
       </c>
       <c r="AS19" s="6">
-        <v>0</v>
+        <v>447.829408</v>
       </c>
       <c r="AT19" s="6">
         <v>0</v>
@@ -6543,7 +6543,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6677,7 +6677,7 @@
         <v>1531.614065</v>
       </c>
       <c r="AS20" s="15">
-        <v>0</v>
+        <v>1490.1352489999999</v>
       </c>
       <c r="AT20" s="15">
         <v>0</v>
@@ -6705,7 +6705,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>1013.434178</v>
       </c>
       <c r="AS21" s="6">
-        <v>0</v>
+        <v>945.84492</v>
       </c>
       <c r="AT21" s="6">
         <v>0</v>
@@ -6867,7 +6867,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>4750.4988849999991</v>
       </c>
       <c r="AS22" s="7">
-        <v>0</v>
+        <v>4837.8717259999994</v>
       </c>
       <c r="AT22" s="7">
         <v>0</v>
@@ -7029,100 +7029,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -7137,9 +7137,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -7152,19 +7149,19 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="17"/>
+    <col min="54" max="16384" width="6.7109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -7221,7 +7218,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7382,7 +7379,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7544,12 +7541,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7710,7 +7707,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7871,7 +7868,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -8032,7 +8029,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8193,7 +8190,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8354,7 +8351,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8515,7 +8512,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8676,7 +8673,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8837,7 +8834,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8892,12 +8889,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -9058,7 +9055,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9219,7 +9216,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9380,7 +9377,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9541,7 +9538,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9702,7 +9699,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9863,7 +9860,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -10024,7 +10021,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10185,38 +10182,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -10239,22 +10236,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -10311,7 +10308,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10472,7 +10469,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10633,12 +10630,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10799,7 +10796,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -10960,7 +10957,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11121,7 +11118,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11282,7 +11279,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11443,7 +11440,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11604,7 +11601,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11765,7 +11762,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11926,7 +11923,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -11981,12 +11978,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12147,7 +12144,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12308,7 +12305,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12469,7 +12466,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12630,7 +12627,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12791,7 +12788,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -12952,7 +12949,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13113,7 +13110,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13274,38 +13271,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13327,19 +13324,19 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -13396,7 +13393,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13557,7 +13554,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13719,12 +13716,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13885,7 +13882,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14046,7 +14043,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14207,7 +14204,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14368,7 +14365,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14529,7 +14526,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14690,7 +14687,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14851,7 +14848,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15012,7 +15009,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15067,12 +15064,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15233,7 +15230,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15394,7 +15391,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15555,7 +15552,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15716,7 +15713,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15877,7 +15874,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16038,7 +16035,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16199,7 +16196,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16360,38 +16357,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16405,19 +16402,19 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -16474,7 +16471,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16635,7 +16632,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16797,12 +16794,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -16963,7 +16960,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17124,7 +17121,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17285,7 +17282,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17446,7 +17443,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17607,7 +17604,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17768,7 +17765,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17929,7 +17926,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18090,7 +18087,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18145,12 +18142,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18311,7 +18308,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18472,7 +18469,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18633,7 +18630,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18794,7 +18791,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -18955,7 +18952,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19116,7 +19113,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19277,7 +19274,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19438,38 +19435,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19483,20 +19480,20 @@
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -19553,7 +19550,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -19717,7 +19714,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -19879,7 +19876,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -20043,12 +20040,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -20212,7 +20209,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -20376,7 +20373,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -20540,7 +20537,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -20704,7 +20701,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -20868,7 +20865,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -21032,7 +21029,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -21196,7 +21193,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -21360,7 +21357,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -21416,12 +21413,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -21585,7 +21582,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -21749,7 +21746,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -21913,7 +21910,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -22077,7 +22074,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -22241,7 +22238,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -22405,7 +22402,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -22569,7 +22566,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -22733,38 +22730,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22779,22 +22776,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -22851,7 +22848,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -23012,7 +23009,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -23174,12 +23171,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -23340,7 +23337,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -23501,7 +23498,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -23662,7 +23659,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -23823,7 +23820,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -23984,7 +23981,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -24145,7 +24142,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -24306,7 +24303,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -24467,7 +24464,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -24522,12 +24519,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -24688,7 +24685,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -24849,7 +24846,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -25010,7 +25007,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -25171,7 +25168,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -25332,7 +25329,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -25493,7 +25490,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -25654,7 +25651,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -25815,40 +25812,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25870,22 +25867,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -25942,7 +25939,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26103,7 +26100,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26265,12 +26262,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26431,7 +26428,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26592,7 +26589,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26753,7 +26750,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26914,7 +26911,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27075,7 +27072,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27236,7 +27233,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27397,7 +27394,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27558,7 +27555,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27613,12 +27610,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27779,7 +27776,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27940,7 +27937,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28101,7 +28098,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28262,7 +28259,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28423,7 +28420,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28584,7 +28581,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28745,7 +28742,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28906,40 +28903,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -28961,22 +28958,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -29033,7 +29030,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29194,7 +29191,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29356,12 +29353,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29495,7 +29492,7 @@
         <v>5643</v>
       </c>
       <c r="AS5" s="15">
-        <v>6028</v>
+        <v>6013</v>
       </c>
       <c r="AT5" s="15">
         <v>5798</v>
@@ -29522,7 +29519,7 @@
         <v>4445</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29656,7 +29653,7 @@
         <v>12345</v>
       </c>
       <c r="AS6" s="15">
-        <v>12529</v>
+        <v>12521</v>
       </c>
       <c r="AT6" s="15">
         <v>13020</v>
@@ -29683,7 +29680,7 @@
         <v>11733</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29817,7 +29814,7 @@
         <v>19120</v>
       </c>
       <c r="AS7" s="15">
-        <v>19503</v>
+        <v>20252</v>
       </c>
       <c r="AT7" s="15">
         <v>19483</v>
@@ -29844,7 +29841,7 @@
         <v>15028</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -29978,7 +29975,7 @@
         <v>4983</v>
       </c>
       <c r="AS8" s="15">
-        <v>4590</v>
+        <v>4584</v>
       </c>
       <c r="AT8" s="15">
         <v>4727</v>
@@ -30005,7 +30002,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30139,7 +30136,7 @@
         <v>9444</v>
       </c>
       <c r="AS9" s="15">
-        <v>10443</v>
+        <v>10442</v>
       </c>
       <c r="AT9" s="15">
         <v>11367</v>
@@ -30166,7 +30163,7 @@
         <v>8123</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30300,7 +30297,7 @@
         <v>14930</v>
       </c>
       <c r="AS10" s="15">
-        <v>15310</v>
+        <v>15298</v>
       </c>
       <c r="AT10" s="15">
         <v>14332</v>
@@ -30327,7 +30324,7 @@
         <v>9903</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30461,7 +30458,7 @@
         <v>39158</v>
       </c>
       <c r="AS11" s="15">
-        <v>36679</v>
+        <v>36566</v>
       </c>
       <c r="AT11" s="15">
         <v>40038</v>
@@ -30488,7 +30485,7 @@
         <v>34137</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30622,7 +30619,7 @@
         <v>105623</v>
       </c>
       <c r="AS12" s="7">
-        <v>105082</v>
+        <v>105676</v>
       </c>
       <c r="AT12" s="7">
         <v>108765</v>
@@ -30649,7 +30646,7 @@
         <v>85879</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30704,12 +30701,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30843,7 +30840,7 @@
         <v>413.19035400000001</v>
       </c>
       <c r="AS15" s="15">
-        <v>447.052076</v>
+        <v>446.03003200000001</v>
       </c>
       <c r="AT15" s="15">
         <v>431.289469</v>
@@ -30870,7 +30867,7 @@
         <v>299.51857200000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -31004,7 +31001,7 @@
         <v>879.88279499999999</v>
       </c>
       <c r="AS16" s="15">
-        <v>894.59904400000005</v>
+        <v>894.27530200000001</v>
       </c>
       <c r="AT16" s="15">
         <v>946.93562999999995</v>
@@ -31031,7 +31028,7 @@
         <v>889.37489700000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31165,7 +31162,7 @@
         <v>572.46850099999995</v>
       </c>
       <c r="AS17" s="15">
-        <v>535.51196000000004</v>
+        <v>535.38713099999995</v>
       </c>
       <c r="AT17" s="15">
         <v>474.83860800000002</v>
@@ -31192,7 +31189,7 @@
         <v>534.04841199999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31326,7 +31323,7 @@
         <v>71.025507000000005</v>
       </c>
       <c r="AS18" s="15">
-        <v>65.691602000000003</v>
+        <v>65.657144000000002</v>
       </c>
       <c r="AT18" s="15">
         <v>63.640169999999998</v>
@@ -31353,7 +31350,7 @@
         <v>38.940157999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31487,7 +31484,7 @@
         <v>422.15675099999999</v>
       </c>
       <c r="AS19" s="15">
-        <v>466.18692499999997</v>
+        <v>466.16468300000003</v>
       </c>
       <c r="AT19" s="15">
         <v>467.72137600000002</v>
@@ -31514,7 +31511,7 @@
         <v>363.77720699999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31648,7 +31645,7 @@
         <v>1545.036443</v>
       </c>
       <c r="AS20" s="15">
-        <v>1507.2264929999999</v>
+        <v>1507.6246900000001</v>
       </c>
       <c r="AT20" s="15">
         <v>1423.9756070000001</v>
@@ -31675,7 +31672,7 @@
         <v>993.71548499999994</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31809,7 +31806,7 @@
         <v>923.15671699999996</v>
       </c>
       <c r="AS21" s="15">
-        <v>760.97466899999995</v>
+        <v>760.18734400000005</v>
       </c>
       <c r="AT21" s="15">
         <v>965.85286299999996</v>
@@ -31836,7 +31833,7 @@
         <v>756.39903700000002</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -31970,7 +31967,7 @@
         <v>4826.9170679999997</v>
       </c>
       <c r="AS22" s="7">
-        <v>4677.2427690000004</v>
+        <v>4675.3263260000003</v>
       </c>
       <c r="AT22" s="7">
         <v>4774.2537229999998</v>
@@ -31997,40 +31994,40 @@
         <v>3875.773768</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32043,8 +32040,5 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GH ACTION Autorun Wed Nov 13 05:26:36 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFDDC1D-2FDD-49E7-A18A-BDDACEC7EEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0CC44D-4E38-44D9-B99C-7C333CE6E935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3977,7 +3977,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
+      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4512,7 +4512,7 @@
         <v>5675</v>
       </c>
       <c r="AT5" s="15">
-        <v>0</v>
+        <v>5428</v>
       </c>
       <c r="AU5" s="15">
         <v>0</v>
@@ -4674,7 +4674,7 @@
         <v>12635</v>
       </c>
       <c r="AT6" s="6">
-        <v>0</v>
+        <v>12916</v>
       </c>
       <c r="AU6" s="6">
         <v>0</v>
@@ -4836,7 +4836,7 @@
         <v>19109</v>
       </c>
       <c r="AT7" s="6">
-        <v>0</v>
+        <v>18714</v>
       </c>
       <c r="AU7" s="6">
         <v>0</v>
@@ -4998,7 +4998,7 @@
         <v>3788</v>
       </c>
       <c r="AT8" s="6">
-        <v>0</v>
+        <v>3686</v>
       </c>
       <c r="AU8" s="6">
         <v>0</v>
@@ -5160,7 +5160,7 @@
         <v>9428</v>
       </c>
       <c r="AT9" s="6">
-        <v>0</v>
+        <v>6290</v>
       </c>
       <c r="AU9" s="6">
         <v>0</v>
@@ -5322,7 +5322,7 @@
         <v>16277</v>
       </c>
       <c r="AT10" s="15">
-        <v>0</v>
+        <v>14405</v>
       </c>
       <c r="AU10" s="15">
         <v>0</v>
@@ -5484,7 +5484,7 @@
         <v>41497</v>
       </c>
       <c r="AT11" s="6">
-        <v>0</v>
+        <v>22253</v>
       </c>
       <c r="AU11" s="6">
         <v>0</v>
@@ -5646,7 +5646,7 @@
         <v>108409</v>
       </c>
       <c r="AT12" s="7">
-        <v>0</v>
+        <v>83692</v>
       </c>
       <c r="AU12" s="7">
         <v>0</v>
@@ -5870,7 +5870,7 @@
         <v>423.848096</v>
       </c>
       <c r="AT15" s="15">
-        <v>0</v>
+        <v>431.78306400000002</v>
       </c>
       <c r="AU15" s="15">
         <v>0</v>
@@ -6032,7 +6032,7 @@
         <v>906.96721200000002</v>
       </c>
       <c r="AT16" s="6">
-        <v>0</v>
+        <v>897.10638900000004</v>
       </c>
       <c r="AU16" s="6">
         <v>0</v>
@@ -6194,7 +6194,7 @@
         <v>568.45972600000005</v>
       </c>
       <c r="AT17" s="6">
-        <v>0</v>
+        <v>450.09578199999999</v>
       </c>
       <c r="AU17" s="6">
         <v>0</v>
@@ -6356,7 +6356,7 @@
         <v>54.787115</v>
       </c>
       <c r="AT18" s="6">
-        <v>0</v>
+        <v>53.773249999999997</v>
       </c>
       <c r="AU18" s="6">
         <v>0</v>
@@ -6518,7 +6518,7 @@
         <v>447.829408</v>
       </c>
       <c r="AT19" s="6">
-        <v>0</v>
+        <v>355.663386</v>
       </c>
       <c r="AU19" s="6">
         <v>0</v>
@@ -6680,7 +6680,7 @@
         <v>1490.1352489999999</v>
       </c>
       <c r="AT20" s="15">
-        <v>0</v>
+        <v>1293.599242</v>
       </c>
       <c r="AU20" s="15">
         <v>0</v>
@@ -6842,7 +6842,7 @@
         <v>945.84492</v>
       </c>
       <c r="AT21" s="6">
-        <v>0</v>
+        <v>518.63106200000004</v>
       </c>
       <c r="AU21" s="6">
         <v>0</v>
@@ -7004,7 +7004,7 @@
         <v>4837.8717259999994</v>
       </c>
       <c r="AT22" s="7">
-        <v>0</v>
+        <v>4000.6521749999997</v>
       </c>
       <c r="AU22" s="7">
         <v>0</v>
@@ -28961,7 +28961,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29495,7 +29495,7 @@
         <v>6013</v>
       </c>
       <c r="AT5" s="15">
-        <v>5798</v>
+        <v>5772</v>
       </c>
       <c r="AU5" s="15">
         <v>6285</v>
@@ -29656,7 +29656,7 @@
         <v>12521</v>
       </c>
       <c r="AT6" s="15">
-        <v>13020</v>
+        <v>13002</v>
       </c>
       <c r="AU6" s="15">
         <v>13283</v>
@@ -29817,7 +29817,7 @@
         <v>20252</v>
       </c>
       <c r="AT7" s="15">
-        <v>19483</v>
+        <v>20140</v>
       </c>
       <c r="AU7" s="15">
         <v>19617</v>
@@ -29978,7 +29978,7 @@
         <v>4584</v>
       </c>
       <c r="AT8" s="15">
-        <v>4727</v>
+        <v>4701</v>
       </c>
       <c r="AU8" s="15">
         <v>4921</v>
@@ -30139,7 +30139,7 @@
         <v>10442</v>
       </c>
       <c r="AT9" s="15">
-        <v>11367</v>
+        <v>11366</v>
       </c>
       <c r="AU9" s="15">
         <v>10430</v>
@@ -30300,7 +30300,7 @@
         <v>15298</v>
       </c>
       <c r="AT10" s="15">
-        <v>14332</v>
+        <v>14306</v>
       </c>
       <c r="AU10" s="15">
         <v>14951</v>
@@ -30461,7 +30461,7 @@
         <v>36566</v>
       </c>
       <c r="AT11" s="15">
-        <v>40038</v>
+        <v>39895</v>
       </c>
       <c r="AU11" s="15">
         <v>38254</v>
@@ -30622,7 +30622,7 @@
         <v>105676</v>
       </c>
       <c r="AT12" s="7">
-        <v>108765</v>
+        <v>109182</v>
       </c>
       <c r="AU12" s="7">
         <v>107741</v>
@@ -30843,7 +30843,7 @@
         <v>446.03003200000001</v>
       </c>
       <c r="AT15" s="15">
-        <v>431.289469</v>
+        <v>429.901228</v>
       </c>
       <c r="AU15" s="15">
         <v>469.00431500000002</v>
@@ -31004,7 +31004,7 @@
         <v>894.27530200000001</v>
       </c>
       <c r="AT16" s="15">
-        <v>946.93562999999995</v>
+        <v>946.150037</v>
       </c>
       <c r="AU16" s="15">
         <v>925.71202000000005</v>
@@ -31165,7 +31165,7 @@
         <v>535.38713099999995</v>
       </c>
       <c r="AT17" s="15">
-        <v>474.83860800000002</v>
+        <v>473.34906000000001</v>
       </c>
       <c r="AU17" s="15">
         <v>555.82336499999997</v>
@@ -31326,7 +31326,7 @@
         <v>65.657144000000002</v>
       </c>
       <c r="AT18" s="15">
-        <v>63.640169999999998</v>
+        <v>62.828195999999998</v>
       </c>
       <c r="AU18" s="15">
         <v>71.092873999999995</v>
@@ -31487,7 +31487,7 @@
         <v>466.16468300000003</v>
       </c>
       <c r="AT19" s="15">
-        <v>467.72137600000002</v>
+        <v>467.80611199999998</v>
       </c>
       <c r="AU19" s="15">
         <v>449.01658300000003</v>
@@ -31648,7 +31648,7 @@
         <v>1507.6246900000001</v>
       </c>
       <c r="AT20" s="15">
-        <v>1423.9756070000001</v>
+        <v>1421.873722</v>
       </c>
       <c r="AU20" s="15">
         <v>1526.804995</v>
@@ -31809,7 +31809,7 @@
         <v>760.18734400000005</v>
       </c>
       <c r="AT21" s="15">
-        <v>965.85286299999996</v>
+        <v>965.35345099999995</v>
       </c>
       <c r="AU21" s="15">
         <v>890.68457100000001</v>
@@ -31970,7 +31970,7 @@
         <v>4675.3263260000003</v>
       </c>
       <c r="AT22" s="7">
-        <v>4774.2537229999998</v>
+        <v>4767.2618060000004</v>
       </c>
       <c r="AU22" s="7">
         <v>4888.138723</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Nov 19 05:26:55 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0CC44D-4E38-44D9-B99C-7C333CE6E935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BBDB8B-22FA-4A3B-8E46-CC8B7F29309C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3977,7 +3977,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4515,7 +4515,7 @@
         <v>5428</v>
       </c>
       <c r="AU5" s="15">
-        <v>0</v>
+        <v>5247</v>
       </c>
       <c r="AV5" s="15">
         <v>0</v>
@@ -4677,7 +4677,7 @@
         <v>12916</v>
       </c>
       <c r="AU6" s="6">
-        <v>0</v>
+        <v>12419</v>
       </c>
       <c r="AV6" s="6">
         <v>0</v>
@@ -4839,7 +4839,7 @@
         <v>18714</v>
       </c>
       <c r="AU7" s="6">
-        <v>0</v>
+        <v>19145</v>
       </c>
       <c r="AV7" s="6">
         <v>0</v>
@@ -5001,7 +5001,7 @@
         <v>3686</v>
       </c>
       <c r="AU8" s="6">
-        <v>0</v>
+        <v>3579</v>
       </c>
       <c r="AV8" s="6">
         <v>0</v>
@@ -5163,7 +5163,7 @@
         <v>6290</v>
       </c>
       <c r="AU9" s="6">
-        <v>0</v>
+        <v>7066</v>
       </c>
       <c r="AV9" s="6">
         <v>0</v>
@@ -5325,7 +5325,7 @@
         <v>14405</v>
       </c>
       <c r="AU10" s="15">
-        <v>0</v>
+        <v>16838</v>
       </c>
       <c r="AV10" s="15">
         <v>0</v>
@@ -5487,7 +5487,7 @@
         <v>22253</v>
       </c>
       <c r="AU11" s="6">
-        <v>0</v>
+        <v>22102</v>
       </c>
       <c r="AV11" s="6">
         <v>0</v>
@@ -5649,7 +5649,7 @@
         <v>83692</v>
       </c>
       <c r="AU12" s="7">
-        <v>0</v>
+        <v>86396</v>
       </c>
       <c r="AV12" s="7">
         <v>0</v>
@@ -5873,7 +5873,7 @@
         <v>431.78306400000002</v>
       </c>
       <c r="AU15" s="15">
-        <v>0</v>
+        <v>393.53971000000001</v>
       </c>
       <c r="AV15" s="15">
         <v>0</v>
@@ -6035,7 +6035,7 @@
         <v>897.10638900000004</v>
       </c>
       <c r="AU16" s="6">
-        <v>0</v>
+        <v>900.00210400000003</v>
       </c>
       <c r="AV16" s="6">
         <v>0</v>
@@ -6197,7 +6197,7 @@
         <v>450.09578199999999</v>
       </c>
       <c r="AU17" s="6">
-        <v>0</v>
+        <v>473.276298</v>
       </c>
       <c r="AV17" s="6">
         <v>0</v>
@@ -6359,7 +6359,7 @@
         <v>53.773249999999997</v>
       </c>
       <c r="AU18" s="6">
-        <v>0</v>
+        <v>45.303784</v>
       </c>
       <c r="AV18" s="6">
         <v>0</v>
@@ -6521,7 +6521,7 @@
         <v>355.663386</v>
       </c>
       <c r="AU19" s="6">
-        <v>0</v>
+        <v>425.83826199999999</v>
       </c>
       <c r="AV19" s="6">
         <v>0</v>
@@ -6683,7 +6683,7 @@
         <v>1293.599242</v>
       </c>
       <c r="AU20" s="15">
-        <v>0</v>
+        <v>1624.1286869999999</v>
       </c>
       <c r="AV20" s="15">
         <v>0</v>
@@ -6845,7 +6845,7 @@
         <v>518.63106200000004</v>
       </c>
       <c r="AU21" s="6">
-        <v>0</v>
+        <v>528.408771</v>
       </c>
       <c r="AV21" s="6">
         <v>0</v>
@@ -7007,7 +7007,7 @@
         <v>4000.6521749999997</v>
       </c>
       <c r="AU22" s="7">
-        <v>0</v>
+        <v>4390.4976159999997</v>
       </c>
       <c r="AV22" s="7">
         <v>0</v>
@@ -28961,7 +28961,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29498,7 +29498,7 @@
         <v>5772</v>
       </c>
       <c r="AU5" s="15">
-        <v>6285</v>
+        <v>6240</v>
       </c>
       <c r="AV5" s="15">
         <v>6041</v>
@@ -29659,7 +29659,7 @@
         <v>13002</v>
       </c>
       <c r="AU6" s="15">
-        <v>13283</v>
+        <v>13213</v>
       </c>
       <c r="AV6" s="15">
         <v>12323</v>
@@ -29820,7 +29820,7 @@
         <v>20140</v>
       </c>
       <c r="AU7" s="15">
-        <v>19617</v>
+        <v>20152</v>
       </c>
       <c r="AV7" s="15">
         <v>18576</v>
@@ -29981,7 +29981,7 @@
         <v>4701</v>
       </c>
       <c r="AU8" s="15">
-        <v>4921</v>
+        <v>4906</v>
       </c>
       <c r="AV8" s="15">
         <v>4378</v>
@@ -30142,7 +30142,7 @@
         <v>11366</v>
       </c>
       <c r="AU9" s="15">
-        <v>10430</v>
+        <v>10324</v>
       </c>
       <c r="AV9" s="15">
         <v>8463</v>
@@ -30303,7 +30303,7 @@
         <v>14306</v>
       </c>
       <c r="AU10" s="15">
-        <v>14951</v>
+        <v>14899</v>
       </c>
       <c r="AV10" s="15">
         <v>14127</v>
@@ -30464,7 +30464,7 @@
         <v>39895</v>
       </c>
       <c r="AU11" s="15">
-        <v>38254</v>
+        <v>38122</v>
       </c>
       <c r="AV11" s="15">
         <v>40158</v>
@@ -30625,7 +30625,7 @@
         <v>109182</v>
       </c>
       <c r="AU12" s="7">
-        <v>107741</v>
+        <v>107856</v>
       </c>
       <c r="AV12" s="7">
         <v>104066</v>
@@ -30846,7 +30846,7 @@
         <v>429.901228</v>
       </c>
       <c r="AU15" s="15">
-        <v>469.00431500000002</v>
+        <v>467.44506699999999</v>
       </c>
       <c r="AV15" s="15">
         <v>464.85895299999999</v>
@@ -31007,7 +31007,7 @@
         <v>946.150037</v>
       </c>
       <c r="AU16" s="15">
-        <v>925.71202000000005</v>
+        <v>924.90387799999996</v>
       </c>
       <c r="AV16" s="15">
         <v>887.33977800000002</v>
@@ -31168,7 +31168,7 @@
         <v>473.34906000000001</v>
       </c>
       <c r="AU17" s="15">
-        <v>555.82336499999997</v>
+        <v>555.19625099999996</v>
       </c>
       <c r="AV17" s="15">
         <v>487.59617100000003</v>
@@ -31329,7 +31329,7 @@
         <v>62.828195999999998</v>
       </c>
       <c r="AU18" s="15">
-        <v>71.092873999999995</v>
+        <v>70.386797000000001</v>
       </c>
       <c r="AV18" s="15">
         <v>65.225431999999998</v>
@@ -31490,7 +31490,7 @@
         <v>467.80611199999998</v>
       </c>
       <c r="AU19" s="15">
-        <v>449.01658300000003</v>
+        <v>448.10832900000003</v>
       </c>
       <c r="AV19" s="15">
         <v>386.00406099999998</v>
@@ -31651,7 +31651,7 @@
         <v>1421.873722</v>
       </c>
       <c r="AU20" s="15">
-        <v>1526.804995</v>
+        <v>1523.652621</v>
       </c>
       <c r="AV20" s="15">
         <v>1414.814081</v>
@@ -31812,7 +31812,7 @@
         <v>965.35345099999995</v>
       </c>
       <c r="AU21" s="15">
-        <v>890.68457100000001</v>
+        <v>888.51850899999999</v>
       </c>
       <c r="AV21" s="15">
         <v>908.04903400000001</v>
@@ -31973,7 +31973,7 @@
         <v>4767.2618060000004</v>
       </c>
       <c r="AU22" s="7">
-        <v>4888.138723</v>
+        <v>4878.2114519999996</v>
       </c>
       <c r="AV22" s="7">
         <v>4613.8875099999996</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Nov 26 05:27:24 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BBDB8B-22FA-4A3B-8E46-CC8B7F29309C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1067A0AF-3386-4859-ADA9-0422A923242B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3973,11 +3973,11 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomRight" activeCell="AG35" sqref="AG35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4518,7 +4518,7 @@
         <v>5247</v>
       </c>
       <c r="AV5" s="15">
-        <v>0</v>
+        <v>5810</v>
       </c>
       <c r="AW5" s="15">
         <v>0</v>
@@ -4680,7 +4680,7 @@
         <v>12419</v>
       </c>
       <c r="AV6" s="6">
-        <v>0</v>
+        <v>12735</v>
       </c>
       <c r="AW6" s="6">
         <v>0</v>
@@ -4842,7 +4842,7 @@
         <v>19145</v>
       </c>
       <c r="AV7" s="6">
-        <v>0</v>
+        <v>18064</v>
       </c>
       <c r="AW7" s="6">
         <v>0</v>
@@ -5004,7 +5004,7 @@
         <v>3579</v>
       </c>
       <c r="AV8" s="6">
-        <v>0</v>
+        <v>3864</v>
       </c>
       <c r="AW8" s="6">
         <v>0</v>
@@ -5166,7 +5166,7 @@
         <v>7066</v>
       </c>
       <c r="AV9" s="6">
-        <v>0</v>
+        <v>8653</v>
       </c>
       <c r="AW9" s="6">
         <v>0</v>
@@ -5328,7 +5328,7 @@
         <v>16838</v>
       </c>
       <c r="AV10" s="15">
-        <v>0</v>
+        <v>15383</v>
       </c>
       <c r="AW10" s="15">
         <v>0</v>
@@ -5490,7 +5490,7 @@
         <v>22102</v>
       </c>
       <c r="AV11" s="6">
-        <v>0</v>
+        <v>42361</v>
       </c>
       <c r="AW11" s="6">
         <v>0</v>
@@ -5652,7 +5652,7 @@
         <v>86396</v>
       </c>
       <c r="AV12" s="7">
-        <v>0</v>
+        <v>106870</v>
       </c>
       <c r="AW12" s="7">
         <v>0</v>
@@ -5876,7 +5876,7 @@
         <v>393.53971000000001</v>
       </c>
       <c r="AV15" s="15">
-        <v>0</v>
+        <v>440.79726099999999</v>
       </c>
       <c r="AW15" s="15">
         <v>0</v>
@@ -6038,7 +6038,7 @@
         <v>900.00210400000003</v>
       </c>
       <c r="AV16" s="6">
-        <v>0</v>
+        <v>941.736717</v>
       </c>
       <c r="AW16" s="6">
         <v>0</v>
@@ -6200,7 +6200,7 @@
         <v>473.276298</v>
       </c>
       <c r="AV17" s="6">
-        <v>0</v>
+        <v>537.12163299999997</v>
       </c>
       <c r="AW17" s="6">
         <v>0</v>
@@ -6362,7 +6362,7 @@
         <v>45.303784</v>
       </c>
       <c r="AV18" s="6">
-        <v>0</v>
+        <v>58.904367000000001</v>
       </c>
       <c r="AW18" s="6">
         <v>0</v>
@@ -6524,7 +6524,7 @@
         <v>425.83826199999999</v>
       </c>
       <c r="AV19" s="6">
-        <v>0</v>
+        <v>406.99744399999997</v>
       </c>
       <c r="AW19" s="6">
         <v>0</v>
@@ -6686,7 +6686,7 @@
         <v>1624.1286869999999</v>
       </c>
       <c r="AV20" s="15">
-        <v>0</v>
+        <v>1445.379508</v>
       </c>
       <c r="AW20" s="15">
         <v>0</v>
@@ -6848,7 +6848,7 @@
         <v>528.408771</v>
       </c>
       <c r="AV21" s="6">
-        <v>0</v>
+        <v>1097.929144</v>
       </c>
       <c r="AW21" s="6">
         <v>0</v>
@@ -7010,7 +7010,7 @@
         <v>4390.4976159999997</v>
       </c>
       <c r="AV22" s="7">
-        <v>0</v>
+        <v>4928.8660739999996</v>
       </c>
       <c r="AW22" s="7">
         <v>0</v>
@@ -25870,7 +25870,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28961,7 +28961,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29501,7 +29501,7 @@
         <v>6240</v>
       </c>
       <c r="AV5" s="15">
-        <v>6041</v>
+        <v>6028</v>
       </c>
       <c r="AW5" s="15">
         <v>6067</v>
@@ -29662,7 +29662,7 @@
         <v>13213</v>
       </c>
       <c r="AV6" s="15">
-        <v>12323</v>
+        <v>12264</v>
       </c>
       <c r="AW6" s="15">
         <v>13140</v>
@@ -29823,7 +29823,7 @@
         <v>20152</v>
       </c>
       <c r="AV7" s="15">
-        <v>18576</v>
+        <v>18707</v>
       </c>
       <c r="AW7" s="15">
         <v>18123</v>
@@ -29984,7 +29984,7 @@
         <v>4906</v>
       </c>
       <c r="AV8" s="15">
-        <v>4378</v>
+        <v>4374</v>
       </c>
       <c r="AW8" s="15">
         <v>4738</v>
@@ -30145,7 +30145,7 @@
         <v>10324</v>
       </c>
       <c r="AV9" s="15">
-        <v>8463</v>
+        <v>8469</v>
       </c>
       <c r="AW9" s="15">
         <v>10685</v>
@@ -30306,7 +30306,7 @@
         <v>14899</v>
       </c>
       <c r="AV10" s="15">
-        <v>14127</v>
+        <v>14221</v>
       </c>
       <c r="AW10" s="15">
         <v>13416</v>
@@ -30467,7 +30467,7 @@
         <v>38122</v>
       </c>
       <c r="AV11" s="15">
-        <v>40158</v>
+        <v>40047</v>
       </c>
       <c r="AW11" s="15">
         <v>42446</v>
@@ -30628,7 +30628,7 @@
         <v>107856</v>
       </c>
       <c r="AV12" s="7">
-        <v>104066</v>
+        <v>104110</v>
       </c>
       <c r="AW12" s="7">
         <v>108615</v>
@@ -30849,7 +30849,7 @@
         <v>467.44506699999999</v>
       </c>
       <c r="AV15" s="15">
-        <v>464.85895299999999</v>
+        <v>463.75915500000002</v>
       </c>
       <c r="AW15" s="15">
         <v>452.84101800000002</v>
@@ -31010,7 +31010,7 @@
         <v>924.90387799999996</v>
       </c>
       <c r="AV16" s="15">
-        <v>887.33977800000002</v>
+        <v>887.30184199999997</v>
       </c>
       <c r="AW16" s="15">
         <v>950.074296</v>
@@ -31171,7 +31171,7 @@
         <v>555.19625099999996</v>
       </c>
       <c r="AV17" s="15">
-        <v>487.59617100000003</v>
+        <v>475.47162500000002</v>
       </c>
       <c r="AW17" s="15">
         <v>512.009274</v>
@@ -31332,7 +31332,7 @@
         <v>70.386797000000001</v>
       </c>
       <c r="AV18" s="15">
-        <v>65.225431999999998</v>
+        <v>65.123716999999999</v>
       </c>
       <c r="AW18" s="15">
         <v>64.451792999999995</v>
@@ -31493,7 +31493,7 @@
         <v>448.10832900000003</v>
       </c>
       <c r="AV19" s="15">
-        <v>386.00406099999998</v>
+        <v>385.99813899999998</v>
       </c>
       <c r="AW19" s="15">
         <v>459.34115800000001</v>
@@ -31654,7 +31654,7 @@
         <v>1523.652621</v>
       </c>
       <c r="AV20" s="15">
-        <v>1414.814081</v>
+        <v>1423.650607</v>
       </c>
       <c r="AW20" s="15">
         <v>1286.8551580000001</v>
@@ -31815,7 +31815,7 @@
         <v>888.51850899999999</v>
       </c>
       <c r="AV21" s="15">
-        <v>908.04903400000001</v>
+        <v>908.04581700000006</v>
       </c>
       <c r="AW21" s="15">
         <v>1021.3936210000001</v>
@@ -31976,7 +31976,7 @@
         <v>4878.2114519999996</v>
       </c>
       <c r="AV22" s="7">
-        <v>4613.8875099999996</v>
+        <v>4609.3509020000001</v>
       </c>
       <c r="AW22" s="7">
         <v>4746.9663180000007</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Dec  3 05:28:31 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1067A0AF-3386-4859-ADA9-0422A923242B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC862109-3BB7-45D7-BD76-85CC1122BF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3977,7 +3977,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="AG35" sqref="AG35"/>
+      <selection pane="bottomRight" activeCell="AH35" sqref="AH35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4521,7 +4521,7 @@
         <v>5810</v>
       </c>
       <c r="AW5" s="15">
-        <v>0</v>
+        <v>5572</v>
       </c>
       <c r="AX5" s="15">
         <v>0</v>
@@ -4683,7 +4683,7 @@
         <v>12735</v>
       </c>
       <c r="AW6" s="6">
-        <v>0</v>
+        <v>12798</v>
       </c>
       <c r="AX6" s="6">
         <v>0</v>
@@ -4845,7 +4845,7 @@
         <v>18064</v>
       </c>
       <c r="AW7" s="6">
-        <v>0</v>
+        <v>18271</v>
       </c>
       <c r="AX7" s="6">
         <v>0</v>
@@ -5007,7 +5007,7 @@
         <v>3864</v>
       </c>
       <c r="AW8" s="6">
-        <v>0</v>
+        <v>3609</v>
       </c>
       <c r="AX8" s="6">
         <v>0</v>
@@ -5169,7 +5169,7 @@
         <v>8653</v>
       </c>
       <c r="AW9" s="6">
-        <v>0</v>
+        <v>8114</v>
       </c>
       <c r="AX9" s="6">
         <v>0</v>
@@ -5331,7 +5331,7 @@
         <v>15383</v>
       </c>
       <c r="AW10" s="15">
-        <v>0</v>
+        <v>13825</v>
       </c>
       <c r="AX10" s="15">
         <v>0</v>
@@ -5493,7 +5493,7 @@
         <v>42361</v>
       </c>
       <c r="AW11" s="6">
-        <v>0</v>
+        <v>40600</v>
       </c>
       <c r="AX11" s="6">
         <v>0</v>
@@ -5655,7 +5655,7 @@
         <v>106870</v>
       </c>
       <c r="AW12" s="7">
-        <v>0</v>
+        <v>102789</v>
       </c>
       <c r="AX12" s="7">
         <v>0</v>
@@ -5879,7 +5879,7 @@
         <v>440.79726099999999</v>
       </c>
       <c r="AW15" s="15">
-        <v>0</v>
+        <v>415.09190000000001</v>
       </c>
       <c r="AX15" s="15">
         <v>0</v>
@@ -6041,7 +6041,7 @@
         <v>941.736717</v>
       </c>
       <c r="AW16" s="6">
-        <v>0</v>
+        <v>941.69424500000002</v>
       </c>
       <c r="AX16" s="6">
         <v>0</v>
@@ -6203,7 +6203,7 @@
         <v>537.12163299999997</v>
       </c>
       <c r="AW17" s="6">
-        <v>0</v>
+        <v>549.75688400000001</v>
       </c>
       <c r="AX17" s="6">
         <v>0</v>
@@ -6365,7 +6365,7 @@
         <v>58.904367000000001</v>
       </c>
       <c r="AW18" s="6">
-        <v>0</v>
+        <v>59.709687000000002</v>
       </c>
       <c r="AX18" s="6">
         <v>0</v>
@@ -6527,7 +6527,7 @@
         <v>406.99744399999997</v>
       </c>
       <c r="AW19" s="6">
-        <v>0</v>
+        <v>378.96353699999997</v>
       </c>
       <c r="AX19" s="6">
         <v>0</v>
@@ -6689,7 +6689,7 @@
         <v>1445.379508</v>
       </c>
       <c r="AW20" s="15">
-        <v>0</v>
+        <v>1271.416577</v>
       </c>
       <c r="AX20" s="15">
         <v>0</v>
@@ -6851,7 +6851,7 @@
         <v>1097.929144</v>
       </c>
       <c r="AW21" s="6">
-        <v>0</v>
+        <v>966.90824399999997</v>
       </c>
       <c r="AX21" s="6">
         <v>0</v>
@@ -7013,7 +7013,7 @@
         <v>4928.8660739999996</v>
       </c>
       <c r="AW22" s="7">
-        <v>0</v>
+        <v>4583.5410739999998</v>
       </c>
       <c r="AX22" s="7">
         <v>0</v>
@@ -25870,7 +25870,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28961,7 +28961,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29504,7 +29504,7 @@
         <v>6028</v>
       </c>
       <c r="AW5" s="15">
-        <v>6067</v>
+        <v>6061</v>
       </c>
       <c r="AX5" s="15">
         <v>5859</v>
@@ -29665,7 +29665,7 @@
         <v>12264</v>
       </c>
       <c r="AW6" s="15">
-        <v>13140</v>
+        <v>13090</v>
       </c>
       <c r="AX6" s="15">
         <v>12760</v>
@@ -29826,7 +29826,7 @@
         <v>18707</v>
       </c>
       <c r="AW7" s="15">
-        <v>18123</v>
+        <v>18479</v>
       </c>
       <c r="AX7" s="15">
         <v>17145</v>
@@ -29987,7 +29987,7 @@
         <v>4374</v>
       </c>
       <c r="AW8" s="15">
-        <v>4738</v>
+        <v>4736</v>
       </c>
       <c r="AX8" s="15">
         <v>5072</v>
@@ -30309,7 +30309,7 @@
         <v>14221</v>
       </c>
       <c r="AW10" s="15">
-        <v>13416</v>
+        <v>13410</v>
       </c>
       <c r="AX10" s="15">
         <v>13980</v>
@@ -30470,7 +30470,7 @@
         <v>40047</v>
       </c>
       <c r="AW11" s="15">
-        <v>42446</v>
+        <v>42340</v>
       </c>
       <c r="AX11" s="15">
         <v>41515</v>
@@ -30631,7 +30631,7 @@
         <v>104110</v>
       </c>
       <c r="AW12" s="7">
-        <v>108615</v>
+        <v>108801</v>
       </c>
       <c r="AX12" s="7">
         <v>105054</v>
@@ -30852,7 +30852,7 @@
         <v>463.75915500000002</v>
       </c>
       <c r="AW15" s="15">
-        <v>452.84101800000002</v>
+        <v>452.88129900000001</v>
       </c>
       <c r="AX15" s="15">
         <v>426.452989</v>
@@ -31013,7 +31013,7 @@
         <v>887.30184199999997</v>
       </c>
       <c r="AW16" s="15">
-        <v>950.074296</v>
+        <v>948.39401199999998</v>
       </c>
       <c r="AX16" s="15">
         <v>945.47032300000001</v>
@@ -31174,7 +31174,7 @@
         <v>475.47162500000002</v>
       </c>
       <c r="AW17" s="15">
-        <v>512.009274</v>
+        <v>510.87128000000001</v>
       </c>
       <c r="AX17" s="15">
         <v>480.54639800000001</v>
@@ -31335,7 +31335,7 @@
         <v>65.123716999999999</v>
       </c>
       <c r="AW18" s="15">
-        <v>64.451792999999995</v>
+        <v>64.426805000000002</v>
       </c>
       <c r="AX18" s="15">
         <v>64.893192999999997</v>
@@ -31496,7 +31496,7 @@
         <v>385.99813899999998</v>
       </c>
       <c r="AW19" s="15">
-        <v>459.34115800000001</v>
+        <v>459.83835599999998</v>
       </c>
       <c r="AX19" s="15">
         <v>413.78705100000002</v>
@@ -31657,7 +31657,7 @@
         <v>1423.650607</v>
       </c>
       <c r="AW20" s="15">
-        <v>1286.8551580000001</v>
+        <v>1284.8599810000001</v>
       </c>
       <c r="AX20" s="15">
         <v>1328.845151</v>
@@ -31818,7 +31818,7 @@
         <v>908.04581700000006</v>
       </c>
       <c r="AW21" s="15">
-        <v>1021.3936210000001</v>
+        <v>1020.322375</v>
       </c>
       <c r="AX21" s="15">
         <v>984.25070500000004</v>
@@ -31979,7 +31979,7 @@
         <v>4609.3509020000001</v>
       </c>
       <c r="AW22" s="7">
-        <v>4746.9663180000007</v>
+        <v>4741.5941080000002</v>
       </c>
       <c r="AX22" s="7">
         <v>4644.2458099999994</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Dec 10 05:28:34 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC862109-3BB7-45D7-BD76-85CC1122BF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D96EB5-E11F-4F2A-8BC0-F42F5681809E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3977,7 +3977,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="AH35" sqref="AH35"/>
+      <selection pane="bottomRight" activeCell="AL31" sqref="AL31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4524,7 +4524,7 @@
         <v>5572</v>
       </c>
       <c r="AX5" s="15">
-        <v>0</v>
+        <v>5285</v>
       </c>
       <c r="AY5" s="15">
         <v>0</v>
@@ -4686,7 +4686,7 @@
         <v>12798</v>
       </c>
       <c r="AX6" s="6">
-        <v>0</v>
+        <v>12141</v>
       </c>
       <c r="AY6" s="6">
         <v>0</v>
@@ -4848,7 +4848,7 @@
         <v>18271</v>
       </c>
       <c r="AX7" s="6">
-        <v>0</v>
+        <v>17022</v>
       </c>
       <c r="AY7" s="6">
         <v>0</v>
@@ -5010,7 +5010,7 @@
         <v>3609</v>
       </c>
       <c r="AX8" s="6">
-        <v>0</v>
+        <v>3408</v>
       </c>
       <c r="AY8" s="6">
         <v>0</v>
@@ -5172,7 +5172,7 @@
         <v>8114</v>
       </c>
       <c r="AX9" s="6">
-        <v>0</v>
+        <v>8578</v>
       </c>
       <c r="AY9" s="6">
         <v>0</v>
@@ -5334,7 +5334,7 @@
         <v>13825</v>
       </c>
       <c r="AX10" s="15">
-        <v>0</v>
+        <v>15468</v>
       </c>
       <c r="AY10" s="15">
         <v>0</v>
@@ -5496,7 +5496,7 @@
         <v>40600</v>
       </c>
       <c r="AX11" s="6">
-        <v>0</v>
+        <v>40199</v>
       </c>
       <c r="AY11" s="6">
         <v>0</v>
@@ -5658,7 +5658,7 @@
         <v>102789</v>
       </c>
       <c r="AX12" s="7">
-        <v>0</v>
+        <v>102101</v>
       </c>
       <c r="AY12" s="7">
         <v>0</v>
@@ -5882,7 +5882,7 @@
         <v>415.09190000000001</v>
       </c>
       <c r="AX15" s="15">
-        <v>0</v>
+        <v>388.26512000000002</v>
       </c>
       <c r="AY15" s="15">
         <v>0</v>
@@ -6044,7 +6044,7 @@
         <v>941.69424500000002</v>
       </c>
       <c r="AX16" s="6">
-        <v>0</v>
+        <v>854.46578099999999</v>
       </c>
       <c r="AY16" s="6">
         <v>0</v>
@@ -6206,7 +6206,7 @@
         <v>549.75688400000001</v>
       </c>
       <c r="AX17" s="6">
-        <v>0</v>
+        <v>465.66764999999998</v>
       </c>
       <c r="AY17" s="6">
         <v>0</v>
@@ -6368,7 +6368,7 @@
         <v>59.709687000000002</v>
       </c>
       <c r="AX18" s="6">
-        <v>0</v>
+        <v>51.402760000000001</v>
       </c>
       <c r="AY18" s="6">
         <v>0</v>
@@ -6530,7 +6530,7 @@
         <v>378.96353699999997</v>
       </c>
       <c r="AX19" s="6">
-        <v>0</v>
+        <v>388.67211900000001</v>
       </c>
       <c r="AY19" s="6">
         <v>0</v>
@@ -6692,7 +6692,7 @@
         <v>1271.416577</v>
       </c>
       <c r="AX20" s="15">
-        <v>0</v>
+        <v>1388.788507</v>
       </c>
       <c r="AY20" s="15">
         <v>0</v>
@@ -6854,7 +6854,7 @@
         <v>966.90824399999997</v>
       </c>
       <c r="AX21" s="6">
-        <v>0</v>
+        <v>959.09063300000003</v>
       </c>
       <c r="AY21" s="6">
         <v>0</v>
@@ -7016,7 +7016,7 @@
         <v>4583.5410739999998</v>
       </c>
       <c r="AX22" s="7">
-        <v>0</v>
+        <v>4496.3525699999991</v>
       </c>
       <c r="AY22" s="7">
         <v>0</v>
@@ -28961,7 +28961,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29507,7 +29507,7 @@
         <v>6061</v>
       </c>
       <c r="AX5" s="15">
-        <v>5859</v>
+        <v>5842</v>
       </c>
       <c r="AY5" s="15">
         <v>5952</v>
@@ -29668,7 +29668,7 @@
         <v>13090</v>
       </c>
       <c r="AX6" s="15">
-        <v>12760</v>
+        <v>12731</v>
       </c>
       <c r="AY6" s="15">
         <v>13045</v>
@@ -29829,7 +29829,7 @@
         <v>18479</v>
       </c>
       <c r="AX7" s="15">
-        <v>17145</v>
+        <v>17518</v>
       </c>
       <c r="AY7" s="15">
         <v>19061</v>
@@ -29990,7 +29990,7 @@
         <v>4736</v>
       </c>
       <c r="AX8" s="15">
-        <v>5072</v>
+        <v>5054</v>
       </c>
       <c r="AY8" s="15">
         <v>5220</v>
@@ -30151,7 +30151,7 @@
         <v>10685</v>
       </c>
       <c r="AX9" s="15">
-        <v>8723</v>
+        <v>8720</v>
       </c>
       <c r="AY9" s="15">
         <v>8890</v>
@@ -30312,7 +30312,7 @@
         <v>13410</v>
       </c>
       <c r="AX10" s="15">
-        <v>13980</v>
+        <v>13974</v>
       </c>
       <c r="AY10" s="15">
         <v>13485</v>
@@ -30473,7 +30473,7 @@
         <v>42340</v>
       </c>
       <c r="AX11" s="15">
-        <v>41515</v>
+        <v>41424</v>
       </c>
       <c r="AY11" s="15">
         <v>43919</v>
@@ -30634,7 +30634,7 @@
         <v>108801</v>
       </c>
       <c r="AX12" s="7">
-        <v>105054</v>
+        <v>105263</v>
       </c>
       <c r="AY12" s="7">
         <v>109572</v>
@@ -30855,7 +30855,7 @@
         <v>452.88129900000001</v>
       </c>
       <c r="AX15" s="15">
-        <v>426.452989</v>
+        <v>425.64727800000003</v>
       </c>
       <c r="AY15" s="15">
         <v>437.59148099999999</v>
@@ -31016,7 +31016,7 @@
         <v>948.39401199999998</v>
       </c>
       <c r="AX16" s="15">
-        <v>945.47032300000001</v>
+        <v>944.53284499999995</v>
       </c>
       <c r="AY16" s="15">
         <v>953.87813300000005</v>
@@ -31177,7 +31177,7 @@
         <v>510.87128000000001</v>
       </c>
       <c r="AX17" s="15">
-        <v>480.54639800000001</v>
+        <v>477.441305</v>
       </c>
       <c r="AY17" s="15">
         <v>489.13018499999998</v>
@@ -31338,7 +31338,7 @@
         <v>64.426805000000002</v>
       </c>
       <c r="AX18" s="15">
-        <v>64.893192999999997</v>
+        <v>64.586344999999994</v>
       </c>
       <c r="AY18" s="15">
         <v>77.609941000000006</v>
@@ -31499,7 +31499,7 @@
         <v>459.83835599999998</v>
       </c>
       <c r="AX19" s="15">
-        <v>413.78705100000002</v>
+        <v>413.75766499999997</v>
       </c>
       <c r="AY19" s="15">
         <v>370.854581</v>
@@ -31660,7 +31660,7 @@
         <v>1284.8599810000001</v>
       </c>
       <c r="AX20" s="15">
-        <v>1328.845151</v>
+        <v>1328.8392249999999</v>
       </c>
       <c r="AY20" s="15">
         <v>1309.9274230000001</v>
@@ -31821,7 +31821,7 @@
         <v>1020.322375</v>
       </c>
       <c r="AX21" s="15">
-        <v>984.25070500000004</v>
+        <v>983.16574400000002</v>
       </c>
       <c r="AY21" s="15">
         <v>999.25665500000002</v>
@@ -31982,7 +31982,7 @@
         <v>4741.5941080000002</v>
       </c>
       <c r="AX22" s="7">
-        <v>4644.2458099999994</v>
+        <v>4637.9704069999998</v>
       </c>
       <c r="AY22" s="7">
         <v>4638.2483990000001</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Dec 17 05:28:18 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D96EB5-E11F-4F2A-8BC0-F42F5681809E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973C3053-CFE0-43E1-ACF0-0E4568C6D085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3977,7 +3977,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="AL31" sqref="AL31"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4527,7 +4527,7 @@
         <v>5285</v>
       </c>
       <c r="AY5" s="15">
-        <v>0</v>
+        <v>5388</v>
       </c>
       <c r="AZ5" s="15">
         <v>0</v>
@@ -4689,7 +4689,7 @@
         <v>12141</v>
       </c>
       <c r="AY6" s="6">
-        <v>0</v>
+        <v>12651</v>
       </c>
       <c r="AZ6" s="6">
         <v>0</v>
@@ -4851,7 +4851,7 @@
         <v>17022</v>
       </c>
       <c r="AY7" s="6">
-        <v>0</v>
+        <v>17509</v>
       </c>
       <c r="AZ7" s="6">
         <v>0</v>
@@ -5013,7 +5013,7 @@
         <v>3408</v>
       </c>
       <c r="AY8" s="6">
-        <v>0</v>
+        <v>3847</v>
       </c>
       <c r="AZ8" s="6">
         <v>0</v>
@@ -5175,7 +5175,7 @@
         <v>8578</v>
       </c>
       <c r="AY9" s="6">
-        <v>0</v>
+        <v>9224</v>
       </c>
       <c r="AZ9" s="6">
         <v>0</v>
@@ -5337,7 +5337,7 @@
         <v>15468</v>
       </c>
       <c r="AY10" s="15">
-        <v>0</v>
+        <v>13762</v>
       </c>
       <c r="AZ10" s="15">
         <v>0</v>
@@ -5499,7 +5499,7 @@
         <v>40199</v>
       </c>
       <c r="AY11" s="6">
-        <v>0</v>
+        <v>40321</v>
       </c>
       <c r="AZ11" s="6">
         <v>0</v>
@@ -5661,7 +5661,7 @@
         <v>102101</v>
       </c>
       <c r="AY12" s="7">
-        <v>0</v>
+        <v>102702</v>
       </c>
       <c r="AZ12" s="7">
         <v>0</v>
@@ -5885,7 +5885,7 @@
         <v>388.26512000000002</v>
       </c>
       <c r="AY15" s="15">
-        <v>0</v>
+        <v>374.37831499999999</v>
       </c>
       <c r="AZ15" s="15">
         <v>0</v>
@@ -6047,7 +6047,7 @@
         <v>854.46578099999999</v>
       </c>
       <c r="AY16" s="6">
-        <v>0</v>
+        <v>907.25786900000003</v>
       </c>
       <c r="AZ16" s="6">
         <v>0</v>
@@ -6209,7 +6209,7 @@
         <v>465.66764999999998</v>
       </c>
       <c r="AY17" s="6">
-        <v>0</v>
+        <v>517.29284800000005</v>
       </c>
       <c r="AZ17" s="6">
         <v>0</v>
@@ -6371,7 +6371,7 @@
         <v>51.402760000000001</v>
       </c>
       <c r="AY18" s="6">
-        <v>0</v>
+        <v>62.586969000000003</v>
       </c>
       <c r="AZ18" s="6">
         <v>0</v>
@@ -6533,7 +6533,7 @@
         <v>388.67211900000001</v>
       </c>
       <c r="AY19" s="6">
-        <v>0</v>
+        <v>460.41769199999999</v>
       </c>
       <c r="AZ19" s="6">
         <v>0</v>
@@ -6695,7 +6695,7 @@
         <v>1388.788507</v>
       </c>
       <c r="AY20" s="15">
-        <v>0</v>
+        <v>1235.1902259999999</v>
       </c>
       <c r="AZ20" s="15">
         <v>0</v>
@@ -6857,7 +6857,7 @@
         <v>959.09063300000003</v>
       </c>
       <c r="AY21" s="6">
-        <v>0</v>
+        <v>984.02678500000002</v>
       </c>
       <c r="AZ21" s="6">
         <v>0</v>
@@ -7019,7 +7019,7 @@
         <v>4496.3525699999991</v>
       </c>
       <c r="AY22" s="7">
-        <v>0</v>
+        <v>4541.1507039999997</v>
       </c>
       <c r="AZ22" s="7">
         <v>0</v>
@@ -28961,7 +28961,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29510,7 +29510,7 @@
         <v>5842</v>
       </c>
       <c r="AY5" s="15">
-        <v>5952</v>
+        <v>5943</v>
       </c>
       <c r="AZ5" s="15">
         <v>5737</v>
@@ -29671,7 +29671,7 @@
         <v>12731</v>
       </c>
       <c r="AY6" s="15">
-        <v>13045</v>
+        <v>13004</v>
       </c>
       <c r="AZ6" s="15">
         <v>14224</v>
@@ -29832,7 +29832,7 @@
         <v>17518</v>
       </c>
       <c r="AY7" s="15">
-        <v>19061</v>
+        <v>19524</v>
       </c>
       <c r="AZ7" s="15">
         <v>18743</v>
@@ -29993,7 +29993,7 @@
         <v>5054</v>
       </c>
       <c r="AY8" s="15">
-        <v>5220</v>
+        <v>5214</v>
       </c>
       <c r="AZ8" s="15">
         <v>3936</v>
@@ -30154,7 +30154,7 @@
         <v>8720</v>
       </c>
       <c r="AY9" s="15">
-        <v>8890</v>
+        <v>8886</v>
       </c>
       <c r="AZ9" s="15">
         <v>8575</v>
@@ -30315,7 +30315,7 @@
         <v>13974</v>
       </c>
       <c r="AY10" s="15">
-        <v>13485</v>
+        <v>13476</v>
       </c>
       <c r="AZ10" s="15">
         <v>13114</v>
@@ -30476,7 +30476,7 @@
         <v>41424</v>
       </c>
       <c r="AY11" s="15">
-        <v>43919</v>
+        <v>43809</v>
       </c>
       <c r="AZ11" s="15">
         <v>41996</v>
@@ -30637,7 +30637,7 @@
         <v>105263</v>
       </c>
       <c r="AY12" s="7">
-        <v>109572</v>
+        <v>109856</v>
       </c>
       <c r="AZ12" s="7">
         <v>106325</v>
@@ -30858,7 +30858,7 @@
         <v>425.64727800000003</v>
       </c>
       <c r="AY15" s="15">
-        <v>437.59148099999999</v>
+        <v>437.325469</v>
       </c>
       <c r="AZ15" s="15">
         <v>450.48192299999999</v>
@@ -31019,7 +31019,7 @@
         <v>944.53284499999995</v>
       </c>
       <c r="AY16" s="15">
-        <v>953.87813300000005</v>
+        <v>952.99238300000002</v>
       </c>
       <c r="AZ16" s="15">
         <v>1078.200255</v>
@@ -31180,7 +31180,7 @@
         <v>477.441305</v>
       </c>
       <c r="AY17" s="15">
-        <v>489.13018499999998</v>
+        <v>488.13959699999998</v>
       </c>
       <c r="AZ17" s="15">
         <v>519.41852500000005</v>
@@ -31341,7 +31341,7 @@
         <v>64.586344999999994</v>
       </c>
       <c r="AY18" s="15">
-        <v>77.609941000000006</v>
+        <v>77.515338</v>
       </c>
       <c r="AZ18" s="15">
         <v>54.823993000000002</v>
@@ -31502,7 +31502,7 @@
         <v>413.75766499999997</v>
       </c>
       <c r="AY19" s="15">
-        <v>370.854581</v>
+        <v>370.727867</v>
       </c>
       <c r="AZ19" s="15">
         <v>352.28804100000002</v>
@@ -31663,7 +31663,7 @@
         <v>1328.8392249999999</v>
       </c>
       <c r="AY20" s="15">
-        <v>1309.9274230000001</v>
+        <v>1309.148817</v>
       </c>
       <c r="AZ20" s="15">
         <v>1274.0086839999999</v>
@@ -31824,7 +31824,7 @@
         <v>983.16574400000002</v>
       </c>
       <c r="AY21" s="15">
-        <v>999.25665500000002</v>
+        <v>998.32605699999999</v>
       </c>
       <c r="AZ21" s="15">
         <v>985.02643899999998</v>
@@ -31985,7 +31985,7 @@
         <v>4637.9704069999998</v>
       </c>
       <c r="AY22" s="7">
-        <v>4638.2483990000001</v>
+        <v>4634.1755279999998</v>
       </c>
       <c r="AZ22" s="7">
         <v>4714.2478599999995</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Dec 24 05:26:14 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973C3053-CFE0-43E1-ACF0-0E4568C6D085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBDB33C2-2DFB-4104-AB5C-9495A534C9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3973,11 +3973,11 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4530,7 +4530,7 @@
         <v>5388</v>
       </c>
       <c r="AZ5" s="15">
-        <v>0</v>
+        <v>5464</v>
       </c>
       <c r="BA5" s="15">
         <v>0</v>
@@ -4692,7 +4692,7 @@
         <v>12651</v>
       </c>
       <c r="AZ6" s="6">
-        <v>0</v>
+        <v>12545</v>
       </c>
       <c r="BA6" s="6">
         <v>0</v>
@@ -4854,7 +4854,7 @@
         <v>17509</v>
       </c>
       <c r="AZ7" s="6">
-        <v>0</v>
+        <v>17625</v>
       </c>
       <c r="BA7" s="6">
         <v>0</v>
@@ -5016,7 +5016,7 @@
         <v>3847</v>
       </c>
       <c r="AZ8" s="6">
-        <v>0</v>
+        <v>3593</v>
       </c>
       <c r="BA8" s="6">
         <v>0</v>
@@ -5178,7 +5178,7 @@
         <v>9224</v>
       </c>
       <c r="AZ9" s="6">
-        <v>0</v>
+        <v>9255</v>
       </c>
       <c r="BA9" s="6">
         <v>0</v>
@@ -5340,7 +5340,7 @@
         <v>13762</v>
       </c>
       <c r="AZ10" s="15">
-        <v>0</v>
+        <v>13120</v>
       </c>
       <c r="BA10" s="15">
         <v>0</v>
@@ -5502,7 +5502,7 @@
         <v>40321</v>
       </c>
       <c r="AZ11" s="6">
-        <v>0</v>
+        <v>40011</v>
       </c>
       <c r="BA11" s="6">
         <v>0</v>
@@ -5664,7 +5664,7 @@
         <v>102702</v>
       </c>
       <c r="AZ12" s="7">
-        <v>0</v>
+        <v>101613</v>
       </c>
       <c r="BA12" s="7">
         <v>0</v>
@@ -5888,7 +5888,7 @@
         <v>374.37831499999999</v>
       </c>
       <c r="AZ15" s="15">
-        <v>0</v>
+        <v>382.25658499999997</v>
       </c>
       <c r="BA15" s="15">
         <v>0</v>
@@ -6050,7 +6050,7 @@
         <v>907.25786900000003</v>
       </c>
       <c r="AZ16" s="6">
-        <v>0</v>
+        <v>868.11476200000004</v>
       </c>
       <c r="BA16" s="6">
         <v>0</v>
@@ -6212,7 +6212,7 @@
         <v>517.29284800000005</v>
       </c>
       <c r="AZ17" s="6">
-        <v>0</v>
+        <v>527.08074299999998</v>
       </c>
       <c r="BA17" s="6">
         <v>0</v>
@@ -6374,7 +6374,7 @@
         <v>62.586969000000003</v>
       </c>
       <c r="AZ18" s="6">
-        <v>0</v>
+        <v>55.552880000000002</v>
       </c>
       <c r="BA18" s="6">
         <v>0</v>
@@ -6536,7 +6536,7 @@
         <v>460.41769199999999</v>
       </c>
       <c r="AZ19" s="6">
-        <v>0</v>
+        <v>431.516952</v>
       </c>
       <c r="BA19" s="6">
         <v>0</v>
@@ -6698,7 +6698,7 @@
         <v>1235.1902259999999</v>
       </c>
       <c r="AZ20" s="15">
-        <v>0</v>
+        <v>1153.768867</v>
       </c>
       <c r="BA20" s="15">
         <v>0</v>
@@ -6860,7 +6860,7 @@
         <v>984.02678500000002</v>
       </c>
       <c r="AZ21" s="6">
-        <v>0</v>
+        <v>989.86285799999996</v>
       </c>
       <c r="BA21" s="6">
         <v>0</v>
@@ -7022,7 +7022,7 @@
         <v>4541.1507039999997</v>
       </c>
       <c r="AZ22" s="7">
-        <v>0</v>
+        <v>4408.1536469999992</v>
       </c>
       <c r="BA22" s="7">
         <v>0</v>
@@ -7137,6 +7137,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -25870,7 +25873,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28949,6 +28952,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -28958,10 +28964,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29513,7 +29519,7 @@
         <v>5943</v>
       </c>
       <c r="AZ5" s="15">
-        <v>5737</v>
+        <v>5724</v>
       </c>
       <c r="BA5" s="15">
         <v>4445</v>
@@ -29674,7 +29680,7 @@
         <v>13004</v>
       </c>
       <c r="AZ6" s="15">
-        <v>14224</v>
+        <v>14181</v>
       </c>
       <c r="BA6" s="15">
         <v>11733</v>
@@ -29835,7 +29841,7 @@
         <v>19524</v>
       </c>
       <c r="AZ7" s="15">
-        <v>18743</v>
+        <v>19286</v>
       </c>
       <c r="BA7" s="15">
         <v>15028</v>
@@ -29996,7 +30002,7 @@
         <v>5214</v>
       </c>
       <c r="AZ8" s="15">
-        <v>3936</v>
+        <v>3923</v>
       </c>
       <c r="BA8" s="15">
         <v>2510</v>
@@ -30157,7 +30163,7 @@
         <v>8886</v>
       </c>
       <c r="AZ9" s="15">
-        <v>8575</v>
+        <v>8576</v>
       </c>
       <c r="BA9" s="15">
         <v>8123</v>
@@ -30318,7 +30324,7 @@
         <v>13476</v>
       </c>
       <c r="AZ10" s="15">
-        <v>13114</v>
+        <v>13131</v>
       </c>
       <c r="BA10" s="15">
         <v>9903</v>
@@ -30479,7 +30485,7 @@
         <v>43809</v>
       </c>
       <c r="AZ11" s="15">
-        <v>41996</v>
+        <v>41905</v>
       </c>
       <c r="BA11" s="15">
         <v>34137</v>
@@ -30640,7 +30646,7 @@
         <v>109856</v>
       </c>
       <c r="AZ12" s="7">
-        <v>106325</v>
+        <v>106726</v>
       </c>
       <c r="BA12" s="7">
         <v>85879</v>
@@ -30861,7 +30867,7 @@
         <v>437.325469</v>
       </c>
       <c r="AZ15" s="15">
-        <v>450.48192299999999</v>
+        <v>448.757631</v>
       </c>
       <c r="BA15" s="15">
         <v>299.51857200000001</v>
@@ -31022,7 +31028,7 @@
         <v>952.99238300000002</v>
       </c>
       <c r="AZ16" s="15">
-        <v>1078.200255</v>
+        <v>1077.8690630000001</v>
       </c>
       <c r="BA16" s="15">
         <v>889.37489700000003</v>
@@ -31183,7 +31189,7 @@
         <v>488.13959699999998</v>
       </c>
       <c r="AZ17" s="15">
-        <v>519.41852500000005</v>
+        <v>488.450468</v>
       </c>
       <c r="BA17" s="15">
         <v>534.04841199999998</v>
@@ -31344,7 +31350,7 @@
         <v>77.515338</v>
       </c>
       <c r="AZ18" s="15">
-        <v>54.823993000000002</v>
+        <v>54.363036999999998</v>
       </c>
       <c r="BA18" s="15">
         <v>38.940157999999997</v>
@@ -31505,7 +31511,7 @@
         <v>370.727867</v>
       </c>
       <c r="AZ19" s="15">
-        <v>352.28804100000002</v>
+        <v>352.56290100000001</v>
       </c>
       <c r="BA19" s="15">
         <v>363.77720699999998</v>
@@ -31666,7 +31672,7 @@
         <v>1309.148817</v>
       </c>
       <c r="AZ20" s="15">
-        <v>1274.0086839999999</v>
+        <v>1275.2088490000001</v>
       </c>
       <c r="BA20" s="15">
         <v>993.71548499999994</v>
@@ -31827,7 +31833,7 @@
         <v>998.32605699999999</v>
       </c>
       <c r="AZ21" s="15">
-        <v>985.02643899999998</v>
+        <v>984.39462500000002</v>
       </c>
       <c r="BA21" s="15">
         <v>756.39903700000002</v>
@@ -31988,7 +31994,7 @@
         <v>4634.1755279999998</v>
       </c>
       <c r="AZ22" s="7">
-        <v>4714.2478599999995</v>
+        <v>4681.6065740000004</v>
       </c>
       <c r="BA22" s="7">
         <v>3875.773768</v>
@@ -32040,5 +32046,8 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GH ACTION Autorun Tue Dec 31 05:25:49 UTC 2024
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBDB33C2-2DFB-4104-AB5C-9495A534C9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FD0FF3-5498-40F8-A843-677D0030FA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -3973,11 +3973,11 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="AK35" sqref="AK35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4533,7 +4533,7 @@
         <v>5464</v>
       </c>
       <c r="BA5" s="15">
-        <v>0</v>
+        <v>4363</v>
       </c>
       <c r="BB5"/>
     </row>
@@ -4695,7 +4695,7 @@
         <v>12545</v>
       </c>
       <c r="BA6" s="6">
-        <v>0</v>
+        <v>11478</v>
       </c>
       <c r="BB6"/>
     </row>
@@ -4857,7 +4857,7 @@
         <v>17625</v>
       </c>
       <c r="BA7" s="6">
-        <v>0</v>
+        <v>16410</v>
       </c>
       <c r="BB7"/>
     </row>
@@ -5019,7 +5019,7 @@
         <v>3593</v>
       </c>
       <c r="BA8" s="6">
-        <v>0</v>
+        <v>2807</v>
       </c>
       <c r="BB8"/>
     </row>
@@ -5181,7 +5181,7 @@
         <v>9255</v>
       </c>
       <c r="BA9" s="6">
-        <v>0</v>
+        <v>8047</v>
       </c>
       <c r="BB9"/>
     </row>
@@ -5343,7 +5343,7 @@
         <v>13120</v>
       </c>
       <c r="BA10" s="15">
-        <v>0</v>
+        <v>12133</v>
       </c>
       <c r="BB10"/>
     </row>
@@ -5505,7 +5505,7 @@
         <v>40011</v>
       </c>
       <c r="BA11" s="6">
-        <v>0</v>
+        <v>29432</v>
       </c>
       <c r="BB11"/>
     </row>
@@ -5667,7 +5667,7 @@
         <v>101613</v>
       </c>
       <c r="BA12" s="7">
-        <v>0</v>
+        <v>84670</v>
       </c>
       <c r="BB12"/>
     </row>
@@ -5891,7 +5891,7 @@
         <v>382.25658499999997</v>
       </c>
       <c r="BA15" s="15">
-        <v>0</v>
+        <v>303.44771800000001</v>
       </c>
       <c r="BB15"/>
     </row>
@@ -6053,7 +6053,7 @@
         <v>868.11476200000004</v>
       </c>
       <c r="BA16" s="6">
-        <v>0</v>
+        <v>868.11864300000002</v>
       </c>
       <c r="BB16"/>
     </row>
@@ -6215,7 +6215,7 @@
         <v>527.08074299999998</v>
       </c>
       <c r="BA17" s="6">
-        <v>0</v>
+        <v>433.165955</v>
       </c>
       <c r="BB17"/>
     </row>
@@ -6377,7 +6377,7 @@
         <v>55.552880000000002</v>
       </c>
       <c r="BA18" s="6">
-        <v>0</v>
+        <v>42.773207999999997</v>
       </c>
       <c r="BB18"/>
     </row>
@@ -6539,7 +6539,7 @@
         <v>431.516952</v>
       </c>
       <c r="BA19" s="6">
-        <v>0</v>
+        <v>374.79168900000002</v>
       </c>
       <c r="BB19"/>
     </row>
@@ -6701,7 +6701,7 @@
         <v>1153.768867</v>
       </c>
       <c r="BA20" s="15">
-        <v>0</v>
+        <v>1143.806075</v>
       </c>
       <c r="BB20"/>
     </row>
@@ -6863,7 +6863,7 @@
         <v>989.86285799999996</v>
       </c>
       <c r="BA21" s="6">
-        <v>0</v>
+        <v>657.70498399999997</v>
       </c>
       <c r="BB21"/>
     </row>
@@ -7025,7 +7025,7 @@
         <v>4408.1536469999992</v>
       </c>
       <c r="BA22" s="7">
-        <v>0</v>
+        <v>3823.8082720000002</v>
       </c>
       <c r="BB22"/>
     </row>
@@ -7137,9 +7137,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -25873,7 +25870,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28952,9 +28949,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -28964,10 +28958,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29522,7 +29516,7 @@
         <v>5724</v>
       </c>
       <c r="BA5" s="15">
-        <v>4445</v>
+        <v>4413</v>
       </c>
     </row>
     <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -29683,7 +29677,7 @@
         <v>14181</v>
       </c>
       <c r="BA6" s="15">
-        <v>11733</v>
+        <v>11673</v>
       </c>
     </row>
     <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -29844,7 +29838,7 @@
         <v>19286</v>
       </c>
       <c r="BA7" s="15">
-        <v>15028</v>
+        <v>15590</v>
       </c>
     </row>
     <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -30005,7 +29999,7 @@
         <v>3923</v>
       </c>
       <c r="BA8" s="15">
-        <v>2510</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -30166,7 +30160,7 @@
         <v>8576</v>
       </c>
       <c r="BA9" s="15">
-        <v>8123</v>
+        <v>8134</v>
       </c>
     </row>
     <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -30327,7 +30321,7 @@
         <v>13131</v>
       </c>
       <c r="BA10" s="15">
-        <v>9903</v>
+        <v>9863</v>
       </c>
     </row>
     <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -30488,7 +30482,7 @@
         <v>41905</v>
       </c>
       <c r="BA11" s="15">
-        <v>34137</v>
+        <v>34066</v>
       </c>
     </row>
     <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -30649,7 +30643,7 @@
         <v>106726</v>
       </c>
       <c r="BA12" s="7">
-        <v>85879</v>
+        <v>86245</v>
       </c>
     </row>
     <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
@@ -30870,7 +30864,7 @@
         <v>448.757631</v>
       </c>
       <c r="BA15" s="15">
-        <v>299.51857200000001</v>
+        <v>298.50642199999999</v>
       </c>
     </row>
     <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -31031,7 +31025,7 @@
         <v>1077.8690630000001</v>
       </c>
       <c r="BA16" s="15">
-        <v>889.37489700000003</v>
+        <v>888.297684</v>
       </c>
     </row>
     <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -31192,7 +31186,7 @@
         <v>488.450468</v>
       </c>
       <c r="BA17" s="15">
-        <v>534.04841199999998</v>
+        <v>533.92582100000004</v>
       </c>
     </row>
     <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -31353,7 +31347,7 @@
         <v>54.363036999999998</v>
       </c>
       <c r="BA18" s="15">
-        <v>38.940157999999997</v>
+        <v>38.857964000000003</v>
       </c>
     </row>
     <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -31514,7 +31508,7 @@
         <v>352.56290100000001</v>
       </c>
       <c r="BA19" s="15">
-        <v>363.77720699999998</v>
+        <v>364.61675700000001</v>
       </c>
     </row>
     <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -31675,7 +31669,7 @@
         <v>1275.2088490000001</v>
       </c>
       <c r="BA20" s="15">
-        <v>993.71548499999994</v>
+        <v>992.76339499999995</v>
       </c>
     </row>
     <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -31836,7 +31830,7 @@
         <v>984.39462500000002</v>
       </c>
       <c r="BA21" s="15">
-        <v>756.39903700000002</v>
+        <v>755.640308</v>
       </c>
     </row>
     <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -31997,7 +31991,7 @@
         <v>4681.6065740000004</v>
       </c>
       <c r="BA22" s="7">
-        <v>3875.773768</v>
+        <v>3872.6083509999999</v>
       </c>
     </row>
     <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -32046,8 +32040,5 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jan 14 05:25:08 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FB4E12-2A05-456C-9FA3-E3E736D928B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A0F18F-E211-41BF-9517-826821C439F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4427,7 +4427,7 @@
         <v>5358</v>
       </c>
       <c r="C5" s="15">
-        <v>5567</v>
+        <v>5540</v>
       </c>
       <c r="D5" s="15">
         <v>5313</v>
@@ -4588,7 +4588,7 @@
         <v>12582</v>
       </c>
       <c r="C6" s="15">
-        <v>11847</v>
+        <v>11791</v>
       </c>
       <c r="D6" s="15">
         <v>11076</v>
@@ -4749,7 +4749,7 @@
         <v>17450</v>
       </c>
       <c r="C7" s="15">
-        <v>18450</v>
+        <v>19106</v>
       </c>
       <c r="D7" s="15">
         <v>15756</v>
@@ -4910,7 +4910,7 @@
         <v>2687</v>
       </c>
       <c r="C8" s="15">
-        <v>2899</v>
+        <v>2897</v>
       </c>
       <c r="D8" s="15">
         <v>2589</v>
@@ -5071,7 +5071,7 @@
         <v>10297</v>
       </c>
       <c r="C9" s="15">
-        <v>8399</v>
+        <v>8396</v>
       </c>
       <c r="D9" s="15">
         <v>5753</v>
@@ -5232,7 +5232,7 @@
         <v>11516</v>
       </c>
       <c r="C10" s="15">
-        <v>12613</v>
+        <v>12621</v>
       </c>
       <c r="D10" s="15">
         <v>10182</v>
@@ -5393,7 +5393,7 @@
         <v>36384</v>
       </c>
       <c r="C11" s="15">
-        <v>38690</v>
+        <v>38539</v>
       </c>
       <c r="D11" s="15">
         <v>32574</v>
@@ -5554,7 +5554,7 @@
         <v>96274</v>
       </c>
       <c r="C12" s="7">
-        <v>98465</v>
+        <v>98890</v>
       </c>
       <c r="D12" s="7">
         <v>83243</v>
@@ -5775,7 +5775,7 @@
         <v>382.683311</v>
       </c>
       <c r="C15" s="15">
-        <v>412.02217400000001</v>
+        <v>411.243494</v>
       </c>
       <c r="D15" s="15">
         <v>396.04362099999997</v>
@@ -5936,7 +5936,7 @@
         <v>929.03476499999999</v>
       </c>
       <c r="C16" s="15">
-        <v>797.86787800000002</v>
+        <v>797.01472000000001</v>
       </c>
       <c r="D16" s="15">
         <v>782.62626299999999</v>
@@ -6097,7 +6097,7 @@
         <v>376.11375500000003</v>
       </c>
       <c r="C17" s="15">
-        <v>569.58045000000004</v>
+        <v>568.96275800000001</v>
       </c>
       <c r="D17" s="15">
         <v>403.53600899999998</v>
@@ -6258,7 +6258,7 @@
         <v>47.517266999999997</v>
       </c>
       <c r="C18" s="15">
-        <v>46.832397999999998</v>
+        <v>46.863571999999998</v>
       </c>
       <c r="D18" s="15">
         <v>39.916519999999998</v>
@@ -6419,7 +6419,7 @@
         <v>418.15840200000002</v>
       </c>
       <c r="C19" s="15">
-        <v>371.36372499999999</v>
+        <v>371.12378000000001</v>
       </c>
       <c r="D19" s="15">
         <v>230.17139</v>
@@ -6580,7 +6580,7 @@
         <v>1130.558683</v>
       </c>
       <c r="C20" s="15">
-        <v>1227.6475809999999</v>
+        <v>1226.6599679999999</v>
       </c>
       <c r="D20" s="15">
         <v>1071.8569259999999</v>
@@ -6741,7 +6741,7 @@
         <v>806.811958</v>
       </c>
       <c r="C21" s="15">
-        <v>886.51915299999996</v>
+        <v>885.46785799999998</v>
       </c>
       <c r="D21" s="15">
         <v>811.52483700000005</v>
@@ -6902,7 +6902,7 @@
         <v>4090.8781410000001</v>
       </c>
       <c r="C22" s="7">
-        <v>4311.8333590000002</v>
+        <v>4307.3361500000001</v>
       </c>
       <c r="D22" s="7">
         <v>3735.6755659999999</v>
@@ -7114,7 +7114,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="J33" sqref="J33"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7520,7 +7520,7 @@
         <v>4730</v>
       </c>
       <c r="C5" s="15">
-        <v>0</v>
+        <v>5872</v>
       </c>
       <c r="D5" s="15">
         <v>0</v>
@@ -7682,7 +7682,7 @@
         <v>12095</v>
       </c>
       <c r="C6" s="6">
-        <v>0</v>
+        <v>13042</v>
       </c>
       <c r="D6" s="6">
         <v>0</v>
@@ -7844,7 +7844,7 @@
         <v>15563</v>
       </c>
       <c r="C7" s="6">
-        <v>0</v>
+        <v>17769</v>
       </c>
       <c r="D7" s="6">
         <v>0</v>
@@ -8006,7 +8006,7 @@
         <v>2558</v>
       </c>
       <c r="C8" s="6">
-        <v>0</v>
+        <v>2603</v>
       </c>
       <c r="D8" s="6">
         <v>0</v>
@@ -8168,7 +8168,7 @@
         <v>8423</v>
       </c>
       <c r="C9" s="6">
-        <v>0</v>
+        <v>9423</v>
       </c>
       <c r="D9" s="6">
         <v>0</v>
@@ -8330,7 +8330,7 @@
         <v>13491</v>
       </c>
       <c r="C10" s="15">
-        <v>0</v>
+        <v>13856</v>
       </c>
       <c r="D10" s="15">
         <v>0</v>
@@ -8492,7 +8492,7 @@
         <v>37245</v>
       </c>
       <c r="C11" s="6">
-        <v>0</v>
+        <v>42824</v>
       </c>
       <c r="D11" s="6">
         <v>0</v>
@@ -8654,7 +8654,7 @@
         <v>94105</v>
       </c>
       <c r="C12" s="7">
-        <v>0</v>
+        <v>105389</v>
       </c>
       <c r="D12" s="7">
         <v>0</v>
@@ -8878,7 +8878,7 @@
         <v>322.07186400000001</v>
       </c>
       <c r="C15" s="15">
-        <v>0</v>
+        <v>459.58167200000003</v>
       </c>
       <c r="D15" s="15">
         <v>0</v>
@@ -9040,7 +9040,7 @@
         <v>859.18348900000001</v>
       </c>
       <c r="C16" s="6">
-        <v>0</v>
+        <v>940.731405</v>
       </c>
       <c r="D16" s="6">
         <v>0</v>
@@ -9202,7 +9202,7 @@
         <v>528.604739</v>
       </c>
       <c r="C17" s="6">
-        <v>0</v>
+        <v>565.80550300000004</v>
       </c>
       <c r="D17" s="6">
         <v>0</v>
@@ -9364,7 +9364,7 @@
         <v>43.254700999999997</v>
       </c>
       <c r="C18" s="6">
-        <v>0</v>
+        <v>47.766359999999999</v>
       </c>
       <c r="D18" s="6">
         <v>0</v>
@@ -9526,7 +9526,7 @@
         <v>429.12917499999998</v>
       </c>
       <c r="C19" s="6">
-        <v>0</v>
+        <v>428.60117700000001</v>
       </c>
       <c r="D19" s="6">
         <v>0</v>
@@ -9688,7 +9688,7 @@
         <v>1284.4908330000001</v>
       </c>
       <c r="C20" s="15">
-        <v>0</v>
+        <v>1319.8847940000001</v>
       </c>
       <c r="D20" s="15">
         <v>0</v>
@@ -9850,7 +9850,7 @@
         <v>816.26813900000002</v>
       </c>
       <c r="C21" s="6">
-        <v>0</v>
+        <v>1079.764948</v>
       </c>
       <c r="D21" s="6">
         <v>0</v>
@@ -10012,7 +10012,7 @@
         <v>4283.0029399999994</v>
       </c>
       <c r="C22" s="7">
-        <v>0</v>
+        <v>4842.135859</v>
       </c>
       <c r="D22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jan 21 05:27:02 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A0F18F-E211-41BF-9517-826821C439F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C4BCAE-48E0-45E6-ABA6-2205FC8263CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4022,7 +4022,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4430,7 +4430,7 @@
         <v>5540</v>
       </c>
       <c r="D5" s="15">
-        <v>5313</v>
+        <v>5300</v>
       </c>
       <c r="E5" s="15">
         <v>6114</v>
@@ -4591,7 +4591,7 @@
         <v>11791</v>
       </c>
       <c r="D6" s="15">
-        <v>11076</v>
+        <v>11049</v>
       </c>
       <c r="E6" s="15">
         <v>13062</v>
@@ -4752,7 +4752,7 @@
         <v>19106</v>
       </c>
       <c r="D7" s="15">
-        <v>15756</v>
+        <v>16246</v>
       </c>
       <c r="E7" s="15">
         <v>17583</v>
@@ -4913,7 +4913,7 @@
         <v>2897</v>
       </c>
       <c r="D8" s="15">
-        <v>2589</v>
+        <v>2580</v>
       </c>
       <c r="E8" s="15">
         <v>3898</v>
@@ -5074,7 +5074,7 @@
         <v>8396</v>
       </c>
       <c r="D9" s="15">
-        <v>5753</v>
+        <v>5655</v>
       </c>
       <c r="E9" s="15">
         <v>7931</v>
@@ -5235,7 +5235,7 @@
         <v>12621</v>
       </c>
       <c r="D10" s="15">
-        <v>10182</v>
+        <v>10176</v>
       </c>
       <c r="E10" s="15">
         <v>12366</v>
@@ -5396,7 +5396,7 @@
         <v>38539</v>
       </c>
       <c r="D11" s="15">
-        <v>32574</v>
+        <v>32477</v>
       </c>
       <c r="E11" s="15">
         <v>40173</v>
@@ -5557,7 +5557,7 @@
         <v>98890</v>
       </c>
       <c r="D12" s="7">
-        <v>83243</v>
+        <v>83483</v>
       </c>
       <c r="E12" s="7">
         <v>101127</v>
@@ -5778,7 +5778,7 @@
         <v>411.243494</v>
       </c>
       <c r="D15" s="15">
-        <v>396.04362099999997</v>
+        <v>395.64064100000002</v>
       </c>
       <c r="E15" s="15">
         <v>441.97207300000002</v>
@@ -5939,7 +5939,7 @@
         <v>797.01472000000001</v>
       </c>
       <c r="D16" s="15">
-        <v>782.62626299999999</v>
+        <v>782.26911800000005</v>
       </c>
       <c r="E16" s="15">
         <v>952.64041699999996</v>
@@ -6100,7 +6100,7 @@
         <v>568.96275800000001</v>
       </c>
       <c r="D17" s="15">
-        <v>403.53600899999998</v>
+        <v>402.09397100000001</v>
       </c>
       <c r="E17" s="15">
         <v>571.26219700000001</v>
@@ -6261,7 +6261,7 @@
         <v>46.863571999999998</v>
       </c>
       <c r="D18" s="15">
-        <v>39.916519999999998</v>
+        <v>39.851851000000003</v>
       </c>
       <c r="E18" s="15">
         <v>56.588912999999998</v>
@@ -6422,7 +6422,7 @@
         <v>371.12378000000001</v>
       </c>
       <c r="D19" s="15">
-        <v>230.17139</v>
+        <v>229.96909099999999</v>
       </c>
       <c r="E19" s="15">
         <v>317.27139399999999</v>
@@ -6583,7 +6583,7 @@
         <v>1226.6599679999999</v>
       </c>
       <c r="D20" s="15">
-        <v>1071.8569259999999</v>
+        <v>1070.25217</v>
       </c>
       <c r="E20" s="15">
         <v>1271.9374800000001</v>
@@ -6744,7 +6744,7 @@
         <v>885.46785799999998</v>
       </c>
       <c r="D21" s="15">
-        <v>811.52483700000005</v>
+        <v>810.51703299999997</v>
       </c>
       <c r="E21" s="15">
         <v>928.78577900000005</v>
@@ -6905,7 +6905,7 @@
         <v>4307.3361500000001</v>
       </c>
       <c r="D22" s="7">
-        <v>3735.6755659999999</v>
+        <v>3730.593875</v>
       </c>
       <c r="E22" s="7">
         <v>4540.4582529999998</v>
@@ -7114,7 +7114,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7523,7 +7523,7 @@
         <v>5872</v>
       </c>
       <c r="D5" s="15">
-        <v>0</v>
+        <v>5997</v>
       </c>
       <c r="E5" s="15">
         <v>0</v>
@@ -7685,7 +7685,7 @@
         <v>13042</v>
       </c>
       <c r="D6" s="6">
-        <v>0</v>
+        <v>12207</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
@@ -7847,7 +7847,7 @@
         <v>17769</v>
       </c>
       <c r="D7" s="6">
-        <v>0</v>
+        <v>16302</v>
       </c>
       <c r="E7" s="6">
         <v>0</v>
@@ -8009,7 +8009,7 @@
         <v>2603</v>
       </c>
       <c r="D8" s="6">
-        <v>0</v>
+        <v>3321</v>
       </c>
       <c r="E8" s="6">
         <v>0</v>
@@ -8171,7 +8171,7 @@
         <v>9423</v>
       </c>
       <c r="D9" s="6">
-        <v>0</v>
+        <v>9212</v>
       </c>
       <c r="E9" s="6">
         <v>0</v>
@@ -8333,7 +8333,7 @@
         <v>13856</v>
       </c>
       <c r="D10" s="15">
-        <v>0</v>
+        <v>14287</v>
       </c>
       <c r="E10" s="15">
         <v>0</v>
@@ -8495,7 +8495,7 @@
         <v>42824</v>
       </c>
       <c r="D11" s="6">
-        <v>0</v>
+        <v>42476</v>
       </c>
       <c r="E11" s="6">
         <v>0</v>
@@ -8657,7 +8657,7 @@
         <v>105389</v>
       </c>
       <c r="D12" s="7">
-        <v>0</v>
+        <v>103802</v>
       </c>
       <c r="E12" s="7">
         <v>0</v>
@@ -8881,7 +8881,7 @@
         <v>459.58167200000003</v>
       </c>
       <c r="D15" s="15">
-        <v>0</v>
+        <v>447.03429399999999</v>
       </c>
       <c r="E15" s="15">
         <v>0</v>
@@ -9043,7 +9043,7 @@
         <v>940.731405</v>
       </c>
       <c r="D16" s="6">
-        <v>0</v>
+        <v>819.21292900000003</v>
       </c>
       <c r="E16" s="6">
         <v>0</v>
@@ -9205,7 +9205,7 @@
         <v>565.80550300000004</v>
       </c>
       <c r="D17" s="6">
-        <v>0</v>
+        <v>547.47224900000003</v>
       </c>
       <c r="E17" s="6">
         <v>0</v>
@@ -9367,7 +9367,7 @@
         <v>47.766359999999999</v>
       </c>
       <c r="D18" s="6">
-        <v>0</v>
+        <v>50.947935999999999</v>
       </c>
       <c r="E18" s="6">
         <v>0</v>
@@ -9529,7 +9529,7 @@
         <v>428.60117700000001</v>
       </c>
       <c r="D19" s="6">
-        <v>0</v>
+        <v>457.96698199999997</v>
       </c>
       <c r="E19" s="6">
         <v>0</v>
@@ -9691,7 +9691,7 @@
         <v>1319.8847940000001</v>
       </c>
       <c r="D20" s="15">
-        <v>0</v>
+        <v>1377.5173259999999</v>
       </c>
       <c r="E20" s="15">
         <v>0</v>
@@ -9853,7 +9853,7 @@
         <v>1079.764948</v>
       </c>
       <c r="D21" s="6">
-        <v>0</v>
+        <v>1067.5123590000001</v>
       </c>
       <c r="E21" s="6">
         <v>0</v>
@@ -10015,7 +10015,7 @@
         <v>4842.135859</v>
       </c>
       <c r="D22" s="7">
-        <v>0</v>
+        <v>4767.6640750000006</v>
       </c>
       <c r="E22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jan 28 05:25:44 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C4BCAE-48E0-45E6-ABA6-2205FC8263CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FED2A6-A634-4B26-878F-5325DC296ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4022,7 +4022,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4433,7 +4433,7 @@
         <v>5300</v>
       </c>
       <c r="E5" s="15">
-        <v>6114</v>
+        <v>6112</v>
       </c>
       <c r="F5" s="15">
         <v>6109</v>
@@ -4594,7 +4594,7 @@
         <v>11049</v>
       </c>
       <c r="E6" s="15">
-        <v>13062</v>
+        <v>13019</v>
       </c>
       <c r="F6" s="15">
         <v>13258</v>
@@ -4755,7 +4755,7 @@
         <v>16246</v>
       </c>
       <c r="E7" s="15">
-        <v>17583</v>
+        <v>18033</v>
       </c>
       <c r="F7" s="15">
         <v>17485</v>
@@ -4916,7 +4916,7 @@
         <v>2580</v>
       </c>
       <c r="E8" s="15">
-        <v>3898</v>
+        <v>3894</v>
       </c>
       <c r="F8" s="15">
         <v>4019</v>
@@ -5077,7 +5077,7 @@
         <v>5655</v>
       </c>
       <c r="E9" s="15">
-        <v>7931</v>
+        <v>7932</v>
       </c>
       <c r="F9" s="15">
         <v>8966</v>
@@ -5238,7 +5238,7 @@
         <v>10176</v>
       </c>
       <c r="E10" s="15">
-        <v>12366</v>
+        <v>12348</v>
       </c>
       <c r="F10" s="15">
         <v>13940</v>
@@ -5399,7 +5399,7 @@
         <v>32477</v>
       </c>
       <c r="E11" s="15">
-        <v>40173</v>
+        <v>40049</v>
       </c>
       <c r="F11" s="15">
         <v>42165</v>
@@ -5560,7 +5560,7 @@
         <v>83483</v>
       </c>
       <c r="E12" s="7">
-        <v>101127</v>
+        <v>101387</v>
       </c>
       <c r="F12" s="7">
         <v>105942</v>
@@ -5781,7 +5781,7 @@
         <v>395.64064100000002</v>
       </c>
       <c r="E15" s="15">
-        <v>441.97207300000002</v>
+        <v>441.34100899999999</v>
       </c>
       <c r="F15" s="15">
         <v>437.040007</v>
@@ -5942,7 +5942,7 @@
         <v>782.26911800000005</v>
       </c>
       <c r="E16" s="15">
-        <v>952.64041699999996</v>
+        <v>952.18820300000004</v>
       </c>
       <c r="F16" s="15">
         <v>964.13352899999995</v>
@@ -6103,7 +6103,7 @@
         <v>402.09397100000001</v>
       </c>
       <c r="E17" s="15">
-        <v>571.26219700000001</v>
+        <v>548.17622900000003</v>
       </c>
       <c r="F17" s="15">
         <v>577.42893400000003</v>
@@ -6264,7 +6264,7 @@
         <v>39.851851000000003</v>
       </c>
       <c r="E18" s="15">
-        <v>56.588912999999998</v>
+        <v>56.533883000000003</v>
       </c>
       <c r="F18" s="15">
         <v>56.952452999999998</v>
@@ -6425,7 +6425,7 @@
         <v>229.96909099999999</v>
       </c>
       <c r="E19" s="15">
-        <v>317.27139399999999</v>
+        <v>317.2758</v>
       </c>
       <c r="F19" s="15">
         <v>379.321258</v>
@@ -6586,7 +6586,7 @@
         <v>1070.25217</v>
       </c>
       <c r="E20" s="15">
-        <v>1271.9374800000001</v>
+        <v>1271.499867</v>
       </c>
       <c r="F20" s="15">
         <v>1404.405921</v>
@@ -6747,7 +6747,7 @@
         <v>810.51703299999997</v>
       </c>
       <c r="E21" s="15">
-        <v>928.78577900000005</v>
+        <v>927.77234299999998</v>
       </c>
       <c r="F21" s="15">
         <v>1020.4252310000001</v>
@@ -6908,7 +6908,7 @@
         <v>3730.593875</v>
       </c>
       <c r="E22" s="7">
-        <v>4540.4582529999998</v>
+        <v>4514.7873339999996</v>
       </c>
       <c r="F22" s="7">
         <v>4839.7073330000003</v>
@@ -7114,7 +7114,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="J36" sqref="J36"/>
+      <selection pane="bottomRight" activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7526,7 +7526,7 @@
         <v>5997</v>
       </c>
       <c r="E5" s="15">
-        <v>0</v>
+        <v>5731</v>
       </c>
       <c r="F5" s="15">
         <v>0</v>
@@ -7688,7 +7688,7 @@
         <v>12207</v>
       </c>
       <c r="E6" s="6">
-        <v>0</v>
+        <v>12660</v>
       </c>
       <c r="F6" s="6">
         <v>0</v>
@@ -7850,7 +7850,7 @@
         <v>16302</v>
       </c>
       <c r="E7" s="6">
-        <v>0</v>
+        <v>16727</v>
       </c>
       <c r="F7" s="6">
         <v>0</v>
@@ -8012,7 +8012,7 @@
         <v>3321</v>
       </c>
       <c r="E8" s="6">
-        <v>0</v>
+        <v>3696</v>
       </c>
       <c r="F8" s="6">
         <v>0</v>
@@ -8174,7 +8174,7 @@
         <v>9212</v>
       </c>
       <c r="E9" s="6">
-        <v>0</v>
+        <v>9218</v>
       </c>
       <c r="F9" s="6">
         <v>0</v>
@@ -8336,7 +8336,7 @@
         <v>14287</v>
       </c>
       <c r="E10" s="15">
-        <v>0</v>
+        <v>13941</v>
       </c>
       <c r="F10" s="15">
         <v>0</v>
@@ -8498,7 +8498,7 @@
         <v>42476</v>
       </c>
       <c r="E11" s="6">
-        <v>0</v>
+        <v>38642</v>
       </c>
       <c r="F11" s="6">
         <v>0</v>
@@ -8660,7 +8660,7 @@
         <v>103802</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
+        <v>100615</v>
       </c>
       <c r="F12" s="7">
         <v>0</v>
@@ -8884,7 +8884,7 @@
         <v>447.03429399999999</v>
       </c>
       <c r="E15" s="15">
-        <v>0</v>
+        <v>422.88258300000001</v>
       </c>
       <c r="F15" s="15">
         <v>0</v>
@@ -9046,7 +9046,7 @@
         <v>819.21292900000003</v>
       </c>
       <c r="E16" s="6">
-        <v>0</v>
+        <v>947.74714100000006</v>
       </c>
       <c r="F16" s="6">
         <v>0</v>
@@ -9208,7 +9208,7 @@
         <v>547.47224900000003</v>
       </c>
       <c r="E17" s="6">
-        <v>0</v>
+        <v>484.21945799999997</v>
       </c>
       <c r="F17" s="6">
         <v>0</v>
@@ -9370,7 +9370,7 @@
         <v>50.947935999999999</v>
       </c>
       <c r="E18" s="6">
-        <v>0</v>
+        <v>56.739410999999997</v>
       </c>
       <c r="F18" s="6">
         <v>0</v>
@@ -9532,7 +9532,7 @@
         <v>457.96698199999997</v>
       </c>
       <c r="E19" s="6">
-        <v>0</v>
+        <v>418.39605499999999</v>
       </c>
       <c r="F19" s="6">
         <v>0</v>
@@ -9694,7 +9694,7 @@
         <v>1377.5173259999999</v>
       </c>
       <c r="E20" s="15">
-        <v>0</v>
+        <v>1450.5708320000001</v>
       </c>
       <c r="F20" s="15">
         <v>0</v>
@@ -9856,7 +9856,7 @@
         <v>1067.5123590000001</v>
       </c>
       <c r="E21" s="6">
-        <v>0</v>
+        <v>920.97551599999997</v>
       </c>
       <c r="F21" s="6">
         <v>0</v>
@@ -10018,7 +10018,7 @@
         <v>4767.6640750000006</v>
       </c>
       <c r="E22" s="7">
-        <v>0</v>
+        <v>4701.5309959999995</v>
       </c>
       <c r="F22" s="7">
         <v>0</v>

</xml_diff>